<commit_message>
Ajuste al reporte de estatus
</commit_message>
<xml_diff>
--- a/00-Documentacion/Listado de reportes totales-TI.xlsx
+++ b/00-Documentacion/Listado de reportes totales-TI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8EF6633-9708-4567-B89F-DDB9A79608D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{166363D8-6128-4048-8092-B855F576FCFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1498AA1A-1ACC-4329-A050-ACA05131B658}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{1498AA1A-1ACC-4329-A050-ACA05131B658}"/>
   </bookViews>
   <sheets>
     <sheet name="General - Analisis" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13094" uniqueCount="1788">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13098" uniqueCount="1792">
   <si>
     <t xml:space="preserve">Reporte </t>
   </si>
@@ -5418,6 +5418,18 @@
   </si>
   <si>
     <t>Complejidad</t>
+  </si>
+  <si>
+    <t>Terminado , por validar</t>
+  </si>
+  <si>
+    <t>detenido</t>
+  </si>
+  <si>
+    <t>En desarrollo</t>
+  </si>
+  <si>
+    <t>Pendiente</t>
   </si>
 </sst>
 </file>
@@ -5532,7 +5544,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5596,6 +5608,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5666,7 +5684,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5754,7 +5772,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -5776,6 +5793,8 @@
     <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6092,7 +6111,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB9B04FF-17D8-4BD0-8305-46A7C5B17D5A}">
   <dimension ref="A1:R1347"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -6183,7 +6202,7 @@
       <c r="C2" s="9" t="s">
         <v>1243</v>
       </c>
-      <c r="D2" s="46" t="s">
+      <c r="D2" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="9" t="s">
@@ -6625,7 +6644,7 @@
       <c r="C14" s="9" t="s">
         <v>1238</v>
       </c>
-      <c r="D14" s="46" t="s">
+      <c r="D14" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E14" s="9" t="s">
@@ -6835,7 +6854,7 @@
       <c r="C19" s="5" t="s">
         <v>1134</v>
       </c>
-      <c r="D19" s="47" t="s">
+      <c r="D19" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E19" s="5" t="s">
@@ -6871,7 +6890,7 @@
       <c r="C20" s="5" t="s">
         <v>1266</v>
       </c>
-      <c r="D20" s="47" t="s">
+      <c r="D20" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E20" s="5" t="s">
@@ -6907,7 +6926,7 @@
       <c r="C21" s="9" t="s">
         <v>1267</v>
       </c>
-      <c r="D21" s="46" t="s">
+      <c r="D21" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E21" s="5" t="s">
@@ -7013,7 +7032,7 @@
       <c r="C24" s="5" t="s">
         <v>1322</v>
       </c>
-      <c r="D24" s="46" t="s">
+      <c r="D24" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E24" s="5" t="s">
@@ -7049,7 +7068,7 @@
       <c r="C25" s="5" t="s">
         <v>1135</v>
       </c>
-      <c r="D25" s="47" t="s">
+      <c r="D25" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E25" s="5" t="s">
@@ -7085,7 +7104,7 @@
       <c r="C26" s="5" t="s">
         <v>1323</v>
       </c>
-      <c r="D26" s="47" t="s">
+      <c r="D26" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E26" s="5" t="s">
@@ -7121,7 +7140,7 @@
       <c r="C27" s="5" t="s">
         <v>1212</v>
       </c>
-      <c r="D27" s="47" t="s">
+      <c r="D27" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E27" s="5" t="s">
@@ -12221,7 +12240,7 @@
       <c r="C153" s="9" t="s">
         <v>1268</v>
       </c>
-      <c r="D153" s="46" t="s">
+      <c r="D153" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E153" s="9" t="s">
@@ -14347,7 +14366,7 @@
       <c r="C212" s="9" t="s">
         <v>1293</v>
       </c>
-      <c r="D212" s="46" t="s">
+      <c r="D212" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E212" s="5" t="s">
@@ -14383,7 +14402,7 @@
       <c r="C213" s="5" t="s">
         <v>1103</v>
       </c>
-      <c r="D213" s="46" t="s">
+      <c r="D213" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E213" s="5" t="s">
@@ -14415,7 +14434,7 @@
       <c r="C214" s="9" t="s">
         <v>1309</v>
       </c>
-      <c r="D214" s="46" t="s">
+      <c r="D214" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E214" s="9" t="s">
@@ -14451,7 +14470,7 @@
       <c r="C215" s="9" t="s">
         <v>1256</v>
       </c>
-      <c r="D215" s="46" t="s">
+      <c r="D215" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E215" s="9" t="s">
@@ -14487,7 +14506,7 @@
       <c r="C216" s="9" t="s">
         <v>1244</v>
       </c>
-      <c r="D216" s="46" t="s">
+      <c r="D216" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E216" s="9" t="s">
@@ -14523,7 +14542,7 @@
       <c r="C217" s="5" t="s">
         <v>1102</v>
       </c>
-      <c r="D217" s="46" t="s">
+      <c r="D217" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E217" s="5" t="s">
@@ -14559,7 +14578,7 @@
       <c r="C218" s="5" t="s">
         <v>1310</v>
       </c>
-      <c r="D218" s="47" t="s">
+      <c r="D218" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E218" s="5" t="s">
@@ -14595,7 +14614,7 @@
       <c r="C219" s="5" t="s">
         <v>1242</v>
       </c>
-      <c r="D219" s="47" t="s">
+      <c r="D219" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E219" s="5" t="s">
@@ -14631,7 +14650,7 @@
       <c r="C220" s="5" t="s">
         <v>1240</v>
       </c>
-      <c r="D220" s="47" t="s">
+      <c r="D220" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E220" s="5" t="s">
@@ -14667,7 +14686,7 @@
       <c r="C221" s="5" t="s">
         <v>1241</v>
       </c>
-      <c r="D221" s="47" t="s">
+      <c r="D221" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E221" s="5" t="s">
@@ -14775,7 +14794,7 @@
       <c r="C224" s="5" t="s">
         <v>1320</v>
       </c>
-      <c r="D224" s="47" t="s">
+      <c r="D224" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E224" s="5" t="s">
@@ -15277,7 +15296,7 @@
       <c r="C238" s="5" t="s">
         <v>1318</v>
       </c>
-      <c r="D238" s="47" t="s">
+      <c r="D238" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E238" s="5" t="s">
@@ -15313,7 +15332,7 @@
       <c r="C239" s="5" t="s">
         <v>1311</v>
       </c>
-      <c r="D239" s="47" t="s">
+      <c r="D239" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E239" s="5" t="s">
@@ -15385,7 +15404,7 @@
       <c r="C241" s="5" t="s">
         <v>1237</v>
       </c>
-      <c r="D241" s="47" t="s">
+      <c r="D241" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E241" s="5" t="s">
@@ -16069,7 +16088,7 @@
       <c r="C260" s="5" t="s">
         <v>1258</v>
       </c>
-      <c r="D260" s="47" t="s">
+      <c r="D260" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E260" s="5" t="s">
@@ -17399,7 +17418,7 @@
       <c r="C294" s="5" t="s">
         <v>1239</v>
       </c>
-      <c r="D294" s="47" t="s">
+      <c r="D294" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E294" s="5" t="s">
@@ -17467,7 +17486,7 @@
       <c r="C296" s="5" t="s">
         <v>1298</v>
       </c>
-      <c r="D296" s="47" t="s">
+      <c r="D296" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E296" s="5" t="s">
@@ -17539,7 +17558,7 @@
       <c r="C298" s="5" t="s">
         <v>1104</v>
       </c>
-      <c r="D298" s="47" t="s">
+      <c r="D298" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E298" s="5" t="s">
@@ -17575,7 +17594,7 @@
       <c r="C299" s="5" t="s">
         <v>1105</v>
       </c>
-      <c r="D299" s="47" t="s">
+      <c r="D299" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E299" s="5" t="s">
@@ -17791,7 +17810,7 @@
       <c r="C305" s="5" t="s">
         <v>1110</v>
       </c>
-      <c r="D305" s="47" t="s">
+      <c r="D305" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E305" s="5" t="s">
@@ -17835,7 +17854,7 @@
       <c r="C306" s="5" t="s">
         <v>1111</v>
       </c>
-      <c r="D306" s="47" t="s">
+      <c r="D306" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E306" s="5" t="s">
@@ -20111,7 +20130,7 @@
       <c r="C365" s="5" t="s">
         <v>1273</v>
       </c>
-      <c r="D365" s="47" t="s">
+      <c r="D365" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E365" s="5" t="s">
@@ -20153,7 +20172,7 @@
       <c r="C366" s="5" t="s">
         <v>1141</v>
       </c>
-      <c r="D366" s="47" t="s">
+      <c r="D366" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E366" s="5" t="s">
@@ -20195,7 +20214,7 @@
       <c r="C367" s="5" t="s">
         <v>1142</v>
       </c>
-      <c r="D367" s="47" t="s">
+      <c r="D367" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E367" s="5" t="s">
@@ -20347,7 +20366,7 @@
       <c r="C371" s="5" t="s">
         <v>1146</v>
       </c>
-      <c r="D371" s="47" t="s">
+      <c r="D371" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E371" s="5" t="s">
@@ -20571,7 +20590,7 @@
       <c r="C377" s="5" t="s">
         <v>1275</v>
       </c>
-      <c r="D377" s="47" t="s">
+      <c r="D377" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E377" s="5" t="s">
@@ -20651,7 +20670,7 @@
       <c r="C379" s="9" t="s">
         <v>1114</v>
       </c>
-      <c r="D379" s="47" t="s">
+      <c r="D379" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E379" s="5" t="s">
@@ -20687,7 +20706,7 @@
       <c r="C380" s="5" t="s">
         <v>1281</v>
       </c>
-      <c r="D380" s="47" t="s">
+      <c r="D380" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E380" s="5" t="s">
@@ -20765,7 +20784,7 @@
       <c r="C382" s="5" t="s">
         <v>1116</v>
       </c>
-      <c r="D382" s="47" t="s">
+      <c r="D382" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E382" s="5" t="s">
@@ -20887,7 +20906,7 @@
       <c r="C385" s="5" t="s">
         <v>1136</v>
       </c>
-      <c r="D385" s="47" t="s">
+      <c r="D385" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E385" s="5" t="s">
@@ -21319,7 +21338,7 @@
       <c r="C397" s="5" t="s">
         <v>1117</v>
       </c>
-      <c r="D397" s="47" t="s">
+      <c r="D397" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E397" s="5" t="s">
@@ -21509,7 +21528,7 @@
       <c r="C402" s="5" t="s">
         <v>1139</v>
       </c>
-      <c r="D402" s="47" t="s">
+      <c r="D402" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E402" s="5" t="s">
@@ -21589,7 +21608,7 @@
       <c r="C404" s="5" t="s">
         <v>1265</v>
       </c>
-      <c r="D404" s="47" t="s">
+      <c r="D404" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E404" s="5" t="s">
@@ -21967,7 +21986,7 @@
       <c r="C414" s="5" t="s">
         <v>1328</v>
       </c>
-      <c r="D414" s="47" t="s">
+      <c r="D414" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E414" s="5" t="s">
@@ -21997,7 +22016,7 @@
       <c r="C415" s="5" t="s">
         <v>1119</v>
       </c>
-      <c r="D415" s="47" t="s">
+      <c r="D415" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E415" s="5" t="s">
@@ -22075,7 +22094,7 @@
       <c r="C417" s="5" t="s">
         <v>1149</v>
       </c>
-      <c r="D417" s="47" t="s">
+      <c r="D417" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E417" s="5" t="s">
@@ -22337,7 +22356,7 @@
       <c r="C424" s="5" t="s">
         <v>1120</v>
       </c>
-      <c r="D424" s="47" t="s">
+      <c r="D424" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E424" s="5" t="s">
@@ -22371,7 +22390,7 @@
       <c r="C425" s="5" t="s">
         <v>1121</v>
       </c>
-      <c r="D425" s="47" t="s">
+      <c r="D425" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E425" s="5" t="s">
@@ -22405,7 +22424,7 @@
       <c r="C426" s="5" t="s">
         <v>1276</v>
       </c>
-      <c r="D426" s="47" t="s">
+      <c r="D426" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E426" s="5" t="s">
@@ -22891,7 +22910,7 @@
       <c r="C439" s="5" t="s">
         <v>1155</v>
       </c>
-      <c r="D439" s="47" t="s">
+      <c r="D439" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E439" s="5" t="s">
@@ -22925,7 +22944,7 @@
       <c r="C440" s="5" t="s">
         <v>1138</v>
       </c>
-      <c r="D440" s="47" t="s">
+      <c r="D440" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E440" s="5" t="s">
@@ -23071,7 +23090,7 @@
       <c r="C444" s="5" t="s">
         <v>1277</v>
       </c>
-      <c r="D444" s="47" t="s">
+      <c r="D444" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E444" s="5" t="s">
@@ -23149,7 +23168,7 @@
       <c r="C446" s="5" t="s">
         <v>1306</v>
       </c>
-      <c r="D446" s="47" t="s">
+      <c r="D446" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E446" s="5" t="s">
@@ -39579,7 +39598,7 @@
       <c r="C836" s="5" t="s">
         <v>1124</v>
       </c>
-      <c r="D836" s="47" t="s">
+      <c r="D836" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E836" s="5" t="s">
@@ -39879,7 +39898,7 @@
       <c r="C844" s="5" t="s">
         <v>1160</v>
       </c>
-      <c r="D844" s="47" t="s">
+      <c r="D844" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E844" s="5" t="s">
@@ -40063,7 +40082,7 @@
       <c r="C849" s="5" t="s">
         <v>1317</v>
       </c>
-      <c r="D849" s="47" t="s">
+      <c r="D849" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E849" s="5" t="s">
@@ -40211,7 +40230,7 @@
       <c r="C853" s="9" t="s">
         <v>1156</v>
       </c>
-      <c r="D853" s="47" t="s">
+      <c r="D853" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E853" s="5" t="s">
@@ -40253,7 +40272,7 @@
       <c r="C854" s="5" t="s">
         <v>1233</v>
       </c>
-      <c r="D854" s="47" t="s">
+      <c r="D854" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E854" s="5" t="s">
@@ -40331,7 +40350,7 @@
       <c r="C856" s="5" t="s">
         <v>1163</v>
       </c>
-      <c r="D856" s="47" t="s">
+      <c r="D856" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E856" s="5" t="s">
@@ -40367,7 +40386,7 @@
       <c r="C857" s="9" t="s">
         <v>1165</v>
       </c>
-      <c r="D857" s="46" t="s">
+      <c r="D857" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E857" s="9" t="s">
@@ -40999,7 +41018,7 @@
       <c r="C873" s="9" t="s">
         <v>1123</v>
       </c>
-      <c r="D873" s="46" t="s">
+      <c r="D873" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E873" s="9" t="s">
@@ -41681,7 +41700,7 @@
       <c r="C892" s="9" t="s">
         <v>1126</v>
       </c>
-      <c r="D892" s="46" t="s">
+      <c r="D892" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E892" s="9" t="s">
@@ -41715,7 +41734,7 @@
       <c r="C893" s="9" t="s">
         <v>1232</v>
       </c>
-      <c r="D893" s="46" t="s">
+      <c r="D893" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E893" s="9" t="s">
@@ -41749,7 +41768,7 @@
       <c r="C894" s="9" t="s">
         <v>1234</v>
       </c>
-      <c r="D894" s="46" t="s">
+      <c r="D894" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E894" s="9" t="s">
@@ -41783,7 +41802,7 @@
       <c r="C895" s="9" t="s">
         <v>1164</v>
       </c>
-      <c r="D895" s="46" t="s">
+      <c r="D895" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E895" s="9" t="s">
@@ -41991,7 +42010,7 @@
       <c r="C900" s="9" t="s">
         <v>1115</v>
       </c>
-      <c r="D900" s="46" t="s">
+      <c r="D900" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E900" s="9" t="s">
@@ -42143,7 +42162,7 @@
       <c r="C904" s="5" t="s">
         <v>1222</v>
       </c>
-      <c r="D904" s="47" t="s">
+      <c r="D904" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E904" s="5" t="s">
@@ -42183,7 +42202,7 @@
       <c r="C905" s="5" t="s">
         <v>1127</v>
       </c>
-      <c r="D905" s="47" t="s">
+      <c r="D905" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E905" s="5" t="s">
@@ -42775,7 +42794,7 @@
       <c r="C921" s="5" t="s">
         <v>1169</v>
       </c>
-      <c r="D921" s="47" t="s">
+      <c r="D921" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E921" s="5" t="s">
@@ -42819,7 +42838,7 @@
       <c r="C922" s="5" t="s">
         <v>1170</v>
       </c>
-      <c r="D922" s="47" t="s">
+      <c r="D922" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E922" s="5" t="s">
@@ -42923,7 +42942,7 @@
       <c r="C925" s="5" t="s">
         <v>1132</v>
       </c>
-      <c r="D925" s="47" t="s">
+      <c r="D925" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E925" s="5" t="s">
@@ -43071,7 +43090,7 @@
       <c r="C929" s="5" t="s">
         <v>1171</v>
       </c>
-      <c r="D929" s="47" t="s">
+      <c r="D929" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E929" s="5" t="s">
@@ -43293,7 +43312,7 @@
       <c r="C935" s="5" t="s">
         <v>1172</v>
       </c>
-      <c r="D935" s="47" t="s">
+      <c r="D935" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E935" s="5" t="s">
@@ -43327,7 +43346,7 @@
       <c r="C936" s="9" t="s">
         <v>1173</v>
       </c>
-      <c r="D936" s="46" t="s">
+      <c r="D936" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E936" s="9" t="s">
@@ -43557,7 +43576,7 @@
       <c r="C942" s="5" t="s">
         <v>1185</v>
       </c>
-      <c r="D942" s="47" t="s">
+      <c r="D942" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E942" s="5" t="s">
@@ -43701,7 +43720,7 @@
       <c r="C946" s="5" t="s">
         <v>1274</v>
       </c>
-      <c r="D946" s="47" t="s">
+      <c r="D946" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E946" s="5" t="s">
@@ -43931,7 +43950,7 @@
       <c r="C952" s="5" t="s">
         <v>1230</v>
       </c>
-      <c r="D952" s="47" t="s">
+      <c r="D952" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E952" s="5" t="s">
@@ -51635,7 +51654,7 @@
       <c r="C1137" s="10" t="s">
         <v>1178</v>
       </c>
-      <c r="D1137" s="48" t="s">
+      <c r="D1137" s="47" t="s">
         <v>4</v>
       </c>
       <c r="E1137" s="10" t="s">
@@ -51669,7 +51688,7 @@
       <c r="C1138" s="10" t="s">
         <v>1133</v>
       </c>
-      <c r="D1138" s="48" t="s">
+      <c r="D1138" s="47" t="s">
         <v>4</v>
       </c>
       <c r="E1138" s="10" t="s">
@@ -51775,7 +51794,7 @@
       <c r="C1141" s="10" t="s">
         <v>1179</v>
       </c>
-      <c r="D1141" s="48" t="s">
+      <c r="D1141" s="47" t="s">
         <v>4</v>
       </c>
       <c r="E1141" s="10" t="s">
@@ -51879,7 +51898,7 @@
       <c r="C1144" s="10" t="s">
         <v>1148</v>
       </c>
-      <c r="D1144" s="48" t="s">
+      <c r="D1144" s="47" t="s">
         <v>5</v>
       </c>
       <c r="E1144" s="10" t="s">
@@ -52019,7 +52038,7 @@
       <c r="C1148" s="10" t="s">
         <v>1223</v>
       </c>
-      <c r="D1148" s="48" t="s">
+      <c r="D1148" s="47" t="s">
         <v>4</v>
       </c>
       <c r="E1148" s="10" t="s">
@@ -52059,7 +52078,7 @@
       <c r="C1149" s="8" t="s">
         <v>1250</v>
       </c>
-      <c r="D1149" s="46" t="s">
+      <c r="D1149" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E1149" s="10" t="s">
@@ -52435,7 +52454,7 @@
       <c r="C1159" s="10" t="s">
         <v>1193</v>
       </c>
-      <c r="D1159" s="48" t="s">
+      <c r="D1159" s="47" t="s">
         <v>4</v>
       </c>
       <c r="E1159" s="10" t="s">
@@ -52475,7 +52494,7 @@
       <c r="C1160" s="10" t="s">
         <v>1255</v>
       </c>
-      <c r="D1160" s="48" t="s">
+      <c r="D1160" s="47" t="s">
         <v>4</v>
       </c>
       <c r="E1160" s="10" t="s">
@@ -52511,7 +52530,7 @@
       <c r="C1161" s="8" t="s">
         <v>1188</v>
       </c>
-      <c r="D1161" s="46" t="s">
+      <c r="D1161" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E1161" s="10" t="s">
@@ -52547,7 +52566,7 @@
       <c r="C1162" s="8" t="s">
         <v>1191</v>
       </c>
-      <c r="D1162" s="46" t="s">
+      <c r="D1162" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E1162" s="10" t="s">
@@ -52589,7 +52608,7 @@
       <c r="C1163" s="10" t="s">
         <v>1189</v>
       </c>
-      <c r="D1163" s="48" t="s">
+      <c r="D1163" s="47" t="s">
         <v>4</v>
       </c>
       <c r="E1163" s="10" t="s">
@@ -52625,7 +52644,7 @@
       <c r="C1164" s="8" t="s">
         <v>1247</v>
       </c>
-      <c r="D1164" s="46" t="s">
+      <c r="D1164" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E1164" s="8" t="s">
@@ -52659,7 +52678,7 @@
       <c r="C1165" s="8" t="s">
         <v>1254</v>
       </c>
-      <c r="D1165" s="46" t="s">
+      <c r="D1165" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E1165" s="8" t="s">
@@ -52697,7 +52716,7 @@
       <c r="C1166" s="8" t="s">
         <v>1192</v>
       </c>
-      <c r="D1166" s="46" t="s">
+      <c r="D1166" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E1166" s="8" t="s">
@@ -52733,7 +52752,7 @@
       <c r="C1167" s="8" t="s">
         <v>1194</v>
       </c>
-      <c r="D1167" s="46" t="s">
+      <c r="D1167" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E1167" s="8" t="s">
@@ -52777,7 +52796,7 @@
       <c r="C1168" s="8" t="s">
         <v>1195</v>
       </c>
-      <c r="D1168" s="45" t="s">
+      <c r="D1168" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E1168" s="8" t="s">
@@ -52819,7 +52838,7 @@
       <c r="C1169" s="8" t="s">
         <v>1129</v>
       </c>
-      <c r="D1169" s="45" t="s">
+      <c r="D1169" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E1169" s="8" t="s">
@@ -52853,7 +52872,7 @@
       <c r="C1170" s="8" t="s">
         <v>1130</v>
       </c>
-      <c r="D1170" s="48" t="s">
+      <c r="D1170" s="47" t="s">
         <v>4</v>
       </c>
       <c r="E1170" s="10" t="s">
@@ -53383,7 +53402,7 @@
       <c r="C1184" s="10" t="s">
         <v>1128</v>
       </c>
-      <c r="D1184" s="48" t="s">
+      <c r="D1184" s="47" t="s">
         <v>4</v>
       </c>
       <c r="E1184" s="10" t="s">
@@ -53547,7 +53566,7 @@
       <c r="C1188" s="10" t="s">
         <v>1131</v>
       </c>
-      <c r="D1188" s="48" t="s">
+      <c r="D1188" s="47" t="s">
         <v>4</v>
       </c>
       <c r="E1188" s="10" t="s">
@@ -53581,7 +53600,7 @@
       <c r="C1189" s="10" t="s">
         <v>1252</v>
       </c>
-      <c r="D1189" s="48" t="s">
+      <c r="D1189" s="47" t="s">
         <v>4</v>
       </c>
       <c r="E1189" s="10" t="s">
@@ -53615,7 +53634,7 @@
       <c r="C1190" s="8" t="s">
         <v>1245</v>
       </c>
-      <c r="D1190" s="45" t="s">
+      <c r="D1190" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E1190" s="10" t="s">
@@ -53825,7 +53844,7 @@
       <c r="C1196" s="8" t="s">
         <v>1197</v>
       </c>
-      <c r="D1196" s="45" t="s">
+      <c r="D1196" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E1196" s="8" t="s">
@@ -53965,7 +53984,7 @@
       <c r="C1200" s="8" t="s">
         <v>1209</v>
       </c>
-      <c r="D1200" s="46" t="s">
+      <c r="D1200" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E1200" s="8" t="s">
@@ -54071,7 +54090,7 @@
       <c r="C1203" s="8" t="s">
         <v>1283</v>
       </c>
-      <c r="D1203" s="48" t="s">
+      <c r="D1203" s="47" t="s">
         <v>4</v>
       </c>
       <c r="E1203" s="10" t="s">
@@ -54113,7 +54132,7 @@
       <c r="C1204" s="10" t="s">
         <v>1326</v>
       </c>
-      <c r="D1204" s="48" t="s">
+      <c r="D1204" s="47" t="s">
         <v>4</v>
       </c>
       <c r="E1204" s="10" t="s">
@@ -54147,7 +54166,7 @@
       <c r="C1205" s="8" t="s">
         <v>1198</v>
       </c>
-      <c r="D1205" s="45" t="s">
+      <c r="D1205" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E1205" s="8" t="s">
@@ -54187,7 +54206,7 @@
       <c r="C1206" s="8" t="s">
         <v>1296</v>
       </c>
-      <c r="D1206" s="45" t="s">
+      <c r="D1206" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E1206" s="8" t="s">
@@ -55131,7 +55150,7 @@
       <c r="C1229" s="10" t="s">
         <v>1202</v>
       </c>
-      <c r="D1229" s="48" t="s">
+      <c r="D1229" s="47" t="s">
         <v>4</v>
       </c>
       <c r="E1229" s="10" t="s">
@@ -55167,7 +55186,7 @@
       <c r="C1230" s="10" t="s">
         <v>1207</v>
       </c>
-      <c r="D1230" s="48" t="s">
+      <c r="D1230" s="47" t="s">
         <v>4</v>
       </c>
       <c r="E1230" s="10" t="s">
@@ -56225,7 +56244,7 @@
       <c r="C1254" s="10" t="s">
         <v>1203</v>
       </c>
-      <c r="D1254" s="48" t="s">
+      <c r="D1254" s="47" t="s">
         <v>4</v>
       </c>
       <c r="E1254" s="10" t="s">
@@ -57681,7 +57700,7 @@
       <c r="C1292" s="8" t="s">
         <v>1231</v>
       </c>
-      <c r="D1292" s="45" t="s">
+      <c r="D1292" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E1292" s="8" t="s">
@@ -57939,7 +57958,7 @@
       <c r="C1299" s="10" t="s">
         <v>1327</v>
       </c>
-      <c r="D1299" s="48" t="s">
+      <c r="D1299" s="47" t="s">
         <v>4</v>
       </c>
       <c r="E1299" s="10" t="s">
@@ -59239,7 +59258,7 @@
       <c r="C1333" s="10" t="s">
         <v>1257</v>
       </c>
-      <c r="D1333" s="45" t="s">
+      <c r="D1333" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E1333" s="10" t="s">
@@ -59275,7 +59294,7 @@
       <c r="C1334" s="10" t="s">
         <v>1280</v>
       </c>
-      <c r="D1334" s="45" t="s">
+      <c r="D1334" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E1334" s="10" t="s">
@@ -59351,7 +59370,7 @@
       <c r="C1336" s="8" t="s">
         <v>1200</v>
       </c>
-      <c r="D1336" s="45" t="s">
+      <c r="D1336" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E1336" s="8" t="s">
@@ -59387,7 +59406,7 @@
       <c r="C1337" s="8" t="s">
         <v>1201</v>
       </c>
-      <c r="D1337" s="45" t="s">
+      <c r="D1337" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E1337" s="8" t="s">
@@ -59423,7 +59442,7 @@
       <c r="C1338" s="8" t="s">
         <v>1294</v>
       </c>
-      <c r="D1338" s="45" t="s">
+      <c r="D1338" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E1338" s="8" t="s">
@@ -59798,7 +59817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF9BE15D-6351-44F9-8E43-517339B371DC}">
   <dimension ref="A1:R124"/>
   <sheetViews>
-    <sheetView topLeftCell="A120" workbookViewId="0">
+    <sheetView topLeftCell="A39" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:R124"/>
     </sheetView>
   </sheetViews>
@@ -59882,13 +59901,13 @@
       <c r="A2" s="9">
         <v>1</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="36" t="s">
         <v>1428</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>1243</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="9" t="s">
@@ -59922,10 +59941,10 @@
       <c r="C3" s="5" t="s">
         <v>554</v>
       </c>
-      <c r="D3" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="38" t="s">
+      <c r="D3" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="37" t="s">
         <v>1096</v>
       </c>
       <c r="F3" s="5"/>
@@ -59958,10 +59977,10 @@
       <c r="C4" s="5" t="s">
         <v>554</v>
       </c>
-      <c r="D4" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="38" t="s">
+      <c r="D4" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="37" t="s">
         <v>1096</v>
       </c>
       <c r="F4" s="5"/>
@@ -59988,16 +60007,16 @@
       <c r="A5" s="9">
         <v>2</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="36" t="s">
         <v>1420</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>554</v>
       </c>
-      <c r="D5" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="38" t="s">
+      <c r="D5" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="37" t="s">
         <v>1074</v>
       </c>
       <c r="F5" s="9"/>
@@ -60028,7 +60047,7 @@
       <c r="C6" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E6" s="5" t="s">
@@ -60066,7 +60085,7 @@
       <c r="C7" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E7" s="5" t="s">
@@ -60104,7 +60123,7 @@
       <c r="C8" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E8" s="5" t="s">
@@ -60142,7 +60161,7 @@
       <c r="C9" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="D9" s="35" t="s">
+      <c r="D9" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E9" s="5" t="s">
@@ -60180,7 +60199,7 @@
       <c r="C10" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="D10" s="35" t="s">
+      <c r="D10" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E10" s="5" t="s">
@@ -60212,16 +60231,16 @@
       <c r="A11" s="9">
         <v>4</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="36" t="s">
         <v>1415</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>1238</v>
       </c>
-      <c r="D11" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" s="37" t="s">
+      <c r="D11" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="36" t="s">
         <v>1732</v>
       </c>
       <c r="F11" s="9"/>
@@ -60245,19 +60264,19 @@
       <c r="R11" s="8"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="39">
+      <c r="A12" s="38">
         <v>6</v>
       </c>
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="36" t="s">
         <v>1615</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>1134</v>
       </c>
-      <c r="D12" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12" s="37" t="s">
+      <c r="D12" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="36" t="s">
         <v>1681</v>
       </c>
       <c r="F12" s="9"/>
@@ -60284,13 +60303,13 @@
       <c r="A13" s="9">
         <v>7</v>
       </c>
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="36" t="s">
         <v>1521</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>1266</v>
       </c>
-      <c r="D13" s="35" t="s">
+      <c r="D13" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E13" t="s">
@@ -60320,13 +60339,13 @@
       <c r="A14" s="9">
         <v>8</v>
       </c>
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="36" t="s">
         <v>1524</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>1267</v>
       </c>
-      <c r="D14" s="35" t="s">
+      <c r="D14" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E14" t="s">
@@ -60353,16 +60372,16 @@
       <c r="R14" s="8"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="39">
+      <c r="A15" s="38">
         <v>10</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="36" t="s">
         <v>1653</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>1322</v>
       </c>
-      <c r="D15" s="35" t="s">
+      <c r="D15" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E15" s="9" t="s">
@@ -60389,16 +60408,16 @@
       <c r="R15" s="8"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="39">
+      <c r="A16" s="38">
         <v>11</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="36" t="s">
         <v>1617</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>1135</v>
       </c>
-      <c r="D16" s="35" t="s">
+      <c r="D16" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E16" s="9" t="s">
@@ -60425,16 +60444,16 @@
       <c r="R16" s="8"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="39">
+      <c r="A17" s="38">
         <v>12</v>
       </c>
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="36" t="s">
         <v>1654</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>1323</v>
       </c>
-      <c r="D17" s="35" t="s">
+      <c r="D17" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E17" s="9" t="s">
@@ -60464,13 +60483,13 @@
       <c r="A18" s="9">
         <v>13</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="36" t="s">
         <v>1343</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>1212</v>
       </c>
-      <c r="D18" s="35" t="s">
+      <c r="D18" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E18" s="9" t="s">
@@ -60500,13 +60519,13 @@
       <c r="A19" s="9">
         <v>23</v>
       </c>
-      <c r="B19" s="37" t="s">
+      <c r="B19" s="36" t="s">
         <v>1525</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>1268</v>
       </c>
-      <c r="D19" s="35" t="s">
+      <c r="D19" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E19" s="9" t="s">
@@ -60536,13 +60555,13 @@
       <c r="A20" s="9">
         <v>26</v>
       </c>
-      <c r="B20" s="37" t="s">
+      <c r="B20" s="36" t="s">
         <v>1581</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>1293</v>
       </c>
-      <c r="D20" s="35" t="s">
+      <c r="D20" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E20" s="9" t="s">
@@ -60569,16 +60588,16 @@
       <c r="R20" s="8"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="39">
+      <c r="A21" s="38">
         <v>27</v>
       </c>
-      <c r="B21" s="37" t="s">
+      <c r="B21" s="36" t="s">
         <v>1330</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>1103</v>
       </c>
-      <c r="D21" s="35" t="s">
+      <c r="D21" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E21" s="9" t="s">
@@ -60601,16 +60620,16 @@
       <c r="R21" s="8"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="39">
+      <c r="A22" s="38">
         <v>28</v>
       </c>
-      <c r="B22" s="37" t="s">
+      <c r="B22" s="36" t="s">
         <v>1616</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>1309</v>
       </c>
-      <c r="D22" s="35" t="s">
+      <c r="D22" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E22" s="9" t="s">
@@ -60640,13 +60659,13 @@
       <c r="A23" s="9">
         <v>29</v>
       </c>
-      <c r="B23" s="37" t="s">
+      <c r="B23" s="36" t="s">
         <v>1487</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>1256</v>
       </c>
-      <c r="D23" s="35" t="s">
+      <c r="D23" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E23" s="9" t="s">
@@ -60676,13 +60695,13 @@
       <c r="A24" s="9">
         <v>30</v>
       </c>
-      <c r="B24" s="37" t="s">
+      <c r="B24" s="36" t="s">
         <v>1429</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>1244</v>
       </c>
-      <c r="D24" s="35" t="s">
+      <c r="D24" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E24" s="9" t="s">
@@ -60712,13 +60731,13 @@
       <c r="A25" s="9">
         <v>31</v>
       </c>
-      <c r="B25" s="37" t="s">
+      <c r="B25" s="36" t="s">
         <v>1430</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>1102</v>
       </c>
-      <c r="D25" s="35" t="s">
+      <c r="D25" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E25" s="9" t="s">
@@ -60745,16 +60764,16 @@
       <c r="R25" s="8"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A26" s="39">
+      <c r="A26" s="38">
         <v>32</v>
       </c>
-      <c r="B26" s="37" t="s">
+      <c r="B26" s="36" t="s">
         <v>1618</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>1310</v>
       </c>
-      <c r="D26" s="35" t="s">
+      <c r="D26" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E26" s="9" t="s">
@@ -60784,13 +60803,13 @@
       <c r="A27" s="9">
         <v>33</v>
       </c>
-      <c r="B27" s="37" t="s">
+      <c r="B27" s="36" t="s">
         <v>1427</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>1242</v>
       </c>
-      <c r="D27" s="35" t="s">
+      <c r="D27" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E27" s="9" t="s">
@@ -60820,13 +60839,13 @@
       <c r="A28" s="9">
         <v>34</v>
       </c>
-      <c r="B28" s="37" t="s">
+      <c r="B28" s="36" t="s">
         <v>1425</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>1240</v>
       </c>
-      <c r="D28" s="35" t="s">
+      <c r="D28" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E28" s="9" t="s">
@@ -60856,13 +60875,13 @@
       <c r="A29" s="9">
         <v>35</v>
       </c>
-      <c r="B29" s="37" t="s">
+      <c r="B29" s="36" t="s">
         <v>1426</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>1241</v>
       </c>
-      <c r="D29" s="35" t="s">
+      <c r="D29" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E29" s="9" t="s">
@@ -60889,16 +60908,16 @@
       <c r="R29" s="8"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="39">
+      <c r="A30" s="38">
         <v>38</v>
       </c>
-      <c r="B30" s="37" t="s">
+      <c r="B30" s="36" t="s">
         <v>1649</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>1320</v>
       </c>
-      <c r="D30" s="35" t="s">
+      <c r="D30" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E30" s="9" t="s">
@@ -60925,16 +60944,16 @@
       <c r="R30" s="8"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="39">
+      <c r="A31" s="38">
         <v>42</v>
       </c>
-      <c r="B31" s="37" t="s">
+      <c r="B31" s="36" t="s">
         <v>1646</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>1318</v>
       </c>
-      <c r="D31" s="35" t="s">
+      <c r="D31" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E31" s="9" t="s">
@@ -60961,16 +60980,16 @@
       <c r="R31" s="8"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="39">
+      <c r="A32" s="38">
         <v>43</v>
       </c>
-      <c r="B32" s="37" t="s">
+      <c r="B32" s="36" t="s">
         <v>1619</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>1311</v>
       </c>
-      <c r="D32" s="35" t="s">
+      <c r="D32" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E32" s="9" t="s">
@@ -61000,13 +61019,13 @@
       <c r="A33" s="9">
         <v>45</v>
       </c>
-      <c r="B33" s="37" t="s">
+      <c r="B33" s="36" t="s">
         <v>1414</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>1237</v>
       </c>
-      <c r="D33" s="35" t="s">
+      <c r="D33" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E33" s="9" t="s">
@@ -61036,13 +61055,13 @@
       <c r="A34" s="9">
         <v>64</v>
       </c>
-      <c r="B34" s="37" t="s">
+      <c r="B34" s="36" t="s">
         <v>1496</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>1258</v>
       </c>
-      <c r="D34" s="35" t="s">
+      <c r="D34" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E34" s="9" t="s">
@@ -61072,13 +61091,13 @@
       <c r="A35" s="9">
         <v>81</v>
       </c>
-      <c r="B35" s="37" t="s">
+      <c r="B35" s="36" t="s">
         <v>1419</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>1239</v>
       </c>
-      <c r="D35" s="35" t="s">
+      <c r="D35" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E35" s="9" t="s">
@@ -61103,16 +61122,16 @@
       <c r="R35" s="8"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" s="39">
+      <c r="A36" s="38">
         <v>83</v>
       </c>
-      <c r="B36" s="37" t="s">
+      <c r="B36" s="36" t="s">
         <v>1592</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>1298</v>
       </c>
-      <c r="D36" s="35" t="s">
+      <c r="D36" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E36" s="9" t="s">
@@ -61140,16 +61159,16 @@
       <c r="A37" s="9">
         <v>85</v>
       </c>
-      <c r="B37" s="37" t="s">
+      <c r="B37" s="36" t="s">
         <v>1485</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>1104</v>
       </c>
-      <c r="D37" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="E37" s="38" t="s">
+      <c r="D37" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="37" t="s">
         <v>1693</v>
       </c>
       <c r="F37" s="9"/>
@@ -61173,16 +61192,16 @@
       <c r="R37" s="8"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A38" s="39">
+      <c r="A38" s="38">
         <v>86</v>
       </c>
-      <c r="B38" s="37" t="s">
+      <c r="B38" s="36" t="s">
         <v>1590</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>1105</v>
       </c>
-      <c r="D38" s="35" t="s">
+      <c r="D38" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E38" s="9" t="s">
@@ -61212,13 +61231,13 @@
       <c r="A39" s="9">
         <v>92</v>
       </c>
-      <c r="B39" s="37" t="s">
+      <c r="B39" s="36" t="s">
         <v>1546</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>1110</v>
       </c>
-      <c r="D39" s="35" t="s">
+      <c r="D39" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E39" s="9" t="s">
@@ -61253,16 +61272,16 @@
       <c r="R39" s="8"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" s="39">
+      <c r="A40" s="38">
         <v>93</v>
       </c>
-      <c r="B40" s="37" t="s">
+      <c r="B40" s="36" t="s">
         <v>1342</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>1111</v>
       </c>
-      <c r="D40" s="35" t="s">
+      <c r="D40" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E40" s="9" t="s">
@@ -61292,13 +61311,13 @@
       <c r="A41" s="9">
         <v>111</v>
       </c>
-      <c r="B41" s="37" t="s">
+      <c r="B41" s="36" t="s">
         <v>1538</v>
       </c>
       <c r="C41" s="9" t="s">
         <v>1273</v>
       </c>
-      <c r="D41" s="35" t="s">
+      <c r="D41" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E41" s="9" t="s">
@@ -61334,13 +61353,13 @@
       <c r="A42" s="9">
         <v>112</v>
       </c>
-      <c r="B42" s="37" t="s">
+      <c r="B42" s="36" t="s">
         <v>1530</v>
       </c>
       <c r="C42" s="9" t="s">
         <v>1141</v>
       </c>
-      <c r="D42" s="35" t="s">
+      <c r="D42" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E42" s="9" t="s">
@@ -61373,16 +61392,16 @@
       <c r="R42" s="8"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" s="39">
+      <c r="A43" s="38">
         <v>113</v>
       </c>
-      <c r="B43" s="37" t="s">
+      <c r="B43" s="36" t="s">
         <v>1614</v>
       </c>
       <c r="C43" s="9" t="s">
         <v>1142</v>
       </c>
-      <c r="D43" s="35" t="s">
+      <c r="D43" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E43" s="9" t="s">
@@ -61412,13 +61431,13 @@
       <c r="A44" s="9">
         <v>116</v>
       </c>
-      <c r="B44" s="37" t="s">
+      <c r="B44" s="36" t="s">
         <v>1433</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>1146</v>
       </c>
-      <c r="D44" s="35" t="s">
+      <c r="D44" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E44" s="9" t="s">
@@ -61448,13 +61467,13 @@
       <c r="A45" s="9">
         <v>120</v>
       </c>
-      <c r="B45" s="37" t="s">
+      <c r="B45" s="36" t="s">
         <v>1540</v>
       </c>
       <c r="C45" s="9" t="s">
         <v>1275</v>
       </c>
-      <c r="D45" s="35" t="s">
+      <c r="D45" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E45" s="9" t="s">
@@ -61492,16 +61511,16 @@
       <c r="A46" s="9">
         <v>122</v>
       </c>
-      <c r="B46" s="37" t="s">
+      <c r="B46" s="36" t="s">
         <v>1375</v>
       </c>
       <c r="C46" s="9" t="s">
         <v>1114</v>
       </c>
-      <c r="D46" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="E46" s="37" t="s">
+      <c r="D46" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="E46" s="36" t="s">
         <v>1094</v>
       </c>
       <c r="F46" s="9"/>
@@ -61528,16 +61547,16 @@
       <c r="A47" s="9">
         <v>123</v>
       </c>
-      <c r="B47" s="37" t="s">
+      <c r="B47" s="36" t="s">
         <v>1553</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>1281</v>
       </c>
-      <c r="D47" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="E47" s="37" t="s">
+      <c r="D47" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="E47" s="36" t="s">
         <v>1101</v>
       </c>
       <c r="F47" s="9"/>
@@ -61567,16 +61586,16 @@
       <c r="R47" s="8"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A48" s="39">
+      <c r="A48" s="38">
         <v>125</v>
       </c>
-      <c r="B48" s="37" t="s">
+      <c r="B48" s="36" t="s">
         <v>1665</v>
       </c>
       <c r="C48" s="9" t="s">
         <v>1116</v>
       </c>
-      <c r="D48" s="35" t="s">
+      <c r="D48" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E48" s="9" t="s">
@@ -61610,13 +61629,13 @@
       <c r="A49" s="9">
         <v>127</v>
       </c>
-      <c r="B49" s="37" t="s">
+      <c r="B49" s="36" t="s">
         <v>1446</v>
       </c>
       <c r="C49" s="9" t="s">
         <v>1136</v>
       </c>
-      <c r="D49" s="35" t="s">
+      <c r="D49" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E49" s="9" t="s">
@@ -61644,13 +61663,13 @@
       <c r="A50" s="9">
         <v>131</v>
       </c>
-      <c r="B50" s="37" t="s">
+      <c r="B50" s="36" t="s">
         <v>1483</v>
       </c>
       <c r="C50" s="9" t="s">
         <v>1117</v>
       </c>
-      <c r="D50" s="35" t="s">
+      <c r="D50" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E50" s="9" t="s">
@@ -61678,13 +61697,13 @@
       <c r="A51" s="9">
         <v>136</v>
       </c>
-      <c r="B51" s="37" t="s">
+      <c r="B51" s="36" t="s">
         <v>1447</v>
       </c>
       <c r="C51" s="9" t="s">
         <v>1139</v>
       </c>
-      <c r="D51" s="35" t="s">
+      <c r="D51" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E51" s="9" t="s">
@@ -61714,13 +61733,13 @@
       <c r="A52" s="9">
         <v>138</v>
       </c>
-      <c r="B52" s="37" t="s">
+      <c r="B52" s="36" t="s">
         <v>1520</v>
       </c>
       <c r="C52" s="9" t="s">
         <v>1265</v>
       </c>
-      <c r="D52" s="35" t="s">
+      <c r="D52" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E52" s="9" t="s">
@@ -61753,16 +61772,16 @@
       <c r="R52" s="8"/>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A53" s="39">
+      <c r="A53" s="38">
         <v>145</v>
       </c>
-      <c r="B53" s="37" t="s">
+      <c r="B53" s="36" t="s">
         <v>1664</v>
       </c>
-      <c r="C53" s="40" t="s">
+      <c r="C53" s="39" t="s">
         <v>1328</v>
       </c>
-      <c r="D53" s="35" t="s">
+      <c r="D53" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E53" s="9" t="s">
@@ -61786,13 +61805,13 @@
       <c r="A54" s="9">
         <v>146</v>
       </c>
-      <c r="B54" s="37" t="s">
+      <c r="B54" s="36" t="s">
         <v>1370</v>
       </c>
       <c r="C54" s="9" t="s">
         <v>1119</v>
       </c>
-      <c r="D54" s="35" t="s">
+      <c r="D54" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E54" s="9" t="s">
@@ -61822,13 +61841,13 @@
       <c r="A55" s="9">
         <v>148</v>
       </c>
-      <c r="B55" s="37" t="s">
+      <c r="B55" s="36" t="s">
         <v>1395</v>
       </c>
       <c r="C55" s="9" t="s">
         <v>1149</v>
       </c>
-      <c r="D55" s="35" t="s">
+      <c r="D55" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E55" s="9" t="s">
@@ -61858,13 +61877,13 @@
       <c r="A56" s="9">
         <v>150</v>
       </c>
-      <c r="B56" s="37" t="s">
+      <c r="B56" s="36" t="s">
         <v>1423</v>
       </c>
       <c r="C56" s="9" t="s">
         <v>1120</v>
       </c>
-      <c r="D56" s="35" t="s">
+      <c r="D56" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E56" s="9" t="s">
@@ -61892,13 +61911,13 @@
       <c r="A57" s="9">
         <v>151</v>
       </c>
-      <c r="B57" s="37" t="s">
+      <c r="B57" s="36" t="s">
         <v>1440</v>
       </c>
       <c r="C57" s="9" t="s">
         <v>1121</v>
       </c>
-      <c r="D57" s="35" t="s">
+      <c r="D57" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E57" s="9" t="s">
@@ -61926,13 +61945,13 @@
       <c r="A58" s="9">
         <v>152</v>
       </c>
-      <c r="B58" s="37" t="s">
+      <c r="B58" s="36" t="s">
         <v>1541</v>
       </c>
       <c r="C58" s="9" t="s">
         <v>1276</v>
       </c>
-      <c r="D58" s="35" t="s">
+      <c r="D58" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E58" s="9" t="s">
@@ -61970,13 +61989,13 @@
       <c r="A59" s="9">
         <v>162</v>
       </c>
-      <c r="B59" s="37" t="s">
+      <c r="B59" s="36" t="s">
         <v>1455</v>
       </c>
       <c r="C59" s="9" t="s">
         <v>1155</v>
       </c>
-      <c r="D59" s="35" t="s">
+      <c r="D59" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E59" s="9" t="s">
@@ -62004,13 +62023,13 @@
       <c r="A60" s="9">
         <v>163</v>
       </c>
-      <c r="B60" s="37" t="s">
+      <c r="B60" s="36" t="s">
         <v>1418</v>
       </c>
       <c r="C60" s="9" t="s">
         <v>1138</v>
       </c>
-      <c r="D60" s="35" t="s">
+      <c r="D60" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E60" s="9" t="s">
@@ -62038,13 +62057,13 @@
       <c r="A61" s="9">
         <v>166</v>
       </c>
-      <c r="B61" s="37" t="s">
+      <c r="B61" s="36" t="s">
         <v>1542</v>
       </c>
       <c r="C61" s="9" t="s">
         <v>1277</v>
       </c>
-      <c r="D61" s="35" t="s">
+      <c r="D61" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E61" s="9" t="s">
@@ -62077,16 +62096,16 @@
       <c r="R61" s="8"/>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A62" s="39">
+      <c r="A62" s="38">
         <v>168</v>
       </c>
-      <c r="B62" s="37" t="s">
+      <c r="B62" s="36" t="s">
         <v>1610</v>
       </c>
       <c r="C62" s="9" t="s">
         <v>1306</v>
       </c>
-      <c r="D62" s="35" t="s">
+      <c r="D62" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E62" s="9" t="s">
@@ -62114,13 +62133,13 @@
       <c r="A63" s="9">
         <v>178</v>
       </c>
-      <c r="B63" s="37" t="s">
+      <c r="B63" s="36" t="s">
         <v>1434</v>
       </c>
       <c r="C63" s="9" t="s">
         <v>1124</v>
       </c>
-      <c r="D63" s="35" t="s">
+      <c r="D63" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E63" s="9" t="s">
@@ -62148,13 +62167,13 @@
       <c r="A64" s="9">
         <v>182</v>
       </c>
-      <c r="B64" s="37" t="s">
+      <c r="B64" s="36" t="s">
         <v>1467</v>
       </c>
       <c r="C64" s="9" t="s">
         <v>1160</v>
       </c>
-      <c r="D64" s="35" t="s">
+      <c r="D64" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E64" s="9" t="s">
@@ -62181,16 +62200,16 @@
       <c r="R64" s="8"/>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A65" s="39">
+      <c r="A65" s="38">
         <v>185</v>
       </c>
-      <c r="B65" s="37" t="s">
+      <c r="B65" s="36" t="s">
         <v>1645</v>
       </c>
       <c r="C65" s="9" t="s">
         <v>1317</v>
       </c>
-      <c r="D65" s="35" t="s">
+      <c r="D65" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E65" s="9" t="s">
@@ -62220,13 +62239,13 @@
       <c r="A66" s="9">
         <v>189</v>
       </c>
-      <c r="B66" s="37" t="s">
+      <c r="B66" s="36" t="s">
         <v>1398</v>
       </c>
       <c r="C66" s="9" t="s">
         <v>1156</v>
       </c>
-      <c r="D66" s="35" t="s">
+      <c r="D66" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E66" s="9" t="s">
@@ -62262,13 +62281,13 @@
       <c r="A67" s="9">
         <v>190</v>
       </c>
-      <c r="B67" s="37" t="s">
+      <c r="B67" s="36" t="s">
         <v>1403</v>
       </c>
       <c r="C67" s="9" t="s">
         <v>1233</v>
       </c>
-      <c r="D67" s="35" t="s">
+      <c r="D67" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E67" s="9" t="s">
@@ -62296,13 +62315,13 @@
       <c r="A68" s="9">
         <v>192</v>
       </c>
-      <c r="B68" s="37" t="s">
+      <c r="B68" s="36" t="s">
         <v>1451</v>
       </c>
       <c r="C68" s="9" t="s">
         <v>1163</v>
       </c>
-      <c r="D68" s="35" t="s">
+      <c r="D68" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E68" s="9" t="s">
@@ -62332,13 +62351,13 @@
       <c r="A69" s="9">
         <v>193</v>
       </c>
-      <c r="B69" s="37" t="s">
+      <c r="B69" s="36" t="s">
         <v>1582</v>
       </c>
       <c r="C69" s="9" t="s">
         <v>1165</v>
       </c>
-      <c r="D69" s="35" t="s">
+      <c r="D69" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E69" s="9" t="s">
@@ -62374,13 +62393,13 @@
       <c r="A70" s="9">
         <v>204</v>
       </c>
-      <c r="B70" s="37" t="s">
+      <c r="B70" s="36" t="s">
         <v>1123</v>
       </c>
       <c r="C70" s="9" t="s">
         <v>1123</v>
       </c>
-      <c r="D70" s="35" t="s">
+      <c r="D70" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E70" s="9" t="s">
@@ -62410,13 +62429,13 @@
       <c r="A71" s="9">
         <v>207</v>
       </c>
-      <c r="B71" s="37" t="s">
+      <c r="B71" s="36" t="s">
         <v>1406</v>
       </c>
       <c r="C71" s="9" t="s">
         <v>1126</v>
       </c>
-      <c r="D71" s="35" t="s">
+      <c r="D71" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E71" s="9" t="s">
@@ -62444,13 +62463,13 @@
       <c r="A72" s="9">
         <v>208</v>
       </c>
-      <c r="B72" s="37" t="s">
+      <c r="B72" s="36" t="s">
         <v>1402</v>
       </c>
       <c r="C72" s="9" t="s">
         <v>1232</v>
       </c>
-      <c r="D72" s="35" t="s">
+      <c r="D72" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E72" s="9" t="s">
@@ -62478,13 +62497,13 @@
       <c r="A73" s="9">
         <v>209</v>
       </c>
-      <c r="B73" s="37" t="s">
+      <c r="B73" s="36" t="s">
         <v>1405</v>
       </c>
       <c r="C73" s="9" t="s">
         <v>1234</v>
       </c>
-      <c r="D73" s="35" t="s">
+      <c r="D73" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E73" s="9" t="s">
@@ -62512,13 +62531,13 @@
       <c r="A74" s="9">
         <v>210</v>
       </c>
-      <c r="B74" s="37" t="s">
+      <c r="B74" s="36" t="s">
         <v>1452</v>
       </c>
       <c r="C74" s="9" t="s">
         <v>1164</v>
       </c>
-      <c r="D74" s="35" t="s">
+      <c r="D74" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E74" s="9" t="s">
@@ -62546,13 +62565,13 @@
       <c r="A75" s="9">
         <v>212</v>
       </c>
-      <c r="B75" s="37" t="s">
+      <c r="B75" s="36" t="s">
         <v>1377</v>
       </c>
       <c r="C75" s="9" t="s">
         <v>1115</v>
       </c>
-      <c r="D75" s="35" t="s">
+      <c r="D75" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E75" s="9" t="s">
@@ -62586,13 +62605,13 @@
       <c r="A76" s="9">
         <v>214</v>
       </c>
-      <c r="B76" s="37" t="s">
+      <c r="B76" s="36" t="s">
         <v>1376</v>
       </c>
       <c r="C76" s="9" t="s">
         <v>1222</v>
       </c>
-      <c r="D76" s="35" t="s">
+      <c r="D76" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E76" s="9" t="s">
@@ -62626,13 +62645,13 @@
       <c r="A77" s="9">
         <v>215</v>
       </c>
-      <c r="B77" s="37" t="s">
+      <c r="B77" s="36" t="s">
         <v>1404</v>
       </c>
       <c r="C77" s="9" t="s">
         <v>1127</v>
       </c>
-      <c r="D77" s="35" t="s">
+      <c r="D77" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E77" s="9" t="s">
@@ -62660,13 +62679,13 @@
       <c r="A78" s="9">
         <v>223</v>
       </c>
-      <c r="B78" s="37" t="s">
+      <c r="B78" s="36" t="s">
         <v>1558</v>
       </c>
       <c r="C78" s="9" t="s">
         <v>1169</v>
       </c>
-      <c r="D78" s="35" t="s">
+      <c r="D78" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E78" s="9" t="s">
@@ -62704,13 +62723,13 @@
       <c r="A79" s="9">
         <v>224</v>
       </c>
-      <c r="B79" s="37" t="s">
+      <c r="B79" s="36" t="s">
         <v>1460</v>
       </c>
       <c r="C79" s="9" t="s">
         <v>1170</v>
       </c>
-      <c r="D79" s="35" t="s">
+      <c r="D79" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E79" s="9" t="s">
@@ -62738,13 +62757,13 @@
       <c r="A80" s="9">
         <v>227</v>
       </c>
-      <c r="B80" s="37" t="s">
+      <c r="B80" s="36" t="s">
         <v>1365</v>
       </c>
       <c r="C80" s="9" t="s">
         <v>1132</v>
       </c>
-      <c r="D80" s="35" t="s">
+      <c r="D80" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E80" s="9" t="s">
@@ -62772,13 +62791,13 @@
       <c r="A81" s="9">
         <v>230</v>
       </c>
-      <c r="B81" s="37" t="s">
+      <c r="B81" s="36" t="s">
         <v>1551</v>
       </c>
       <c r="C81" s="9" t="s">
         <v>1171</v>
       </c>
-      <c r="D81" s="35" t="s">
+      <c r="D81" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E81" s="9" t="s">
@@ -62816,13 +62835,13 @@
       <c r="A82" s="9">
         <v>232</v>
       </c>
-      <c r="B82" s="37" t="s">
+      <c r="B82" s="36" t="s">
         <v>1432</v>
       </c>
       <c r="C82" s="9" t="s">
         <v>1172</v>
       </c>
-      <c r="D82" s="35" t="s">
+      <c r="D82" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E82" s="9" t="s">
@@ -62850,13 +62869,13 @@
       <c r="A83" s="9">
         <v>233</v>
       </c>
-      <c r="B83" s="37" t="s">
+      <c r="B83" s="36" t="s">
         <v>1396</v>
       </c>
       <c r="C83" s="9" t="s">
         <v>1173</v>
       </c>
-      <c r="D83" s="35" t="s">
+      <c r="D83" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E83" s="9" t="s">
@@ -62888,13 +62907,13 @@
       <c r="A84" s="9">
         <v>238</v>
       </c>
-      <c r="B84" s="37" t="s">
+      <c r="B84" s="36" t="s">
         <v>1488</v>
       </c>
       <c r="C84" s="9" t="s">
         <v>1185</v>
       </c>
-      <c r="D84" s="35" t="s">
+      <c r="D84" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E84" s="9" t="s">
@@ -62922,13 +62941,13 @@
       <c r="A85" s="9">
         <v>241</v>
       </c>
-      <c r="B85" s="37" t="s">
+      <c r="B85" s="36" t="s">
         <v>1539</v>
       </c>
       <c r="C85" s="9" t="s">
         <v>1274</v>
       </c>
-      <c r="D85" s="35" t="s">
+      <c r="D85" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E85" s="9" t="s">
@@ -62964,13 +62983,13 @@
       <c r="A86" s="9">
         <v>243</v>
       </c>
-      <c r="B86" s="37" t="s">
+      <c r="B86" s="36" t="s">
         <v>1391</v>
       </c>
       <c r="C86" s="9" t="s">
         <v>1230</v>
       </c>
-      <c r="D86" s="35" t="s">
+      <c r="D86" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E86" s="9" t="s">
@@ -62998,13 +63017,13 @@
       <c r="A87" s="8">
         <v>253</v>
       </c>
-      <c r="B87" s="41" t="s">
+      <c r="B87" s="40" t="s">
         <v>1353</v>
       </c>
       <c r="C87" s="8" t="s">
         <v>1178</v>
       </c>
-      <c r="D87" s="35" t="s">
+      <c r="D87" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E87" s="9" t="s">
@@ -63032,13 +63051,13 @@
       <c r="A88" s="8">
         <v>254</v>
       </c>
-      <c r="B88" s="41" t="s">
+      <c r="B88" s="40" t="s">
         <v>1424</v>
       </c>
       <c r="C88" s="8" t="s">
         <v>1133</v>
       </c>
-      <c r="D88" s="35" t="s">
+      <c r="D88" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E88" s="9" t="s">
@@ -63066,13 +63085,13 @@
       <c r="A89" s="8">
         <v>257</v>
       </c>
-      <c r="B89" s="41" t="s">
+      <c r="B89" s="40" t="s">
         <v>1457</v>
       </c>
       <c r="C89" s="8" t="s">
         <v>1179</v>
       </c>
-      <c r="D89" s="35" t="s">
+      <c r="D89" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E89" s="9" t="s">
@@ -63097,16 +63116,16 @@
       <c r="R89" s="8"/>
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A90" s="42">
+      <c r="A90" s="41">
         <v>260</v>
       </c>
-      <c r="B90" s="41" t="s">
+      <c r="B90" s="40" t="s">
         <v>1587</v>
       </c>
       <c r="C90" s="8" t="s">
         <v>1148</v>
       </c>
-      <c r="D90" s="36" t="s">
+      <c r="D90" s="35" t="s">
         <v>5</v>
       </c>
       <c r="E90" s="9" t="s">
@@ -63134,16 +63153,16 @@
       <c r="A91" s="8">
         <v>264</v>
       </c>
-      <c r="B91" s="41" t="s">
+      <c r="B91" s="40" t="s">
         <v>1378</v>
       </c>
       <c r="C91" s="8" t="s">
         <v>1223</v>
       </c>
-      <c r="D91" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="E91" s="37" t="s">
+      <c r="D91" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="E91" s="36" t="s">
         <v>1687</v>
       </c>
       <c r="F91" s="8"/>
@@ -63174,13 +63193,13 @@
       <c r="A92" s="8">
         <v>265</v>
       </c>
-      <c r="B92" s="41" t="s">
+      <c r="B92" s="40" t="s">
         <v>1449</v>
       </c>
       <c r="C92" s="8" t="s">
         <v>1250</v>
       </c>
-      <c r="D92" s="35" t="s">
+      <c r="D92" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E92" s="9" t="s">
@@ -63207,16 +63226,16 @@
       <c r="R92" s="8"/>
     </row>
     <row r="93" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A93" s="42">
+      <c r="A93" s="41">
         <v>270</v>
       </c>
-      <c r="B93" s="41" t="s">
+      <c r="B93" s="40" t="s">
         <v>1666</v>
       </c>
       <c r="C93" s="8" t="s">
         <v>1193</v>
       </c>
-      <c r="D93" s="35" t="s">
+      <c r="D93" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E93" s="8" t="s">
@@ -63250,16 +63269,16 @@
       <c r="A94" s="8">
         <v>271</v>
       </c>
-      <c r="B94" s="41" t="s">
+      <c r="B94" s="40" t="s">
         <v>1486</v>
       </c>
       <c r="C94" s="8" t="s">
         <v>1255</v>
       </c>
-      <c r="D94" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="E94" s="41" t="s">
+      <c r="D94" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="E94" s="40" t="s">
         <v>1684</v>
       </c>
       <c r="F94" s="8"/>
@@ -63286,13 +63305,13 @@
       <c r="A95" s="8">
         <v>272</v>
       </c>
-      <c r="B95" s="41" t="s">
+      <c r="B95" s="40" t="s">
         <v>1490</v>
       </c>
       <c r="C95" s="8" t="s">
         <v>1188</v>
       </c>
-      <c r="D95" s="35" t="s">
+      <c r="D95" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E95" s="8" t="s">
@@ -63322,16 +63341,16 @@
       <c r="A96" s="8">
         <v>273</v>
       </c>
-      <c r="B96" s="41" t="s">
+      <c r="B96" s="40" t="s">
         <v>1559</v>
       </c>
       <c r="C96" s="8" t="s">
         <v>1191</v>
       </c>
-      <c r="D96" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="E96" s="43" t="s">
+      <c r="D96" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="E96" s="42" t="s">
         <v>1101</v>
       </c>
       <c r="F96" s="8"/>
@@ -63364,16 +63383,16 @@
       <c r="A97" s="8">
         <v>274</v>
       </c>
-      <c r="B97" s="41" t="s">
+      <c r="B97" s="40" t="s">
         <v>1489</v>
       </c>
       <c r="C97" s="8" t="s">
         <v>1189</v>
       </c>
-      <c r="D97" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="E97" s="44" t="s">
+      <c r="D97" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="E97" s="43" t="s">
         <v>1681</v>
       </c>
       <c r="F97" s="8"/>
@@ -63400,16 +63419,16 @@
       <c r="A98" s="8">
         <v>275</v>
       </c>
-      <c r="B98" s="41" t="s">
+      <c r="B98" s="40" t="s">
         <v>1441</v>
       </c>
       <c r="C98" s="8" t="s">
         <v>1247</v>
       </c>
-      <c r="D98" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="E98" s="37" t="s">
+      <c r="D98" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="E98" s="36" t="s">
         <v>1096</v>
       </c>
       <c r="F98" s="8"/>
@@ -63434,16 +63453,16 @@
       <c r="A99" s="8">
         <v>276</v>
       </c>
-      <c r="B99" s="41" t="s">
+      <c r="B99" s="40" t="s">
         <v>1484</v>
       </c>
       <c r="C99" s="8" t="s">
         <v>1254</v>
       </c>
-      <c r="D99" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="E99" s="37" t="s">
+      <c r="D99" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="E99" s="36" t="s">
         <v>1692</v>
       </c>
       <c r="F99" s="8"/>
@@ -63472,13 +63491,13 @@
       <c r="A100" s="8">
         <v>277</v>
       </c>
-      <c r="B100" s="41" t="s">
+      <c r="B100" s="40" t="s">
         <v>1350</v>
       </c>
       <c r="C100" s="8" t="s">
         <v>1192</v>
       </c>
-      <c r="D100" s="35" t="s">
+      <c r="D100" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E100" s="9" t="s">
@@ -63508,13 +63527,13 @@
       <c r="A101" s="8">
         <v>278</v>
       </c>
-      <c r="B101" s="41" t="s">
+      <c r="B101" s="40" t="s">
         <v>1556</v>
       </c>
       <c r="C101" s="8" t="s">
         <v>1194</v>
       </c>
-      <c r="D101" s="35" t="s">
+      <c r="D101" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E101" s="9" t="s">
@@ -63552,13 +63571,13 @@
       <c r="A102" s="8">
         <v>279</v>
       </c>
-      <c r="B102" s="41" t="s">
+      <c r="B102" s="40" t="s">
         <v>1557</v>
       </c>
       <c r="C102" s="8" t="s">
         <v>1195</v>
       </c>
-      <c r="D102" s="35" t="s">
+      <c r="D102" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E102" s="9" t="s">
@@ -63594,13 +63613,13 @@
       <c r="A103" s="8">
         <v>280</v>
       </c>
-      <c r="B103" s="41" t="s">
+      <c r="B103" s="40" t="s">
         <v>1465</v>
       </c>
       <c r="C103" s="8" t="s">
         <v>1129</v>
       </c>
-      <c r="D103" s="35" t="s">
+      <c r="D103" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E103" s="9" t="s">
@@ -63628,13 +63647,13 @@
       <c r="A104" s="8">
         <v>281</v>
       </c>
-      <c r="B104" s="41" t="s">
+      <c r="B104" s="40" t="s">
         <v>1464</v>
       </c>
       <c r="C104" s="8" t="s">
         <v>1130</v>
       </c>
-      <c r="D104" s="35" t="s">
+      <c r="D104" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E104" s="8" t="s">
@@ -63662,13 +63681,13 @@
       <c r="A105" s="8">
         <v>289</v>
       </c>
-      <c r="B105" s="41" t="s">
+      <c r="B105" s="40" t="s">
         <v>1462</v>
       </c>
       <c r="C105" s="8" t="s">
         <v>1128</v>
       </c>
-      <c r="D105" s="35" t="s">
+      <c r="D105" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E105" s="8" t="s">
@@ -63696,13 +63715,13 @@
       <c r="A106" s="8">
         <v>291</v>
       </c>
-      <c r="B106" s="41" t="s">
+      <c r="B106" s="40" t="s">
         <v>1463</v>
       </c>
       <c r="C106" s="8" t="s">
         <v>1131</v>
       </c>
-      <c r="D106" s="35" t="s">
+      <c r="D106" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E106" s="8" t="s">
@@ -63730,13 +63749,13 @@
       <c r="A107" s="8">
         <v>292</v>
       </c>
-      <c r="B107" s="41" t="s">
+      <c r="B107" s="40" t="s">
         <v>1461</v>
       </c>
       <c r="C107" s="8" t="s">
         <v>1252</v>
       </c>
-      <c r="D107" s="35" t="s">
+      <c r="D107" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E107" s="8" t="s">
@@ -63764,13 +63783,13 @@
       <c r="A108" s="8">
         <v>293</v>
       </c>
-      <c r="B108" s="41" t="s">
+      <c r="B108" s="40" t="s">
         <v>1431</v>
       </c>
       <c r="C108" s="8" t="s">
         <v>1245</v>
       </c>
-      <c r="D108" s="35" t="s">
+      <c r="D108" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E108" s="8" t="s">
@@ -63798,13 +63817,13 @@
       <c r="A109" s="8">
         <v>299</v>
       </c>
-      <c r="B109" s="41" t="s">
+      <c r="B109" s="40" t="s">
         <v>1469</v>
       </c>
       <c r="C109" s="8" t="s">
         <v>1197</v>
       </c>
-      <c r="D109" s="35" t="s">
+      <c r="D109" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E109" s="9" t="s">
@@ -63831,16 +63850,16 @@
       <c r="R109" s="8"/>
     </row>
     <row r="110" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A110" s="42">
+      <c r="A110" s="41">
         <v>302</v>
       </c>
-      <c r="B110" s="41" t="s">
+      <c r="B110" s="40" t="s">
         <v>1332</v>
       </c>
       <c r="C110" s="8" t="s">
         <v>1209</v>
       </c>
-      <c r="D110" s="35" t="s">
+      <c r="D110" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E110" s="9" t="s">
@@ -63868,13 +63887,13 @@
       <c r="A111" s="8">
         <v>305</v>
       </c>
-      <c r="B111" s="41" t="s">
+      <c r="B111" s="40" t="s">
         <v>1555</v>
       </c>
       <c r="C111" s="8" t="s">
         <v>1283</v>
       </c>
-      <c r="D111" s="35" t="s">
+      <c r="D111" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E111" s="8" t="s">
@@ -63907,16 +63926,16 @@
       <c r="R111" s="8"/>
     </row>
     <row r="112" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A112" s="42">
+      <c r="A112" s="41">
         <v>306</v>
       </c>
-      <c r="B112" s="41" t="s">
+      <c r="B112" s="40" t="s">
         <v>1659</v>
       </c>
       <c r="C112" s="8" t="s">
         <v>1326</v>
       </c>
-      <c r="D112" s="35" t="s">
+      <c r="D112" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E112" s="8" t="s">
@@ -63941,16 +63960,16 @@
       <c r="R112" s="8"/>
     </row>
     <row r="113" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A113" s="42">
+      <c r="A113" s="41">
         <v>307</v>
       </c>
-      <c r="B113" s="41" t="s">
+      <c r="B113" s="40" t="s">
         <v>1663</v>
       </c>
       <c r="C113" s="8" t="s">
         <v>1198</v>
       </c>
-      <c r="D113" s="35" t="s">
+      <c r="D113" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E113" s="9" t="s">
@@ -63981,16 +64000,16 @@
       <c r="R113" s="8"/>
     </row>
     <row r="114" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A114" s="42">
+      <c r="A114" s="41">
         <v>308</v>
       </c>
-      <c r="B114" s="41" t="s">
+      <c r="B114" s="40" t="s">
         <v>1588</v>
       </c>
       <c r="C114" s="8" t="s">
         <v>1296</v>
       </c>
-      <c r="D114" s="35" t="s">
+      <c r="D114" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E114" s="9" t="s">
@@ -64020,13 +64039,13 @@
       <c r="A115" s="8">
         <v>313</v>
       </c>
-      <c r="B115" s="41" t="s">
+      <c r="B115" s="40" t="s">
         <v>1474</v>
       </c>
       <c r="C115" s="8" t="s">
         <v>1202</v>
       </c>
-      <c r="D115" s="35" t="s">
+      <c r="D115" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E115" s="10" t="s">
@@ -64053,16 +64072,16 @@
       <c r="R115" s="8"/>
     </row>
     <row r="116" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A116" s="42">
+      <c r="A116" s="41">
         <v>314</v>
       </c>
-      <c r="B116" s="41" t="s">
+      <c r="B116" s="40" t="s">
         <v>1661</v>
       </c>
       <c r="C116" s="8" t="s">
         <v>1207</v>
       </c>
-      <c r="D116" s="35" t="s">
+      <c r="D116" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E116" s="8" t="s">
@@ -64092,13 +64111,13 @@
       <c r="A117" s="8">
         <v>319</v>
       </c>
-      <c r="B117" s="41" t="s">
+      <c r="B117" s="40" t="s">
         <v>1354</v>
       </c>
       <c r="C117" s="8" t="s">
         <v>1203</v>
       </c>
-      <c r="D117" s="35" t="s">
+      <c r="D117" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E117" s="8" t="s">
@@ -64126,13 +64145,13 @@
       <c r="A118" s="8">
         <v>324</v>
       </c>
-      <c r="B118" s="41" t="s">
+      <c r="B118" s="40" t="s">
         <v>1394</v>
       </c>
       <c r="C118" s="8" t="s">
         <v>1231</v>
       </c>
-      <c r="D118" s="35" t="s">
+      <c r="D118" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E118" s="9" t="s">
@@ -64157,16 +64176,16 @@
       <c r="R118" s="8"/>
     </row>
     <row r="119" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A119" s="42">
+      <c r="A119" s="41">
         <v>327</v>
       </c>
-      <c r="B119" s="41" t="s">
+      <c r="B119" s="40" t="s">
         <v>1660</v>
       </c>
       <c r="C119" s="8" t="s">
         <v>1327</v>
       </c>
-      <c r="D119" s="35" t="s">
+      <c r="D119" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E119" s="8" t="s">
@@ -64196,13 +64215,13 @@
       <c r="A120" s="8">
         <v>339</v>
       </c>
-      <c r="B120" s="41" t="s">
+      <c r="B120" s="40" t="s">
         <v>1493</v>
       </c>
       <c r="C120" s="8" t="s">
         <v>1257</v>
       </c>
-      <c r="D120" s="35" t="s">
+      <c r="D120" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E120" s="8" t="s">
@@ -64232,13 +64251,13 @@
       <c r="A121" s="8">
         <v>340</v>
       </c>
-      <c r="B121" s="41" t="s">
+      <c r="B121" s="40" t="s">
         <v>1549</v>
       </c>
       <c r="C121" s="8" t="s">
         <v>1280</v>
       </c>
-      <c r="D121" s="35" t="s">
+      <c r="D121" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E121" s="8" t="s">
@@ -64271,16 +64290,16 @@
       <c r="R121" s="8"/>
     </row>
     <row r="122" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A122" s="42">
+      <c r="A122" s="41">
         <v>342</v>
       </c>
-      <c r="B122" s="41" t="s">
+      <c r="B122" s="40" t="s">
         <v>1601</v>
       </c>
       <c r="C122" s="8" t="s">
         <v>1200</v>
       </c>
-      <c r="D122" s="35" t="s">
+      <c r="D122" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E122" s="9" t="s">
@@ -64310,13 +64329,13 @@
       <c r="A123" s="8">
         <v>343</v>
       </c>
-      <c r="B123" s="41" t="s">
+      <c r="B123" s="40" t="s">
         <v>1416</v>
       </c>
       <c r="C123" s="8" t="s">
         <v>1201</v>
       </c>
-      <c r="D123" s="35" t="s">
+      <c r="D123" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E123" s="9" t="s">
@@ -64343,16 +64362,16 @@
       <c r="R123" s="8"/>
     </row>
     <row r="124" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A124" s="42">
+      <c r="A124" s="41">
         <v>344</v>
       </c>
-      <c r="B124" s="41" t="s">
+      <c r="B124" s="40" t="s">
         <v>1584</v>
       </c>
       <c r="C124" s="8" t="s">
         <v>1294</v>
       </c>
-      <c r="D124" s="35" t="s">
+      <c r="D124" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E124" s="9" t="s">
@@ -64383,10 +64402,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9585C0FF-65C5-4BD8-9936-5C9A63F7E604}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64436,7 +64455,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="33" t="s">
         <v>1778</v>
       </c>
       <c r="B2" s="15" t="s">
@@ -64469,7 +64488,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="49" t="s">
         <v>1778</v>
       </c>
       <c r="B3" s="15" t="s">
@@ -64502,7 +64521,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="49" t="s">
         <v>1778</v>
       </c>
       <c r="B4" s="15" t="s">
@@ -64565,7 +64584,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
         <v>1779</v>
       </c>
@@ -64596,8 +64615,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
         <v>1779</v>
       </c>
       <c r="B7" s="12"/>
@@ -64628,7 +64647,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="48" t="s">
         <v>1778</v>
       </c>
       <c r="B8" s="15" t="s">
@@ -65160,6 +65179,30 @@
       </c>
       <c r="J24" s="12">
         <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="33"/>
+      <c r="B26" t="s">
+        <v>1788</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="49"/>
+      <c r="B27" t="s">
+        <v>1789</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="48"/>
+      <c r="B28" t="s">
+        <v>1790</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="12"/>
+      <c r="B29" t="s">
+        <v>1791</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modificación Reporte   DAF empresa 29 mxn  (EGR_ING_Pend_Fact)     se regenero el reportes - Quedo pendiente el orden del reporte del mes , se envio bosch_pedimento2    analisis y desglose de procedimientos preparacion de documentacion de procedimiento, descripcion de parametros,tipos Documentacion Actualizacion de listado de repores agrego estatis y observacion
</commit_message>
<xml_diff>
--- a/00-Documentacion/Listado de reportes totales-TI.xlsx
+++ b/00-Documentacion/Listado de reportes totales-TI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{166363D8-6128-4048-8092-B855F576FCFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB4D95E-CCD6-486D-9BCA-2C8A4D290D9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{1498AA1A-1ACC-4329-A050-ACA05131B658}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13098" uniqueCount="1792">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13112" uniqueCount="1800">
   <si>
     <t xml:space="preserve">Reporte </t>
   </si>
@@ -5431,12 +5431,36 @@
   <si>
     <t>Pendiente</t>
   </si>
+  <si>
+    <t>estatus</t>
+  </si>
+  <si>
+    <t>observaciones</t>
+  </si>
+  <si>
+    <t>terminado</t>
+  </si>
+  <si>
+    <t>proceso</t>
+  </si>
+  <si>
+    <t>tiene grafica de barras</t>
+  </si>
+  <si>
+    <t>ajustes a funcion mensual , Gustavo</t>
+  </si>
+  <si>
+    <t>ajustes a los totales , Gustavo</t>
+  </si>
+  <si>
+    <t>se modifico la funcion  logis.display_fecha_confirmacion4</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5542,6 +5566,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -5684,7 +5714,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5795,6 +5825,12 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -64402,10 +64438,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9585C0FF-65C5-4BD8-9936-5C9A63F7E604}">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64420,9 +64456,10 @@
     <col min="8" max="8" width="19.85546875" customWidth="1"/>
     <col min="9" max="9" width="8.85546875" customWidth="1"/>
     <col min="10" max="10" width="21.5703125" customWidth="1"/>
+    <col min="12" max="12" width="52.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>1781</v>
       </c>
@@ -64453,8 +64490,14 @@
       <c r="J1" s="13" t="s">
         <v>1777</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K1" s="50" t="s">
+        <v>1792</v>
+      </c>
+      <c r="L1" s="50" t="s">
+        <v>1793</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
         <v>1778</v>
       </c>
@@ -64486,8 +64529,11 @@
         <f>2+1</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>1794</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="49" t="s">
         <v>1778</v>
       </c>
@@ -64519,8 +64565,14 @@
         <f>3+1</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>1794</v>
+      </c>
+      <c r="L3" t="s">
+        <v>1797</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="49" t="s">
         <v>1778</v>
       </c>
@@ -64552,8 +64604,14 @@
         <f>4+1</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>1794</v>
+      </c>
+      <c r="L4" t="s">
+        <v>1798</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>1779</v>
       </c>
@@ -64583,8 +64641,11 @@
         <f>4+1</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>1795</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="33" t="s">
         <v>1779</v>
       </c>
@@ -64614,8 +64675,11 @@
         <f>2+1</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K6" t="s">
+        <v>1794</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="33" t="s">
         <v>1779</v>
       </c>
@@ -64645,8 +64709,11 @@
         <f>2+1</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K7" t="s">
+        <v>1794</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="48" t="s">
         <v>1778</v>
       </c>
@@ -64678,8 +64745,14 @@
         <f>4+1</f>
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K8" t="s">
+        <v>1795</v>
+      </c>
+      <c r="L8" t="s">
+        <v>1796</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>1778</v>
       </c>
@@ -64710,8 +64783,14 @@
       <c r="J9" s="12">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K9" t="s">
+        <v>1795</v>
+      </c>
+      <c r="L9" t="s">
+        <v>1799</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>1778</v>
       </c>
@@ -64743,7 +64822,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>1778</v>
       </c>
@@ -64776,12 +64855,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>1779</v>
       </c>
       <c r="B12" s="12"/>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="51" t="s">
         <v>1768</v>
       </c>
       <c r="D12" s="21" t="s">
@@ -64807,7 +64886,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>1778</v>
       </c>
@@ -64839,94 +64918,101 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
-        <v>1779</v>
-      </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="19" t="s">
-        <v>1770</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>1764</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>1771</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>8</v>
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>1778</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>1754</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>1754</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>1755</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>1756</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>21</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>1707</v>
+        <v>1684</v>
       </c>
       <c r="H14" s="12">
         <v>12</v>
       </c>
       <c r="I14" s="12">
-        <v>5</v>
-      </c>
-      <c r="J14" s="12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="J14" s="28">
+        <f>5+2</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>1779</v>
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="19" t="s">
-        <v>1562</v>
-      </c>
-      <c r="D15" s="21" t="s">
-        <v>1773</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>1769</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>1101</v>
+        <v>1766</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>1767</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>1765</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>1249</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>1682</v>
       </c>
       <c r="H15" s="12">
         <v>13</v>
       </c>
       <c r="I15" s="12">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="J15" s="12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
-        <v>1779</v>
-      </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="19" t="s">
-        <v>1775</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>1764</v>
-      </c>
-      <c r="E16" s="26" t="s">
-        <v>1765</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>227</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>1690</v>
+        <f>15+5</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>1778</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>1739</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>1742</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>1743</v>
+      </c>
+      <c r="E16" s="29" t="s">
+        <v>1744</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>481</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>1681</v>
       </c>
       <c r="H16" s="12">
         <v>14</v>
       </c>
       <c r="I16" s="12">
+        <v>35</v>
+      </c>
+      <c r="J16" s="12">
+        <f>3+8</f>
         <v>11</v>
-      </c>
-      <c r="J16" s="12">
-        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -64935,60 +65021,59 @@
       </c>
       <c r="B17" s="12"/>
       <c r="C17" s="19" t="s">
-        <v>1761</v>
+        <v>1775</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>1762</v>
+        <v>1764</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>1763</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>6</v>
+        <v>1765</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>227</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>1725</v>
+        <v>1690</v>
       </c>
       <c r="H17" s="12">
         <v>15</v>
       </c>
       <c r="I17" s="12">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J17" s="12">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
-        <v>1778</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>1758</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>1758</v>
-      </c>
-      <c r="D18" s="24" t="s">
-        <v>1759</v>
-      </c>
-      <c r="E18" s="25" t="s">
-        <v>1744</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>1779</v>
+      </c>
+      <c r="B18" s="12"/>
+      <c r="C18" s="19" t="s">
+        <v>1643</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>1764</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>1765</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="G18" s="10" t="s">
-        <v>1696</v>
+        <v>1681</v>
       </c>
       <c r="H18" s="12">
         <v>16</v>
       </c>
       <c r="I18" s="12">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="J18" s="12">
-        <v>16</v>
+        <f>9+2</f>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -64997,126 +65082,120 @@
       </c>
       <c r="B19" s="12"/>
       <c r="C19" s="19" t="s">
-        <v>1766</v>
+        <v>1761</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>1767</v>
+        <v>1762</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>1765</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>1249</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>1682</v>
+        <v>1763</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>1725</v>
       </c>
       <c r="H19" s="12">
         <v>17</v>
       </c>
       <c r="I19" s="12">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="J19" s="12">
-        <f>15+5</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
-        <v>1778</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>1754</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>1754</v>
-      </c>
-      <c r="D20" s="24" t="s">
-        <v>1755</v>
-      </c>
-      <c r="E20" s="27" t="s">
-        <v>1756</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>21</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>1779</v>
+      </c>
+      <c r="B20" s="12"/>
+      <c r="C20" s="19" t="s">
+        <v>1770</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>1764</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>1771</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>8</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>1684</v>
+        <v>1707</v>
       </c>
       <c r="H20" s="12">
         <v>18</v>
       </c>
       <c r="I20" s="12">
-        <v>32</v>
-      </c>
-      <c r="J20" s="28">
-        <f>5+2</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
-        <v>1778</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>1739</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>1742</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>1743</v>
-      </c>
-      <c r="E21" s="29" t="s">
-        <v>1744</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>481</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>1681</v>
+        <v>5</v>
+      </c>
+      <c r="J20" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
+        <v>1779</v>
+      </c>
+      <c r="B21" s="12"/>
+      <c r="C21" s="19" t="s">
+        <v>1562</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>1773</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>1769</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>1101</v>
       </c>
       <c r="H21" s="12">
         <v>19</v>
       </c>
       <c r="I21" s="12">
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="J21" s="12">
-        <f>3+8</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
-        <v>1779</v>
-      </c>
-      <c r="B22" s="12"/>
-      <c r="C22" s="19" t="s">
-        <v>1643</v>
-      </c>
-      <c r="D22" s="21" t="s">
-        <v>1764</v>
-      </c>
-      <c r="E22" s="26" t="s">
-        <v>1765</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>1778</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>1758</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>1758</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>1759</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>1744</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>1681</v>
+        <v>1696</v>
       </c>
       <c r="H22" s="12">
         <v>20</v>
       </c>
       <c r="I22" s="12">
-        <v>61</v>
+        <v>12</v>
       </c>
       <c r="J22" s="12">
-        <f>9+2</f>
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
crear proceso de identificación de rango  ( coordenadas de Excel posiciones )
ajustar al parámetros de coordenadas espacio a títulos.
modificación de procedimiento Excel para asignar título de hoja
actualizacion de listado de reportes
</commit_message>
<xml_diff>
--- a/00-Documentacion/Listado de reportes totales-TI.xlsx
+++ b/00-Documentacion/Listado de reportes totales-TI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A3E1B9-D08B-44F1-ACB2-756D951D42E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB1A141-1A12-4F2E-ACD9-0D09CBD934B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{1498AA1A-1ACC-4329-A050-ACA05131B658}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13112" uniqueCount="1801">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13111" uniqueCount="1802">
   <si>
     <t xml:space="preserve">Reporte </t>
   </si>
@@ -5291,9 +5291,6 @@
     <t>CORRECTO</t>
   </si>
   <si>
-    <t>Interfaces</t>
-  </si>
-  <si>
     <t>En Espera Por Periodicidad</t>
   </si>
   <si>
@@ -5457,6 +5454,12 @@
   </si>
   <si>
     <t>no encuentro ecl command</t>
+  </si>
+  <si>
+    <t>bosch_pedim2,Bosch Pedimentos3</t>
+  </si>
+  <si>
+    <t>bosch_pedim2,bosch_pedim3</t>
   </si>
 </sst>
 </file>
@@ -5717,7 +5720,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -5771,9 +5774,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -6241,7 +6241,7 @@
       <c r="C2" s="9" t="s">
         <v>1243</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="9" t="s">
@@ -6683,7 +6683,7 @@
       <c r="C14" s="9" t="s">
         <v>1238</v>
       </c>
-      <c r="D14" s="45" t="s">
+      <c r="D14" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E14" s="9" t="s">
@@ -6893,7 +6893,7 @@
       <c r="C19" s="5" t="s">
         <v>1134</v>
       </c>
-      <c r="D19" s="46" t="s">
+      <c r="D19" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E19" s="5" t="s">
@@ -6929,7 +6929,7 @@
       <c r="C20" s="5" t="s">
         <v>1266</v>
       </c>
-      <c r="D20" s="46" t="s">
+      <c r="D20" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E20" s="5" t="s">
@@ -6965,7 +6965,7 @@
       <c r="C21" s="9" t="s">
         <v>1267</v>
       </c>
-      <c r="D21" s="45" t="s">
+      <c r="D21" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E21" s="5" t="s">
@@ -7071,7 +7071,7 @@
       <c r="C24" s="5" t="s">
         <v>1322</v>
       </c>
-      <c r="D24" s="45" t="s">
+      <c r="D24" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E24" s="5" t="s">
@@ -7107,7 +7107,7 @@
       <c r="C25" s="5" t="s">
         <v>1135</v>
       </c>
-      <c r="D25" s="46" t="s">
+      <c r="D25" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E25" s="5" t="s">
@@ -7143,7 +7143,7 @@
       <c r="C26" s="5" t="s">
         <v>1323</v>
       </c>
-      <c r="D26" s="46" t="s">
+      <c r="D26" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E26" s="5" t="s">
@@ -7179,7 +7179,7 @@
       <c r="C27" s="5" t="s">
         <v>1212</v>
       </c>
-      <c r="D27" s="46" t="s">
+      <c r="D27" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E27" s="5" t="s">
@@ -12279,7 +12279,7 @@
       <c r="C153" s="9" t="s">
         <v>1268</v>
       </c>
-      <c r="D153" s="45" t="s">
+      <c r="D153" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E153" s="9" t="s">
@@ -14405,7 +14405,7 @@
       <c r="C212" s="9" t="s">
         <v>1293</v>
       </c>
-      <c r="D212" s="45" t="s">
+      <c r="D212" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E212" s="5" t="s">
@@ -14441,7 +14441,7 @@
       <c r="C213" s="5" t="s">
         <v>1103</v>
       </c>
-      <c r="D213" s="45" t="s">
+      <c r="D213" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E213" s="5" t="s">
@@ -14473,7 +14473,7 @@
       <c r="C214" s="9" t="s">
         <v>1309</v>
       </c>
-      <c r="D214" s="45" t="s">
+      <c r="D214" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E214" s="9" t="s">
@@ -14509,7 +14509,7 @@
       <c r="C215" s="9" t="s">
         <v>1256</v>
       </c>
-      <c r="D215" s="45" t="s">
+      <c r="D215" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E215" s="9" t="s">
@@ -14545,7 +14545,7 @@
       <c r="C216" s="9" t="s">
         <v>1244</v>
       </c>
-      <c r="D216" s="45" t="s">
+      <c r="D216" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E216" s="9" t="s">
@@ -14581,7 +14581,7 @@
       <c r="C217" s="5" t="s">
         <v>1102</v>
       </c>
-      <c r="D217" s="45" t="s">
+      <c r="D217" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E217" s="5" t="s">
@@ -14617,7 +14617,7 @@
       <c r="C218" s="5" t="s">
         <v>1310</v>
       </c>
-      <c r="D218" s="46" t="s">
+      <c r="D218" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E218" s="5" t="s">
@@ -14653,7 +14653,7 @@
       <c r="C219" s="5" t="s">
         <v>1242</v>
       </c>
-      <c r="D219" s="46" t="s">
+      <c r="D219" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E219" s="5" t="s">
@@ -14689,7 +14689,7 @@
       <c r="C220" s="5" t="s">
         <v>1240</v>
       </c>
-      <c r="D220" s="46" t="s">
+      <c r="D220" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E220" s="5" t="s">
@@ -14725,7 +14725,7 @@
       <c r="C221" s="5" t="s">
         <v>1241</v>
       </c>
-      <c r="D221" s="46" t="s">
+      <c r="D221" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E221" s="5" t="s">
@@ -14833,7 +14833,7 @@
       <c r="C224" s="5" t="s">
         <v>1320</v>
       </c>
-      <c r="D224" s="46" t="s">
+      <c r="D224" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E224" s="5" t="s">
@@ -15335,7 +15335,7 @@
       <c r="C238" s="5" t="s">
         <v>1318</v>
       </c>
-      <c r="D238" s="46" t="s">
+      <c r="D238" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E238" s="5" t="s">
@@ -15371,7 +15371,7 @@
       <c r="C239" s="5" t="s">
         <v>1311</v>
       </c>
-      <c r="D239" s="46" t="s">
+      <c r="D239" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E239" s="5" t="s">
@@ -15443,7 +15443,7 @@
       <c r="C241" s="5" t="s">
         <v>1237</v>
       </c>
-      <c r="D241" s="46" t="s">
+      <c r="D241" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E241" s="5" t="s">
@@ -16127,7 +16127,7 @@
       <c r="C260" s="5" t="s">
         <v>1258</v>
       </c>
-      <c r="D260" s="46" t="s">
+      <c r="D260" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E260" s="5" t="s">
@@ -17457,7 +17457,7 @@
       <c r="C294" s="5" t="s">
         <v>1239</v>
       </c>
-      <c r="D294" s="46" t="s">
+      <c r="D294" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E294" s="5" t="s">
@@ -17525,7 +17525,7 @@
       <c r="C296" s="5" t="s">
         <v>1298</v>
       </c>
-      <c r="D296" s="46" t="s">
+      <c r="D296" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E296" s="5" t="s">
@@ -17597,7 +17597,7 @@
       <c r="C298" s="5" t="s">
         <v>1104</v>
       </c>
-      <c r="D298" s="46" t="s">
+      <c r="D298" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E298" s="5" t="s">
@@ -17633,7 +17633,7 @@
       <c r="C299" s="5" t="s">
         <v>1105</v>
       </c>
-      <c r="D299" s="46" t="s">
+      <c r="D299" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E299" s="5" t="s">
@@ -17849,7 +17849,7 @@
       <c r="C305" s="5" t="s">
         <v>1110</v>
       </c>
-      <c r="D305" s="46" t="s">
+      <c r="D305" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E305" s="5" t="s">
@@ -17893,7 +17893,7 @@
       <c r="C306" s="5" t="s">
         <v>1111</v>
       </c>
-      <c r="D306" s="46" t="s">
+      <c r="D306" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E306" s="5" t="s">
@@ -20169,7 +20169,7 @@
       <c r="C365" s="5" t="s">
         <v>1273</v>
       </c>
-      <c r="D365" s="46" t="s">
+      <c r="D365" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E365" s="5" t="s">
@@ -20211,7 +20211,7 @@
       <c r="C366" s="5" t="s">
         <v>1141</v>
       </c>
-      <c r="D366" s="46" t="s">
+      <c r="D366" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E366" s="5" t="s">
@@ -20253,7 +20253,7 @@
       <c r="C367" s="5" t="s">
         <v>1142</v>
       </c>
-      <c r="D367" s="46" t="s">
+      <c r="D367" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E367" s="5" t="s">
@@ -20405,7 +20405,7 @@
       <c r="C371" s="5" t="s">
         <v>1146</v>
       </c>
-      <c r="D371" s="46" t="s">
+      <c r="D371" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E371" s="5" t="s">
@@ -20629,7 +20629,7 @@
       <c r="C377" s="5" t="s">
         <v>1275</v>
       </c>
-      <c r="D377" s="46" t="s">
+      <c r="D377" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E377" s="5" t="s">
@@ -20709,7 +20709,7 @@
       <c r="C379" s="9" t="s">
         <v>1114</v>
       </c>
-      <c r="D379" s="46" t="s">
+      <c r="D379" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E379" s="5" t="s">
@@ -20745,7 +20745,7 @@
       <c r="C380" s="5" t="s">
         <v>1281</v>
       </c>
-      <c r="D380" s="46" t="s">
+      <c r="D380" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E380" s="5" t="s">
@@ -20823,7 +20823,7 @@
       <c r="C382" s="5" t="s">
         <v>1116</v>
       </c>
-      <c r="D382" s="46" t="s">
+      <c r="D382" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E382" s="5" t="s">
@@ -20945,7 +20945,7 @@
       <c r="C385" s="5" t="s">
         <v>1136</v>
       </c>
-      <c r="D385" s="46" t="s">
+      <c r="D385" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E385" s="5" t="s">
@@ -21377,7 +21377,7 @@
       <c r="C397" s="5" t="s">
         <v>1117</v>
       </c>
-      <c r="D397" s="46" t="s">
+      <c r="D397" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E397" s="5" t="s">
@@ -21567,7 +21567,7 @@
       <c r="C402" s="5" t="s">
         <v>1139</v>
       </c>
-      <c r="D402" s="46" t="s">
+      <c r="D402" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E402" s="5" t="s">
@@ -21647,7 +21647,7 @@
       <c r="C404" s="5" t="s">
         <v>1265</v>
       </c>
-      <c r="D404" s="46" t="s">
+      <c r="D404" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E404" s="5" t="s">
@@ -22025,7 +22025,7 @@
       <c r="C414" s="5" t="s">
         <v>1328</v>
       </c>
-      <c r="D414" s="46" t="s">
+      <c r="D414" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E414" s="5" t="s">
@@ -22055,7 +22055,7 @@
       <c r="C415" s="5" t="s">
         <v>1119</v>
       </c>
-      <c r="D415" s="46" t="s">
+      <c r="D415" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E415" s="5" t="s">
@@ -22133,7 +22133,7 @@
       <c r="C417" s="5" t="s">
         <v>1149</v>
       </c>
-      <c r="D417" s="46" t="s">
+      <c r="D417" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E417" s="5" t="s">
@@ -22395,7 +22395,7 @@
       <c r="C424" s="5" t="s">
         <v>1120</v>
       </c>
-      <c r="D424" s="46" t="s">
+      <c r="D424" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E424" s="5" t="s">
@@ -22429,7 +22429,7 @@
       <c r="C425" s="5" t="s">
         <v>1121</v>
       </c>
-      <c r="D425" s="46" t="s">
+      <c r="D425" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E425" s="5" t="s">
@@ -22463,7 +22463,7 @@
       <c r="C426" s="5" t="s">
         <v>1276</v>
       </c>
-      <c r="D426" s="46" t="s">
+      <c r="D426" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E426" s="5" t="s">
@@ -22949,7 +22949,7 @@
       <c r="C439" s="5" t="s">
         <v>1155</v>
       </c>
-      <c r="D439" s="46" t="s">
+      <c r="D439" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E439" s="5" t="s">
@@ -22983,7 +22983,7 @@
       <c r="C440" s="5" t="s">
         <v>1138</v>
       </c>
-      <c r="D440" s="46" t="s">
+      <c r="D440" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E440" s="5" t="s">
@@ -23129,7 +23129,7 @@
       <c r="C444" s="5" t="s">
         <v>1277</v>
       </c>
-      <c r="D444" s="46" t="s">
+      <c r="D444" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E444" s="5" t="s">
@@ -23207,7 +23207,7 @@
       <c r="C446" s="5" t="s">
         <v>1306</v>
       </c>
-      <c r="D446" s="46" t="s">
+      <c r="D446" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E446" s="5" t="s">
@@ -39637,7 +39637,7 @@
       <c r="C836" s="5" t="s">
         <v>1124</v>
       </c>
-      <c r="D836" s="46" t="s">
+      <c r="D836" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E836" s="5" t="s">
@@ -39937,7 +39937,7 @@
       <c r="C844" s="5" t="s">
         <v>1160</v>
       </c>
-      <c r="D844" s="46" t="s">
+      <c r="D844" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E844" s="5" t="s">
@@ -40121,7 +40121,7 @@
       <c r="C849" s="5" t="s">
         <v>1317</v>
       </c>
-      <c r="D849" s="46" t="s">
+      <c r="D849" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E849" s="5" t="s">
@@ -40269,7 +40269,7 @@
       <c r="C853" s="9" t="s">
         <v>1156</v>
       </c>
-      <c r="D853" s="46" t="s">
+      <c r="D853" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E853" s="5" t="s">
@@ -40311,7 +40311,7 @@
       <c r="C854" s="5" t="s">
         <v>1233</v>
       </c>
-      <c r="D854" s="46" t="s">
+      <c r="D854" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E854" s="5" t="s">
@@ -40389,7 +40389,7 @@
       <c r="C856" s="5" t="s">
         <v>1163</v>
       </c>
-      <c r="D856" s="46" t="s">
+      <c r="D856" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E856" s="5" t="s">
@@ -40425,7 +40425,7 @@
       <c r="C857" s="9" t="s">
         <v>1165</v>
       </c>
-      <c r="D857" s="45" t="s">
+      <c r="D857" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E857" s="9" t="s">
@@ -41057,7 +41057,7 @@
       <c r="C873" s="9" t="s">
         <v>1123</v>
       </c>
-      <c r="D873" s="45" t="s">
+      <c r="D873" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E873" s="9" t="s">
@@ -41739,7 +41739,7 @@
       <c r="C892" s="9" t="s">
         <v>1126</v>
       </c>
-      <c r="D892" s="45" t="s">
+      <c r="D892" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E892" s="9" t="s">
@@ -41773,7 +41773,7 @@
       <c r="C893" s="9" t="s">
         <v>1232</v>
       </c>
-      <c r="D893" s="45" t="s">
+      <c r="D893" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E893" s="9" t="s">
@@ -41807,7 +41807,7 @@
       <c r="C894" s="9" t="s">
         <v>1234</v>
       </c>
-      <c r="D894" s="45" t="s">
+      <c r="D894" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E894" s="9" t="s">
@@ -41841,7 +41841,7 @@
       <c r="C895" s="9" t="s">
         <v>1164</v>
       </c>
-      <c r="D895" s="45" t="s">
+      <c r="D895" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E895" s="9" t="s">
@@ -42049,7 +42049,7 @@
       <c r="C900" s="9" t="s">
         <v>1115</v>
       </c>
-      <c r="D900" s="45" t="s">
+      <c r="D900" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E900" s="9" t="s">
@@ -42201,7 +42201,7 @@
       <c r="C904" s="5" t="s">
         <v>1222</v>
       </c>
-      <c r="D904" s="46" t="s">
+      <c r="D904" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E904" s="5" t="s">
@@ -42241,7 +42241,7 @@
       <c r="C905" s="5" t="s">
         <v>1127</v>
       </c>
-      <c r="D905" s="46" t="s">
+      <c r="D905" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E905" s="5" t="s">
@@ -42833,7 +42833,7 @@
       <c r="C921" s="5" t="s">
         <v>1169</v>
       </c>
-      <c r="D921" s="46" t="s">
+      <c r="D921" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E921" s="5" t="s">
@@ -42877,7 +42877,7 @@
       <c r="C922" s="5" t="s">
         <v>1170</v>
       </c>
-      <c r="D922" s="46" t="s">
+      <c r="D922" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E922" s="5" t="s">
@@ -42981,7 +42981,7 @@
       <c r="C925" s="5" t="s">
         <v>1132</v>
       </c>
-      <c r="D925" s="46" t="s">
+      <c r="D925" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E925" s="5" t="s">
@@ -43129,7 +43129,7 @@
       <c r="C929" s="5" t="s">
         <v>1171</v>
       </c>
-      <c r="D929" s="46" t="s">
+      <c r="D929" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E929" s="5" t="s">
@@ -43351,7 +43351,7 @@
       <c r="C935" s="5" t="s">
         <v>1172</v>
       </c>
-      <c r="D935" s="46" t="s">
+      <c r="D935" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E935" s="5" t="s">
@@ -43385,7 +43385,7 @@
       <c r="C936" s="9" t="s">
         <v>1173</v>
       </c>
-      <c r="D936" s="45" t="s">
+      <c r="D936" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E936" s="9" t="s">
@@ -43615,7 +43615,7 @@
       <c r="C942" s="5" t="s">
         <v>1185</v>
       </c>
-      <c r="D942" s="46" t="s">
+      <c r="D942" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E942" s="5" t="s">
@@ -43759,7 +43759,7 @@
       <c r="C946" s="5" t="s">
         <v>1274</v>
       </c>
-      <c r="D946" s="46" t="s">
+      <c r="D946" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E946" s="5" t="s">
@@ -43989,7 +43989,7 @@
       <c r="C952" s="5" t="s">
         <v>1230</v>
       </c>
-      <c r="D952" s="46" t="s">
+      <c r="D952" s="45" t="s">
         <v>4</v>
       </c>
       <c r="E952" s="5" t="s">
@@ -51693,7 +51693,7 @@
       <c r="C1137" s="10" t="s">
         <v>1178</v>
       </c>
-      <c r="D1137" s="47" t="s">
+      <c r="D1137" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E1137" s="10" t="s">
@@ -51727,7 +51727,7 @@
       <c r="C1138" s="10" t="s">
         <v>1133</v>
       </c>
-      <c r="D1138" s="47" t="s">
+      <c r="D1138" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E1138" s="10" t="s">
@@ -51833,7 +51833,7 @@
       <c r="C1141" s="10" t="s">
         <v>1179</v>
       </c>
-      <c r="D1141" s="47" t="s">
+      <c r="D1141" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E1141" s="10" t="s">
@@ -51937,7 +51937,7 @@
       <c r="C1144" s="10" t="s">
         <v>1148</v>
       </c>
-      <c r="D1144" s="47" t="s">
+      <c r="D1144" s="46" t="s">
         <v>5</v>
       </c>
       <c r="E1144" s="10" t="s">
@@ -52077,7 +52077,7 @@
       <c r="C1148" s="10" t="s">
         <v>1223</v>
       </c>
-      <c r="D1148" s="47" t="s">
+      <c r="D1148" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E1148" s="10" t="s">
@@ -52117,7 +52117,7 @@
       <c r="C1149" s="8" t="s">
         <v>1250</v>
       </c>
-      <c r="D1149" s="45" t="s">
+      <c r="D1149" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E1149" s="10" t="s">
@@ -52493,7 +52493,7 @@
       <c r="C1159" s="10" t="s">
         <v>1193</v>
       </c>
-      <c r="D1159" s="47" t="s">
+      <c r="D1159" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E1159" s="10" t="s">
@@ -52533,7 +52533,7 @@
       <c r="C1160" s="10" t="s">
         <v>1255</v>
       </c>
-      <c r="D1160" s="47" t="s">
+      <c r="D1160" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E1160" s="10" t="s">
@@ -52569,7 +52569,7 @@
       <c r="C1161" s="8" t="s">
         <v>1188</v>
       </c>
-      <c r="D1161" s="45" t="s">
+      <c r="D1161" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E1161" s="10" t="s">
@@ -52605,7 +52605,7 @@
       <c r="C1162" s="8" t="s">
         <v>1191</v>
       </c>
-      <c r="D1162" s="45" t="s">
+      <c r="D1162" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E1162" s="10" t="s">
@@ -52647,7 +52647,7 @@
       <c r="C1163" s="10" t="s">
         <v>1189</v>
       </c>
-      <c r="D1163" s="47" t="s">
+      <c r="D1163" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E1163" s="10" t="s">
@@ -52683,7 +52683,7 @@
       <c r="C1164" s="8" t="s">
         <v>1247</v>
       </c>
-      <c r="D1164" s="45" t="s">
+      <c r="D1164" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E1164" s="8" t="s">
@@ -52717,7 +52717,7 @@
       <c r="C1165" s="8" t="s">
         <v>1254</v>
       </c>
-      <c r="D1165" s="45" t="s">
+      <c r="D1165" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E1165" s="8" t="s">
@@ -52755,7 +52755,7 @@
       <c r="C1166" s="8" t="s">
         <v>1192</v>
       </c>
-      <c r="D1166" s="45" t="s">
+      <c r="D1166" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E1166" s="8" t="s">
@@ -52791,7 +52791,7 @@
       <c r="C1167" s="8" t="s">
         <v>1194</v>
       </c>
-      <c r="D1167" s="45" t="s">
+      <c r="D1167" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E1167" s="8" t="s">
@@ -52835,7 +52835,7 @@
       <c r="C1168" s="8" t="s">
         <v>1195</v>
       </c>
-      <c r="D1168" s="44" t="s">
+      <c r="D1168" s="43" t="s">
         <v>4</v>
       </c>
       <c r="E1168" s="8" t="s">
@@ -52877,7 +52877,7 @@
       <c r="C1169" s="8" t="s">
         <v>1129</v>
       </c>
-      <c r="D1169" s="44" t="s">
+      <c r="D1169" s="43" t="s">
         <v>4</v>
       </c>
       <c r="E1169" s="8" t="s">
@@ -52911,7 +52911,7 @@
       <c r="C1170" s="8" t="s">
         <v>1130</v>
       </c>
-      <c r="D1170" s="47" t="s">
+      <c r="D1170" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E1170" s="10" t="s">
@@ -53441,7 +53441,7 @@
       <c r="C1184" s="10" t="s">
         <v>1128</v>
       </c>
-      <c r="D1184" s="47" t="s">
+      <c r="D1184" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E1184" s="10" t="s">
@@ -53605,7 +53605,7 @@
       <c r="C1188" s="10" t="s">
         <v>1131</v>
       </c>
-      <c r="D1188" s="47" t="s">
+      <c r="D1188" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E1188" s="10" t="s">
@@ -53639,7 +53639,7 @@
       <c r="C1189" s="10" t="s">
         <v>1252</v>
       </c>
-      <c r="D1189" s="47" t="s">
+      <c r="D1189" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E1189" s="10" t="s">
@@ -53673,7 +53673,7 @@
       <c r="C1190" s="8" t="s">
         <v>1245</v>
       </c>
-      <c r="D1190" s="44" t="s">
+      <c r="D1190" s="43" t="s">
         <v>4</v>
       </c>
       <c r="E1190" s="10" t="s">
@@ -53883,7 +53883,7 @@
       <c r="C1196" s="8" t="s">
         <v>1197</v>
       </c>
-      <c r="D1196" s="44" t="s">
+      <c r="D1196" s="43" t="s">
         <v>4</v>
       </c>
       <c r="E1196" s="8" t="s">
@@ -54023,7 +54023,7 @@
       <c r="C1200" s="8" t="s">
         <v>1209</v>
       </c>
-      <c r="D1200" s="45" t="s">
+      <c r="D1200" s="44" t="s">
         <v>4</v>
       </c>
       <c r="E1200" s="8" t="s">
@@ -54129,7 +54129,7 @@
       <c r="C1203" s="8" t="s">
         <v>1283</v>
       </c>
-      <c r="D1203" s="47" t="s">
+      <c r="D1203" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E1203" s="10" t="s">
@@ -54171,7 +54171,7 @@
       <c r="C1204" s="10" t="s">
         <v>1326</v>
       </c>
-      <c r="D1204" s="47" t="s">
+      <c r="D1204" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E1204" s="10" t="s">
@@ -54205,7 +54205,7 @@
       <c r="C1205" s="8" t="s">
         <v>1198</v>
       </c>
-      <c r="D1205" s="44" t="s">
+      <c r="D1205" s="43" t="s">
         <v>4</v>
       </c>
       <c r="E1205" s="8" t="s">
@@ -54245,7 +54245,7 @@
       <c r="C1206" s="8" t="s">
         <v>1296</v>
       </c>
-      <c r="D1206" s="44" t="s">
+      <c r="D1206" s="43" t="s">
         <v>4</v>
       </c>
       <c r="E1206" s="8" t="s">
@@ -54321,7 +54321,7 @@
         <v>4</v>
       </c>
       <c r="E1208" s="8" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="F1208" s="8"/>
       <c r="G1208" s="8" t="s">
@@ -54363,7 +54363,7 @@
         <v>4</v>
       </c>
       <c r="E1209" s="8" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="F1209" s="8"/>
       <c r="G1209" s="8" t="s">
@@ -54405,7 +54405,7 @@
         <v>4</v>
       </c>
       <c r="E1210" s="8" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="F1210" s="10"/>
       <c r="G1210" s="10" t="s">
@@ -54447,7 +54447,7 @@
         <v>4</v>
       </c>
       <c r="E1211" s="8" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="F1211" s="8"/>
       <c r="G1211" s="8" t="s">
@@ -54489,7 +54489,7 @@
         <v>4</v>
       </c>
       <c r="E1212" s="8" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="F1212" s="10"/>
       <c r="G1212" s="10" t="s">
@@ -54531,7 +54531,7 @@
         <v>4</v>
       </c>
       <c r="E1213" s="8" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="F1213" s="10"/>
       <c r="G1213" s="10" t="s">
@@ -54573,7 +54573,7 @@
         <v>4</v>
       </c>
       <c r="E1214" s="8" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="F1214" s="8"/>
       <c r="G1214" s="8" t="s">
@@ -54615,7 +54615,7 @@
         <v>4</v>
       </c>
       <c r="E1215" s="8" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="F1215" s="8"/>
       <c r="G1215" s="8" t="s">
@@ -54657,7 +54657,7 @@
         <v>4</v>
       </c>
       <c r="E1216" s="8" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="F1216" s="8"/>
       <c r="G1216" s="8" t="s">
@@ -54699,7 +54699,7 @@
         <v>4</v>
       </c>
       <c r="E1217" s="8" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="F1217" s="10"/>
       <c r="G1217" s="10" t="s">
@@ -54741,7 +54741,7 @@
         <v>4</v>
       </c>
       <c r="E1218" s="8" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="F1218" s="10"/>
       <c r="G1218" s="10" t="s">
@@ -54783,7 +54783,7 @@
         <v>4</v>
       </c>
       <c r="E1219" s="8" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="F1219" s="10"/>
       <c r="G1219" s="10" t="s">
@@ -54825,7 +54825,7 @@
         <v>4</v>
       </c>
       <c r="E1220" s="8" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="F1220" s="10"/>
       <c r="G1220" s="10" t="s">
@@ -54867,7 +54867,7 @@
         <v>4</v>
       </c>
       <c r="E1221" s="8" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="F1221" s="10"/>
       <c r="G1221" s="10" t="s">
@@ -54909,7 +54909,7 @@
         <v>4</v>
       </c>
       <c r="E1222" s="8" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="F1222" s="10"/>
       <c r="G1222" s="10" t="s">
@@ -54951,7 +54951,7 @@
         <v>4</v>
       </c>
       <c r="E1223" s="8" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="F1223" s="10"/>
       <c r="G1223" s="10"/>
@@ -54991,7 +54991,7 @@
         <v>4</v>
       </c>
       <c r="E1224" s="8" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="F1224" s="10"/>
       <c r="G1224" s="10" t="s">
@@ -55033,7 +55033,7 @@
         <v>4</v>
       </c>
       <c r="E1225" s="8" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="F1225" s="10"/>
       <c r="G1225" s="10" t="s">
@@ -55075,7 +55075,7 @@
         <v>4</v>
       </c>
       <c r="E1226" s="8" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="F1226" s="10"/>
       <c r="G1226" s="10" t="s">
@@ -55189,7 +55189,7 @@
       <c r="C1229" s="10" t="s">
         <v>1202</v>
       </c>
-      <c r="D1229" s="47" t="s">
+      <c r="D1229" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E1229" s="10" t="s">
@@ -55225,7 +55225,7 @@
       <c r="C1230" s="10" t="s">
         <v>1207</v>
       </c>
-      <c r="D1230" s="47" t="s">
+      <c r="D1230" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E1230" s="10" t="s">
@@ -56283,7 +56283,7 @@
       <c r="C1254" s="10" t="s">
         <v>1203</v>
       </c>
-      <c r="D1254" s="47" t="s">
+      <c r="D1254" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E1254" s="10" t="s">
@@ -57739,7 +57739,7 @@
       <c r="C1292" s="8" t="s">
         <v>1231</v>
       </c>
-      <c r="D1292" s="44" t="s">
+      <c r="D1292" s="43" t="s">
         <v>4</v>
       </c>
       <c r="E1292" s="8" t="s">
@@ -57997,7 +57997,7 @@
       <c r="C1299" s="10" t="s">
         <v>1327</v>
       </c>
-      <c r="D1299" s="47" t="s">
+      <c r="D1299" s="46" t="s">
         <v>4</v>
       </c>
       <c r="E1299" s="10" t="s">
@@ -59297,7 +59297,7 @@
       <c r="C1333" s="10" t="s">
         <v>1257</v>
       </c>
-      <c r="D1333" s="44" t="s">
+      <c r="D1333" s="43" t="s">
         <v>4</v>
       </c>
       <c r="E1333" s="10" t="s">
@@ -59333,7 +59333,7 @@
       <c r="C1334" s="10" t="s">
         <v>1280</v>
       </c>
-      <c r="D1334" s="44" t="s">
+      <c r="D1334" s="43" t="s">
         <v>4</v>
       </c>
       <c r="E1334" s="10" t="s">
@@ -59409,7 +59409,7 @@
       <c r="C1336" s="8" t="s">
         <v>1200</v>
       </c>
-      <c r="D1336" s="44" t="s">
+      <c r="D1336" s="43" t="s">
         <v>4</v>
       </c>
       <c r="E1336" s="8" t="s">
@@ -59445,7 +59445,7 @@
       <c r="C1337" s="8" t="s">
         <v>1201</v>
       </c>
-      <c r="D1337" s="44" t="s">
+      <c r="D1337" s="43" t="s">
         <v>4</v>
       </c>
       <c r="E1337" s="8" t="s">
@@ -59481,7 +59481,7 @@
       <c r="C1338" s="8" t="s">
         <v>1294</v>
       </c>
-      <c r="D1338" s="44" t="s">
+      <c r="D1338" s="43" t="s">
         <v>4</v>
       </c>
       <c r="E1338" s="8" t="s">
@@ -59940,13 +59940,13 @@
       <c r="A2" s="9">
         <v>1</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="35" t="s">
         <v>1428</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>1243</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="9" t="s">
@@ -59980,10 +59980,10 @@
       <c r="C3" s="5" t="s">
         <v>554</v>
       </c>
-      <c r="D3" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="37" t="s">
+      <c r="D3" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="36" t="s">
         <v>1096</v>
       </c>
       <c r="F3" s="5"/>
@@ -60016,10 +60016,10 @@
       <c r="C4" s="5" t="s">
         <v>554</v>
       </c>
-      <c r="D4" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="37" t="s">
+      <c r="D4" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="36" t="s">
         <v>1096</v>
       </c>
       <c r="F4" s="5"/>
@@ -60046,16 +60046,16 @@
       <c r="A5" s="9">
         <v>2</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="35" t="s">
         <v>1420</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>554</v>
       </c>
-      <c r="D5" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="37" t="s">
+      <c r="D5" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="36" t="s">
         <v>1074</v>
       </c>
       <c r="F5" s="9"/>
@@ -60086,7 +60086,7 @@
       <c r="C6" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="D6" s="34" t="s">
+      <c r="D6" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E6" s="5" t="s">
@@ -60124,7 +60124,7 @@
       <c r="C7" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="D7" s="34" t="s">
+      <c r="D7" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E7" s="5" t="s">
@@ -60162,7 +60162,7 @@
       <c r="C8" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="D8" s="34" t="s">
+      <c r="D8" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E8" s="5" t="s">
@@ -60200,7 +60200,7 @@
       <c r="C9" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="D9" s="34" t="s">
+      <c r="D9" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E9" s="5" t="s">
@@ -60238,7 +60238,7 @@
       <c r="C10" s="5" t="s">
         <v>481</v>
       </c>
-      <c r="D10" s="34" t="s">
+      <c r="D10" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E10" s="5" t="s">
@@ -60270,16 +60270,16 @@
       <c r="A11" s="9">
         <v>4</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="35" t="s">
         <v>1415</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>1238</v>
       </c>
-      <c r="D11" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" s="36" t="s">
+      <c r="D11" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="35" t="s">
         <v>1732</v>
       </c>
       <c r="F11" s="9"/>
@@ -60303,19 +60303,19 @@
       <c r="R11" s="8"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="38">
+      <c r="A12" s="37">
         <v>6</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="35" t="s">
         <v>1615</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>1134</v>
       </c>
-      <c r="D12" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12" s="36" t="s">
+      <c r="D12" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" s="35" t="s">
         <v>1681</v>
       </c>
       <c r="F12" s="9"/>
@@ -60342,13 +60342,13 @@
       <c r="A13" s="9">
         <v>7</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="35" t="s">
         <v>1521</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>1266</v>
       </c>
-      <c r="D13" s="34" t="s">
+      <c r="D13" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E13" t="s">
@@ -60378,13 +60378,13 @@
       <c r="A14" s="9">
         <v>8</v>
       </c>
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="35" t="s">
         <v>1524</v>
       </c>
       <c r="C14" s="9" t="s">
         <v>1267</v>
       </c>
-      <c r="D14" s="34" t="s">
+      <c r="D14" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E14" t="s">
@@ -60411,16 +60411,16 @@
       <c r="R14" s="8"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="38">
+      <c r="A15" s="37">
         <v>10</v>
       </c>
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="35" t="s">
         <v>1653</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>1322</v>
       </c>
-      <c r="D15" s="34" t="s">
+      <c r="D15" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E15" s="9" t="s">
@@ -60447,16 +60447,16 @@
       <c r="R15" s="8"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="38">
+      <c r="A16" s="37">
         <v>11</v>
       </c>
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="35" t="s">
         <v>1617</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>1135</v>
       </c>
-      <c r="D16" s="34" t="s">
+      <c r="D16" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E16" s="9" t="s">
@@ -60483,16 +60483,16 @@
       <c r="R16" s="8"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="38">
+      <c r="A17" s="37">
         <v>12</v>
       </c>
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="35" t="s">
         <v>1654</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>1323</v>
       </c>
-      <c r="D17" s="34" t="s">
+      <c r="D17" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E17" s="9" t="s">
@@ -60522,13 +60522,13 @@
       <c r="A18" s="9">
         <v>13</v>
       </c>
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="35" t="s">
         <v>1343</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>1212</v>
       </c>
-      <c r="D18" s="34" t="s">
+      <c r="D18" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E18" s="9" t="s">
@@ -60558,13 +60558,13 @@
       <c r="A19" s="9">
         <v>23</v>
       </c>
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="35" t="s">
         <v>1525</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>1268</v>
       </c>
-      <c r="D19" s="34" t="s">
+      <c r="D19" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E19" s="9" t="s">
@@ -60594,13 +60594,13 @@
       <c r="A20" s="9">
         <v>26</v>
       </c>
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="35" t="s">
         <v>1581</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>1293</v>
       </c>
-      <c r="D20" s="34" t="s">
+      <c r="D20" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E20" s="9" t="s">
@@ -60627,16 +60627,16 @@
       <c r="R20" s="8"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="38">
+      <c r="A21" s="37">
         <v>27</v>
       </c>
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="35" t="s">
         <v>1330</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>1103</v>
       </c>
-      <c r="D21" s="34" t="s">
+      <c r="D21" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E21" s="9" t="s">
@@ -60659,16 +60659,16 @@
       <c r="R21" s="8"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="38">
+      <c r="A22" s="37">
         <v>28</v>
       </c>
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="35" t="s">
         <v>1616</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>1309</v>
       </c>
-      <c r="D22" s="34" t="s">
+      <c r="D22" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E22" s="9" t="s">
@@ -60698,13 +60698,13 @@
       <c r="A23" s="9">
         <v>29</v>
       </c>
-      <c r="B23" s="36" t="s">
+      <c r="B23" s="35" t="s">
         <v>1487</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>1256</v>
       </c>
-      <c r="D23" s="34" t="s">
+      <c r="D23" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E23" s="9" t="s">
@@ -60734,13 +60734,13 @@
       <c r="A24" s="9">
         <v>30</v>
       </c>
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="35" t="s">
         <v>1429</v>
       </c>
       <c r="C24" s="9" t="s">
         <v>1244</v>
       </c>
-      <c r="D24" s="34" t="s">
+      <c r="D24" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E24" s="9" t="s">
@@ -60770,13 +60770,13 @@
       <c r="A25" s="9">
         <v>31</v>
       </c>
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="35" t="s">
         <v>1430</v>
       </c>
       <c r="C25" s="9" t="s">
         <v>1102</v>
       </c>
-      <c r="D25" s="34" t="s">
+      <c r="D25" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E25" s="9" t="s">
@@ -60803,16 +60803,16 @@
       <c r="R25" s="8"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A26" s="38">
+      <c r="A26" s="37">
         <v>32</v>
       </c>
-      <c r="B26" s="36" t="s">
+      <c r="B26" s="35" t="s">
         <v>1618</v>
       </c>
       <c r="C26" s="9" t="s">
         <v>1310</v>
       </c>
-      <c r="D26" s="34" t="s">
+      <c r="D26" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E26" s="9" t="s">
@@ -60842,13 +60842,13 @@
       <c r="A27" s="9">
         <v>33</v>
       </c>
-      <c r="B27" s="36" t="s">
+      <c r="B27" s="35" t="s">
         <v>1427</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>1242</v>
       </c>
-      <c r="D27" s="34" t="s">
+      <c r="D27" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E27" s="9" t="s">
@@ -60878,13 +60878,13 @@
       <c r="A28" s="9">
         <v>34</v>
       </c>
-      <c r="B28" s="36" t="s">
+      <c r="B28" s="35" t="s">
         <v>1425</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>1240</v>
       </c>
-      <c r="D28" s="34" t="s">
+      <c r="D28" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E28" s="9" t="s">
@@ -60914,13 +60914,13 @@
       <c r="A29" s="9">
         <v>35</v>
       </c>
-      <c r="B29" s="36" t="s">
+      <c r="B29" s="35" t="s">
         <v>1426</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>1241</v>
       </c>
-      <c r="D29" s="34" t="s">
+      <c r="D29" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E29" s="9" t="s">
@@ -60947,16 +60947,16 @@
       <c r="R29" s="8"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="38">
+      <c r="A30" s="37">
         <v>38</v>
       </c>
-      <c r="B30" s="36" t="s">
+      <c r="B30" s="35" t="s">
         <v>1649</v>
       </c>
       <c r="C30" s="9" t="s">
         <v>1320</v>
       </c>
-      <c r="D30" s="34" t="s">
+      <c r="D30" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E30" s="9" t="s">
@@ -60983,16 +60983,16 @@
       <c r="R30" s="8"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A31" s="38">
+      <c r="A31" s="37">
         <v>42</v>
       </c>
-      <c r="B31" s="36" t="s">
+      <c r="B31" s="35" t="s">
         <v>1646</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>1318</v>
       </c>
-      <c r="D31" s="34" t="s">
+      <c r="D31" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E31" s="9" t="s">
@@ -61019,16 +61019,16 @@
       <c r="R31" s="8"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="38">
+      <c r="A32" s="37">
         <v>43</v>
       </c>
-      <c r="B32" s="36" t="s">
+      <c r="B32" s="35" t="s">
         <v>1619</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>1311</v>
       </c>
-      <c r="D32" s="34" t="s">
+      <c r="D32" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E32" s="9" t="s">
@@ -61058,13 +61058,13 @@
       <c r="A33" s="9">
         <v>45</v>
       </c>
-      <c r="B33" s="36" t="s">
+      <c r="B33" s="35" t="s">
         <v>1414</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>1237</v>
       </c>
-      <c r="D33" s="34" t="s">
+      <c r="D33" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E33" s="9" t="s">
@@ -61094,13 +61094,13 @@
       <c r="A34" s="9">
         <v>64</v>
       </c>
-      <c r="B34" s="36" t="s">
+      <c r="B34" s="35" t="s">
         <v>1496</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>1258</v>
       </c>
-      <c r="D34" s="34" t="s">
+      <c r="D34" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E34" s="9" t="s">
@@ -61130,13 +61130,13 @@
       <c r="A35" s="9">
         <v>81</v>
       </c>
-      <c r="B35" s="36" t="s">
+      <c r="B35" s="35" t="s">
         <v>1419</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>1239</v>
       </c>
-      <c r="D35" s="34" t="s">
+      <c r="D35" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E35" s="9" t="s">
@@ -61161,16 +61161,16 @@
       <c r="R35" s="8"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" s="38">
+      <c r="A36" s="37">
         <v>83</v>
       </c>
-      <c r="B36" s="36" t="s">
+      <c r="B36" s="35" t="s">
         <v>1592</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>1298</v>
       </c>
-      <c r="D36" s="34" t="s">
+      <c r="D36" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E36" s="9" t="s">
@@ -61198,16 +61198,16 @@
       <c r="A37" s="9">
         <v>85</v>
       </c>
-      <c r="B37" s="36" t="s">
+      <c r="B37" s="35" t="s">
         <v>1485</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>1104</v>
       </c>
-      <c r="D37" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="E37" s="37" t="s">
+      <c r="D37" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="36" t="s">
         <v>1693</v>
       </c>
       <c r="F37" s="9"/>
@@ -61231,16 +61231,16 @@
       <c r="R37" s="8"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A38" s="38">
+      <c r="A38" s="37">
         <v>86</v>
       </c>
-      <c r="B38" s="36" t="s">
+      <c r="B38" s="35" t="s">
         <v>1590</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>1105</v>
       </c>
-      <c r="D38" s="34" t="s">
+      <c r="D38" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E38" s="9" t="s">
@@ -61270,13 +61270,13 @@
       <c r="A39" s="9">
         <v>92</v>
       </c>
-      <c r="B39" s="36" t="s">
+      <c r="B39" s="35" t="s">
         <v>1546</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>1110</v>
       </c>
-      <c r="D39" s="34" t="s">
+      <c r="D39" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E39" s="9" t="s">
@@ -61311,16 +61311,16 @@
       <c r="R39" s="8"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" s="38">
+      <c r="A40" s="37">
         <v>93</v>
       </c>
-      <c r="B40" s="36" t="s">
+      <c r="B40" s="35" t="s">
         <v>1342</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>1111</v>
       </c>
-      <c r="D40" s="34" t="s">
+      <c r="D40" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E40" s="9" t="s">
@@ -61350,13 +61350,13 @@
       <c r="A41" s="9">
         <v>111</v>
       </c>
-      <c r="B41" s="36" t="s">
+      <c r="B41" s="35" t="s">
         <v>1538</v>
       </c>
       <c r="C41" s="9" t="s">
         <v>1273</v>
       </c>
-      <c r="D41" s="34" t="s">
+      <c r="D41" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E41" s="9" t="s">
@@ -61392,13 +61392,13 @@
       <c r="A42" s="9">
         <v>112</v>
       </c>
-      <c r="B42" s="36" t="s">
+      <c r="B42" s="35" t="s">
         <v>1530</v>
       </c>
       <c r="C42" s="9" t="s">
         <v>1141</v>
       </c>
-      <c r="D42" s="34" t="s">
+      <c r="D42" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E42" s="9" t="s">
@@ -61431,16 +61431,16 @@
       <c r="R42" s="8"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" s="38">
+      <c r="A43" s="37">
         <v>113</v>
       </c>
-      <c r="B43" s="36" t="s">
+      <c r="B43" s="35" t="s">
         <v>1614</v>
       </c>
       <c r="C43" s="9" t="s">
         <v>1142</v>
       </c>
-      <c r="D43" s="34" t="s">
+      <c r="D43" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E43" s="9" t="s">
@@ -61470,13 +61470,13 @@
       <c r="A44" s="9">
         <v>116</v>
       </c>
-      <c r="B44" s="36" t="s">
+      <c r="B44" s="35" t="s">
         <v>1433</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>1146</v>
       </c>
-      <c r="D44" s="34" t="s">
+      <c r="D44" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E44" s="9" t="s">
@@ -61506,13 +61506,13 @@
       <c r="A45" s="9">
         <v>120</v>
       </c>
-      <c r="B45" s="36" t="s">
+      <c r="B45" s="35" t="s">
         <v>1540</v>
       </c>
       <c r="C45" s="9" t="s">
         <v>1275</v>
       </c>
-      <c r="D45" s="34" t="s">
+      <c r="D45" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E45" s="9" t="s">
@@ -61550,16 +61550,16 @@
       <c r="A46" s="9">
         <v>122</v>
       </c>
-      <c r="B46" s="36" t="s">
+      <c r="B46" s="35" t="s">
         <v>1375</v>
       </c>
       <c r="C46" s="9" t="s">
         <v>1114</v>
       </c>
-      <c r="D46" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="E46" s="36" t="s">
+      <c r="D46" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E46" s="35" t="s">
         <v>1094</v>
       </c>
       <c r="F46" s="9"/>
@@ -61586,16 +61586,16 @@
       <c r="A47" s="9">
         <v>123</v>
       </c>
-      <c r="B47" s="36" t="s">
+      <c r="B47" s="35" t="s">
         <v>1553</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>1281</v>
       </c>
-      <c r="D47" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="E47" s="36" t="s">
+      <c r="D47" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E47" s="35" t="s">
         <v>1101</v>
       </c>
       <c r="F47" s="9"/>
@@ -61625,16 +61625,16 @@
       <c r="R47" s="8"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A48" s="38">
+      <c r="A48" s="37">
         <v>125</v>
       </c>
-      <c r="B48" s="36" t="s">
+      <c r="B48" s="35" t="s">
         <v>1665</v>
       </c>
       <c r="C48" s="9" t="s">
         <v>1116</v>
       </c>
-      <c r="D48" s="34" t="s">
+      <c r="D48" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E48" s="9" t="s">
@@ -61668,13 +61668,13 @@
       <c r="A49" s="9">
         <v>127</v>
       </c>
-      <c r="B49" s="36" t="s">
+      <c r="B49" s="35" t="s">
         <v>1446</v>
       </c>
       <c r="C49" s="9" t="s">
         <v>1136</v>
       </c>
-      <c r="D49" s="34" t="s">
+      <c r="D49" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E49" s="9" t="s">
@@ -61702,13 +61702,13 @@
       <c r="A50" s="9">
         <v>131</v>
       </c>
-      <c r="B50" s="36" t="s">
+      <c r="B50" s="35" t="s">
         <v>1483</v>
       </c>
       <c r="C50" s="9" t="s">
         <v>1117</v>
       </c>
-      <c r="D50" s="34" t="s">
+      <c r="D50" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E50" s="9" t="s">
@@ -61736,13 +61736,13 @@
       <c r="A51" s="9">
         <v>136</v>
       </c>
-      <c r="B51" s="36" t="s">
+      <c r="B51" s="35" t="s">
         <v>1447</v>
       </c>
       <c r="C51" s="9" t="s">
         <v>1139</v>
       </c>
-      <c r="D51" s="34" t="s">
+      <c r="D51" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E51" s="9" t="s">
@@ -61772,13 +61772,13 @@
       <c r="A52" s="9">
         <v>138</v>
       </c>
-      <c r="B52" s="36" t="s">
+      <c r="B52" s="35" t="s">
         <v>1520</v>
       </c>
       <c r="C52" s="9" t="s">
         <v>1265</v>
       </c>
-      <c r="D52" s="34" t="s">
+      <c r="D52" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E52" s="9" t="s">
@@ -61811,16 +61811,16 @@
       <c r="R52" s="8"/>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A53" s="38">
+      <c r="A53" s="37">
         <v>145</v>
       </c>
-      <c r="B53" s="36" t="s">
+      <c r="B53" s="35" t="s">
         <v>1664</v>
       </c>
-      <c r="C53" s="39" t="s">
+      <c r="C53" s="38" t="s">
         <v>1328</v>
       </c>
-      <c r="D53" s="34" t="s">
+      <c r="D53" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E53" s="9" t="s">
@@ -61844,13 +61844,13 @@
       <c r="A54" s="9">
         <v>146</v>
       </c>
-      <c r="B54" s="36" t="s">
+      <c r="B54" s="35" t="s">
         <v>1370</v>
       </c>
       <c r="C54" s="9" t="s">
         <v>1119</v>
       </c>
-      <c r="D54" s="34" t="s">
+      <c r="D54" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E54" s="9" t="s">
@@ -61880,13 +61880,13 @@
       <c r="A55" s="9">
         <v>148</v>
       </c>
-      <c r="B55" s="36" t="s">
+      <c r="B55" s="35" t="s">
         <v>1395</v>
       </c>
       <c r="C55" s="9" t="s">
         <v>1149</v>
       </c>
-      <c r="D55" s="34" t="s">
+      <c r="D55" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E55" s="9" t="s">
@@ -61916,13 +61916,13 @@
       <c r="A56" s="9">
         <v>150</v>
       </c>
-      <c r="B56" s="36" t="s">
+      <c r="B56" s="35" t="s">
         <v>1423</v>
       </c>
       <c r="C56" s="9" t="s">
         <v>1120</v>
       </c>
-      <c r="D56" s="34" t="s">
+      <c r="D56" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E56" s="9" t="s">
@@ -61950,13 +61950,13 @@
       <c r="A57" s="9">
         <v>151</v>
       </c>
-      <c r="B57" s="36" t="s">
+      <c r="B57" s="35" t="s">
         <v>1440</v>
       </c>
       <c r="C57" s="9" t="s">
         <v>1121</v>
       </c>
-      <c r="D57" s="34" t="s">
+      <c r="D57" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E57" s="9" t="s">
@@ -61984,13 +61984,13 @@
       <c r="A58" s="9">
         <v>152</v>
       </c>
-      <c r="B58" s="36" t="s">
+      <c r="B58" s="35" t="s">
         <v>1541</v>
       </c>
       <c r="C58" s="9" t="s">
         <v>1276</v>
       </c>
-      <c r="D58" s="34" t="s">
+      <c r="D58" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E58" s="9" t="s">
@@ -62028,13 +62028,13 @@
       <c r="A59" s="9">
         <v>162</v>
       </c>
-      <c r="B59" s="36" t="s">
+      <c r="B59" s="35" t="s">
         <v>1455</v>
       </c>
       <c r="C59" s="9" t="s">
         <v>1155</v>
       </c>
-      <c r="D59" s="34" t="s">
+      <c r="D59" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E59" s="9" t="s">
@@ -62062,13 +62062,13 @@
       <c r="A60" s="9">
         <v>163</v>
       </c>
-      <c r="B60" s="36" t="s">
+      <c r="B60" s="35" t="s">
         <v>1418</v>
       </c>
       <c r="C60" s="9" t="s">
         <v>1138</v>
       </c>
-      <c r="D60" s="34" t="s">
+      <c r="D60" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E60" s="9" t="s">
@@ -62096,13 +62096,13 @@
       <c r="A61" s="9">
         <v>166</v>
       </c>
-      <c r="B61" s="36" t="s">
+      <c r="B61" s="35" t="s">
         <v>1542</v>
       </c>
       <c r="C61" s="9" t="s">
         <v>1277</v>
       </c>
-      <c r="D61" s="34" t="s">
+      <c r="D61" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E61" s="9" t="s">
@@ -62135,16 +62135,16 @@
       <c r="R61" s="8"/>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A62" s="38">
+      <c r="A62" s="37">
         <v>168</v>
       </c>
-      <c r="B62" s="36" t="s">
+      <c r="B62" s="35" t="s">
         <v>1610</v>
       </c>
       <c r="C62" s="9" t="s">
         <v>1306</v>
       </c>
-      <c r="D62" s="34" t="s">
+      <c r="D62" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E62" s="9" t="s">
@@ -62172,13 +62172,13 @@
       <c r="A63" s="9">
         <v>178</v>
       </c>
-      <c r="B63" s="36" t="s">
+      <c r="B63" s="35" t="s">
         <v>1434</v>
       </c>
       <c r="C63" s="9" t="s">
         <v>1124</v>
       </c>
-      <c r="D63" s="34" t="s">
+      <c r="D63" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E63" s="9" t="s">
@@ -62206,13 +62206,13 @@
       <c r="A64" s="9">
         <v>182</v>
       </c>
-      <c r="B64" s="36" t="s">
+      <c r="B64" s="35" t="s">
         <v>1467</v>
       </c>
       <c r="C64" s="9" t="s">
         <v>1160</v>
       </c>
-      <c r="D64" s="34" t="s">
+      <c r="D64" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E64" s="9" t="s">
@@ -62239,16 +62239,16 @@
       <c r="R64" s="8"/>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A65" s="38">
+      <c r="A65" s="37">
         <v>185</v>
       </c>
-      <c r="B65" s="36" t="s">
+      <c r="B65" s="35" t="s">
         <v>1645</v>
       </c>
       <c r="C65" s="9" t="s">
         <v>1317</v>
       </c>
-      <c r="D65" s="34" t="s">
+      <c r="D65" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E65" s="9" t="s">
@@ -62278,13 +62278,13 @@
       <c r="A66" s="9">
         <v>189</v>
       </c>
-      <c r="B66" s="36" t="s">
+      <c r="B66" s="35" t="s">
         <v>1398</v>
       </c>
       <c r="C66" s="9" t="s">
         <v>1156</v>
       </c>
-      <c r="D66" s="34" t="s">
+      <c r="D66" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E66" s="9" t="s">
@@ -62320,13 +62320,13 @@
       <c r="A67" s="9">
         <v>190</v>
       </c>
-      <c r="B67" s="36" t="s">
+      <c r="B67" s="35" t="s">
         <v>1403</v>
       </c>
       <c r="C67" s="9" t="s">
         <v>1233</v>
       </c>
-      <c r="D67" s="34" t="s">
+      <c r="D67" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E67" s="9" t="s">
@@ -62354,13 +62354,13 @@
       <c r="A68" s="9">
         <v>192</v>
       </c>
-      <c r="B68" s="36" t="s">
+      <c r="B68" s="35" t="s">
         <v>1451</v>
       </c>
       <c r="C68" s="9" t="s">
         <v>1163</v>
       </c>
-      <c r="D68" s="34" t="s">
+      <c r="D68" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E68" s="9" t="s">
@@ -62390,13 +62390,13 @@
       <c r="A69" s="9">
         <v>193</v>
       </c>
-      <c r="B69" s="36" t="s">
+      <c r="B69" s="35" t="s">
         <v>1582</v>
       </c>
       <c r="C69" s="9" t="s">
         <v>1165</v>
       </c>
-      <c r="D69" s="34" t="s">
+      <c r="D69" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E69" s="9" t="s">
@@ -62432,13 +62432,13 @@
       <c r="A70" s="9">
         <v>204</v>
       </c>
-      <c r="B70" s="36" t="s">
+      <c r="B70" s="35" t="s">
         <v>1123</v>
       </c>
       <c r="C70" s="9" t="s">
         <v>1123</v>
       </c>
-      <c r="D70" s="34" t="s">
+      <c r="D70" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E70" s="9" t="s">
@@ -62468,13 +62468,13 @@
       <c r="A71" s="9">
         <v>207</v>
       </c>
-      <c r="B71" s="36" t="s">
+      <c r="B71" s="35" t="s">
         <v>1406</v>
       </c>
       <c r="C71" s="9" t="s">
         <v>1126</v>
       </c>
-      <c r="D71" s="34" t="s">
+      <c r="D71" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E71" s="9" t="s">
@@ -62502,13 +62502,13 @@
       <c r="A72" s="9">
         <v>208</v>
       </c>
-      <c r="B72" s="36" t="s">
+      <c r="B72" s="35" t="s">
         <v>1402</v>
       </c>
       <c r="C72" s="9" t="s">
         <v>1232</v>
       </c>
-      <c r="D72" s="34" t="s">
+      <c r="D72" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E72" s="9" t="s">
@@ -62536,13 +62536,13 @@
       <c r="A73" s="9">
         <v>209</v>
       </c>
-      <c r="B73" s="36" t="s">
+      <c r="B73" s="35" t="s">
         <v>1405</v>
       </c>
       <c r="C73" s="9" t="s">
         <v>1234</v>
       </c>
-      <c r="D73" s="34" t="s">
+      <c r="D73" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E73" s="9" t="s">
@@ -62570,13 +62570,13 @@
       <c r="A74" s="9">
         <v>210</v>
       </c>
-      <c r="B74" s="36" t="s">
+      <c r="B74" s="35" t="s">
         <v>1452</v>
       </c>
       <c r="C74" s="9" t="s">
         <v>1164</v>
       </c>
-      <c r="D74" s="34" t="s">
+      <c r="D74" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E74" s="9" t="s">
@@ -62604,13 +62604,13 @@
       <c r="A75" s="9">
         <v>212</v>
       </c>
-      <c r="B75" s="36" t="s">
+      <c r="B75" s="35" t="s">
         <v>1377</v>
       </c>
       <c r="C75" s="9" t="s">
         <v>1115</v>
       </c>
-      <c r="D75" s="34" t="s">
+      <c r="D75" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E75" s="9" t="s">
@@ -62644,13 +62644,13 @@
       <c r="A76" s="9">
         <v>214</v>
       </c>
-      <c r="B76" s="36" t="s">
+      <c r="B76" s="35" t="s">
         <v>1376</v>
       </c>
       <c r="C76" s="9" t="s">
         <v>1222</v>
       </c>
-      <c r="D76" s="34" t="s">
+      <c r="D76" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E76" s="9" t="s">
@@ -62684,13 +62684,13 @@
       <c r="A77" s="9">
         <v>215</v>
       </c>
-      <c r="B77" s="36" t="s">
+      <c r="B77" s="35" t="s">
         <v>1404</v>
       </c>
       <c r="C77" s="9" t="s">
         <v>1127</v>
       </c>
-      <c r="D77" s="34" t="s">
+      <c r="D77" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E77" s="9" t="s">
@@ -62718,13 +62718,13 @@
       <c r="A78" s="9">
         <v>223</v>
       </c>
-      <c r="B78" s="36" t="s">
+      <c r="B78" s="35" t="s">
         <v>1558</v>
       </c>
       <c r="C78" s="9" t="s">
         <v>1169</v>
       </c>
-      <c r="D78" s="34" t="s">
+      <c r="D78" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E78" s="9" t="s">
@@ -62762,13 +62762,13 @@
       <c r="A79" s="9">
         <v>224</v>
       </c>
-      <c r="B79" s="36" t="s">
+      <c r="B79" s="35" t="s">
         <v>1460</v>
       </c>
       <c r="C79" s="9" t="s">
         <v>1170</v>
       </c>
-      <c r="D79" s="34" t="s">
+      <c r="D79" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E79" s="9" t="s">
@@ -62796,13 +62796,13 @@
       <c r="A80" s="9">
         <v>227</v>
       </c>
-      <c r="B80" s="36" t="s">
+      <c r="B80" s="35" t="s">
         <v>1365</v>
       </c>
       <c r="C80" s="9" t="s">
         <v>1132</v>
       </c>
-      <c r="D80" s="34" t="s">
+      <c r="D80" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E80" s="9" t="s">
@@ -62830,13 +62830,13 @@
       <c r="A81" s="9">
         <v>230</v>
       </c>
-      <c r="B81" s="36" t="s">
+      <c r="B81" s="35" t="s">
         <v>1551</v>
       </c>
       <c r="C81" s="9" t="s">
         <v>1171</v>
       </c>
-      <c r="D81" s="34" t="s">
+      <c r="D81" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E81" s="9" t="s">
@@ -62874,13 +62874,13 @@
       <c r="A82" s="9">
         <v>232</v>
       </c>
-      <c r="B82" s="36" t="s">
+      <c r="B82" s="35" t="s">
         <v>1432</v>
       </c>
       <c r="C82" s="9" t="s">
         <v>1172</v>
       </c>
-      <c r="D82" s="34" t="s">
+      <c r="D82" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E82" s="9" t="s">
@@ -62908,13 +62908,13 @@
       <c r="A83" s="9">
         <v>233</v>
       </c>
-      <c r="B83" s="36" t="s">
+      <c r="B83" s="35" t="s">
         <v>1396</v>
       </c>
       <c r="C83" s="9" t="s">
         <v>1173</v>
       </c>
-      <c r="D83" s="34" t="s">
+      <c r="D83" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E83" s="9" t="s">
@@ -62946,13 +62946,13 @@
       <c r="A84" s="9">
         <v>238</v>
       </c>
-      <c r="B84" s="36" t="s">
+      <c r="B84" s="35" t="s">
         <v>1488</v>
       </c>
       <c r="C84" s="9" t="s">
         <v>1185</v>
       </c>
-      <c r="D84" s="34" t="s">
+      <c r="D84" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E84" s="9" t="s">
@@ -62980,13 +62980,13 @@
       <c r="A85" s="9">
         <v>241</v>
       </c>
-      <c r="B85" s="36" t="s">
+      <c r="B85" s="35" t="s">
         <v>1539</v>
       </c>
       <c r="C85" s="9" t="s">
         <v>1274</v>
       </c>
-      <c r="D85" s="34" t="s">
+      <c r="D85" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E85" s="9" t="s">
@@ -63022,13 +63022,13 @@
       <c r="A86" s="9">
         <v>243</v>
       </c>
-      <c r="B86" s="36" t="s">
+      <c r="B86" s="35" t="s">
         <v>1391</v>
       </c>
       <c r="C86" s="9" t="s">
         <v>1230</v>
       </c>
-      <c r="D86" s="34" t="s">
+      <c r="D86" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E86" s="9" t="s">
@@ -63056,13 +63056,13 @@
       <c r="A87" s="8">
         <v>253</v>
       </c>
-      <c r="B87" s="40" t="s">
+      <c r="B87" s="39" t="s">
         <v>1353</v>
       </c>
       <c r="C87" s="8" t="s">
         <v>1178</v>
       </c>
-      <c r="D87" s="34" t="s">
+      <c r="D87" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E87" s="9" t="s">
@@ -63090,13 +63090,13 @@
       <c r="A88" s="8">
         <v>254</v>
       </c>
-      <c r="B88" s="40" t="s">
+      <c r="B88" s="39" t="s">
         <v>1424</v>
       </c>
       <c r="C88" s="8" t="s">
         <v>1133</v>
       </c>
-      <c r="D88" s="34" t="s">
+      <c r="D88" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E88" s="9" t="s">
@@ -63124,13 +63124,13 @@
       <c r="A89" s="8">
         <v>257</v>
       </c>
-      <c r="B89" s="40" t="s">
+      <c r="B89" s="39" t="s">
         <v>1457</v>
       </c>
       <c r="C89" s="8" t="s">
         <v>1179</v>
       </c>
-      <c r="D89" s="34" t="s">
+      <c r="D89" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E89" s="9" t="s">
@@ -63155,16 +63155,16 @@
       <c r="R89" s="8"/>
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A90" s="41">
+      <c r="A90" s="40">
         <v>260</v>
       </c>
-      <c r="B90" s="40" t="s">
+      <c r="B90" s="39" t="s">
         <v>1587</v>
       </c>
       <c r="C90" s="8" t="s">
         <v>1148</v>
       </c>
-      <c r="D90" s="35" t="s">
+      <c r="D90" s="34" t="s">
         <v>5</v>
       </c>
       <c r="E90" s="9" t="s">
@@ -63192,16 +63192,16 @@
       <c r="A91" s="8">
         <v>264</v>
       </c>
-      <c r="B91" s="40" t="s">
+      <c r="B91" s="39" t="s">
         <v>1378</v>
       </c>
       <c r="C91" s="8" t="s">
         <v>1223</v>
       </c>
-      <c r="D91" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="E91" s="36" t="s">
+      <c r="D91" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E91" s="35" t="s">
         <v>1687</v>
       </c>
       <c r="F91" s="8"/>
@@ -63232,13 +63232,13 @@
       <c r="A92" s="8">
         <v>265</v>
       </c>
-      <c r="B92" s="40" t="s">
+      <c r="B92" s="39" t="s">
         <v>1449</v>
       </c>
       <c r="C92" s="8" t="s">
         <v>1250</v>
       </c>
-      <c r="D92" s="34" t="s">
+      <c r="D92" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E92" s="9" t="s">
@@ -63265,16 +63265,16 @@
       <c r="R92" s="8"/>
     </row>
     <row r="93" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A93" s="41">
+      <c r="A93" s="40">
         <v>270</v>
       </c>
-      <c r="B93" s="40" t="s">
+      <c r="B93" s="39" t="s">
         <v>1666</v>
       </c>
       <c r="C93" s="8" t="s">
         <v>1193</v>
       </c>
-      <c r="D93" s="34" t="s">
+      <c r="D93" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E93" s="8" t="s">
@@ -63308,16 +63308,16 @@
       <c r="A94" s="8">
         <v>271</v>
       </c>
-      <c r="B94" s="40" t="s">
+      <c r="B94" s="39" t="s">
         <v>1486</v>
       </c>
       <c r="C94" s="8" t="s">
         <v>1255</v>
       </c>
-      <c r="D94" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="E94" s="40" t="s">
+      <c r="D94" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E94" s="39" t="s">
         <v>1684</v>
       </c>
       <c r="F94" s="8"/>
@@ -63344,13 +63344,13 @@
       <c r="A95" s="8">
         <v>272</v>
       </c>
-      <c r="B95" s="40" t="s">
+      <c r="B95" s="39" t="s">
         <v>1490</v>
       </c>
       <c r="C95" s="8" t="s">
         <v>1188</v>
       </c>
-      <c r="D95" s="34" t="s">
+      <c r="D95" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E95" s="8" t="s">
@@ -63380,16 +63380,16 @@
       <c r="A96" s="8">
         <v>273</v>
       </c>
-      <c r="B96" s="40" t="s">
+      <c r="B96" s="39" t="s">
         <v>1559</v>
       </c>
       <c r="C96" s="8" t="s">
         <v>1191</v>
       </c>
-      <c r="D96" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="E96" s="42" t="s">
+      <c r="D96" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E96" s="41" t="s">
         <v>1101</v>
       </c>
       <c r="F96" s="8"/>
@@ -63422,16 +63422,16 @@
       <c r="A97" s="8">
         <v>274</v>
       </c>
-      <c r="B97" s="40" t="s">
+      <c r="B97" s="39" t="s">
         <v>1489</v>
       </c>
       <c r="C97" s="8" t="s">
         <v>1189</v>
       </c>
-      <c r="D97" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="E97" s="43" t="s">
+      <c r="D97" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E97" s="42" t="s">
         <v>1681</v>
       </c>
       <c r="F97" s="8"/>
@@ -63458,16 +63458,16 @@
       <c r="A98" s="8">
         <v>275</v>
       </c>
-      <c r="B98" s="40" t="s">
+      <c r="B98" s="39" t="s">
         <v>1441</v>
       </c>
       <c r="C98" s="8" t="s">
         <v>1247</v>
       </c>
-      <c r="D98" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="E98" s="36" t="s">
+      <c r="D98" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E98" s="35" t="s">
         <v>1096</v>
       </c>
       <c r="F98" s="8"/>
@@ -63492,16 +63492,16 @@
       <c r="A99" s="8">
         <v>276</v>
       </c>
-      <c r="B99" s="40" t="s">
+      <c r="B99" s="39" t="s">
         <v>1484</v>
       </c>
       <c r="C99" s="8" t="s">
         <v>1254</v>
       </c>
-      <c r="D99" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="E99" s="36" t="s">
+      <c r="D99" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E99" s="35" t="s">
         <v>1692</v>
       </c>
       <c r="F99" s="8"/>
@@ -63530,13 +63530,13 @@
       <c r="A100" s="8">
         <v>277</v>
       </c>
-      <c r="B100" s="40" t="s">
+      <c r="B100" s="39" t="s">
         <v>1350</v>
       </c>
       <c r="C100" s="8" t="s">
         <v>1192</v>
       </c>
-      <c r="D100" s="34" t="s">
+      <c r="D100" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E100" s="9" t="s">
@@ -63566,13 +63566,13 @@
       <c r="A101" s="8">
         <v>278</v>
       </c>
-      <c r="B101" s="40" t="s">
+      <c r="B101" s="39" t="s">
         <v>1556</v>
       </c>
       <c r="C101" s="8" t="s">
         <v>1194</v>
       </c>
-      <c r="D101" s="34" t="s">
+      <c r="D101" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E101" s="9" t="s">
@@ -63610,13 +63610,13 @@
       <c r="A102" s="8">
         <v>279</v>
       </c>
-      <c r="B102" s="40" t="s">
+      <c r="B102" s="39" t="s">
         <v>1557</v>
       </c>
       <c r="C102" s="8" t="s">
         <v>1195</v>
       </c>
-      <c r="D102" s="34" t="s">
+      <c r="D102" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E102" s="9" t="s">
@@ -63652,13 +63652,13 @@
       <c r="A103" s="8">
         <v>280</v>
       </c>
-      <c r="B103" s="40" t="s">
+      <c r="B103" s="39" t="s">
         <v>1465</v>
       </c>
       <c r="C103" s="8" t="s">
         <v>1129</v>
       </c>
-      <c r="D103" s="34" t="s">
+      <c r="D103" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E103" s="9" t="s">
@@ -63686,13 +63686,13 @@
       <c r="A104" s="8">
         <v>281</v>
       </c>
-      <c r="B104" s="40" t="s">
+      <c r="B104" s="39" t="s">
         <v>1464</v>
       </c>
       <c r="C104" s="8" t="s">
         <v>1130</v>
       </c>
-      <c r="D104" s="34" t="s">
+      <c r="D104" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E104" s="8" t="s">
@@ -63720,13 +63720,13 @@
       <c r="A105" s="8">
         <v>289</v>
       </c>
-      <c r="B105" s="40" t="s">
+      <c r="B105" s="39" t="s">
         <v>1462</v>
       </c>
       <c r="C105" s="8" t="s">
         <v>1128</v>
       </c>
-      <c r="D105" s="34" t="s">
+      <c r="D105" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E105" s="8" t="s">
@@ -63754,13 +63754,13 @@
       <c r="A106" s="8">
         <v>291</v>
       </c>
-      <c r="B106" s="40" t="s">
+      <c r="B106" s="39" t="s">
         <v>1463</v>
       </c>
       <c r="C106" s="8" t="s">
         <v>1131</v>
       </c>
-      <c r="D106" s="34" t="s">
+      <c r="D106" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E106" s="8" t="s">
@@ -63788,13 +63788,13 @@
       <c r="A107" s="8">
         <v>292</v>
       </c>
-      <c r="B107" s="40" t="s">
+      <c r="B107" s="39" t="s">
         <v>1461</v>
       </c>
       <c r="C107" s="8" t="s">
         <v>1252</v>
       </c>
-      <c r="D107" s="34" t="s">
+      <c r="D107" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E107" s="8" t="s">
@@ -63822,13 +63822,13 @@
       <c r="A108" s="8">
         <v>293</v>
       </c>
-      <c r="B108" s="40" t="s">
+      <c r="B108" s="39" t="s">
         <v>1431</v>
       </c>
       <c r="C108" s="8" t="s">
         <v>1245</v>
       </c>
-      <c r="D108" s="34" t="s">
+      <c r="D108" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E108" s="8" t="s">
@@ -63856,13 +63856,13 @@
       <c r="A109" s="8">
         <v>299</v>
       </c>
-      <c r="B109" s="40" t="s">
+      <c r="B109" s="39" t="s">
         <v>1469</v>
       </c>
       <c r="C109" s="8" t="s">
         <v>1197</v>
       </c>
-      <c r="D109" s="34" t="s">
+      <c r="D109" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E109" s="9" t="s">
@@ -63889,16 +63889,16 @@
       <c r="R109" s="8"/>
     </row>
     <row r="110" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A110" s="41">
+      <c r="A110" s="40">
         <v>302</v>
       </c>
-      <c r="B110" s="40" t="s">
+      <c r="B110" s="39" t="s">
         <v>1332</v>
       </c>
       <c r="C110" s="8" t="s">
         <v>1209</v>
       </c>
-      <c r="D110" s="34" t="s">
+      <c r="D110" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E110" s="9" t="s">
@@ -63926,13 +63926,13 @@
       <c r="A111" s="8">
         <v>305</v>
       </c>
-      <c r="B111" s="40" t="s">
+      <c r="B111" s="39" t="s">
         <v>1555</v>
       </c>
       <c r="C111" s="8" t="s">
         <v>1283</v>
       </c>
-      <c r="D111" s="34" t="s">
+      <c r="D111" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E111" s="8" t="s">
@@ -63965,16 +63965,16 @@
       <c r="R111" s="8"/>
     </row>
     <row r="112" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A112" s="41">
+      <c r="A112" s="40">
         <v>306</v>
       </c>
-      <c r="B112" s="40" t="s">
+      <c r="B112" s="39" t="s">
         <v>1659</v>
       </c>
       <c r="C112" s="8" t="s">
         <v>1326</v>
       </c>
-      <c r="D112" s="34" t="s">
+      <c r="D112" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E112" s="8" t="s">
@@ -63999,16 +63999,16 @@
       <c r="R112" s="8"/>
     </row>
     <row r="113" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A113" s="41">
+      <c r="A113" s="40">
         <v>307</v>
       </c>
-      <c r="B113" s="40" t="s">
+      <c r="B113" s="39" t="s">
         <v>1663</v>
       </c>
       <c r="C113" s="8" t="s">
         <v>1198</v>
       </c>
-      <c r="D113" s="34" t="s">
+      <c r="D113" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E113" s="9" t="s">
@@ -64039,16 +64039,16 @@
       <c r="R113" s="8"/>
     </row>
     <row r="114" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A114" s="41">
+      <c r="A114" s="40">
         <v>308</v>
       </c>
-      <c r="B114" s="40" t="s">
+      <c r="B114" s="39" t="s">
         <v>1588</v>
       </c>
       <c r="C114" s="8" t="s">
         <v>1296</v>
       </c>
-      <c r="D114" s="34" t="s">
+      <c r="D114" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E114" s="9" t="s">
@@ -64078,13 +64078,13 @@
       <c r="A115" s="8">
         <v>313</v>
       </c>
-      <c r="B115" s="40" t="s">
+      <c r="B115" s="39" t="s">
         <v>1474</v>
       </c>
       <c r="C115" s="8" t="s">
         <v>1202</v>
       </c>
-      <c r="D115" s="34" t="s">
+      <c r="D115" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E115" s="10" t="s">
@@ -64111,16 +64111,16 @@
       <c r="R115" s="8"/>
     </row>
     <row r="116" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A116" s="41">
+      <c r="A116" s="40">
         <v>314</v>
       </c>
-      <c r="B116" s="40" t="s">
+      <c r="B116" s="39" t="s">
         <v>1661</v>
       </c>
       <c r="C116" s="8" t="s">
         <v>1207</v>
       </c>
-      <c r="D116" s="34" t="s">
+      <c r="D116" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E116" s="8" t="s">
@@ -64150,13 +64150,13 @@
       <c r="A117" s="8">
         <v>319</v>
       </c>
-      <c r="B117" s="40" t="s">
+      <c r="B117" s="39" t="s">
         <v>1354</v>
       </c>
       <c r="C117" s="8" t="s">
         <v>1203</v>
       </c>
-      <c r="D117" s="34" t="s">
+      <c r="D117" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E117" s="8" t="s">
@@ -64184,13 +64184,13 @@
       <c r="A118" s="8">
         <v>324</v>
       </c>
-      <c r="B118" s="40" t="s">
+      <c r="B118" s="39" t="s">
         <v>1394</v>
       </c>
       <c r="C118" s="8" t="s">
         <v>1231</v>
       </c>
-      <c r="D118" s="34" t="s">
+      <c r="D118" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E118" s="9" t="s">
@@ -64215,16 +64215,16 @@
       <c r="R118" s="8"/>
     </row>
     <row r="119" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A119" s="41">
+      <c r="A119" s="40">
         <v>327</v>
       </c>
-      <c r="B119" s="40" t="s">
+      <c r="B119" s="39" t="s">
         <v>1660</v>
       </c>
       <c r="C119" s="8" t="s">
         <v>1327</v>
       </c>
-      <c r="D119" s="34" t="s">
+      <c r="D119" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E119" s="8" t="s">
@@ -64254,13 +64254,13 @@
       <c r="A120" s="8">
         <v>339</v>
       </c>
-      <c r="B120" s="40" t="s">
+      <c r="B120" s="39" t="s">
         <v>1493</v>
       </c>
       <c r="C120" s="8" t="s">
         <v>1257</v>
       </c>
-      <c r="D120" s="34" t="s">
+      <c r="D120" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E120" s="8" t="s">
@@ -64290,13 +64290,13 @@
       <c r="A121" s="8">
         <v>340</v>
       </c>
-      <c r="B121" s="40" t="s">
+      <c r="B121" s="39" t="s">
         <v>1549</v>
       </c>
       <c r="C121" s="8" t="s">
         <v>1280</v>
       </c>
-      <c r="D121" s="34" t="s">
+      <c r="D121" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E121" s="8" t="s">
@@ -64329,16 +64329,16 @@
       <c r="R121" s="8"/>
     </row>
     <row r="122" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A122" s="41">
+      <c r="A122" s="40">
         <v>342</v>
       </c>
-      <c r="B122" s="40" t="s">
+      <c r="B122" s="39" t="s">
         <v>1601</v>
       </c>
       <c r="C122" s="8" t="s">
         <v>1200</v>
       </c>
-      <c r="D122" s="34" t="s">
+      <c r="D122" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E122" s="9" t="s">
@@ -64368,13 +64368,13 @@
       <c r="A123" s="8">
         <v>343</v>
       </c>
-      <c r="B123" s="40" t="s">
+      <c r="B123" s="39" t="s">
         <v>1416</v>
       </c>
       <c r="C123" s="8" t="s">
         <v>1201</v>
       </c>
-      <c r="D123" s="34" t="s">
+      <c r="D123" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E123" s="9" t="s">
@@ -64401,16 +64401,16 @@
       <c r="R123" s="8"/>
     </row>
     <row r="124" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A124" s="41">
+      <c r="A124" s="40">
         <v>344</v>
       </c>
-      <c r="B124" s="40" t="s">
+      <c r="B124" s="39" t="s">
         <v>1584</v>
       </c>
       <c r="C124" s="8" t="s">
         <v>1294</v>
       </c>
-      <c r="D124" s="34" t="s">
+      <c r="D124" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E124" s="9" t="s">
@@ -64443,8 +64443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9585C0FF-65C5-4BD8-9936-5C9A63F7E604}">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64464,10 +64464,10 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
+        <v>1780</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>1781</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>1782</v>
       </c>
       <c r="C1" s="13" t="s">
         <v>1737</v>
@@ -64479,42 +64479,42 @@
         <v>37</v>
       </c>
       <c r="F1" s="13" t="s">
+        <v>1782</v>
+      </c>
+      <c r="G1" s="13" t="s">
         <v>1783</v>
       </c>
-      <c r="G1" s="13" t="s">
-        <v>1784</v>
-      </c>
       <c r="H1" s="13" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="I1" s="13" t="s">
+        <v>1775</v>
+      </c>
+      <c r="J1" s="13" t="s">
         <v>1776</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="K1" s="49" t="s">
+        <v>1791</v>
+      </c>
+      <c r="L1" s="49" t="s">
+        <v>1792</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
         <v>1777</v>
-      </c>
-      <c r="K1" s="50" t="s">
-        <v>1792</v>
-      </c>
-      <c r="L1" s="50" t="s">
-        <v>1793</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
-        <v>1778</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>1739</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
       <c r="F2" s="10" t="s">
         <v>19</v>
@@ -64533,23 +64533,23 @@
         <v>3</v>
       </c>
       <c r="K2" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="49" t="s">
-        <v>1778</v>
+      <c r="A3" s="48" t="s">
+        <v>1777</v>
       </c>
       <c r="B3" s="15" t="s">
+        <v>1750</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>1750</v>
+      </c>
+      <c r="D3" s="23" t="s">
         <v>1751</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>1751</v>
-      </c>
-      <c r="D3" s="24" t="s">
-        <v>1752</v>
-      </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="24" t="s">
         <v>1744</v>
       </c>
       <c r="F3" s="12" t="s">
@@ -64569,26 +64569,26 @@
         <v>4</v>
       </c>
       <c r="K3" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
       <c r="L3" t="s">
-        <v>1797</v>
+        <v>1796</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="49" t="s">
-        <v>1778</v>
+      <c r="A4" s="48" t="s">
+        <v>1777</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>1753</v>
+        <v>1752</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>1753</v>
-      </c>
-      <c r="D4" s="24" t="s">
         <v>1752</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="D4" s="23" t="s">
+        <v>1751</v>
+      </c>
+      <c r="E4" s="24" t="s">
         <v>1744</v>
       </c>
       <c r="F4" s="12" t="s">
@@ -64608,22 +64608,22 @@
         <v>5</v>
       </c>
       <c r="L4" t="s">
-        <v>1800</v>
+        <v>1799</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
       <c r="B5" s="12"/>
       <c r="C5" s="19" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>1764</v>
+        <v>1763</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>1769</v>
+        <v>1768</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>13</v>
@@ -64642,25 +64642,25 @@
         <v>5</v>
       </c>
       <c r="K5" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
       <c r="L5" t="s">
-        <v>1798</v>
+        <v>1797</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="s">
-        <v>1779</v>
+      <c r="A6" s="32" t="s">
+        <v>1778</v>
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="19" t="s">
-        <v>1774</v>
+        <v>1773</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>1767</v>
+        <v>1766</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>1769</v>
+        <v>1768</v>
       </c>
       <c r="F6" s="10" t="s">
         <v>15</v>
@@ -64679,22 +64679,22 @@
         <v>3</v>
       </c>
       <c r="K6" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="33" t="s">
-        <v>1779</v>
+      <c r="A7" s="32" t="s">
+        <v>1778</v>
       </c>
       <c r="B7" s="12"/>
       <c r="C7" s="21" t="s">
         <v>1586</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>1764</v>
+        <v>1763</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>1769</v>
+        <v>1768</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>12</v>
@@ -64713,24 +64713,24 @@
         <v>3</v>
       </c>
       <c r="K7" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="48" t="s">
-        <v>1778</v>
+      <c r="A8" s="47" t="s">
+        <v>1777</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>1739</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>1750</v>
+        <v>1749</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>16</v>
@@ -64749,30 +64749,28 @@
         <v>5</v>
       </c>
       <c r="K8" t="s">
+        <v>1794</v>
+      </c>
+      <c r="L8" t="s">
         <v>1795</v>
-      </c>
-      <c r="L8" t="s">
-        <v>1796</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>1739</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="16"/>
+      <c r="D9" s="17" t="s">
+        <v>1785</v>
+      </c>
+      <c r="E9" s="22" t="s">
         <v>1745</v>
       </c>
-      <c r="D9" s="17" t="s">
-        <v>1786</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>1746</v>
-      </c>
       <c r="F9" s="12" t="s">
-        <v>1218</v>
+        <v>1800</v>
       </c>
       <c r="G9" s="12" t="s">
         <v>1716</v>
@@ -64787,30 +64785,30 @@
         <v>3</v>
       </c>
       <c r="K9" t="s">
-        <v>1795</v>
+        <v>1794</v>
       </c>
       <c r="L9" t="s">
-        <v>1799</v>
+        <v>1798</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="B10" s="15" t="s">
         <v>1739</v>
       </c>
-      <c r="C10" s="22" t="s">
-        <v>1747</v>
-      </c>
-      <c r="D10" s="17" t="s">
-        <v>1786</v>
-      </c>
-      <c r="E10" s="23" t="s">
+      <c r="C10" s="15" t="s">
         <v>1746</v>
       </c>
+      <c r="D10" s="15" t="s">
+        <v>1785</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>1745</v>
+      </c>
       <c r="F10" s="12" t="s">
-        <v>1218</v>
+        <v>1801</v>
       </c>
       <c r="G10" s="12" t="s">
         <v>1716</v>
@@ -64825,150 +64823,151 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>1757</v>
+        <v>1753</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>1757</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>1780</v>
-      </c>
-      <c r="E11" s="25" t="s">
-        <v>1746</v>
+        <v>1753</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>1754</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>1755</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>1682</v>
+        <v>21</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>1684</v>
       </c>
       <c r="H11" s="12">
         <v>9</v>
       </c>
       <c r="I11" s="12">
+        <v>32</v>
+      </c>
+      <c r="J11" s="12">
+        <f>3+8</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>1777</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>1756</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>1756</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>1779</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>1745</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>1682</v>
+      </c>
+      <c r="H12" s="12">
+        <v>10</v>
+      </c>
+      <c r="I12" s="12">
         <v>9</v>
       </c>
-      <c r="J11" s="12">
+      <c r="J12" s="27">
+        <f>5+2</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>1778</v>
+      </c>
+      <c r="B13" s="12"/>
+      <c r="C13" s="50" t="s">
+        <v>1767</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>1763</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>1764</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>1682</v>
+      </c>
+      <c r="H13" s="12">
+        <v>11</v>
+      </c>
+      <c r="I13" s="12">
+        <v>13</v>
+      </c>
+      <c r="J13" s="12">
         <f>4+1</f>
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
-        <v>1779</v>
-      </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="51" t="s">
-        <v>1768</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>1764</v>
-      </c>
-      <c r="E12" s="26" t="s">
-        <v>1765</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>1682</v>
-      </c>
-      <c r="H12" s="12">
-        <v>10</v>
-      </c>
-      <c r="I12" s="12">
-        <v>13</v>
-      </c>
-      <c r="J12" s="12">
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>1777</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>1739</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>1352</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>1747</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>1745</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>1076</v>
+      </c>
+      <c r="H14" s="12">
+        <v>12</v>
+      </c>
+      <c r="I14" s="12">
+        <v>2</v>
+      </c>
+      <c r="J14" s="12">
         <f>6+7</f>
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
-        <v>1778</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>1739</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>1352</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>1748</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>1746</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>1076</v>
-      </c>
-      <c r="H13" s="12">
-        <v>11</v>
-      </c>
-      <c r="I13" s="12">
-        <v>2</v>
-      </c>
-      <c r="J13" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
-        <v>1778</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>1754</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>1754</v>
-      </c>
-      <c r="D14" s="24" t="s">
-        <v>1755</v>
-      </c>
-      <c r="E14" s="27" t="s">
-        <v>1756</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>1684</v>
-      </c>
-      <c r="H14" s="12">
-        <v>12</v>
-      </c>
-      <c r="I14" s="12">
-        <v>32</v>
-      </c>
-      <c r="J14" s="28">
-        <f>5+2</f>
-        <v>7</v>
-      </c>
-    </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="19" t="s">
+        <v>1765</v>
+      </c>
+      <c r="D15" s="19" t="s">
         <v>1766</v>
       </c>
-      <c r="D15" s="19" t="s">
-        <v>1767</v>
-      </c>
-      <c r="E15" s="26" t="s">
-        <v>1765</v>
-      </c>
-      <c r="F15" s="8" t="s">
+      <c r="E15" s="25" t="s">
+        <v>1764</v>
+      </c>
+      <c r="F15" s="12" t="s">
         <v>1249</v>
       </c>
       <c r="G15" s="8" t="s">
@@ -64981,56 +64980,55 @@
         <v>29</v>
       </c>
       <c r="J15" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>1777</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>1739</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>1742</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>1743</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>1744</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>1681</v>
+      </c>
+      <c r="H16" s="12">
+        <v>14</v>
+      </c>
+      <c r="I16" s="12">
+        <v>35</v>
+      </c>
+      <c r="J16" s="12">
         <f>15+5</f>
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
-        <v>1778</v>
-      </c>
-      <c r="B16" s="15" t="s">
-        <v>1739</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>1742</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>1743</v>
-      </c>
-      <c r="E16" s="29" t="s">
-        <v>1744</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>481</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>1681</v>
-      </c>
-      <c r="H16" s="12">
-        <v>14</v>
-      </c>
-      <c r="I16" s="12">
-        <v>35</v>
-      </c>
-      <c r="J16" s="12">
-        <f>3+8</f>
-        <v>11</v>
-      </c>
-    </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
       <c r="B17" s="12"/>
       <c r="C17" s="19" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
       <c r="D17" s="19" t="s">
+        <v>1763</v>
+      </c>
+      <c r="E17" s="25" t="s">
         <v>1764</v>
-      </c>
-      <c r="E17" s="26" t="s">
-        <v>1765</v>
       </c>
       <c r="F17" s="10" t="s">
         <v>227</v>
@@ -65050,17 +65048,17 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
       <c r="B18" s="12"/>
       <c r="C18" s="19" t="s">
         <v>1643</v>
       </c>
       <c r="D18" s="21" t="s">
+        <v>1763</v>
+      </c>
+      <c r="E18" s="25" t="s">
         <v>1764</v>
-      </c>
-      <c r="E18" s="26" t="s">
-        <v>1765</v>
       </c>
       <c r="F18" s="12" t="s">
         <v>7</v>
@@ -65081,17 +65079,17 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
       <c r="B19" s="12"/>
       <c r="C19" s="19" t="s">
+        <v>1760</v>
+      </c>
+      <c r="D19" s="19" t="s">
         <v>1761</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="E19" s="25" t="s">
         <v>1762</v>
-      </c>
-      <c r="E19" s="26" t="s">
-        <v>1763</v>
       </c>
       <c r="F19" s="12" t="s">
         <v>6</v>
@@ -65111,17 +65109,17 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
       <c r="B20" s="12"/>
       <c r="C20" s="19" t="s">
+        <v>1769</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>1763</v>
+      </c>
+      <c r="E20" s="20" t="s">
         <v>1770</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>1764</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>1771</v>
       </c>
       <c r="F20" s="10" t="s">
         <v>8</v>
@@ -65141,17 +65139,17 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
       <c r="B21" s="12"/>
       <c r="C21" s="19" t="s">
         <v>1562</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>1769</v>
+        <v>1768</v>
       </c>
       <c r="F21" s="10" t="s">
         <v>14</v>
@@ -65171,18 +65169,18 @@
     </row>
     <row r="22" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="B22" s="15" t="s">
+        <v>1757</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>1757</v>
+      </c>
+      <c r="D22" s="23" t="s">
         <v>1758</v>
       </c>
-      <c r="C22" s="15" t="s">
-        <v>1758</v>
-      </c>
-      <c r="D22" s="24" t="s">
-        <v>1759</v>
-      </c>
-      <c r="E22" s="25" t="s">
+      <c r="E22" s="24" t="s">
         <v>1744</v>
       </c>
       <c r="F22" s="12" t="s">
@@ -65203,17 +65201,17 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="19" t="s">
         <v>1622</v>
       </c>
       <c r="D23" s="21" t="s">
-        <v>1764</v>
+        <v>1763</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>1769</v>
+        <v>1768</v>
       </c>
       <c r="F23" s="10" t="s">
         <v>11</v>
@@ -65233,25 +65231,25 @@
     </row>
     <row r="24" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="B24" s="15" t="s">
         <v>1739</v>
       </c>
-      <c r="C24" s="30" t="s">
+      <c r="C24" s="29" t="s">
         <v>1740</v>
       </c>
-      <c r="D24" s="31" t="s">
-        <v>1785</v>
-      </c>
-      <c r="E24" s="32" t="s">
+      <c r="D24" s="30" t="s">
+        <v>1784</v>
+      </c>
+      <c r="E24" s="31" t="s">
         <v>1741</v>
       </c>
       <c r="F24" s="12" t="s">
         <v>17</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="H24" s="12">
         <v>22</v>
@@ -65264,27 +65262,27 @@
       </c>
     </row>
     <row r="26" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="33"/>
+      <c r="A26" s="32"/>
       <c r="B26" t="s">
+        <v>1787</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="48"/>
+      <c r="B27" t="s">
         <v>1788</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="49"/>
-      <c r="B27" t="s">
+    <row r="28" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="47"/>
+      <c r="B28" t="s">
         <v>1789</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="48"/>
-      <c r="B28" t="s">
-        <v>1790</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
       <c r="B29" t="s">
-        <v>1791</v>
+        <v>1790</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agregar configuración de graficas (tipo) , opción de series
actualizacion de plan
</commit_message>
<xml_diff>
--- a/00-Documentacion/Listado de reportes totales-TI.xlsx
+++ b/00-Documentacion/Listado de reportes totales-TI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A13788-763A-474F-8DFB-FF467637D941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65C673B-495D-4B52-9B7C-502B119872DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{1498AA1A-1ACC-4329-A050-ACA05131B658}"/>
   </bookViews>
@@ -6104,6 +6104,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6117,9 +6120,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -7757,7 +7757,7 @@
       </c>
       <c r="R33" s="8"/>
     </row>
-    <row r="34" spans="1:18" ht="51.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" ht="39" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>14</v>
       </c>
@@ -15039,7 +15039,7 @@
       <c r="Q221" s="8"/>
       <c r="R221" s="8"/>
     </row>
-    <row r="222" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A222" s="5">
         <v>36</v>
       </c>
@@ -15075,7 +15075,7 @@
       <c r="Q222" s="8"/>
       <c r="R222" s="8"/>
     </row>
-    <row r="223" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A223" s="5">
         <v>37</v>
       </c>
@@ -15147,7 +15147,7 @@
       <c r="Q224" s="8"/>
       <c r="R224" s="8"/>
     </row>
-    <row r="225" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A225" s="5">
         <v>39</v>
       </c>
@@ -15179,7 +15179,7 @@
       <c r="Q225" s="8"/>
       <c r="R225" s="8"/>
     </row>
-    <row r="226" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A226" s="5">
         <v>39</v>
       </c>
@@ -15685,7 +15685,7 @@
       <c r="Q239" s="8"/>
       <c r="R239" s="8"/>
     </row>
-    <row r="240" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A240" s="5">
         <v>44</v>
       </c>
@@ -15757,7 +15757,7 @@
       <c r="Q241" s="8"/>
       <c r="R241" s="8"/>
     </row>
-    <row r="242" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A242" s="5">
         <v>46</v>
       </c>
@@ -15793,7 +15793,7 @@
       <c r="Q242" s="8"/>
       <c r="R242" s="8"/>
     </row>
-    <row r="243" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A243" s="5">
         <v>47</v>
       </c>
@@ -15829,7 +15829,7 @@
       <c r="Q243" s="8"/>
       <c r="R243" s="8"/>
     </row>
-    <row r="244" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A244" s="5">
         <v>48</v>
       </c>
@@ -15865,7 +15865,7 @@
       <c r="Q244" s="8"/>
       <c r="R244" s="8"/>
     </row>
-    <row r="245" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A245" s="5">
         <v>49</v>
       </c>
@@ -15901,7 +15901,7 @@
       <c r="Q245" s="8"/>
       <c r="R245" s="8"/>
     </row>
-    <row r="246" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A246" s="5">
         <v>50</v>
       </c>
@@ -15937,7 +15937,7 @@
       <c r="Q246" s="8"/>
       <c r="R246" s="8"/>
     </row>
-    <row r="247" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A247" s="5">
         <v>51</v>
       </c>
@@ -15973,7 +15973,7 @@
       <c r="Q247" s="8"/>
       <c r="R247" s="8"/>
     </row>
-    <row r="248" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A248" s="5">
         <v>52</v>
       </c>
@@ -16009,7 +16009,7 @@
       <c r="Q248" s="8"/>
       <c r="R248" s="8"/>
     </row>
-    <row r="249" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A249" s="5">
         <v>53</v>
       </c>
@@ -16189,7 +16189,7 @@
       <c r="Q253" s="8"/>
       <c r="R253" s="8"/>
     </row>
-    <row r="254" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A254" s="5">
         <v>58</v>
       </c>
@@ -16261,7 +16261,7 @@
       <c r="Q255" s="8"/>
       <c r="R255" s="8"/>
     </row>
-    <row r="256" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A256" s="5">
         <v>60</v>
       </c>
@@ -16369,7 +16369,7 @@
       <c r="Q258" s="8"/>
       <c r="R258" s="8"/>
     </row>
-    <row r="259" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A259" s="5">
         <v>63</v>
       </c>
@@ -16441,7 +16441,7 @@
       <c r="Q260" s="8"/>
       <c r="R260" s="8"/>
     </row>
-    <row r="261" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A261" s="5">
         <v>65</v>
       </c>
@@ -16477,7 +16477,7 @@
       <c r="Q261" s="8"/>
       <c r="R261" s="8"/>
     </row>
-    <row r="262" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A262" s="5">
         <v>66</v>
       </c>
@@ -16555,7 +16555,7 @@
       <c r="Q263" s="8"/>
       <c r="R263" s="8"/>
     </row>
-    <row r="264" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A264" s="5">
         <v>68</v>
       </c>
@@ -16623,7 +16623,7 @@
       <c r="Q265" s="8"/>
       <c r="R265" s="8"/>
     </row>
-    <row r="266" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A266" s="5">
         <v>70</v>
       </c>
@@ -16735,7 +16735,7 @@
       </c>
       <c r="R268" s="8"/>
     </row>
-    <row r="269" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A269" s="5">
         <v>73</v>
       </c>
@@ -16913,7 +16913,7 @@
       <c r="Q273" s="8"/>
       <c r="R273" s="8"/>
     </row>
-    <row r="274" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A274" s="5">
         <v>77</v>
       </c>
@@ -16955,7 +16955,7 @@
       </c>
       <c r="R274" s="8"/>
     </row>
-    <row r="275" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A275" s="5">
         <v>78</v>
       </c>
@@ -16989,7 +16989,7 @@
       <c r="Q275" s="8"/>
       <c r="R275" s="8"/>
     </row>
-    <row r="276" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A276" s="5">
         <v>79</v>
       </c>
@@ -17695,7 +17695,7 @@
       </c>
       <c r="R292" s="8"/>
     </row>
-    <row r="293" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A293" s="5">
         <v>80</v>
       </c>
@@ -17769,7 +17769,7 @@
       <c r="Q294" s="8"/>
       <c r="R294" s="8"/>
     </row>
-    <row r="295" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A295" s="5">
         <v>82</v>
       </c>
@@ -17837,7 +17837,7 @@
       <c r="Q296" s="8"/>
       <c r="R296" s="8"/>
     </row>
-    <row r="297" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A297" s="5">
         <v>84</v>
       </c>
@@ -17947,7 +17947,7 @@
       <c r="Q299" s="8"/>
       <c r="R299" s="8"/>
     </row>
-    <row r="300" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A300" s="5">
         <v>87</v>
       </c>
@@ -17981,7 +17981,7 @@
       <c r="Q300" s="8"/>
       <c r="R300" s="8"/>
     </row>
-    <row r="301" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A301" s="5">
         <v>88</v>
       </c>
@@ -18015,7 +18015,7 @@
       <c r="Q301" s="8"/>
       <c r="R301" s="8"/>
     </row>
-    <row r="302" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A302" s="5">
         <v>89</v>
       </c>
@@ -18051,7 +18051,7 @@
       <c r="Q302" s="8"/>
       <c r="R302" s="8"/>
     </row>
-    <row r="303" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A303" s="5">
         <v>90</v>
       </c>
@@ -18093,7 +18093,7 @@
       </c>
       <c r="R303" s="8"/>
     </row>
-    <row r="304" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A304" s="5">
         <v>91</v>
       </c>
@@ -18207,7 +18207,7 @@
       <c r="Q306" s="8"/>
       <c r="R306" s="8"/>
     </row>
-    <row r="307" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A307" s="5">
         <v>94</v>
       </c>
@@ -18247,7 +18247,7 @@
       </c>
       <c r="R307" s="8"/>
     </row>
-    <row r="308" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A308" s="5">
         <v>95</v>
       </c>
@@ -18323,7 +18323,7 @@
       </c>
       <c r="R309" s="8"/>
     </row>
-    <row r="310" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A310" s="5">
         <v>97</v>
       </c>
@@ -18473,7 +18473,7 @@
       <c r="Q313" s="8"/>
       <c r="R313" s="8"/>
     </row>
-    <row r="314" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A314" s="5">
         <v>98</v>
       </c>
@@ -18579,7 +18579,7 @@
       <c r="Q316" s="8"/>
       <c r="R316" s="8"/>
     </row>
-    <row r="317" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A317" s="5">
         <v>99</v>
       </c>
@@ -18623,7 +18623,7 @@
       </c>
       <c r="R317" s="8"/>
     </row>
-    <row r="318" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A318" s="5">
         <v>100</v>
       </c>
@@ -19035,7 +19035,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="328" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A328" s="5">
         <v>102</v>
       </c>
@@ -19077,7 +19077,7 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="329" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A329" s="5">
         <v>103</v>
       </c>
@@ -19151,7 +19151,7 @@
       </c>
       <c r="R330" s="8"/>
     </row>
-    <row r="331" spans="1:18" ht="39" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A331" s="5">
         <v>104</v>
       </c>
@@ -19193,7 +19193,7 @@
       </c>
       <c r="R331" s="8"/>
     </row>
-    <row r="332" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A332" s="5">
         <v>105</v>
       </c>
@@ -19389,7 +19389,7 @@
       <c r="Q336" s="8"/>
       <c r="R336" s="8"/>
     </row>
-    <row r="337" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A337" s="5">
         <v>106</v>
       </c>
@@ -19575,7 +19575,7 @@
       <c r="Q341" s="8"/>
       <c r="R341" s="8"/>
     </row>
-    <row r="342" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A342" s="5">
         <v>108</v>
       </c>
@@ -19611,7 +19611,7 @@
       <c r="Q342" s="8"/>
       <c r="R342" s="8"/>
     </row>
-    <row r="343" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A343" s="5">
         <v>108</v>
       </c>
@@ -19649,7 +19649,7 @@
       <c r="Q343" s="8"/>
       <c r="R343" s="8"/>
     </row>
-    <row r="344" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A344" s="5">
         <v>108</v>
       </c>
@@ -20333,7 +20333,7 @@
       <c r="Q361" s="8"/>
       <c r="R361" s="8"/>
     </row>
-    <row r="362" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A362" s="5">
         <v>109</v>
       </c>
@@ -20373,7 +20373,7 @@
         <v>1701</v>
       </c>
     </row>
-    <row r="363" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A363" s="5">
         <v>110</v>
       </c>
@@ -20567,7 +20567,7 @@
       <c r="Q367" s="8"/>
       <c r="R367" s="8"/>
     </row>
-    <row r="368" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A368" s="5">
         <v>114</v>
       </c>
@@ -20719,7 +20719,7 @@
       <c r="Q371" s="8"/>
       <c r="R371" s="8"/>
     </row>
-    <row r="372" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A372" s="5">
         <v>117</v>
       </c>
@@ -20759,7 +20759,7 @@
       </c>
       <c r="R372" s="8"/>
     </row>
-    <row r="373" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A373" s="5">
         <v>118</v>
       </c>
@@ -20951,7 +20951,7 @@
       </c>
       <c r="R377" s="8"/>
     </row>
-    <row r="378" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A378" s="5">
         <v>121</v>
       </c>
@@ -21065,7 +21065,7 @@
       </c>
       <c r="R380" s="8"/>
     </row>
-    <row r="381" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A381" s="5">
         <v>124</v>
       </c>
@@ -21141,7 +21141,7 @@
       <c r="Q382" s="8"/>
       <c r="R382" s="8"/>
     </row>
-    <row r="383" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A383" s="5">
         <v>126</v>
       </c>
@@ -21435,7 +21435,7 @@
       <c r="Q390" s="8"/>
       <c r="R390" s="8"/>
     </row>
-    <row r="391" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A391" s="9">
         <v>129</v>
       </c>
@@ -21477,7 +21477,7 @@
       </c>
       <c r="R391" s="8"/>
     </row>
-    <row r="392" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A392" s="5">
         <v>130</v>
       </c>
@@ -21689,7 +21689,7 @@
       <c r="Q397" s="8"/>
       <c r="R397" s="8"/>
     </row>
-    <row r="398" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A398" s="5">
         <v>132</v>
       </c>
@@ -21727,7 +21727,7 @@
       <c r="Q398" s="8"/>
       <c r="R398" s="8"/>
     </row>
-    <row r="399" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A399" s="5">
         <v>133</v>
       </c>
@@ -21807,7 +21807,7 @@
       <c r="Q400" s="8"/>
       <c r="R400" s="8"/>
     </row>
-    <row r="401" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A401" s="5">
         <v>135</v>
       </c>
@@ -21881,7 +21881,7 @@
       <c r="Q402" s="8"/>
       <c r="R402" s="8"/>
     </row>
-    <row r="403" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A403" s="5">
         <v>137</v>
       </c>
@@ -21967,7 +21967,7 @@
       <c r="Q404" s="8"/>
       <c r="R404" s="8"/>
     </row>
-    <row r="405" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A405" s="5">
         <v>139</v>
       </c>
@@ -22043,7 +22043,7 @@
       <c r="Q406" s="8"/>
       <c r="R406" s="8"/>
     </row>
-    <row r="407" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A407" s="5">
         <v>141</v>
       </c>
@@ -22081,7 +22081,7 @@
       <c r="Q407" s="8"/>
       <c r="R407" s="8"/>
     </row>
-    <row r="408" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A408" s="5">
         <v>142</v>
       </c>
@@ -22369,7 +22369,7 @@
       <c r="Q415" s="8"/>
       <c r="R415" s="8"/>
     </row>
-    <row r="416" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A416" s="5">
         <v>147</v>
       </c>
@@ -22561,7 +22561,7 @@
       <c r="Q420" s="8"/>
       <c r="R420" s="8"/>
     </row>
-    <row r="421" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A421" s="5">
         <v>149</v>
       </c>
@@ -22823,7 +22823,7 @@
       <c r="Q427" s="8"/>
       <c r="R427" s="8"/>
     </row>
-    <row r="428" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A428" s="5">
         <v>153</v>
       </c>
@@ -22891,7 +22891,7 @@
       <c r="Q429" s="8"/>
       <c r="R429" s="8"/>
     </row>
-    <row r="430" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A430" s="5">
         <v>155</v>
       </c>
@@ -22963,7 +22963,7 @@
       <c r="Q431" s="8"/>
       <c r="R431" s="8"/>
     </row>
-    <row r="432" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A432" s="5">
         <v>157</v>
       </c>
@@ -22997,7 +22997,7 @@
       <c r="Q432" s="8"/>
       <c r="R432" s="8"/>
     </row>
-    <row r="433" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A433" s="5">
         <v>158</v>
       </c>
@@ -23073,7 +23073,7 @@
       <c r="Q434" s="8"/>
       <c r="R434" s="8"/>
     </row>
-    <row r="435" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A435" s="5">
         <v>159</v>
       </c>
@@ -23111,7 +23111,7 @@
       <c r="Q435" s="8"/>
       <c r="R435" s="8"/>
     </row>
-    <row r="436" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A436" s="5">
         <v>160</v>
       </c>
@@ -23189,7 +23189,7 @@
       </c>
       <c r="R437" s="8"/>
     </row>
-    <row r="438" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A438" s="5">
         <v>161</v>
       </c>
@@ -23369,7 +23369,7 @@
       <c r="Q442" s="8"/>
       <c r="R442" s="8"/>
     </row>
-    <row r="443" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A443" s="5">
         <v>165</v>
       </c>
@@ -23449,7 +23449,7 @@
       </c>
       <c r="R444" s="8"/>
     </row>
-    <row r="445" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A445" s="5">
         <v>167</v>
       </c>
@@ -23519,7 +23519,7 @@
       <c r="Q446" s="8"/>
       <c r="R446" s="8"/>
     </row>
-    <row r="447" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A447" s="5">
         <v>169</v>
       </c>
@@ -23593,7 +23593,7 @@
       <c r="Q448" s="8"/>
       <c r="R448" s="8"/>
     </row>
-    <row r="449" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A449" s="5">
         <v>170</v>
       </c>
@@ -23629,7 +23629,7 @@
       <c r="Q449" s="8"/>
       <c r="R449" s="8"/>
     </row>
-    <row r="450" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A450" s="5">
         <v>171</v>
       </c>
@@ -23673,7 +23673,7 @@
       </c>
       <c r="R450" s="8"/>
     </row>
-    <row r="451" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A451" s="5">
         <v>172</v>
       </c>
@@ -33237,7 +33237,7 @@
       </c>
       <c r="R668" s="8"/>
     </row>
-    <row r="669" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="669" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A669" s="9">
         <v>174</v>
       </c>
@@ -33277,7 +33277,7 @@
       </c>
       <c r="R669" s="8"/>
     </row>
-    <row r="670" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="670" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A670" s="5">
         <v>174</v>
       </c>
@@ -33477,7 +33477,7 @@
       </c>
       <c r="R674" s="8"/>
     </row>
-    <row r="675" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="675" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A675" s="9">
         <v>174</v>
       </c>
@@ -33597,7 +33597,7 @@
       </c>
       <c r="R677" s="8"/>
     </row>
-    <row r="678" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="678" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A678" s="9">
         <v>174</v>
       </c>
@@ -33677,7 +33677,7 @@
       </c>
       <c r="R679" s="8"/>
     </row>
-    <row r="680" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="680" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A680" s="9">
         <v>174</v>
       </c>
@@ -33797,7 +33797,7 @@
       </c>
       <c r="R682" s="8"/>
     </row>
-    <row r="683" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="683" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A683" s="9">
         <v>174</v>
       </c>
@@ -33917,7 +33917,7 @@
       </c>
       <c r="R685" s="8"/>
     </row>
-    <row r="686" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="686" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A686" s="5">
         <v>174</v>
       </c>
@@ -34277,7 +34277,7 @@
       </c>
       <c r="R694" s="8"/>
     </row>
-    <row r="695" spans="1:18" ht="39" x14ac:dyDescent="0.25">
+    <row r="695" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A695" s="5">
         <v>174</v>
       </c>
@@ -34437,7 +34437,7 @@
       </c>
       <c r="R698" s="8"/>
     </row>
-    <row r="699" spans="1:18" ht="39" x14ac:dyDescent="0.25">
+    <row r="699" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A699" s="5">
         <v>174</v>
       </c>
@@ -34477,7 +34477,7 @@
       </c>
       <c r="R699" s="8"/>
     </row>
-    <row r="700" spans="1:18" ht="39" x14ac:dyDescent="0.25">
+    <row r="700" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A700" s="5">
         <v>174</v>
       </c>
@@ -34637,7 +34637,7 @@
       </c>
       <c r="R703" s="8"/>
     </row>
-    <row r="704" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="704" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A704" s="9">
         <v>174</v>
       </c>
@@ -34837,7 +34837,7 @@
       </c>
       <c r="R708" s="8"/>
     </row>
-    <row r="709" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="709" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A709" s="9">
         <v>174</v>
       </c>
@@ -34917,7 +34917,7 @@
       </c>
       <c r="R710" s="8"/>
     </row>
-    <row r="711" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="711" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A711" s="9">
         <v>174</v>
       </c>
@@ -35037,7 +35037,7 @@
       </c>
       <c r="R713" s="8"/>
     </row>
-    <row r="714" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="714" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A714" s="9">
         <v>174</v>
       </c>
@@ -35197,7 +35197,7 @@
       </c>
       <c r="R717" s="8"/>
     </row>
-    <row r="718" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="718" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A718" s="9">
         <v>174</v>
       </c>
@@ -35277,7 +35277,7 @@
       </c>
       <c r="R719" s="8"/>
     </row>
-    <row r="720" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="720" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A720" s="9">
         <v>174</v>
       </c>
@@ -35357,7 +35357,7 @@
       </c>
       <c r="R721" s="8"/>
     </row>
-    <row r="722" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="722" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A722" s="9">
         <v>174</v>
       </c>
@@ -36997,7 +36997,7 @@
       </c>
       <c r="R762" s="8"/>
     </row>
-    <row r="763" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="763" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A763" s="9">
         <v>174</v>
       </c>
@@ -37237,7 +37237,7 @@
       </c>
       <c r="R768" s="8"/>
     </row>
-    <row r="769" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="769" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A769" s="9">
         <v>174</v>
       </c>
@@ -39949,7 +39949,7 @@
       <c r="Q836" s="8"/>
       <c r="R836" s="8"/>
     </row>
-    <row r="837" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="837" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A837" s="5">
         <v>179</v>
       </c>
@@ -40251,7 +40251,7 @@
       <c r="Q844" s="8"/>
       <c r="R844" s="8"/>
     </row>
-    <row r="845" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="845" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A845" s="5">
         <v>183</v>
       </c>
@@ -40857,7 +40857,7 @@
       <c r="Q860" s="8"/>
       <c r="R860" s="8"/>
     </row>
-    <row r="861" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="861" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A861" s="9">
         <v>195</v>
       </c>
@@ -40899,7 +40899,7 @@
       </c>
       <c r="R861" s="8"/>
     </row>
-    <row r="862" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="862" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A862" s="5">
         <v>196</v>
       </c>
@@ -40941,7 +40941,7 @@
       <c r="Q862" s="8"/>
       <c r="R862" s="8"/>
     </row>
-    <row r="863" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="863" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A863" s="5">
         <v>196</v>
       </c>
@@ -41125,7 +41125,7 @@
       <c r="Q867" s="8"/>
       <c r="R867" s="8"/>
     </row>
-    <row r="868" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="868" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A868" s="5">
         <v>201</v>
       </c>
@@ -42961,7 +42961,7 @@
       <c r="Q916" s="8"/>
       <c r="R916" s="8"/>
     </row>
-    <row r="917" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="917" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A917" s="5">
         <v>221</v>
       </c>
@@ -43077,7 +43077,7 @@
       <c r="Q919" s="8"/>
       <c r="R919" s="8"/>
     </row>
-    <row r="920" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="920" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A920" s="5">
         <v>222</v>
       </c>
@@ -43223,7 +43223,7 @@
       <c r="Q923" s="8"/>
       <c r="R923" s="8"/>
     </row>
-    <row r="924" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="924" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A924" s="5">
         <v>226</v>
       </c>
@@ -43293,7 +43293,7 @@
       <c r="Q925" s="8"/>
       <c r="R925" s="8"/>
     </row>
-    <row r="926" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="926" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A926" s="5">
         <v>228</v>
       </c>
@@ -43783,7 +43783,7 @@
       </c>
       <c r="R938" s="8"/>
     </row>
-    <row r="939" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="939" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A939" s="5">
         <v>236</v>
       </c>
@@ -43857,7 +43857,7 @@
       <c r="Q940" s="8"/>
       <c r="R940" s="8"/>
     </row>
-    <row r="941" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="941" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A941" s="5">
         <v>237</v>
       </c>
@@ -43963,7 +43963,7 @@
       <c r="Q943" s="8"/>
       <c r="R943" s="8"/>
     </row>
-    <row r="944" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="944" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A944" s="5">
         <v>240</v>
       </c>
@@ -44193,7 +44193,7 @@
       <c r="Q949" s="8"/>
       <c r="R949" s="8"/>
     </row>
-    <row r="950" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="950" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A950" s="5">
         <v>242</v>
       </c>
@@ -44805,7 +44805,7 @@
       </c>
       <c r="R964" s="8"/>
     </row>
-    <row r="965" spans="1:18" ht="39" x14ac:dyDescent="0.25">
+    <row r="965" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A965" s="5">
         <v>244</v>
       </c>
@@ -48459,7 +48459,7 @@
       </c>
       <c r="R1051" s="8"/>
     </row>
-    <row r="1052" spans="1:18" ht="39" x14ac:dyDescent="0.25">
+    <row r="1052" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1052" s="10">
         <v>244</v>
       </c>
@@ -51105,7 +51105,7 @@
       </c>
       <c r="R1114" s="8"/>
     </row>
-    <row r="1115" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1115" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1115" s="10">
         <v>244</v>
       </c>
@@ -51715,7 +51715,7 @@
       <c r="Q1129" s="8"/>
       <c r="R1129" s="8"/>
     </row>
-    <row r="1130" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1130" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1130" s="10">
         <v>248</v>
       </c>
@@ -51827,7 +51827,7 @@
       <c r="Q1132" s="8"/>
       <c r="R1132" s="8"/>
     </row>
-    <row r="1133" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1133" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1133" s="10">
         <v>249</v>
       </c>
@@ -51863,7 +51863,7 @@
       <c r="Q1133" s="8"/>
       <c r="R1133" s="8"/>
     </row>
-    <row r="1134" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1134" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1134" s="10">
         <v>250</v>
       </c>
@@ -51897,7 +51897,7 @@
       <c r="Q1134" s="8"/>
       <c r="R1134" s="8"/>
     </row>
-    <row r="1135" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1135" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1135" s="10">
         <v>251</v>
       </c>
@@ -52075,7 +52075,7 @@
       <c r="Q1139" s="8"/>
       <c r="R1139" s="8"/>
     </row>
-    <row r="1140" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1140" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1140" s="10">
         <v>256</v>
       </c>
@@ -52181,7 +52181,7 @@
       <c r="Q1142" s="8"/>
       <c r="R1142" s="8"/>
     </row>
-    <row r="1143" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1143" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1143" s="10">
         <v>259</v>
       </c>
@@ -52215,7 +52215,7 @@
       <c r="Q1143" s="8"/>
       <c r="R1143" s="8"/>
     </row>
-    <row r="1144" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1144" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1144" s="10">
         <v>260</v>
       </c>
@@ -52249,7 +52249,7 @@
       <c r="Q1144" s="8"/>
       <c r="R1144" s="8"/>
     </row>
-    <row r="1145" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1145" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1145" s="10">
         <v>261</v>
       </c>
@@ -52285,7 +52285,7 @@
       <c r="Q1145" s="8"/>
       <c r="R1145" s="8"/>
     </row>
-    <row r="1146" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1146" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1146" s="10">
         <v>262</v>
       </c>
@@ -52321,7 +52321,7 @@
       <c r="Q1146" s="8"/>
       <c r="R1146" s="8"/>
     </row>
-    <row r="1147" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1147" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1147" s="10">
         <v>263</v>
       </c>
@@ -52431,7 +52431,7 @@
       <c r="Q1149" s="8"/>
       <c r="R1149" s="8"/>
     </row>
-    <row r="1150" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1150" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1150" s="10">
         <v>266</v>
       </c>
@@ -53753,7 +53753,7 @@
       <c r="Q1184" s="8"/>
       <c r="R1184" s="8"/>
     </row>
-    <row r="1185" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1185" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1185" s="10">
         <v>290</v>
       </c>
@@ -53985,7 +53985,7 @@
       <c r="Q1190" s="8"/>
       <c r="R1190" s="8"/>
     </row>
-    <row r="1191" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1191" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1191" s="10">
         <v>294</v>
       </c>
@@ -55433,7 +55433,7 @@
       </c>
       <c r="R1227" s="8"/>
     </row>
-    <row r="1228" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1228" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1228" s="10">
         <v>312</v>
       </c>
@@ -55539,7 +55539,7 @@
       <c r="Q1230" s="8"/>
       <c r="R1230" s="8"/>
     </row>
-    <row r="1231" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1231" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1231" s="10">
         <v>315</v>
       </c>
@@ -56595,7 +56595,7 @@
       <c r="Q1254" s="8"/>
       <c r="R1254" s="8"/>
     </row>
-    <row r="1255" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1255" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1255" s="8">
         <v>320</v>
       </c>
@@ -57447,7 +57447,7 @@
       <c r="Q1276" s="8"/>
       <c r="R1276" s="8"/>
     </row>
-    <row r="1277" spans="1:18" ht="39" x14ac:dyDescent="0.25">
+    <row r="1277" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1277" s="10">
         <v>323</v>
       </c>
@@ -57485,7 +57485,7 @@
       <c r="Q1277" s="8"/>
       <c r="R1277" s="8"/>
     </row>
-    <row r="1278" spans="1:18" ht="39" x14ac:dyDescent="0.25">
+    <row r="1278" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1278" s="10">
         <v>323</v>
       </c>
@@ -57789,7 +57789,7 @@
       <c r="Q1285" s="8"/>
       <c r="R1285" s="8"/>
     </row>
-    <row r="1286" spans="1:18" ht="39" x14ac:dyDescent="0.25">
+    <row r="1286" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1286" s="10">
         <v>323</v>
       </c>
@@ -58979,7 +58979,7 @@
       </c>
       <c r="R1317" s="8"/>
     </row>
-    <row r="1318" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1318" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1318" s="10">
         <v>333</v>
       </c>
@@ -59309,7 +59309,7 @@
       <c r="Q1325" s="8"/>
       <c r="R1325" s="8"/>
     </row>
-    <row r="1326" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1326" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1326" s="10">
         <v>334</v>
       </c>
@@ -59347,7 +59347,7 @@
       <c r="Q1326" s="8"/>
       <c r="R1326" s="8"/>
     </row>
-    <row r="1327" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1327" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1327" s="10">
         <v>335</v>
       </c>
@@ -64731,8 +64731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9585C0FF-65C5-4BD8-9936-5C9A63F7E604}">
   <dimension ref="A1:CE30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64811,104 +64811,104 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:83" x14ac:dyDescent="0.25">
-      <c r="Q1" s="64">
+      <c r="Q1" s="65">
         <v>45536</v>
       </c>
-      <c r="R1" s="65"/>
-      <c r="S1" s="65"/>
-      <c r="T1" s="65"/>
-      <c r="U1" s="64">
+      <c r="R1" s="66"/>
+      <c r="S1" s="66"/>
+      <c r="T1" s="66"/>
+      <c r="U1" s="65">
         <v>45566</v>
       </c>
-      <c r="V1" s="64"/>
-      <c r="W1" s="64"/>
-      <c r="X1" s="64"/>
-      <c r="Y1" s="64"/>
-      <c r="Z1" s="61">
+      <c r="V1" s="65"/>
+      <c r="W1" s="65"/>
+      <c r="X1" s="65"/>
+      <c r="Y1" s="65"/>
+      <c r="Z1" s="62">
         <v>45597</v>
       </c>
-      <c r="AA1" s="62"/>
-      <c r="AB1" s="62"/>
-      <c r="AC1" s="63"/>
-      <c r="AD1" s="61">
+      <c r="AA1" s="63"/>
+      <c r="AB1" s="63"/>
+      <c r="AC1" s="64"/>
+      <c r="AD1" s="62">
         <v>45627</v>
       </c>
-      <c r="AE1" s="62"/>
-      <c r="AF1" s="62"/>
-      <c r="AG1" s="63"/>
-      <c r="AH1" s="61">
+      <c r="AE1" s="63"/>
+      <c r="AF1" s="63"/>
+      <c r="AG1" s="64"/>
+      <c r="AH1" s="62">
         <v>45658</v>
       </c>
-      <c r="AI1" s="62"/>
-      <c r="AJ1" s="62"/>
-      <c r="AK1" s="62"/>
-      <c r="AL1" s="63"/>
-      <c r="AM1" s="61">
+      <c r="AI1" s="63"/>
+      <c r="AJ1" s="63"/>
+      <c r="AK1" s="63"/>
+      <c r="AL1" s="64"/>
+      <c r="AM1" s="62">
         <v>45689</v>
       </c>
-      <c r="AN1" s="62"/>
-      <c r="AO1" s="62"/>
-      <c r="AP1" s="63"/>
-      <c r="AQ1" s="61">
+      <c r="AN1" s="63"/>
+      <c r="AO1" s="63"/>
+      <c r="AP1" s="64"/>
+      <c r="AQ1" s="62">
         <v>45717</v>
       </c>
-      <c r="AR1" s="62"/>
-      <c r="AS1" s="62"/>
-      <c r="AT1" s="63"/>
-      <c r="AU1" s="61">
+      <c r="AR1" s="63"/>
+      <c r="AS1" s="63"/>
+      <c r="AT1" s="64"/>
+      <c r="AU1" s="62">
         <v>45748</v>
       </c>
-      <c r="AV1" s="62"/>
-      <c r="AW1" s="62"/>
-      <c r="AX1" s="63"/>
-      <c r="AY1" s="61">
+      <c r="AV1" s="63"/>
+      <c r="AW1" s="63"/>
+      <c r="AX1" s="64"/>
+      <c r="AY1" s="62">
         <v>45778</v>
       </c>
-      <c r="AZ1" s="62"/>
-      <c r="BA1" s="62"/>
-      <c r="BB1" s="62"/>
-      <c r="BC1" s="63"/>
-      <c r="BD1" s="61">
+      <c r="AZ1" s="63"/>
+      <c r="BA1" s="63"/>
+      <c r="BB1" s="63"/>
+      <c r="BC1" s="64"/>
+      <c r="BD1" s="62">
         <v>45809</v>
       </c>
-      <c r="BE1" s="62"/>
-      <c r="BF1" s="62"/>
-      <c r="BG1" s="62"/>
-      <c r="BH1" s="61">
+      <c r="BE1" s="63"/>
+      <c r="BF1" s="63"/>
+      <c r="BG1" s="63"/>
+      <c r="BH1" s="62">
         <v>45839</v>
       </c>
-      <c r="BI1" s="62"/>
-      <c r="BJ1" s="62"/>
-      <c r="BK1" s="62"/>
-      <c r="BL1" s="63"/>
-      <c r="BM1" s="61">
+      <c r="BI1" s="63"/>
+      <c r="BJ1" s="63"/>
+      <c r="BK1" s="63"/>
+      <c r="BL1" s="64"/>
+      <c r="BM1" s="62">
         <v>45870</v>
       </c>
-      <c r="BN1" s="62"/>
-      <c r="BO1" s="62"/>
-      <c r="BP1" s="62"/>
-      <c r="BQ1" s="61">
+      <c r="BN1" s="63"/>
+      <c r="BO1" s="63"/>
+      <c r="BP1" s="63"/>
+      <c r="BQ1" s="62">
         <v>45901</v>
       </c>
-      <c r="BR1" s="62"/>
-      <c r="BS1" s="62"/>
-      <c r="BT1" s="62"/>
-      <c r="BU1" s="61">
+      <c r="BR1" s="63"/>
+      <c r="BS1" s="63"/>
+      <c r="BT1" s="63"/>
+      <c r="BU1" s="62">
         <v>45931</v>
       </c>
-      <c r="BV1" s="62"/>
-      <c r="BW1" s="62"/>
-      <c r="BX1" s="62"/>
-      <c r="BZ1" s="61">
+      <c r="BV1" s="63"/>
+      <c r="BW1" s="63"/>
+      <c r="BX1" s="63"/>
+      <c r="BZ1" s="62">
         <v>45962</v>
       </c>
-      <c r="CA1" s="62"/>
-      <c r="CB1" s="62"/>
-      <c r="CC1" s="62"/>
-      <c r="CD1" s="66" t="s">
+      <c r="CA1" s="63"/>
+      <c r="CB1" s="63"/>
+      <c r="CC1" s="63"/>
+      <c r="CD1" s="61" t="s">
         <v>1856</v>
       </c>
-      <c r="CE1" s="66"/>
+      <c r="CE1" s="61"/>
     </row>
     <row r="2" spans="1:83" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
@@ -65781,7 +65781,7 @@
       <c r="P8" s="55">
         <v>45538</v>
       </c>
-      <c r="Q8" s="59"/>
+      <c r="Q8" s="58"/>
       <c r="R8" s="12"/>
       <c r="S8" s="12"/>
       <c r="T8" s="12"/>
@@ -68262,22 +68262,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="AM1:AP1"/>
+    <mergeCell ref="AQ1:AT1"/>
+    <mergeCell ref="AU1:AX1"/>
+    <mergeCell ref="AY1:BC1"/>
+    <mergeCell ref="BD1:BG1"/>
+    <mergeCell ref="Q1:T1"/>
+    <mergeCell ref="U1:Y1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AD1:AG1"/>
+    <mergeCell ref="AH1:AL1"/>
     <mergeCell ref="CD1:CE1"/>
     <mergeCell ref="BH1:BL1"/>
     <mergeCell ref="BM1:BP1"/>
     <mergeCell ref="BQ1:BT1"/>
     <mergeCell ref="BU1:BX1"/>
     <mergeCell ref="BZ1:CC1"/>
-    <mergeCell ref="Q1:T1"/>
-    <mergeCell ref="U1:Y1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AD1:AG1"/>
-    <mergeCell ref="AH1:AL1"/>
-    <mergeCell ref="AM1:AP1"/>
-    <mergeCell ref="AQ1:AT1"/>
-    <mergeCell ref="AU1:AX1"/>
-    <mergeCell ref="AY1:BC1"/>
-    <mergeCell ref="BD1:BG1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
generación de pruebas Internas (terminado)
actualizacion plan de trabajo
</commit_message>
<xml_diff>
--- a/00-Documentacion/Listado de reportes totales-TI.xlsx
+++ b/00-Documentacion/Listado de reportes totales-TI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E64DE8-A94B-483D-9CCC-429AC98AA980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2210E913-C8D6-4E02-A8D5-E09B539F5720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{1498AA1A-1ACC-4329-A050-ACA05131B658}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13250" uniqueCount="1869">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13251" uniqueCount="1869">
   <si>
     <t xml:space="preserve">Reporte </t>
   </si>
@@ -5998,7 +5998,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6124,10 +6124,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6141,6 +6137,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -64752,8 +64751,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9585C0FF-65C5-4BD8-9936-5C9A63F7E604}">
   <dimension ref="A1:CG31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="N8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AG18" sqref="AG18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64834,104 +64833,104 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="S1" s="68">
+      <c r="S1" s="66">
         <v>45536</v>
       </c>
-      <c r="T1" s="69"/>
-      <c r="U1" s="69"/>
-      <c r="V1" s="69"/>
-      <c r="W1" s="68">
+      <c r="T1" s="67"/>
+      <c r="U1" s="67"/>
+      <c r="V1" s="67"/>
+      <c r="W1" s="66">
         <v>45566</v>
       </c>
-      <c r="X1" s="68"/>
-      <c r="Y1" s="68"/>
-      <c r="Z1" s="68"/>
-      <c r="AA1" s="68"/>
-      <c r="AB1" s="65">
+      <c r="X1" s="66"/>
+      <c r="Y1" s="66"/>
+      <c r="Z1" s="66"/>
+      <c r="AA1" s="66"/>
+      <c r="AB1" s="63">
         <v>45597</v>
       </c>
-      <c r="AC1" s="66"/>
-      <c r="AD1" s="66"/>
-      <c r="AE1" s="67"/>
-      <c r="AF1" s="65">
+      <c r="AC1" s="64"/>
+      <c r="AD1" s="64"/>
+      <c r="AE1" s="65"/>
+      <c r="AF1" s="63">
         <v>45627</v>
       </c>
-      <c r="AG1" s="66"/>
-      <c r="AH1" s="66"/>
-      <c r="AI1" s="67"/>
-      <c r="AJ1" s="65">
+      <c r="AG1" s="64"/>
+      <c r="AH1" s="64"/>
+      <c r="AI1" s="65"/>
+      <c r="AJ1" s="63">
         <v>45658</v>
       </c>
-      <c r="AK1" s="66"/>
-      <c r="AL1" s="66"/>
-      <c r="AM1" s="66"/>
-      <c r="AN1" s="67"/>
-      <c r="AO1" s="65">
+      <c r="AK1" s="64"/>
+      <c r="AL1" s="64"/>
+      <c r="AM1" s="64"/>
+      <c r="AN1" s="65"/>
+      <c r="AO1" s="63">
         <v>45689</v>
       </c>
-      <c r="AP1" s="66"/>
-      <c r="AQ1" s="66"/>
-      <c r="AR1" s="67"/>
-      <c r="AS1" s="65">
+      <c r="AP1" s="64"/>
+      <c r="AQ1" s="64"/>
+      <c r="AR1" s="65"/>
+      <c r="AS1" s="63">
         <v>45717</v>
       </c>
-      <c r="AT1" s="66"/>
-      <c r="AU1" s="66"/>
-      <c r="AV1" s="67"/>
-      <c r="AW1" s="65">
+      <c r="AT1" s="64"/>
+      <c r="AU1" s="64"/>
+      <c r="AV1" s="65"/>
+      <c r="AW1" s="63">
         <v>45748</v>
       </c>
-      <c r="AX1" s="66"/>
-      <c r="AY1" s="66"/>
-      <c r="AZ1" s="67"/>
-      <c r="BA1" s="65">
+      <c r="AX1" s="64"/>
+      <c r="AY1" s="64"/>
+      <c r="AZ1" s="65"/>
+      <c r="BA1" s="63">
         <v>45778</v>
       </c>
-      <c r="BB1" s="66"/>
-      <c r="BC1" s="66"/>
-      <c r="BD1" s="66"/>
-      <c r="BE1" s="67"/>
-      <c r="BF1" s="65">
+      <c r="BB1" s="64"/>
+      <c r="BC1" s="64"/>
+      <c r="BD1" s="64"/>
+      <c r="BE1" s="65"/>
+      <c r="BF1" s="63">
         <v>45809</v>
       </c>
-      <c r="BG1" s="66"/>
-      <c r="BH1" s="66"/>
-      <c r="BI1" s="66"/>
-      <c r="BJ1" s="65">
+      <c r="BG1" s="64"/>
+      <c r="BH1" s="64"/>
+      <c r="BI1" s="64"/>
+      <c r="BJ1" s="63">
         <v>45839</v>
       </c>
-      <c r="BK1" s="66"/>
-      <c r="BL1" s="66"/>
-      <c r="BM1" s="66"/>
-      <c r="BN1" s="67"/>
-      <c r="BO1" s="65">
+      <c r="BK1" s="64"/>
+      <c r="BL1" s="64"/>
+      <c r="BM1" s="64"/>
+      <c r="BN1" s="65"/>
+      <c r="BO1" s="63">
         <v>45870</v>
       </c>
-      <c r="BP1" s="66"/>
-      <c r="BQ1" s="66"/>
-      <c r="BR1" s="66"/>
-      <c r="BS1" s="65">
+      <c r="BP1" s="64"/>
+      <c r="BQ1" s="64"/>
+      <c r="BR1" s="64"/>
+      <c r="BS1" s="63">
         <v>45901</v>
       </c>
-      <c r="BT1" s="66"/>
-      <c r="BU1" s="66"/>
-      <c r="BV1" s="66"/>
-      <c r="BW1" s="65">
+      <c r="BT1" s="64"/>
+      <c r="BU1" s="64"/>
+      <c r="BV1" s="64"/>
+      <c r="BW1" s="63">
         <v>45931</v>
       </c>
-      <c r="BX1" s="66"/>
-      <c r="BY1" s="66"/>
-      <c r="BZ1" s="66"/>
-      <c r="CB1" s="65">
+      <c r="BX1" s="64"/>
+      <c r="BY1" s="64"/>
+      <c r="BZ1" s="64"/>
+      <c r="CB1" s="63">
         <v>45962</v>
       </c>
-      <c r="CC1" s="66"/>
-      <c r="CD1" s="66"/>
-      <c r="CE1" s="66"/>
-      <c r="CF1" s="64" t="s">
+      <c r="CC1" s="64"/>
+      <c r="CD1" s="64"/>
+      <c r="CE1" s="64"/>
+      <c r="CF1" s="68" t="s">
         <v>1854</v>
       </c>
-      <c r="CG1" s="64"/>
+      <c r="CG1" s="68"/>
     </row>
     <row r="2" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
@@ -66654,7 +66653,7 @@
         <v>1864</v>
       </c>
       <c r="P15" s="12" t="s">
-        <v>1859</v>
+        <v>1865</v>
       </c>
       <c r="Q15" s="51">
         <v>45547</v>
@@ -66663,9 +66662,9 @@
         <v>45558</v>
       </c>
       <c r="S15" s="54"/>
-      <c r="T15" s="63"/>
-      <c r="U15" s="63"/>
-      <c r="V15" s="63"/>
+      <c r="T15" s="12"/>
+      <c r="U15" s="12"/>
+      <c r="V15" s="12"/>
       <c r="W15" s="12"/>
       <c r="X15" s="12"/>
       <c r="Y15" s="12"/>
@@ -66758,7 +66757,9 @@
       <c r="O16" s="12" t="s">
         <v>1864</v>
       </c>
-      <c r="P16" s="12"/>
+      <c r="P16" s="12" t="s">
+        <v>1859</v>
+      </c>
       <c r="Q16" s="51">
         <v>45559</v>
       </c>
@@ -68400,22 +68401,22 @@
     </sortState>
   </autoFilter>
   <mergeCells count="16">
-    <mergeCell ref="AO1:AR1"/>
-    <mergeCell ref="AS1:AV1"/>
-    <mergeCell ref="AW1:AZ1"/>
-    <mergeCell ref="BA1:BE1"/>
-    <mergeCell ref="BF1:BI1"/>
-    <mergeCell ref="S1:V1"/>
-    <mergeCell ref="W1:AA1"/>
-    <mergeCell ref="AB1:AE1"/>
-    <mergeCell ref="AF1:AI1"/>
-    <mergeCell ref="AJ1:AN1"/>
     <mergeCell ref="CF1:CG1"/>
     <mergeCell ref="BJ1:BN1"/>
     <mergeCell ref="BO1:BR1"/>
     <mergeCell ref="BS1:BV1"/>
     <mergeCell ref="BW1:BZ1"/>
     <mergeCell ref="CB1:CE1"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="W1:AA1"/>
+    <mergeCell ref="AB1:AE1"/>
+    <mergeCell ref="AF1:AI1"/>
+    <mergeCell ref="AJ1:AN1"/>
+    <mergeCell ref="AO1:AR1"/>
+    <mergeCell ref="AS1:AV1"/>
+    <mergeCell ref="AW1:AZ1"/>
+    <mergeCell ref="BA1:BE1"/>
+    <mergeCell ref="BF1:BI1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
validación de procedimiento de pedimento2
SC_RS.SPG_RS_COEX_PEDIMENTOS_BOSCH.P_DAT_FOLIOS_RECTIFICACION, cambiar nombres de la columnas
generación de clase
definición de parámetros
</commit_message>
<xml_diff>
--- a/00-Documentacion/Listado de reportes totales-TI.xlsx
+++ b/00-Documentacion/Listado de reportes totales-TI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41099BE4-F1F4-4CFB-B616-3C0C2E3CB16E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{227D65E7-DCF6-4F1B-AD47-BF58D472AF95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{1498AA1A-1ACC-4329-A050-ACA05131B658}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13251" uniqueCount="1870">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13251" uniqueCount="1869">
   <si>
     <t xml:space="preserve">Reporte </t>
   </si>
@@ -5658,9 +5658,6 @@
   </si>
   <si>
     <t>|</t>
-  </si>
-  <si>
-    <t>Ajustes</t>
   </si>
   <si>
     <t>bosch_pedim2_xls</t>
@@ -6127,9 +6124,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6145,7 +6140,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -64755,8 +64752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9585C0FF-65C5-4BD8-9936-5C9A63F7E604}">
   <dimension ref="A1:CG31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AC11" sqref="AC11"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="V17" sqref="V17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64931,10 +64928,10 @@
       <c r="CC1" s="65"/>
       <c r="CD1" s="65"/>
       <c r="CE1" s="65"/>
-      <c r="CF1" s="63" t="s">
+      <c r="CF1" s="69" t="s">
         <v>1854</v>
       </c>
-      <c r="CG1" s="63"/>
+      <c r="CG1" s="69"/>
     </row>
     <row r="2" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
@@ -66743,7 +66740,7 @@
       <c r="E16" s="17"/>
       <c r="F16" s="22"/>
       <c r="G16" s="12" t="s">
-        <v>1869</v>
+        <v>1868</v>
       </c>
       <c r="H16" s="12" t="s">
         <v>1716</v>
@@ -66773,9 +66770,9 @@
       <c r="S16" s="54"/>
       <c r="T16" s="12"/>
       <c r="U16" s="12"/>
-      <c r="V16" s="69"/>
-      <c r="W16" s="69"/>
-      <c r="X16" s="69"/>
+      <c r="V16" s="63"/>
+      <c r="W16" s="63"/>
+      <c r="X16" s="63"/>
       <c r="Y16" s="12"/>
       <c r="AA16" s="12"/>
       <c r="AB16" s="12"/>
@@ -66980,7 +66977,7 @@
         <v>9</v>
       </c>
       <c r="O18" s="12" t="s">
-        <v>1868</v>
+        <v>1864</v>
       </c>
       <c r="P18" s="12"/>
       <c r="Q18" s="51">
@@ -68405,22 +68402,22 @@
     </sortState>
   </autoFilter>
   <mergeCells count="16">
-    <mergeCell ref="AO1:AR1"/>
-    <mergeCell ref="AS1:AV1"/>
-    <mergeCell ref="AW1:AZ1"/>
-    <mergeCell ref="BA1:BE1"/>
-    <mergeCell ref="BF1:BI1"/>
-    <mergeCell ref="S1:V1"/>
-    <mergeCell ref="W1:AA1"/>
-    <mergeCell ref="AB1:AE1"/>
-    <mergeCell ref="AF1:AI1"/>
-    <mergeCell ref="AJ1:AN1"/>
     <mergeCell ref="CF1:CG1"/>
     <mergeCell ref="BJ1:BN1"/>
     <mergeCell ref="BO1:BR1"/>
     <mergeCell ref="BS1:BV1"/>
     <mergeCell ref="BW1:BZ1"/>
     <mergeCell ref="CB1:CE1"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="W1:AA1"/>
+    <mergeCell ref="AB1:AE1"/>
+    <mergeCell ref="AF1:AI1"/>
+    <mergeCell ref="AJ1:AN1"/>
+    <mergeCell ref="AO1:AR1"/>
+    <mergeCell ref="AS1:AV1"/>
+    <mergeCell ref="AW1:AZ1"/>
+    <mergeCell ref="BA1:BE1"/>
+    <mergeCell ref="BF1:BI1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Agrego detalles del Reporte de Evolución en el cuadro de seguimiento.
</commit_message>
<xml_diff>
--- a/00-Documentacion/Listado de reportes totales-TI.xlsx
+++ b/00-Documentacion/Listado de reportes totales-TI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\source\repos\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0FC6630-9A33-4B97-804D-B3D5123782EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF6ED99-7045-4DD4-ABAF-A89CE282C454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10185" yWindow="375" windowWidth="9000" windowHeight="10290" activeTab="2" xr2:uid="{1498AA1A-1ACC-4329-A050-ACA05131B658}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{1498AA1A-1ACC-4329-A050-ACA05131B658}"/>
   </bookViews>
   <sheets>
     <sheet name="General - Analisis" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13258" uniqueCount="1874">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13260" uniqueCount="1876">
   <si>
     <t xml:space="preserve">Reporte </t>
   </si>
@@ -5676,6 +5676,12 @@
   </si>
   <si>
     <t>ZReportes DG</t>
+  </si>
+  <si>
+    <t>Semanal en día Domingo</t>
+  </si>
+  <si>
+    <t>excel, correo</t>
   </si>
 </sst>
 </file>
@@ -5877,7 +5883,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -5985,35 +5991,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6132,14 +6114,8 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6155,7 +6131,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -8715,7 +8693,7 @@
       </c>
       <c r="R54" s="8"/>
     </row>
-    <row r="55" spans="1:18" ht="39" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>14</v>
       </c>
@@ -9243,7 +9221,7 @@
       </c>
       <c r="R66" s="8"/>
     </row>
-    <row r="67" spans="1:18" ht="51.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" ht="39" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
         <v>14</v>
       </c>
@@ -16547,7 +16525,7 @@
       <c r="Q262" s="8"/>
       <c r="R262" s="8"/>
     </row>
-    <row r="263" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A263" s="5">
         <v>67</v>
       </c>
@@ -21959,7 +21937,7 @@
       </c>
       <c r="R403" s="8"/>
     </row>
-    <row r="404" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A404" s="5">
         <v>138</v>
       </c>
@@ -24975,7 +24953,7 @@
       </c>
       <c r="R479" s="8"/>
     </row>
-    <row r="480" spans="1:18" ht="39" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A480" s="5">
         <v>173</v>
       </c>
@@ -26867,7 +26845,7 @@
       </c>
       <c r="R522" s="8"/>
     </row>
-    <row r="523" spans="1:18" ht="39" x14ac:dyDescent="0.25">
+    <row r="523" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A523" s="5">
         <v>173</v>
       </c>
@@ -37871,7 +37849,7 @@
       </c>
       <c r="R783" s="8"/>
     </row>
-    <row r="784" spans="1:18" ht="39" x14ac:dyDescent="0.25">
+    <row r="784" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A784" s="5">
         <v>174</v>
       </c>
@@ -51307,7 +51285,7 @@
       </c>
       <c r="R1118" s="8"/>
     </row>
-    <row r="1119" spans="1:18" ht="39" x14ac:dyDescent="0.25">
+    <row r="1119" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1119" s="10">
         <v>244</v>
       </c>
@@ -56967,7 +56945,7 @@
       <c r="Q1263" s="8"/>
       <c r="R1263" s="8"/>
     </row>
-    <row r="1264" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1264" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1264" s="10">
         <v>322</v>
       </c>
@@ -64765,8 +64743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9585C0FF-65C5-4BD8-9936-5C9A63F7E604}">
   <dimension ref="A1:CG31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64847,104 +64825,104 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="S1" s="67">
+      <c r="S1" s="63">
         <v>45536</v>
       </c>
-      <c r="T1" s="68"/>
-      <c r="U1" s="68"/>
-      <c r="V1" s="68"/>
-      <c r="W1" s="67">
+      <c r="T1" s="64"/>
+      <c r="U1" s="64"/>
+      <c r="V1" s="64"/>
+      <c r="W1" s="63">
         <v>45566</v>
       </c>
-      <c r="X1" s="67"/>
-      <c r="Y1" s="67"/>
-      <c r="Z1" s="67"/>
-      <c r="AA1" s="67"/>
-      <c r="AB1" s="64">
+      <c r="X1" s="63"/>
+      <c r="Y1" s="63"/>
+      <c r="Z1" s="63"/>
+      <c r="AA1" s="63"/>
+      <c r="AB1" s="60">
         <v>45597</v>
       </c>
-      <c r="AC1" s="65"/>
-      <c r="AD1" s="65"/>
-      <c r="AE1" s="66"/>
-      <c r="AF1" s="64">
+      <c r="AC1" s="61"/>
+      <c r="AD1" s="61"/>
+      <c r="AE1" s="62"/>
+      <c r="AF1" s="60">
         <v>45627</v>
       </c>
-      <c r="AG1" s="65"/>
-      <c r="AH1" s="65"/>
-      <c r="AI1" s="66"/>
-      <c r="AJ1" s="64">
+      <c r="AG1" s="61"/>
+      <c r="AH1" s="61"/>
+      <c r="AI1" s="62"/>
+      <c r="AJ1" s="60">
         <v>45658</v>
       </c>
-      <c r="AK1" s="65"/>
-      <c r="AL1" s="65"/>
-      <c r="AM1" s="65"/>
-      <c r="AN1" s="66"/>
-      <c r="AO1" s="64">
+      <c r="AK1" s="61"/>
+      <c r="AL1" s="61"/>
+      <c r="AM1" s="61"/>
+      <c r="AN1" s="62"/>
+      <c r="AO1" s="60">
         <v>45689</v>
       </c>
-      <c r="AP1" s="65"/>
-      <c r="AQ1" s="65"/>
-      <c r="AR1" s="66"/>
-      <c r="AS1" s="64">
+      <c r="AP1" s="61"/>
+      <c r="AQ1" s="61"/>
+      <c r="AR1" s="62"/>
+      <c r="AS1" s="60">
         <v>45717</v>
       </c>
-      <c r="AT1" s="65"/>
-      <c r="AU1" s="65"/>
-      <c r="AV1" s="66"/>
-      <c r="AW1" s="64">
+      <c r="AT1" s="61"/>
+      <c r="AU1" s="61"/>
+      <c r="AV1" s="62"/>
+      <c r="AW1" s="60">
         <v>45748</v>
       </c>
-      <c r="AX1" s="65"/>
-      <c r="AY1" s="65"/>
-      <c r="AZ1" s="66"/>
-      <c r="BA1" s="64">
+      <c r="AX1" s="61"/>
+      <c r="AY1" s="61"/>
+      <c r="AZ1" s="62"/>
+      <c r="BA1" s="60">
         <v>45778</v>
       </c>
-      <c r="BB1" s="65"/>
-      <c r="BC1" s="65"/>
-      <c r="BD1" s="65"/>
-      <c r="BE1" s="66"/>
-      <c r="BF1" s="64">
+      <c r="BB1" s="61"/>
+      <c r="BC1" s="61"/>
+      <c r="BD1" s="61"/>
+      <c r="BE1" s="62"/>
+      <c r="BF1" s="60">
         <v>45809</v>
       </c>
-      <c r="BG1" s="65"/>
-      <c r="BH1" s="65"/>
-      <c r="BI1" s="65"/>
-      <c r="BJ1" s="64">
+      <c r="BG1" s="61"/>
+      <c r="BH1" s="61"/>
+      <c r="BI1" s="61"/>
+      <c r="BJ1" s="60">
         <v>45839</v>
       </c>
-      <c r="BK1" s="65"/>
-      <c r="BL1" s="65"/>
-      <c r="BM1" s="65"/>
-      <c r="BN1" s="66"/>
-      <c r="BO1" s="64">
+      <c r="BK1" s="61"/>
+      <c r="BL1" s="61"/>
+      <c r="BM1" s="61"/>
+      <c r="BN1" s="62"/>
+      <c r="BO1" s="60">
         <v>45870</v>
       </c>
-      <c r="BP1" s="65"/>
-      <c r="BQ1" s="65"/>
-      <c r="BR1" s="65"/>
-      <c r="BS1" s="64">
+      <c r="BP1" s="61"/>
+      <c r="BQ1" s="61"/>
+      <c r="BR1" s="61"/>
+      <c r="BS1" s="60">
         <v>45901</v>
       </c>
-      <c r="BT1" s="65"/>
-      <c r="BU1" s="65"/>
-      <c r="BV1" s="65"/>
-      <c r="BW1" s="64">
+      <c r="BT1" s="61"/>
+      <c r="BU1" s="61"/>
+      <c r="BV1" s="61"/>
+      <c r="BW1" s="60">
         <v>45931</v>
       </c>
-      <c r="BX1" s="65"/>
-      <c r="BY1" s="65"/>
-      <c r="BZ1" s="65"/>
-      <c r="CB1" s="64">
+      <c r="BX1" s="61"/>
+      <c r="BY1" s="61"/>
+      <c r="BZ1" s="61"/>
+      <c r="CB1" s="60">
         <v>45962</v>
       </c>
-      <c r="CC1" s="65"/>
-      <c r="CD1" s="65"/>
-      <c r="CE1" s="65"/>
-      <c r="CF1" s="63" t="s">
+      <c r="CC1" s="61"/>
+      <c r="CD1" s="61"/>
+      <c r="CE1" s="61"/>
+      <c r="CF1" s="65" t="s">
         <v>1854</v>
       </c>
-      <c r="CG1" s="63"/>
+      <c r="CG1" s="65"/>
     </row>
     <row r="2" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
@@ -65001,7 +64979,7 @@
       <c r="R2" s="52" t="s">
         <v>1793</v>
       </c>
-      <c r="S2" s="61" t="s">
+      <c r="S2" s="58" t="s">
         <v>1794</v>
       </c>
       <c r="T2" s="46" t="s">
@@ -66335,7 +66313,6 @@
       <c r="T12" s="12"/>
       <c r="U12" s="12"/>
       <c r="V12" s="12"/>
-      <c r="W12" s="69"/>
       <c r="X12" s="12"/>
       <c r="Y12" s="12"/>
       <c r="Z12" s="12"/>
@@ -66800,7 +66777,6 @@
       <c r="W16" s="12"/>
       <c r="X16" s="12"/>
       <c r="Y16" s="12"/>
-      <c r="Z16" s="69"/>
       <c r="AA16" s="12"/>
       <c r="AB16" s="12"/>
       <c r="AC16" s="12"/>
@@ -66901,9 +66877,9 @@
       <c r="S17" s="53"/>
       <c r="T17" s="12"/>
       <c r="U17" s="12"/>
-      <c r="V17" s="62"/>
-      <c r="W17" s="62"/>
-      <c r="X17" s="62"/>
+      <c r="V17" s="59"/>
+      <c r="W17" s="59"/>
+      <c r="X17" s="59"/>
       <c r="Y17" s="12"/>
       <c r="Z17" s="12"/>
       <c r="AA17" s="12"/>
@@ -67242,7 +67218,6 @@
       <c r="Y20" s="12"/>
       <c r="Z20" s="12"/>
       <c r="AA20" s="12"/>
-      <c r="AB20" s="69"/>
       <c r="AC20" s="12"/>
       <c r="AD20" s="12"/>
       <c r="AE20" s="12"/>
@@ -67367,7 +67342,6 @@
       <c r="AJ21" s="12"/>
       <c r="AK21" s="12"/>
       <c r="AL21" s="12"/>
-      <c r="AM21" s="69"/>
       <c r="AN21" s="12"/>
       <c r="AO21" s="12"/>
       <c r="AP21" s="12"/>
@@ -67477,7 +67451,6 @@
       <c r="AD22" s="12"/>
       <c r="AE22" s="12"/>
       <c r="AF22" s="12"/>
-      <c r="AG22" s="69"/>
       <c r="AH22" s="12"/>
       <c r="AI22" s="12"/>
       <c r="AJ22" s="12"/>
@@ -67723,10 +67696,6 @@
       <c r="AY24" s="12"/>
       <c r="AZ24" s="12"/>
       <c r="BA24" s="12"/>
-      <c r="BB24" s="69"/>
-      <c r="BC24" s="69"/>
-      <c r="BD24" s="69"/>
-      <c r="BE24" s="69"/>
       <c r="BF24" s="12"/>
       <c r="BG24" s="12"/>
       <c r="BH24" s="12"/>
@@ -67824,7 +67793,6 @@
       <c r="AK25" s="12"/>
       <c r="AL25" s="12"/>
       <c r="AM25" s="12"/>
-      <c r="AN25" s="69"/>
       <c r="AO25" s="12"/>
       <c r="AP25" s="12"/>
       <c r="AQ25" s="12"/>
@@ -67834,7 +67802,6 @@
       <c r="AU25" s="12"/>
       <c r="AV25" s="12"/>
       <c r="AW25" s="12"/>
-      <c r="AX25" s="69"/>
       <c r="AY25" s="12"/>
       <c r="AZ25" s="12"/>
       <c r="BA25" s="12"/>
@@ -68069,7 +68036,6 @@
       <c r="BB27" s="12"/>
       <c r="BC27" s="12"/>
       <c r="BD27" s="12"/>
-      <c r="BE27" s="69"/>
       <c r="BF27" s="12"/>
       <c r="BG27" s="12"/>
       <c r="BH27" s="12"/>
@@ -68301,10 +68267,6 @@
       <c r="BR29" s="12"/>
       <c r="BS29" s="12"/>
       <c r="BT29" s="12"/>
-      <c r="BU29" s="69"/>
-      <c r="BV29" s="69"/>
-      <c r="BW29" s="69"/>
-      <c r="BX29" s="69"/>
       <c r="BY29" s="12"/>
       <c r="BZ29" s="12"/>
       <c r="CA29" s="12"/>
@@ -68436,88 +68398,92 @@
         <v>1872</v>
       </c>
       <c r="E31" s="29" t="s">
-        <v>1783</v>
-      </c>
-      <c r="F31" s="69"/>
-      <c r="G31" s="69"/>
-      <c r="H31" s="69"/>
-      <c r="I31" s="69"/>
-      <c r="J31" s="69"/>
-      <c r="K31" s="69"/>
-      <c r="L31" s="69"/>
-      <c r="M31" s="69"/>
-      <c r="N31" s="69"/>
-      <c r="O31" s="58"/>
-      <c r="P31" s="58"/>
-      <c r="Q31" s="59"/>
-      <c r="R31" s="60"/>
-      <c r="S31" s="69"/>
-      <c r="T31" s="69"/>
-      <c r="U31" s="69"/>
-      <c r="V31" s="69"/>
-      <c r="W31" s="69"/>
-      <c r="X31" s="69"/>
-      <c r="Y31" s="69"/>
-      <c r="Z31" s="69"/>
-      <c r="AA31" s="69"/>
-      <c r="AB31" s="69"/>
-      <c r="AC31" s="69"/>
-      <c r="AD31" s="69"/>
-      <c r="AE31" s="69"/>
-      <c r="AF31" s="69"/>
-      <c r="AG31" s="69"/>
-      <c r="AH31" s="69"/>
-      <c r="AI31" s="69"/>
-      <c r="AJ31" s="69"/>
-      <c r="AK31" s="69"/>
-      <c r="AL31" s="69"/>
-      <c r="AM31" s="69"/>
-      <c r="AN31" s="69"/>
-      <c r="AO31" s="69"/>
-      <c r="AP31" s="69"/>
-      <c r="AQ31" s="69"/>
-      <c r="AR31" s="69"/>
-      <c r="AS31" s="69"/>
-      <c r="AT31" s="69"/>
-      <c r="AU31" s="69"/>
-      <c r="AV31" s="69"/>
-      <c r="AW31" s="69"/>
-      <c r="AX31" s="69"/>
-      <c r="AY31" s="69"/>
-      <c r="AZ31" s="69"/>
-      <c r="BA31" s="69"/>
-      <c r="BB31" s="69"/>
-      <c r="BC31" s="69"/>
-      <c r="BD31" s="69"/>
-      <c r="BE31" s="69"/>
-      <c r="BF31" s="69"/>
-      <c r="BG31" s="69"/>
-      <c r="BH31" s="69"/>
-      <c r="BI31" s="69"/>
-      <c r="BJ31" s="69"/>
-      <c r="BK31" s="69"/>
-      <c r="BL31" s="69"/>
-      <c r="BM31" s="69"/>
-      <c r="BN31" s="69"/>
-      <c r="BO31" s="69"/>
-      <c r="BP31" s="69"/>
-      <c r="BQ31" s="69"/>
-      <c r="BR31" s="69"/>
-      <c r="BS31" s="69"/>
-      <c r="BT31" s="69"/>
-      <c r="BU31" s="69"/>
-      <c r="BV31" s="69"/>
-      <c r="BW31" s="69"/>
-      <c r="BX31" s="69"/>
-      <c r="BY31" s="69"/>
-      <c r="BZ31" s="69"/>
-      <c r="CA31" s="69"/>
-      <c r="CB31" s="69"/>
-      <c r="CC31" s="69"/>
-      <c r="CD31" s="69"/>
-      <c r="CE31" s="69"/>
-      <c r="CF31" s="69"/>
-      <c r="CG31" s="69"/>
+        <v>1874</v>
+      </c>
+      <c r="F31" s="12"/>
+      <c r="G31" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="H31" s="49" t="s">
+        <v>1875</v>
+      </c>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="12"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="12"/>
+      <c r="P31" s="12"/>
+      <c r="Q31" s="50"/>
+      <c r="R31" s="12"/>
+      <c r="S31" s="12"/>
+      <c r="T31" s="12"/>
+      <c r="U31" s="12"/>
+      <c r="V31" s="12"/>
+      <c r="W31" s="12"/>
+      <c r="X31" s="12"/>
+      <c r="Y31" s="12"/>
+      <c r="Z31" s="12"/>
+      <c r="AA31" s="12"/>
+      <c r="AB31" s="12"/>
+      <c r="AC31" s="12"/>
+      <c r="AD31" s="12"/>
+      <c r="AE31" s="12"/>
+      <c r="AF31" s="12"/>
+      <c r="AG31" s="12"/>
+      <c r="AH31" s="12"/>
+      <c r="AI31" s="12"/>
+      <c r="AJ31" s="12"/>
+      <c r="AK31" s="12"/>
+      <c r="AL31" s="12"/>
+      <c r="AM31" s="12"/>
+      <c r="AN31" s="12"/>
+      <c r="AO31" s="12"/>
+      <c r="AP31" s="12"/>
+      <c r="AQ31" s="12"/>
+      <c r="AR31" s="12"/>
+      <c r="AS31" s="12"/>
+      <c r="AT31" s="12"/>
+      <c r="AU31" s="12"/>
+      <c r="AV31" s="12"/>
+      <c r="AW31" s="12"/>
+      <c r="AX31" s="12"/>
+      <c r="AY31" s="12"/>
+      <c r="AZ31" s="12"/>
+      <c r="BA31" s="12"/>
+      <c r="BB31" s="12"/>
+      <c r="BC31" s="12"/>
+      <c r="BD31" s="12"/>
+      <c r="BE31" s="12"/>
+      <c r="BF31" s="12"/>
+      <c r="BG31" s="12"/>
+      <c r="BH31" s="12"/>
+      <c r="BI31" s="12"/>
+      <c r="BJ31" s="12"/>
+      <c r="BK31" s="12"/>
+      <c r="BL31" s="12"/>
+      <c r="BM31" s="12"/>
+      <c r="BN31" s="12"/>
+      <c r="BO31" s="12"/>
+      <c r="BP31" s="12"/>
+      <c r="BQ31" s="12"/>
+      <c r="BR31" s="12"/>
+      <c r="BS31" s="12"/>
+      <c r="BT31" s="12"/>
+      <c r="BU31" s="12"/>
+      <c r="BV31" s="12"/>
+      <c r="BW31" s="12"/>
+      <c r="BX31" s="12"/>
+      <c r="BY31" s="12"/>
+      <c r="BZ31" s="12"/>
+      <c r="CA31" s="12"/>
+      <c r="CB31" s="12"/>
+      <c r="CC31" s="12"/>
+      <c r="CD31" s="12"/>
+      <c r="CE31" s="12"/>
+      <c r="CF31" s="12"/>
+      <c r="CG31" s="12"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:CG31" xr:uid="{9585C0FF-65C5-4BD8-9936-5C9A63F7E604}">
@@ -68526,22 +68492,22 @@
     </sortState>
   </autoFilter>
   <mergeCells count="16">
-    <mergeCell ref="AO1:AR1"/>
-    <mergeCell ref="AS1:AV1"/>
-    <mergeCell ref="AW1:AZ1"/>
-    <mergeCell ref="BA1:BE1"/>
-    <mergeCell ref="BF1:BI1"/>
-    <mergeCell ref="S1:V1"/>
-    <mergeCell ref="W1:AA1"/>
-    <mergeCell ref="AB1:AE1"/>
-    <mergeCell ref="AF1:AI1"/>
-    <mergeCell ref="AJ1:AN1"/>
     <mergeCell ref="CF1:CG1"/>
     <mergeCell ref="BJ1:BN1"/>
     <mergeCell ref="BO1:BR1"/>
     <mergeCell ref="BS1:BV1"/>
     <mergeCell ref="BW1:BZ1"/>
     <mergeCell ref="CB1:CE1"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="W1:AA1"/>
+    <mergeCell ref="AB1:AE1"/>
+    <mergeCell ref="AF1:AI1"/>
+    <mergeCell ref="AJ1:AN1"/>
+    <mergeCell ref="AO1:AR1"/>
+    <mergeCell ref="AS1:AV1"/>
+    <mergeCell ref="AW1:AZ1"/>
+    <mergeCell ref="BA1:BE1"/>
+    <mergeCell ref="BF1:BI1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
actualización de lista de reporte por migrar (cargas)
</commit_message>
<xml_diff>
--- a/00-Documentacion/Listado de reportes totales-TI.xlsx
+++ b/00-Documentacion/Listado de reportes totales-TI.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\source\repos\migracion_spooler\00-Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF6ED99-7045-4DD4-ABAF-A89CE282C454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12124FDA-6528-4EB8-AE7B-6DA3FEC91E64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{1498AA1A-1ACC-4329-A050-ACA05131B658}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13260" uniqueCount="1876">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13288" uniqueCount="1882">
   <si>
     <t xml:space="preserve">Reporte </t>
   </si>
@@ -5682,6 +5682,24 @@
   </si>
   <si>
     <t>excel, correo</t>
+  </si>
+  <si>
+    <t>ZDocumentacion</t>
+  </si>
+  <si>
+    <t>Sin Factura – Excel</t>
+  </si>
+  <si>
+    <t>Con Factura</t>
+  </si>
+  <si>
+    <t>Con Documento Fuente</t>
+  </si>
+  <si>
+    <t>Carga de Facturas a Documento Fuente</t>
+  </si>
+  <si>
+    <t>Documentacion</t>
   </si>
 </sst>
 </file>
@@ -5995,7 +6013,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6133,6 +6151,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -64741,10 +64765,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9585C0FF-65C5-4BD8-9936-5C9A63F7E604}">
-  <dimension ref="A1:CG31"/>
+  <dimension ref="A1:CG35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -68389,23 +68413,23 @@
         <v>1777</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>1873</v>
+        <v>1876</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>1871</v>
-      </c>
-      <c r="D31" s="19" t="s">
-        <v>1872</v>
-      </c>
-      <c r="E31" s="29" t="s">
-        <v>1874</v>
+        <v>1881</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>1877</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>1838</v>
       </c>
       <c r="F31" s="12"/>
-      <c r="G31" s="49" t="s">
-        <v>26</v>
-      </c>
-      <c r="H31" s="49" t="s">
-        <v>1875</v>
+      <c r="G31" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H31" s="10" t="s">
+        <v>1075</v>
       </c>
       <c r="I31" s="12"/>
       <c r="J31" s="12"/>
@@ -68415,7 +68439,7 @@
       <c r="N31" s="12"/>
       <c r="O31" s="12"/>
       <c r="P31" s="12"/>
-      <c r="Q31" s="50"/>
+      <c r="Q31" s="12"/>
       <c r="R31" s="12"/>
       <c r="S31" s="12"/>
       <c r="T31" s="12"/>
@@ -68485,9 +68509,413 @@
       <c r="CF31" s="12"/>
       <c r="CG31" s="12"/>
     </row>
+    <row r="32" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>1777</v>
+      </c>
+      <c r="B32" s="66" t="s">
+        <v>1876</v>
+      </c>
+      <c r="C32" s="66" t="s">
+        <v>1881</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>1878</v>
+      </c>
+      <c r="E32" s="17" t="s">
+        <v>1838</v>
+      </c>
+      <c r="F32" s="12"/>
+      <c r="G32" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>1075</v>
+      </c>
+      <c r="I32" s="12"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="12"/>
+      <c r="M32" s="12"/>
+      <c r="N32" s="12"/>
+      <c r="O32" s="12"/>
+      <c r="P32" s="12"/>
+      <c r="Q32" s="12"/>
+      <c r="R32" s="12"/>
+      <c r="S32" s="12"/>
+      <c r="T32" s="12"/>
+      <c r="U32" s="12"/>
+      <c r="V32" s="12"/>
+      <c r="W32" s="12"/>
+      <c r="X32" s="12"/>
+      <c r="Y32" s="12"/>
+      <c r="Z32" s="12"/>
+      <c r="AA32" s="12"/>
+      <c r="AB32" s="12"/>
+      <c r="AC32" s="12"/>
+      <c r="AD32" s="12"/>
+      <c r="AE32" s="12"/>
+      <c r="AF32" s="12"/>
+      <c r="AG32" s="12"/>
+      <c r="AH32" s="12"/>
+      <c r="AI32" s="12"/>
+      <c r="AJ32" s="12"/>
+      <c r="AK32" s="12"/>
+      <c r="AL32" s="12"/>
+      <c r="AM32" s="12"/>
+      <c r="AN32" s="12"/>
+      <c r="AO32" s="12"/>
+      <c r="AP32" s="12"/>
+      <c r="AQ32" s="12"/>
+      <c r="AR32" s="12"/>
+      <c r="AS32" s="12"/>
+      <c r="AT32" s="12"/>
+      <c r="AU32" s="12"/>
+      <c r="AV32" s="12"/>
+      <c r="AW32" s="12"/>
+      <c r="AX32" s="12"/>
+      <c r="AY32" s="12"/>
+      <c r="AZ32" s="12"/>
+      <c r="BA32" s="12"/>
+      <c r="BB32" s="12"/>
+      <c r="BC32" s="12"/>
+      <c r="BD32" s="12"/>
+      <c r="BE32" s="12"/>
+      <c r="BF32" s="12"/>
+      <c r="BG32" s="12"/>
+      <c r="BH32" s="12"/>
+      <c r="BI32" s="12"/>
+      <c r="BJ32" s="12"/>
+      <c r="BK32" s="12"/>
+      <c r="BL32" s="12"/>
+      <c r="BM32" s="12"/>
+      <c r="BN32" s="12"/>
+      <c r="BO32" s="12"/>
+      <c r="BP32" s="12"/>
+      <c r="BQ32" s="12"/>
+      <c r="BR32" s="12"/>
+      <c r="BS32" s="12"/>
+      <c r="BT32" s="12"/>
+      <c r="BU32" s="12"/>
+      <c r="BV32" s="12"/>
+      <c r="BW32" s="12"/>
+      <c r="BX32" s="12"/>
+      <c r="BY32" s="12"/>
+      <c r="BZ32" s="12"/>
+      <c r="CA32" s="12"/>
+      <c r="CB32" s="12"/>
+      <c r="CC32" s="12"/>
+      <c r="CD32" s="12"/>
+      <c r="CE32" s="12"/>
+      <c r="CF32" s="12"/>
+      <c r="CG32" s="12"/>
+    </row>
+    <row r="33" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
+        <v>1777</v>
+      </c>
+      <c r="B33" s="66" t="s">
+        <v>1876</v>
+      </c>
+      <c r="C33" s="66" t="s">
+        <v>1881</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>1879</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>1838</v>
+      </c>
+      <c r="F33" s="12"/>
+      <c r="G33" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>1075</v>
+      </c>
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="12"/>
+      <c r="M33" s="12"/>
+      <c r="N33" s="12"/>
+      <c r="O33" s="12"/>
+      <c r="P33" s="12"/>
+      <c r="Q33" s="12"/>
+      <c r="R33" s="12"/>
+      <c r="S33" s="12"/>
+      <c r="T33" s="12"/>
+      <c r="U33" s="12"/>
+      <c r="V33" s="12"/>
+      <c r="W33" s="12"/>
+      <c r="X33" s="12"/>
+      <c r="Y33" s="12"/>
+      <c r="Z33" s="12"/>
+      <c r="AA33" s="12"/>
+      <c r="AB33" s="12"/>
+      <c r="AC33" s="12"/>
+      <c r="AD33" s="12"/>
+      <c r="AE33" s="12"/>
+      <c r="AF33" s="12"/>
+      <c r="AG33" s="12"/>
+      <c r="AH33" s="12"/>
+      <c r="AI33" s="12"/>
+      <c r="AJ33" s="12"/>
+      <c r="AK33" s="12"/>
+      <c r="AL33" s="12"/>
+      <c r="AM33" s="12"/>
+      <c r="AN33" s="12"/>
+      <c r="AO33" s="12"/>
+      <c r="AP33" s="12"/>
+      <c r="AQ33" s="12"/>
+      <c r="AR33" s="12"/>
+      <c r="AS33" s="12"/>
+      <c r="AT33" s="12"/>
+      <c r="AU33" s="12"/>
+      <c r="AV33" s="12"/>
+      <c r="AW33" s="12"/>
+      <c r="AX33" s="12"/>
+      <c r="AY33" s="12"/>
+      <c r="AZ33" s="12"/>
+      <c r="BA33" s="12"/>
+      <c r="BB33" s="12"/>
+      <c r="BC33" s="12"/>
+      <c r="BD33" s="12"/>
+      <c r="BE33" s="12"/>
+      <c r="BF33" s="12"/>
+      <c r="BG33" s="12"/>
+      <c r="BH33" s="12"/>
+      <c r="BI33" s="12"/>
+      <c r="BJ33" s="12"/>
+      <c r="BK33" s="12"/>
+      <c r="BL33" s="12"/>
+      <c r="BM33" s="12"/>
+      <c r="BN33" s="12"/>
+      <c r="BO33" s="12"/>
+      <c r="BP33" s="12"/>
+      <c r="BQ33" s="12"/>
+      <c r="BR33" s="12"/>
+      <c r="BS33" s="12"/>
+      <c r="BT33" s="12"/>
+      <c r="BU33" s="12"/>
+      <c r="BV33" s="12"/>
+      <c r="BW33" s="12"/>
+      <c r="BX33" s="12"/>
+      <c r="BY33" s="12"/>
+      <c r="BZ33" s="12"/>
+      <c r="CA33" s="12"/>
+      <c r="CB33" s="12"/>
+      <c r="CC33" s="12"/>
+      <c r="CD33" s="12"/>
+      <c r="CE33" s="12"/>
+      <c r="CF33" s="12"/>
+      <c r="CG33" s="12"/>
+    </row>
+    <row r="34" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="14" t="s">
+        <v>1777</v>
+      </c>
+      <c r="B34" s="66" t="s">
+        <v>1876</v>
+      </c>
+      <c r="C34" s="66" t="s">
+        <v>1881</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>1880</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>1838</v>
+      </c>
+      <c r="F34" s="12"/>
+      <c r="G34" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>1075</v>
+      </c>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="12"/>
+      <c r="N34" s="12"/>
+      <c r="O34" s="12"/>
+      <c r="P34" s="12"/>
+      <c r="Q34" s="12"/>
+      <c r="R34" s="12"/>
+      <c r="S34" s="12"/>
+      <c r="T34" s="12"/>
+      <c r="U34" s="12"/>
+      <c r="V34" s="12"/>
+      <c r="W34" s="12"/>
+      <c r="X34" s="12"/>
+      <c r="Y34" s="12"/>
+      <c r="Z34" s="12"/>
+      <c r="AA34" s="12"/>
+      <c r="AB34" s="12"/>
+      <c r="AC34" s="12"/>
+      <c r="AD34" s="12"/>
+      <c r="AE34" s="12"/>
+      <c r="AF34" s="12"/>
+      <c r="AG34" s="12"/>
+      <c r="AH34" s="12"/>
+      <c r="AI34" s="12"/>
+      <c r="AJ34" s="12"/>
+      <c r="AK34" s="12"/>
+      <c r="AL34" s="12"/>
+      <c r="AM34" s="12"/>
+      <c r="AN34" s="12"/>
+      <c r="AO34" s="12"/>
+      <c r="AP34" s="12"/>
+      <c r="AQ34" s="12"/>
+      <c r="AR34" s="12"/>
+      <c r="AS34" s="12"/>
+      <c r="AT34" s="12"/>
+      <c r="AU34" s="12"/>
+      <c r="AV34" s="12"/>
+      <c r="AW34" s="12"/>
+      <c r="AX34" s="12"/>
+      <c r="AY34" s="12"/>
+      <c r="AZ34" s="12"/>
+      <c r="BA34" s="12"/>
+      <c r="BB34" s="12"/>
+      <c r="BC34" s="12"/>
+      <c r="BD34" s="12"/>
+      <c r="BE34" s="12"/>
+      <c r="BF34" s="12"/>
+      <c r="BG34" s="12"/>
+      <c r="BH34" s="12"/>
+      <c r="BI34" s="12"/>
+      <c r="BJ34" s="12"/>
+      <c r="BK34" s="12"/>
+      <c r="BL34" s="12"/>
+      <c r="BM34" s="12"/>
+      <c r="BN34" s="12"/>
+      <c r="BO34" s="12"/>
+      <c r="BP34" s="12"/>
+      <c r="BQ34" s="12"/>
+      <c r="BR34" s="12"/>
+      <c r="BS34" s="12"/>
+      <c r="BT34" s="12"/>
+      <c r="BU34" s="12"/>
+      <c r="BV34" s="12"/>
+      <c r="BW34" s="12"/>
+      <c r="BX34" s="12"/>
+      <c r="BY34" s="12"/>
+      <c r="BZ34" s="12"/>
+      <c r="CA34" s="12"/>
+      <c r="CB34" s="12"/>
+      <c r="CC34" s="12"/>
+      <c r="CD34" s="12"/>
+      <c r="CE34" s="12"/>
+      <c r="CF34" s="12"/>
+      <c r="CG34" s="12"/>
+    </row>
+    <row r="35" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="14" t="s">
+        <v>1777</v>
+      </c>
+      <c r="B35" s="67" t="s">
+        <v>1873</v>
+      </c>
+      <c r="C35" s="67" t="s">
+        <v>1871</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>1872</v>
+      </c>
+      <c r="E35" s="29" t="s">
+        <v>1874</v>
+      </c>
+      <c r="F35" s="12"/>
+      <c r="G35" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>1875</v>
+      </c>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="12"/>
+      <c r="M35" s="12"/>
+      <c r="N35" s="12"/>
+      <c r="O35" s="12"/>
+      <c r="P35" s="12"/>
+      <c r="Q35" s="12"/>
+      <c r="R35" s="12"/>
+      <c r="S35" s="12"/>
+      <c r="T35" s="12"/>
+      <c r="U35" s="12"/>
+      <c r="V35" s="12"/>
+      <c r="W35" s="12"/>
+      <c r="X35" s="12"/>
+      <c r="Y35" s="12"/>
+      <c r="Z35" s="12"/>
+      <c r="AA35" s="12"/>
+      <c r="AB35" s="12"/>
+      <c r="AC35" s="12"/>
+      <c r="AD35" s="12"/>
+      <c r="AE35" s="12"/>
+      <c r="AF35" s="12"/>
+      <c r="AG35" s="12"/>
+      <c r="AH35" s="12"/>
+      <c r="AI35" s="12"/>
+      <c r="AJ35" s="12"/>
+      <c r="AK35" s="12"/>
+      <c r="AL35" s="12"/>
+      <c r="AM35" s="12"/>
+      <c r="AN35" s="12"/>
+      <c r="AO35" s="12"/>
+      <c r="AP35" s="12"/>
+      <c r="AQ35" s="12"/>
+      <c r="AR35" s="12"/>
+      <c r="AS35" s="12"/>
+      <c r="AT35" s="12"/>
+      <c r="AU35" s="12"/>
+      <c r="AV35" s="12"/>
+      <c r="AW35" s="12"/>
+      <c r="AX35" s="12"/>
+      <c r="AY35" s="12"/>
+      <c r="AZ35" s="12"/>
+      <c r="BA35" s="12"/>
+      <c r="BB35" s="12"/>
+      <c r="BC35" s="12"/>
+      <c r="BD35" s="12"/>
+      <c r="BE35" s="12"/>
+      <c r="BF35" s="12"/>
+      <c r="BG35" s="12"/>
+      <c r="BH35" s="12"/>
+      <c r="BI35" s="12"/>
+      <c r="BJ35" s="12"/>
+      <c r="BK35" s="12"/>
+      <c r="BL35" s="12"/>
+      <c r="BM35" s="12"/>
+      <c r="BN35" s="12"/>
+      <c r="BO35" s="12"/>
+      <c r="BP35" s="12"/>
+      <c r="BQ35" s="12"/>
+      <c r="BR35" s="12"/>
+      <c r="BS35" s="12"/>
+      <c r="BT35" s="12"/>
+      <c r="BU35" s="12"/>
+      <c r="BV35" s="12"/>
+      <c r="BW35" s="12"/>
+      <c r="BX35" s="12"/>
+      <c r="BY35" s="12"/>
+      <c r="BZ35" s="12"/>
+      <c r="CA35" s="12"/>
+      <c r="CB35" s="12"/>
+      <c r="CC35" s="12"/>
+      <c r="CD35" s="12"/>
+      <c r="CE35" s="12"/>
+      <c r="CF35" s="12"/>
+      <c r="CG35" s="12"/>
+    </row>
   </sheetData>
   <autoFilter ref="A2:CG31" xr:uid="{9585C0FF-65C5-4BD8-9936-5C9A63F7E604}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:CG31">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:CG35">
       <sortCondition ref="B2:B31"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Actualizar plan de trabajo (ajustar fechas)
bosch_pedimento2_xls
Configuración  de cuentas
Generación (archivo, correo )
</commit_message>
<xml_diff>
--- a/00-Documentacion/Listado de reportes totales-TI.xlsx
+++ b/00-Documentacion/Listado de reportes totales-TI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0B2E19-4CAB-446A-B9AB-B3A50F3B2F98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B74622-26D9-4DE7-AB1D-D5686353CF95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{1498AA1A-1ACC-4329-A050-ACA05131B658}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13288" uniqueCount="1881">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13293" uniqueCount="1881">
   <si>
     <t xml:space="preserve">Reporte </t>
   </si>
@@ -5678,9 +5678,6 @@
     <t>ZReportes DG</t>
   </si>
   <si>
-    <t>Semanal en día Domingo</t>
-  </si>
-  <si>
     <t>ZDocumentacion</t>
   </si>
   <si>
@@ -5696,7 +5693,10 @@
     <t>Carga de Facturas a Documento Fuente</t>
   </si>
   <si>
-    <t>Documentacion</t>
+    <t>Restrutura de Esquemas de Objetos</t>
+  </si>
+  <si>
+    <t>Ajustes</t>
   </si>
 </sst>
 </file>
@@ -6010,7 +6010,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6134,9 +6134,6 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6152,6 +6149,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -64759,17 +64773,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9585C0FF-65C5-4BD8-9936-5C9A63F7E604}">
-  <dimension ref="A1:CG35"/>
+  <dimension ref="A1:CH39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" topLeftCell="BH1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="CG11" sqref="CG11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.7109375" hidden="1" customWidth="1"/>
-    <col min="3" max="4" width="50.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.85546875" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="50.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="55.42578125" customWidth="1"/>
     <col min="6" max="6" width="37.7109375" customWidth="1"/>
     <col min="7" max="7" width="28" customWidth="1"/>
@@ -64839,110 +64854,110 @@
     <col min="81" max="82" width="7" bestFit="1" customWidth="1"/>
     <col min="83" max="83" width="8" bestFit="1" customWidth="1"/>
     <col min="84" max="84" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="S1" s="65">
+    <row r="1" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="S1" s="64">
         <v>45536</v>
       </c>
-      <c r="T1" s="66"/>
-      <c r="U1" s="66"/>
-      <c r="V1" s="66"/>
-      <c r="W1" s="65">
+      <c r="T1" s="65"/>
+      <c r="U1" s="65"/>
+      <c r="V1" s="65"/>
+      <c r="W1" s="64">
         <v>45566</v>
       </c>
-      <c r="X1" s="65"/>
-      <c r="Y1" s="65"/>
-      <c r="Z1" s="65"/>
-      <c r="AA1" s="65"/>
-      <c r="AB1" s="62">
+      <c r="X1" s="64"/>
+      <c r="Y1" s="64"/>
+      <c r="Z1" s="64"/>
+      <c r="AA1" s="64"/>
+      <c r="AB1" s="61">
         <v>45597</v>
       </c>
-      <c r="AC1" s="63"/>
-      <c r="AD1" s="63"/>
-      <c r="AE1" s="64"/>
-      <c r="AF1" s="62">
+      <c r="AC1" s="62"/>
+      <c r="AD1" s="62"/>
+      <c r="AE1" s="63"/>
+      <c r="AF1" s="61">
         <v>45627</v>
       </c>
-      <c r="AG1" s="63"/>
-      <c r="AH1" s="63"/>
-      <c r="AI1" s="64"/>
-      <c r="AJ1" s="62">
+      <c r="AG1" s="62"/>
+      <c r="AH1" s="62"/>
+      <c r="AI1" s="63"/>
+      <c r="AJ1" s="61">
         <v>45658</v>
       </c>
-      <c r="AK1" s="63"/>
-      <c r="AL1" s="63"/>
-      <c r="AM1" s="63"/>
-      <c r="AN1" s="64"/>
-      <c r="AO1" s="62">
+      <c r="AK1" s="62"/>
+      <c r="AL1" s="62"/>
+      <c r="AM1" s="62"/>
+      <c r="AN1" s="63"/>
+      <c r="AO1" s="61">
         <v>45689</v>
       </c>
-      <c r="AP1" s="63"/>
-      <c r="AQ1" s="63"/>
-      <c r="AR1" s="64"/>
-      <c r="AS1" s="62">
+      <c r="AP1" s="62"/>
+      <c r="AQ1" s="62"/>
+      <c r="AR1" s="63"/>
+      <c r="AS1" s="61">
         <v>45717</v>
       </c>
-      <c r="AT1" s="63"/>
-      <c r="AU1" s="63"/>
-      <c r="AV1" s="64"/>
-      <c r="AW1" s="62">
+      <c r="AT1" s="62"/>
+      <c r="AU1" s="62"/>
+      <c r="AV1" s="63"/>
+      <c r="AW1" s="61">
         <v>45748</v>
       </c>
-      <c r="AX1" s="63"/>
-      <c r="AY1" s="63"/>
-      <c r="AZ1" s="64"/>
-      <c r="BA1" s="62">
+      <c r="AX1" s="62"/>
+      <c r="AY1" s="62"/>
+      <c r="AZ1" s="63"/>
+      <c r="BA1" s="61">
         <v>45778</v>
       </c>
-      <c r="BB1" s="63"/>
-      <c r="BC1" s="63"/>
-      <c r="BD1" s="63"/>
-      <c r="BE1" s="64"/>
-      <c r="BF1" s="62">
+      <c r="BB1" s="62"/>
+      <c r="BC1" s="62"/>
+      <c r="BD1" s="62"/>
+      <c r="BE1" s="63"/>
+      <c r="BF1" s="61">
         <v>45809</v>
       </c>
-      <c r="BG1" s="63"/>
-      <c r="BH1" s="63"/>
-      <c r="BI1" s="63"/>
-      <c r="BJ1" s="62">
+      <c r="BG1" s="62"/>
+      <c r="BH1" s="62"/>
+      <c r="BI1" s="62"/>
+      <c r="BJ1" s="61">
         <v>45839</v>
       </c>
-      <c r="BK1" s="63"/>
-      <c r="BL1" s="63"/>
-      <c r="BM1" s="63"/>
-      <c r="BN1" s="64"/>
-      <c r="BO1" s="62">
+      <c r="BK1" s="62"/>
+      <c r="BL1" s="62"/>
+      <c r="BM1" s="62"/>
+      <c r="BN1" s="63"/>
+      <c r="BO1" s="61">
         <v>45870</v>
       </c>
-      <c r="BP1" s="63"/>
-      <c r="BQ1" s="63"/>
-      <c r="BR1" s="63"/>
-      <c r="BS1" s="62">
+      <c r="BP1" s="62"/>
+      <c r="BQ1" s="62"/>
+      <c r="BR1" s="62"/>
+      <c r="BS1" s="61">
         <v>45901</v>
       </c>
-      <c r="BT1" s="63"/>
-      <c r="BU1" s="63"/>
-      <c r="BV1" s="63"/>
-      <c r="BW1" s="62">
+      <c r="BT1" s="62"/>
+      <c r="BU1" s="62"/>
+      <c r="BV1" s="62"/>
+      <c r="BW1" s="61">
         <v>45931</v>
       </c>
-      <c r="BX1" s="63"/>
-      <c r="BY1" s="63"/>
-      <c r="BZ1" s="63"/>
-      <c r="CB1" s="62">
+      <c r="BX1" s="62"/>
+      <c r="BY1" s="62"/>
+      <c r="BZ1" s="62"/>
+      <c r="CB1" s="61">
         <v>45962</v>
       </c>
-      <c r="CC1" s="63"/>
-      <c r="CD1" s="63"/>
-      <c r="CE1" s="63"/>
-      <c r="CF1" s="61" t="s">
+      <c r="CC1" s="62"/>
+      <c r="CD1" s="62"/>
+      <c r="CE1" s="62"/>
+      <c r="CF1" s="66" t="s">
         <v>1854</v>
       </c>
-      <c r="CG1" s="61"/>
-    </row>
-    <row r="2" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CG1" s="66"/>
+    </row>
+    <row r="2" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>1780</v>
       </c>
@@ -65199,7 +65214,7 @@
         <v>1866</v>
       </c>
     </row>
-    <row r="3" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>1778</v>
       </c>
@@ -65315,7 +65330,7 @@
       <c r="CF3" s="12"/>
       <c r="CG3" s="12"/>
     </row>
-    <row r="4" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>1778</v>
       </c>
@@ -65433,7 +65448,7 @@
       <c r="CF4" s="12"/>
       <c r="CG4" s="12"/>
     </row>
-    <row r="5" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>1777</v>
       </c>
@@ -65553,7 +65568,7 @@
       <c r="CF5" s="12"/>
       <c r="CG5" s="12"/>
     </row>
-    <row r="6" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>1777</v>
       </c>
@@ -65677,7 +65692,7 @@
       <c r="CF6" s="12"/>
       <c r="CG6" s="12"/>
     </row>
-    <row r="7" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>1778</v>
       </c>
@@ -65799,7 +65814,7 @@
       <c r="CF7" s="12"/>
       <c r="CG7" s="12"/>
     </row>
-    <row r="8" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>1777</v>
       </c>
@@ -65923,7 +65938,7 @@
       <c r="CF8" s="12"/>
       <c r="CG8" s="12"/>
     </row>
-    <row r="9" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>1777</v>
       </c>
@@ -65979,7 +65994,7 @@
       <c r="R9" s="56">
         <v>45546</v>
       </c>
-      <c r="S9" s="53"/>
+      <c r="S9" s="12"/>
       <c r="T9" s="12"/>
       <c r="U9" s="12"/>
       <c r="V9" s="12"/>
@@ -66047,7 +66062,7 @@
       <c r="CF9" s="12"/>
       <c r="CG9" s="12"/>
     </row>
-    <row r="10" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>1777</v>
       </c>
@@ -66090,10 +66105,10 @@
       <c r="O10" s="12"/>
       <c r="P10" s="12"/>
       <c r="Q10" s="50">
-        <v>45653</v>
+        <v>45659</v>
       </c>
       <c r="R10" s="56">
-        <v>45674</v>
+        <v>45680</v>
       </c>
       <c r="S10" s="53"/>
       <c r="T10" s="12"/>
@@ -66112,10 +66127,10 @@
       <c r="AG10" s="12"/>
       <c r="AH10" s="12"/>
       <c r="AI10" s="12"/>
-      <c r="AJ10" s="48"/>
+      <c r="AJ10" s="12"/>
       <c r="AK10" s="48"/>
       <c r="AL10" s="48"/>
-      <c r="AM10" s="12"/>
+      <c r="AM10" s="48"/>
       <c r="AN10" s="12"/>
       <c r="AO10" s="12"/>
       <c r="AP10" s="12"/>
@@ -66163,23 +66178,21 @@
       <c r="CF10" s="12"/>
       <c r="CG10" s="12"/>
     </row>
-    <row r="11" spans="1:85" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>1778</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>1869</v>
       </c>
-      <c r="C11" s="15" t="s">
-        <v>1869</v>
-      </c>
+      <c r="C11" s="12"/>
       <c r="D11" s="19" t="s">
         <v>1760</v>
       </c>
       <c r="E11" s="19" t="s">
         <v>1761</v>
       </c>
-      <c r="F11" s="25" t="s">
+      <c r="F11" s="71" t="s">
         <v>1762</v>
       </c>
       <c r="G11" s="12" t="s">
@@ -66205,10 +66218,10 @@
       <c r="O11" s="12"/>
       <c r="P11" s="12"/>
       <c r="Q11" s="50">
-        <v>45838</v>
+        <v>45844</v>
       </c>
       <c r="R11" s="56">
-        <v>45860</v>
+        <v>45866</v>
       </c>
       <c r="S11" s="53"/>
       <c r="T11" s="12"/>
@@ -66217,10 +66230,10 @@
       <c r="W11" s="12"/>
       <c r="X11" s="12"/>
       <c r="Y11" s="12"/>
-      <c r="Z11" s="12" t="s">
+      <c r="Z11" s="12"/>
+      <c r="AA11" s="12" t="s">
         <v>1835</v>
       </c>
-      <c r="AA11" s="12"/>
       <c r="AB11" s="12"/>
       <c r="AC11" s="12"/>
       <c r="AD11" s="12"/>
@@ -66255,11 +66268,11 @@
       <c r="BG11" s="12"/>
       <c r="BH11" s="12"/>
       <c r="BI11" s="12"/>
-      <c r="BJ11" s="48"/>
+      <c r="BJ11" s="12"/>
       <c r="BK11" s="48"/>
       <c r="BL11" s="48"/>
       <c r="BM11" s="48"/>
-      <c r="BN11" s="12"/>
+      <c r="BN11" s="48"/>
       <c r="BO11" s="12"/>
       <c r="BP11" s="12"/>
       <c r="BQ11" s="12"/>
@@ -66280,7 +66293,7 @@
       <c r="CF11" s="12"/>
       <c r="CG11" s="12"/>
     </row>
-    <row r="12" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>1777</v>
       </c>
@@ -66322,15 +66335,16 @@
       <c r="O12" s="12"/>
       <c r="P12" s="12"/>
       <c r="Q12" s="50">
-        <v>45923</v>
+        <v>45929</v>
       </c>
       <c r="R12" s="56">
-        <v>45947</v>
+        <v>45953</v>
       </c>
       <c r="S12" s="53"/>
       <c r="T12" s="12"/>
       <c r="U12" s="12"/>
       <c r="V12" s="12"/>
+      <c r="W12" s="12"/>
       <c r="X12" s="12"/>
       <c r="Y12" s="12"/>
       <c r="Z12" s="12"/>
@@ -66381,11 +66395,11 @@
       <c r="BS12" s="12"/>
       <c r="BT12" s="12"/>
       <c r="BU12" s="12"/>
-      <c r="BV12" s="48"/>
+      <c r="BV12" s="12"/>
       <c r="BW12" s="48"/>
       <c r="BX12" s="48"/>
       <c r="BY12" s="48"/>
-      <c r="BZ12" s="12"/>
+      <c r="BZ12" s="48"/>
       <c r="CA12" s="12"/>
       <c r="CB12" s="12"/>
       <c r="CC12" s="12"/>
@@ -66394,56 +66408,59 @@
       <c r="CF12" s="12"/>
       <c r="CG12" s="12"/>
     </row>
-    <row r="13" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
-        <v>1778</v>
+    <row r="13" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>1777</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>1757</v>
-      </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="19" t="s">
-        <v>1622</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>1763</v>
-      </c>
-      <c r="F13" s="20" t="s">
-        <v>1768</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="10" t="s">
-        <v>1706</v>
+        <v>1756</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>1756</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>1756</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>1779</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>1745</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>1682</v>
       </c>
       <c r="I13" s="12">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="J13" s="12">
-        <v>76</v>
+        <v>9</v>
       </c>
       <c r="K13" s="12">
-        <v>8</v>
+        <f>4+1</f>
+        <v>5</v>
       </c>
       <c r="L13" s="54"/>
       <c r="M13" s="12"/>
       <c r="N13" s="12">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="O13" s="12"/>
       <c r="P13" s="12"/>
       <c r="Q13" s="50">
-        <v>45950</v>
+        <v>45681</v>
       </c>
       <c r="R13" s="56">
-        <v>45973</v>
+        <v>45702</v>
       </c>
       <c r="S13" s="53"/>
       <c r="T13" s="12"/>
       <c r="U13" s="12"/>
       <c r="V13" s="12"/>
-      <c r="W13" s="12"/>
+      <c r="W13" s="68"/>
       <c r="X13" s="12"/>
       <c r="Y13" s="12"/>
       <c r="Z13" s="12"/>
@@ -66460,9 +66477,9 @@
       <c r="AK13" s="12"/>
       <c r="AL13" s="12"/>
       <c r="AM13" s="12"/>
-      <c r="AN13" s="12"/>
-      <c r="AO13" s="12"/>
-      <c r="AP13" s="12"/>
+      <c r="AN13" s="48"/>
+      <c r="AO13" s="48"/>
+      <c r="AP13" s="48"/>
       <c r="AQ13" s="12"/>
       <c r="AR13" s="12"/>
       <c r="AS13" s="12"/>
@@ -66498,49 +66515,48 @@
       <c r="BW13" s="12"/>
       <c r="BX13" s="12"/>
       <c r="BY13" s="12"/>
-      <c r="BZ13" s="48"/>
-      <c r="CA13" s="48"/>
-      <c r="CB13" s="48"/>
-      <c r="CC13" s="48"/>
+      <c r="BZ13" s="12"/>
+      <c r="CA13" s="12"/>
+      <c r="CB13" s="12"/>
+      <c r="CC13" s="12"/>
       <c r="CD13" s="12"/>
       <c r="CE13" s="12"/>
-      <c r="CF13" s="46"/>
-      <c r="CG13" s="46"/>
-    </row>
-    <row r="14" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
-        <v>1777</v>
+      <c r="CF13" s="12"/>
+      <c r="CG13" s="12"/>
+      <c r="CH13" s="12"/>
+    </row>
+    <row r="14" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>1778</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>1756</v>
       </c>
-      <c r="C14" s="15" t="s">
-        <v>1756</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>1756</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>1779</v>
-      </c>
-      <c r="F14" s="24" t="s">
-        <v>1745</v>
+      <c r="C14" s="12"/>
+      <c r="D14" s="45" t="s">
+        <v>1767</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>1763</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>1764</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="H14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="10" t="s">
         <v>1682</v>
       </c>
       <c r="I14" s="12">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J14" s="12">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="K14" s="12">
-        <f>4+1</f>
-        <v>5</v>
+        <f>6+7</f>
+        <v>13</v>
       </c>
       <c r="L14" s="54"/>
       <c r="M14" s="12"/>
@@ -66550,10 +66566,10 @@
       <c r="O14" s="12"/>
       <c r="P14" s="12"/>
       <c r="Q14" s="50">
-        <v>45677</v>
+        <v>45705</v>
       </c>
       <c r="R14" s="56">
-        <v>45698</v>
+        <v>45725</v>
       </c>
       <c r="S14" s="53"/>
       <c r="T14" s="12"/>
@@ -66575,13 +66591,13 @@
       <c r="AJ14" s="12"/>
       <c r="AK14" s="12"/>
       <c r="AL14" s="12"/>
-      <c r="AM14" s="48"/>
-      <c r="AN14" s="48"/>
-      <c r="AO14" s="48"/>
+      <c r="AM14" s="12"/>
+      <c r="AN14" s="12"/>
+      <c r="AO14" s="12"/>
       <c r="AP14" s="12"/>
-      <c r="AQ14" s="12"/>
-      <c r="AR14" s="12"/>
-      <c r="AS14" s="12"/>
+      <c r="AQ14" s="48"/>
+      <c r="AR14" s="48"/>
+      <c r="AS14" s="48"/>
       <c r="AT14" s="12"/>
       <c r="AU14" s="12"/>
       <c r="AV14" s="12"/>
@@ -66622,8 +66638,9 @@
       <c r="CE14" s="12"/>
       <c r="CF14" s="12"/>
       <c r="CG14" s="12"/>
-    </row>
-    <row r="15" spans="1:85" x14ac:dyDescent="0.25">
+      <c r="CH14" s="12"/>
+    </row>
+    <row r="15" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>1778</v>
       </c>
@@ -66631,8 +66648,8 @@
         <v>1756</v>
       </c>
       <c r="C15" s="12"/>
-      <c r="D15" s="45" t="s">
-        <v>1767</v>
+      <c r="D15" s="19" t="s">
+        <v>1643</v>
       </c>
       <c r="E15" s="21" t="s">
         <v>1763</v>
@@ -66641,20 +66658,20 @@
         <v>1764</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
       <c r="I15" s="12">
+        <v>16</v>
+      </c>
+      <c r="J15" s="12">
+        <v>61</v>
+      </c>
+      <c r="K15" s="12">
+        <f>9+2</f>
         <v>11</v>
-      </c>
-      <c r="J15" s="12">
-        <v>13</v>
-      </c>
-      <c r="K15" s="12">
-        <f>6+7</f>
-        <v>13</v>
       </c>
       <c r="L15" s="54"/>
       <c r="M15" s="12"/>
@@ -66664,10 +66681,10 @@
       <c r="O15" s="12"/>
       <c r="P15" s="12"/>
       <c r="Q15" s="50">
-        <v>45699</v>
+        <v>45820</v>
       </c>
       <c r="R15" s="56">
-        <v>45719</v>
+        <v>45841</v>
       </c>
       <c r="S15" s="53"/>
       <c r="T15" s="12"/>
@@ -66692,9 +66709,9 @@
       <c r="AM15" s="12"/>
       <c r="AN15" s="12"/>
       <c r="AO15" s="12"/>
-      <c r="AP15" s="48"/>
-      <c r="AQ15" s="48"/>
-      <c r="AR15" s="48"/>
+      <c r="AP15" s="12"/>
+      <c r="AQ15" s="12"/>
+      <c r="AR15" s="12"/>
       <c r="AS15" s="12"/>
       <c r="AT15" s="12"/>
       <c r="AU15" s="12"/>
@@ -66710,9 +66727,9 @@
       <c r="BE15" s="12"/>
       <c r="BF15" s="12"/>
       <c r="BG15" s="12"/>
-      <c r="BH15" s="12"/>
-      <c r="BI15" s="12"/>
-      <c r="BJ15" s="12"/>
+      <c r="BH15" s="48"/>
+      <c r="BI15" s="48"/>
+      <c r="BJ15" s="48"/>
       <c r="BK15" s="12"/>
       <c r="BL15" s="12"/>
       <c r="BM15" s="12"/>
@@ -66736,57 +66753,52 @@
       <c r="CE15" s="12"/>
       <c r="CF15" s="12"/>
       <c r="CG15" s="12"/>
-    </row>
-    <row r="16" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
-        <v>1777</v>
+      <c r="CH15" s="12"/>
+    </row>
+    <row r="16" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>1778</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>1739</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>1739</v>
-      </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="17" t="s">
-        <v>1784</v>
-      </c>
-      <c r="F16" s="22" t="s">
-        <v>1745</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>1218</v>
-      </c>
-      <c r="H16" s="12" t="s">
-        <v>1716</v>
+        <v>1756</v>
+      </c>
+      <c r="C16" s="12"/>
+      <c r="D16" s="19" t="s">
+        <v>1622</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>1763</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>1768</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>1706</v>
       </c>
       <c r="I16" s="12">
+        <v>21</v>
+      </c>
+      <c r="J16" s="12">
+        <v>76</v>
+      </c>
+      <c r="K16" s="12">
         <v>8</v>
       </c>
-      <c r="J16" s="12">
-        <v>10</v>
-      </c>
-      <c r="K16" s="12">
-        <v>3</v>
-      </c>
-      <c r="L16" s="54" t="s">
-        <v>1791</v>
-      </c>
+      <c r="L16" s="54"/>
       <c r="M16" s="12"/>
       <c r="N16" s="12">
-        <v>6</v>
-      </c>
-      <c r="O16" s="12" t="s">
-        <v>1864</v>
-      </c>
-      <c r="P16" s="12" t="s">
-        <v>1865</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
       <c r="Q16" s="50">
-        <v>45547</v>
+        <v>45956</v>
       </c>
       <c r="R16" s="56">
-        <v>45558</v>
+        <v>45979</v>
       </c>
       <c r="S16" s="53"/>
       <c r="T16" s="12"/>
@@ -66795,6 +66807,7 @@
       <c r="W16" s="12"/>
       <c r="X16" s="12"/>
       <c r="Y16" s="12"/>
+      <c r="Z16" s="12"/>
       <c r="AA16" s="12"/>
       <c r="AB16" s="12"/>
       <c r="AC16" s="12"/>
@@ -66847,25 +66860,34 @@
       <c r="BX16" s="12"/>
       <c r="BY16" s="12"/>
       <c r="BZ16" s="12"/>
-      <c r="CA16" s="12"/>
-      <c r="CB16" s="12"/>
-      <c r="CC16" s="12"/>
-      <c r="CD16" s="12"/>
+      <c r="CA16" s="48"/>
+      <c r="CB16" s="48"/>
+      <c r="CC16" s="48"/>
+      <c r="CD16" s="48"/>
       <c r="CE16" s="12"/>
       <c r="CF16" s="12"/>
-      <c r="CG16" s="12"/>
-    </row>
-    <row r="17" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
+      <c r="CG16" s="46"/>
+      <c r="CH16" s="12"/>
+    </row>
+    <row r="17" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>1777</v>
+      </c>
       <c r="B17" s="15" t="s">
         <v>1739</v>
       </c>
-      <c r="C17" s="15"/>
+      <c r="C17" s="15" t="s">
+        <v>1739</v>
+      </c>
       <c r="D17" s="16"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="22"/>
+      <c r="E17" s="17" t="s">
+        <v>1784</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>1745</v>
+      </c>
       <c r="G17" s="12" t="s">
-        <v>1868</v>
+        <v>1218</v>
       </c>
       <c r="H17" s="12" t="s">
         <v>1716</v>
@@ -66873,9 +66895,15 @@
       <c r="I17" s="12">
         <v>8</v>
       </c>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="54"/>
+      <c r="J17" s="12">
+        <v>10</v>
+      </c>
+      <c r="K17" s="12">
+        <v>3</v>
+      </c>
+      <c r="L17" s="54" t="s">
+        <v>1791</v>
+      </c>
       <c r="M17" s="12"/>
       <c r="N17" s="12">
         <v>6</v>
@@ -66884,23 +66912,23 @@
         <v>1864</v>
       </c>
       <c r="P17" s="12" t="s">
-        <v>1859</v>
+        <v>1865</v>
       </c>
       <c r="Q17" s="50">
-        <v>45559</v>
+        <v>45547</v>
       </c>
       <c r="R17" s="56">
-        <v>45573</v>
+        <v>45558</v>
       </c>
       <c r="S17" s="53"/>
       <c r="T17" s="12"/>
       <c r="U17" s="12"/>
-      <c r="V17" s="59"/>
-      <c r="W17" s="59"/>
-      <c r="X17" s="59"/>
+      <c r="V17" s="12"/>
+      <c r="W17" s="12"/>
+      <c r="X17" s="12"/>
       <c r="Y17" s="12"/>
       <c r="Z17" s="12"/>
-      <c r="AA17" s="12"/>
+      <c r="AA17" s="68"/>
       <c r="AB17" s="12"/>
       <c r="AC17" s="12"/>
       <c r="AD17" s="12"/>
@@ -66959,28 +66987,19 @@
       <c r="CE17" s="12"/>
       <c r="CF17" s="12"/>
       <c r="CG17" s="12"/>
-    </row>
-    <row r="18" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
-        <v>1777</v>
-      </c>
+      <c r="CH17" s="12"/>
+    </row>
+    <row r="18" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
       <c r="B18" s="15" t="s">
         <v>1739</v>
       </c>
-      <c r="C18" s="15" t="s">
-        <v>1739</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>1746</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>1784</v>
-      </c>
-      <c r="F18" s="22" t="s">
-        <v>1745</v>
-      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="12"/>
       <c r="G18" s="12" t="s">
-        <v>187</v>
+        <v>1868</v>
       </c>
       <c r="H18" s="12" t="s">
         <v>1716</v>
@@ -66988,35 +67007,33 @@
       <c r="I18" s="12">
         <v>8</v>
       </c>
-      <c r="J18" s="12">
-        <v>10</v>
-      </c>
-      <c r="K18" s="12">
-        <v>3</v>
-      </c>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
       <c r="L18" s="54"/>
       <c r="M18" s="12"/>
       <c r="N18" s="12">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="O18" s="12" t="s">
         <v>1864</v>
       </c>
-      <c r="P18" s="12"/>
+      <c r="P18" s="12" t="s">
+        <v>1859</v>
+      </c>
       <c r="Q18" s="50">
-        <v>45574</v>
+        <v>45559</v>
       </c>
       <c r="R18" s="56">
-        <v>45587</v>
+        <v>45573</v>
       </c>
       <c r="S18" s="53"/>
       <c r="T18" s="12"/>
       <c r="U18" s="12"/>
-      <c r="V18" s="12"/>
-      <c r="W18" s="12"/>
-      <c r="X18" s="48"/>
-      <c r="Y18" s="48"/>
-      <c r="Z18" s="48"/>
+      <c r="V18" s="59"/>
+      <c r="W18" s="59"/>
+      <c r="X18" s="59"/>
+      <c r="Y18" s="12"/>
+      <c r="Z18" s="12"/>
       <c r="AA18" s="12"/>
       <c r="AB18" s="12"/>
       <c r="AC18" s="12"/>
@@ -67076,18 +67093,29 @@
       <c r="CE18" s="12"/>
       <c r="CF18" s="12"/>
       <c r="CG18" s="12"/>
-    </row>
-    <row r="19" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
+      <c r="CH18" s="12"/>
+    </row>
+    <row r="19" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>1777</v>
+      </c>
       <c r="B19" s="15" t="s">
         <v>1739</v>
       </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="22"/>
+      <c r="C19" s="15" t="s">
+        <v>1739</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>1746</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>1784</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>1745</v>
+      </c>
       <c r="G19" s="12" t="s">
-        <v>777</v>
+        <v>187</v>
       </c>
       <c r="H19" s="12" t="s">
         <v>1716</v>
@@ -67095,22 +67123,26 @@
       <c r="I19" s="12">
         <v>8</v>
       </c>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
+      <c r="J19" s="12">
+        <v>10</v>
+      </c>
+      <c r="K19" s="12">
+        <v>3</v>
+      </c>
       <c r="L19" s="54"/>
       <c r="M19" s="12"/>
       <c r="N19" s="12">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="O19" s="12" t="s">
         <v>1864</v>
       </c>
       <c r="P19" s="12"/>
       <c r="Q19" s="50">
-        <v>45588</v>
+        <v>45579</v>
       </c>
       <c r="R19" s="56">
-        <v>45603</v>
+        <v>45589</v>
       </c>
       <c r="S19" s="53"/>
       <c r="T19" s="12"/>
@@ -67118,10 +67150,10 @@
       <c r="V19" s="12"/>
       <c r="W19" s="12"/>
       <c r="X19" s="12"/>
-      <c r="Y19" s="12"/>
+      <c r="Y19" s="48"/>
       <c r="Z19" s="48"/>
       <c r="AA19" s="48"/>
-      <c r="AB19" s="48"/>
+      <c r="AB19" s="12"/>
       <c r="AC19" s="12"/>
       <c r="AD19" s="12"/>
       <c r="AE19" s="12"/>
@@ -67179,53 +67211,42 @@
       <c r="CE19" s="12"/>
       <c r="CF19" s="12"/>
       <c r="CG19" s="12"/>
-    </row>
-    <row r="20" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
-        <v>1777</v>
-      </c>
+      <c r="CH19" s="12"/>
+    </row>
+    <row r="20" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="14"/>
       <c r="B20" s="15" t="s">
         <v>1739</v>
       </c>
-      <c r="C20" s="15" t="s">
-        <v>1739</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>1352</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>1747</v>
-      </c>
-      <c r="F20" s="18" t="s">
-        <v>1745</v>
-      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="22"/>
       <c r="G20" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="H20" s="10" t="s">
-        <v>1076</v>
+        <v>777</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>1716</v>
       </c>
       <c r="I20" s="12">
-        <v>12</v>
-      </c>
-      <c r="J20" s="12">
-        <v>2</v>
-      </c>
-      <c r="K20" s="12">
-        <v>2</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
       <c r="L20" s="54"/>
-      <c r="M20" s="12"/>
+      <c r="M20" s="49"/>
       <c r="N20" s="12">
-        <v>15</v>
-      </c>
-      <c r="O20" s="12"/>
+        <v>3</v>
+      </c>
+      <c r="O20" s="12" t="s">
+        <v>1880</v>
+      </c>
       <c r="P20" s="12"/>
       <c r="Q20" s="50">
-        <v>45720</v>
+        <v>45590</v>
       </c>
       <c r="R20" s="56">
-        <v>45742</v>
+        <v>45604</v>
       </c>
       <c r="S20" s="53"/>
       <c r="T20" s="12"/>
@@ -67235,8 +67256,9 @@
       <c r="X20" s="12"/>
       <c r="Y20" s="12"/>
       <c r="Z20" s="12"/>
-      <c r="AA20" s="12"/>
-      <c r="AC20" s="12"/>
+      <c r="AA20" s="48"/>
+      <c r="AB20" s="48"/>
+      <c r="AC20" s="48"/>
       <c r="AD20" s="12"/>
       <c r="AE20" s="12"/>
       <c r="AF20" s="12"/>
@@ -67252,9 +67274,9 @@
       <c r="AP20" s="12"/>
       <c r="AQ20" s="12"/>
       <c r="AR20" s="12"/>
-      <c r="AS20" s="48"/>
-      <c r="AT20" s="48"/>
-      <c r="AU20" s="48"/>
+      <c r="AS20" s="12"/>
+      <c r="AT20" s="12"/>
+      <c r="AU20" s="12"/>
       <c r="AV20" s="12"/>
       <c r="AW20" s="12"/>
       <c r="AX20" s="12"/>
@@ -67293,52 +67315,54 @@
       <c r="CE20" s="12"/>
       <c r="CF20" s="12"/>
       <c r="CG20" s="12"/>
-    </row>
-    <row r="21" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
-        <v>1778</v>
+      <c r="CH20" s="12"/>
+    </row>
+    <row r="21" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>1777</v>
       </c>
       <c r="B21" s="15" t="s">
         <v>1739</v>
       </c>
-      <c r="C21" s="12"/>
-      <c r="D21" s="19" t="s">
-        <v>1765</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>1766</v>
-      </c>
-      <c r="F21" s="25" t="s">
-        <v>1764</v>
+      <c r="C21" s="15" t="s">
+        <v>1739</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>1352</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>1747</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>1745</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>1249</v>
-      </c>
-      <c r="H21" s="8" t="s">
-        <v>1682</v>
+        <v>24</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>1076</v>
       </c>
       <c r="I21" s="12">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J21" s="12">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="K21" s="12">
-        <f>15+5</f>
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="L21" s="54"/>
       <c r="M21" s="12"/>
       <c r="N21" s="12">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="O21" s="12"/>
       <c r="P21" s="12"/>
       <c r="Q21" s="50">
-        <v>45743</v>
+        <v>45726</v>
       </c>
       <c r="R21" s="56">
-        <v>45763</v>
+        <v>45748</v>
       </c>
       <c r="S21" s="53"/>
       <c r="T21" s="12"/>
@@ -67350,7 +67374,6 @@
       <c r="Z21" s="12"/>
       <c r="AA21" s="12"/>
       <c r="AB21" s="12"/>
-      <c r="AC21" s="12"/>
       <c r="AD21" s="12"/>
       <c r="AE21" s="12"/>
       <c r="AF21" s="12"/>
@@ -67360,17 +67383,18 @@
       <c r="AJ21" s="12"/>
       <c r="AK21" s="12"/>
       <c r="AL21" s="12"/>
+      <c r="AM21" s="12"/>
       <c r="AN21" s="12"/>
       <c r="AO21" s="12"/>
       <c r="AP21" s="12"/>
       <c r="AQ21" s="12"/>
       <c r="AR21" s="12"/>
       <c r="AS21" s="12"/>
-      <c r="AT21" s="12"/>
-      <c r="AU21" s="12"/>
+      <c r="AT21" s="48"/>
+      <c r="AU21" s="48"/>
       <c r="AV21" s="48"/>
-      <c r="AW21" s="48"/>
-      <c r="AX21" s="48"/>
+      <c r="AW21" s="12"/>
+      <c r="AX21" s="12"/>
       <c r="AY21" s="12"/>
       <c r="AZ21" s="12"/>
       <c r="BA21" s="12"/>
@@ -67406,41 +67430,40 @@
       <c r="CE21" s="12"/>
       <c r="CF21" s="12"/>
       <c r="CG21" s="12"/>
-    </row>
-    <row r="22" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
-        <v>1777</v>
+      <c r="CH21" s="12"/>
+    </row>
+    <row r="22" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
+        <v>1778</v>
       </c>
       <c r="B22" s="15" t="s">
         <v>1739</v>
       </c>
-      <c r="C22" s="15" t="s">
-        <v>1739</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>1742</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>1743</v>
-      </c>
-      <c r="F22" s="28" t="s">
-        <v>1744</v>
+      <c r="C22" s="12"/>
+      <c r="D22" s="19" t="s">
+        <v>1765</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>1766</v>
+      </c>
+      <c r="F22" s="25" t="s">
+        <v>1764</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>18</v>
+        <v>1249</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>1681</v>
+        <v>1682</v>
       </c>
       <c r="I22" s="12">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J22" s="12">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="K22" s="12">
-        <f>3+8</f>
-        <v>11</v>
+        <f>15+5</f>
+        <v>20</v>
       </c>
       <c r="L22" s="54"/>
       <c r="M22" s="12"/>
@@ -67450,10 +67473,10 @@
       <c r="O22" s="12"/>
       <c r="P22" s="12"/>
       <c r="Q22" s="50">
-        <v>45764</v>
+        <v>45749</v>
       </c>
       <c r="R22" s="56">
-        <v>45784</v>
+        <v>45769</v>
       </c>
       <c r="S22" s="53"/>
       <c r="T22" s="12"/>
@@ -67469,13 +67492,13 @@
       <c r="AD22" s="12"/>
       <c r="AE22" s="12"/>
       <c r="AF22" s="12"/>
+      <c r="AG22" s="12"/>
       <c r="AH22" s="12"/>
       <c r="AI22" s="12"/>
       <c r="AJ22" s="12"/>
       <c r="AK22" s="12"/>
       <c r="AL22" s="12"/>
       <c r="AM22" s="12"/>
-      <c r="AN22" s="12"/>
       <c r="AO22" s="12"/>
       <c r="AP22" s="12"/>
       <c r="AQ22" s="12"/>
@@ -67484,13 +67507,11 @@
       <c r="AT22" s="12"/>
       <c r="AU22" s="12"/>
       <c r="AV22" s="12"/>
-      <c r="AW22" s="12"/>
-      <c r="AX22" s="12"/>
+      <c r="AW22" s="48"/>
+      <c r="AX22" s="48"/>
       <c r="AY22" s="48"/>
-      <c r="AZ22" s="48"/>
-      <c r="BA22" s="48" t="s">
-        <v>1867</v>
-      </c>
+      <c r="AZ22" s="12"/>
+      <c r="BA22" s="12"/>
       <c r="BB22" s="12"/>
       <c r="BC22" s="12"/>
       <c r="BD22" s="12"/>
@@ -67523,52 +67544,55 @@
       <c r="CE22" s="12"/>
       <c r="CF22" s="12"/>
       <c r="CG22" s="12"/>
-    </row>
-    <row r="23" spans="1:85" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
-        <v>1778</v>
+      <c r="CH22" s="12"/>
+    </row>
+    <row r="23" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>1777</v>
       </c>
       <c r="B23" s="15" t="s">
         <v>1739</v>
       </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="19" t="s">
-        <v>1643</v>
-      </c>
-      <c r="E23" s="21" t="s">
-        <v>1763</v>
-      </c>
-      <c r="F23" s="25" t="s">
-        <v>1764</v>
+      <c r="C23" s="15" t="s">
+        <v>1739</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>1742</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>1743</v>
+      </c>
+      <c r="F23" s="28" t="s">
+        <v>1744</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="H23" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23" s="8" t="s">
         <v>1681</v>
       </c>
       <c r="I23" s="12">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J23" s="12">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="K23" s="12">
-        <f>9+2</f>
+        <f>3+8</f>
         <v>11</v>
       </c>
       <c r="L23" s="54"/>
       <c r="M23" s="12"/>
       <c r="N23" s="12">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O23" s="12"/>
       <c r="P23" s="12"/>
       <c r="Q23" s="50">
-        <v>45814</v>
+        <v>45770</v>
       </c>
       <c r="R23" s="56">
-        <v>45835</v>
+        <v>45790</v>
       </c>
       <c r="S23" s="53"/>
       <c r="T23" s="12"/>
@@ -67585,7 +67609,6 @@
       <c r="AE23" s="12"/>
       <c r="AF23" s="12"/>
       <c r="AG23" s="12"/>
-      <c r="AH23" s="12"/>
       <c r="AI23" s="12"/>
       <c r="AJ23" s="12"/>
       <c r="AK23" s="12"/>
@@ -67601,14 +67624,20 @@
       <c r="AU23" s="12"/>
       <c r="AV23" s="12"/>
       <c r="AW23" s="12"/>
-      <c r="BB23" s="12"/>
+      <c r="AX23" s="12"/>
+      <c r="AY23" s="12"/>
+      <c r="AZ23" s="48"/>
+      <c r="BA23" s="48"/>
+      <c r="BB23" s="48" t="s">
+        <v>1867</v>
+      </c>
       <c r="BC23" s="12"/>
       <c r="BD23" s="12"/>
       <c r="BE23" s="12"/>
       <c r="BF23" s="12"/>
-      <c r="BG23" s="48"/>
-      <c r="BH23" s="48"/>
-      <c r="BI23" s="48"/>
+      <c r="BG23" s="12"/>
+      <c r="BH23" s="12"/>
+      <c r="BI23" s="12"/>
       <c r="BJ23" s="12"/>
       <c r="BK23" s="12"/>
       <c r="BL23" s="12"/>
@@ -67633,8 +67662,9 @@
       <c r="CE23" s="12"/>
       <c r="CF23" s="12"/>
       <c r="CG23" s="12"/>
-    </row>
-    <row r="24" spans="1:85" x14ac:dyDescent="0.25">
+      <c r="CH23" s="12"/>
+    </row>
+    <row r="24" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>1778</v>
       </c>
@@ -67674,10 +67704,10 @@
       <c r="O24" s="12"/>
       <c r="P24" s="12"/>
       <c r="Q24" s="50">
-        <v>45861</v>
+        <v>45867</v>
       </c>
       <c r="R24" s="56">
-        <v>45897</v>
+        <v>45903</v>
       </c>
       <c r="S24" s="53"/>
       <c r="T24" s="12"/>
@@ -67711,9 +67741,13 @@
       <c r="AV24" s="12"/>
       <c r="AW24" s="12"/>
       <c r="AX24" s="12"/>
-      <c r="AY24" s="12"/>
-      <c r="AZ24" s="12"/>
-      <c r="BA24" s="12"/>
+      <c r="AY24" s="68"/>
+      <c r="AZ24" s="68"/>
+      <c r="BA24" s="68"/>
+      <c r="BB24" s="68"/>
+      <c r="BC24" s="12"/>
+      <c r="BD24" s="12"/>
+      <c r="BE24" s="12"/>
       <c r="BF24" s="12"/>
       <c r="BG24" s="12"/>
       <c r="BH24" s="12"/>
@@ -67723,11 +67757,11 @@
       <c r="BL24" s="12"/>
       <c r="BM24" s="12"/>
       <c r="BN24" s="12"/>
-      <c r="BO24" s="48"/>
+      <c r="BO24" s="12"/>
       <c r="BP24" s="48"/>
       <c r="BQ24" s="48"/>
       <c r="BR24" s="48"/>
-      <c r="BS24" s="12"/>
+      <c r="BS24" s="48"/>
       <c r="BT24" s="12"/>
       <c r="BU24" s="12"/>
       <c r="BV24" s="12"/>
@@ -67742,8 +67776,9 @@
       <c r="CE24" s="12"/>
       <c r="CF24" s="12"/>
       <c r="CG24" s="12"/>
-    </row>
-    <row r="25" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CH24" s="12"/>
+    </row>
+    <row r="25" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>1777</v>
       </c>
@@ -67753,7 +67788,7 @@
       <c r="C25" s="15" t="s">
         <v>1739</v>
       </c>
-      <c r="D25" s="15" t="s">
+      <c r="D25" s="19" t="s">
         <v>1740</v>
       </c>
       <c r="E25" s="29" t="s">
@@ -67784,11 +67819,11 @@
       </c>
       <c r="O25" s="12"/>
       <c r="P25" s="12"/>
-      <c r="Q25" s="50">
-        <v>45974</v>
-      </c>
-      <c r="R25" s="56">
-        <v>46003</v>
+      <c r="Q25" s="12">
+        <v>45980</v>
+      </c>
+      <c r="R25" s="54">
+        <v>46009</v>
       </c>
       <c r="S25" s="53"/>
       <c r="T25" s="12"/>
@@ -67811,6 +67846,7 @@
       <c r="AK25" s="12"/>
       <c r="AL25" s="12"/>
       <c r="AM25" s="12"/>
+      <c r="AN25" s="12"/>
       <c r="AO25" s="12"/>
       <c r="AP25" s="12"/>
       <c r="AQ25" s="12"/>
@@ -67820,14 +67856,15 @@
       <c r="AU25" s="12"/>
       <c r="AV25" s="12"/>
       <c r="AW25" s="12"/>
+      <c r="AX25" s="12"/>
       <c r="AY25" s="12"/>
       <c r="AZ25" s="12"/>
       <c r="BA25" s="12"/>
       <c r="BB25" s="12"/>
-      <c r="BC25" s="12"/>
-      <c r="BD25" s="12"/>
-      <c r="BE25" s="12"/>
-      <c r="BF25" s="12"/>
+      <c r="BC25" s="68"/>
+      <c r="BD25" s="68"/>
+      <c r="BE25" s="68"/>
+      <c r="BF25" s="68"/>
       <c r="BG25" s="12"/>
       <c r="BH25" s="12"/>
       <c r="BI25" s="12"/>
@@ -67851,21 +67888,20 @@
       <c r="CA25" s="12"/>
       <c r="CB25" s="12"/>
       <c r="CC25" s="12"/>
-      <c r="CD25" s="48"/>
+      <c r="CD25" s="12"/>
       <c r="CE25" s="48"/>
       <c r="CF25" s="48"/>
       <c r="CG25" s="48"/>
-    </row>
-    <row r="26" spans="1:85" x14ac:dyDescent="0.25">
+      <c r="CH25" s="12"/>
+    </row>
+    <row r="26" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>1778</v>
       </c>
       <c r="B26" s="15" t="s">
         <v>1870</v>
       </c>
-      <c r="C26" s="15" t="s">
-        <v>1870</v>
-      </c>
+      <c r="C26" s="12"/>
       <c r="D26" s="19" t="s">
         <v>1774</v>
       </c>
@@ -67898,10 +67934,10 @@
       <c r="O26" s="12"/>
       <c r="P26" s="12"/>
       <c r="Q26" s="50">
-        <v>45785</v>
+        <v>45791</v>
       </c>
       <c r="R26" s="56">
-        <v>45813</v>
+        <v>45819</v>
       </c>
       <c r="S26" s="53"/>
       <c r="T26" s="12"/>
@@ -67925,7 +67961,7 @@
       <c r="AL26" s="12"/>
       <c r="AM26" s="12"/>
       <c r="AN26" s="12"/>
-      <c r="AO26" s="12"/>
+      <c r="AO26" s="68"/>
       <c r="AP26" s="12"/>
       <c r="AQ26" s="12"/>
       <c r="AR26" s="12"/>
@@ -67935,15 +67971,14 @@
       <c r="AV26" s="12"/>
       <c r="AW26" s="12"/>
       <c r="AX26" s="12"/>
-      <c r="AY26" s="12"/>
       <c r="AZ26" s="12"/>
       <c r="BA26" s="12"/>
-      <c r="BB26" s="48"/>
+      <c r="BB26" s="12"/>
       <c r="BC26" s="48"/>
       <c r="BD26" s="48"/>
       <c r="BE26" s="48"/>
       <c r="BF26" s="48"/>
-      <c r="BG26" s="12"/>
+      <c r="BG26" s="48"/>
       <c r="BH26" s="12"/>
       <c r="BI26" s="12"/>
       <c r="BJ26" s="12"/>
@@ -67970,15 +68005,16 @@
       <c r="CE26" s="12"/>
       <c r="CF26" s="12"/>
       <c r="CG26" s="12"/>
-    </row>
-    <row r="27" spans="1:85" x14ac:dyDescent="0.25">
+      <c r="CH26" s="12"/>
+    </row>
+    <row r="27" spans="1:86" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>1778</v>
       </c>
       <c r="B27" s="15" t="s">
         <v>1870</v>
       </c>
-      <c r="C27" s="15"/>
+      <c r="C27" s="12"/>
       <c r="D27" s="19" t="s">
         <v>1562</v>
       </c>
@@ -68011,10 +68047,10 @@
       <c r="O27" s="12"/>
       <c r="P27" s="12"/>
       <c r="Q27" s="50">
-        <v>45898</v>
+        <v>45904</v>
       </c>
       <c r="R27" s="56">
-        <v>45922</v>
+        <v>45928</v>
       </c>
       <c r="S27" s="53"/>
       <c r="T27" s="12"/>
@@ -68054,6 +68090,7 @@
       <c r="BB27" s="12"/>
       <c r="BC27" s="12"/>
       <c r="BD27" s="12"/>
+      <c r="BE27" s="12"/>
       <c r="BF27" s="12"/>
       <c r="BG27" s="12"/>
       <c r="BH27" s="12"/>
@@ -68067,10 +68104,10 @@
       <c r="BP27" s="12"/>
       <c r="BQ27" s="12"/>
       <c r="BR27" s="12"/>
-      <c r="BS27" s="48"/>
+      <c r="BS27" s="12"/>
       <c r="BT27" s="48"/>
       <c r="BU27" s="48"/>
-      <c r="BV27" s="12"/>
+      <c r="BV27" s="48"/>
       <c r="BW27" s="12"/>
       <c r="BX27" s="12"/>
       <c r="BY27" s="12"/>
@@ -68082,8 +68119,9 @@
       <c r="CE27" s="12"/>
       <c r="CF27" s="12"/>
       <c r="CG27" s="12"/>
-    </row>
-    <row r="28" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CH27" s="12"/>
+    </row>
+    <row r="28" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>1778</v>
       </c>
@@ -68119,10 +68157,10 @@
       <c r="O28" s="49"/>
       <c r="P28" s="49"/>
       <c r="Q28" s="51">
-        <v>45604</v>
+        <v>45607</v>
       </c>
       <c r="R28" s="57">
-        <v>45621</v>
+        <v>45624</v>
       </c>
       <c r="S28" s="53"/>
       <c r="T28" s="12"/>
@@ -68134,10 +68172,10 @@
       <c r="Z28" s="12"/>
       <c r="AA28" s="12"/>
       <c r="AB28" s="12"/>
-      <c r="AC28" s="48"/>
+      <c r="AC28" s="12"/>
       <c r="AD28" s="48"/>
       <c r="AE28" s="48"/>
-      <c r="AF28" s="12"/>
+      <c r="AF28" s="48"/>
       <c r="AG28" s="12"/>
       <c r="AH28" s="12"/>
       <c r="AI28" s="12"/>
@@ -68163,7 +68201,7 @@
       <c r="BC28" s="12"/>
       <c r="BD28" s="12"/>
       <c r="BE28" s="12"/>
-      <c r="BF28" s="12"/>
+      <c r="BF28" s="68"/>
       <c r="BG28" s="12"/>
       <c r="BH28" s="12"/>
       <c r="BI28" s="12"/>
@@ -68191,8 +68229,9 @@
       <c r="CE28" s="12"/>
       <c r="CF28" s="12"/>
       <c r="CG28" s="12"/>
-    </row>
-    <row r="29" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CH28" s="12"/>
+    </row>
+    <row r="29" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>1778</v>
       </c>
@@ -68226,10 +68265,10 @@
       <c r="O29" s="49"/>
       <c r="P29" s="49"/>
       <c r="Q29" s="51">
-        <v>45622</v>
+        <v>45625</v>
       </c>
       <c r="R29" s="57">
-        <v>45636</v>
+        <v>45639</v>
       </c>
       <c r="S29" s="53"/>
       <c r="T29" s="12"/>
@@ -68243,10 +68282,10 @@
       <c r="AB29" s="12"/>
       <c r="AC29" s="12"/>
       <c r="AD29" s="12"/>
-      <c r="AE29" s="48"/>
+      <c r="AE29" s="12"/>
       <c r="AF29" s="48"/>
       <c r="AG29" s="48"/>
-      <c r="AH29" s="12"/>
+      <c r="AH29" s="48"/>
       <c r="AI29" s="12"/>
       <c r="AJ29" s="12"/>
       <c r="AK29" s="12"/>
@@ -68285,6 +68324,10 @@
       <c r="BR29" s="12"/>
       <c r="BS29" s="12"/>
       <c r="BT29" s="12"/>
+      <c r="BU29" s="12"/>
+      <c r="BV29" s="12"/>
+      <c r="BW29" s="12"/>
+      <c r="BX29" s="12"/>
       <c r="BY29" s="12"/>
       <c r="BZ29" s="12"/>
       <c r="CA29" s="12"/>
@@ -68294,8 +68337,9 @@
       <c r="CE29" s="12"/>
       <c r="CF29" s="12"/>
       <c r="CG29" s="12"/>
-    </row>
-    <row r="30" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CH29" s="12"/>
+    </row>
+    <row r="30" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>1778</v>
       </c>
@@ -68322,17 +68366,17 @@
       <c r="J30" s="49"/>
       <c r="K30" s="49"/>
       <c r="L30" s="55"/>
-      <c r="M30" s="49"/>
+      <c r="M30" s="12"/>
       <c r="N30" s="49">
         <v>10</v>
       </c>
       <c r="O30" s="49"/>
       <c r="P30" s="49"/>
       <c r="Q30" s="51">
-        <v>45637</v>
+        <v>45642</v>
       </c>
       <c r="R30" s="57">
-        <v>45652</v>
+        <v>45657</v>
       </c>
       <c r="S30" s="53"/>
       <c r="T30" s="12"/>
@@ -68348,10 +68392,10 @@
       <c r="AD30" s="12"/>
       <c r="AE30" s="12"/>
       <c r="AF30" s="12"/>
-      <c r="AG30" s="48"/>
+      <c r="AG30" s="12"/>
       <c r="AH30" s="48"/>
       <c r="AI30" s="48"/>
-      <c r="AJ30" s="12"/>
+      <c r="AJ30" s="48"/>
       <c r="AK30" s="12"/>
       <c r="AL30" s="12"/>
       <c r="AM30" s="12"/>
@@ -68389,10 +68433,10 @@
       <c r="BS30" s="12"/>
       <c r="BT30" s="12"/>
       <c r="BU30" s="12"/>
-      <c r="BV30" s="12"/>
-      <c r="BW30" s="12"/>
-      <c r="BX30" s="12"/>
-      <c r="BY30" s="12"/>
+      <c r="BV30" s="68"/>
+      <c r="BW30" s="68"/>
+      <c r="BX30" s="68"/>
+      <c r="BY30" s="68"/>
       <c r="BZ30" s="12"/>
       <c r="CA30" s="12"/>
       <c r="CB30" s="12"/>
@@ -68401,24 +68445,25 @@
       <c r="CE30" s="12"/>
       <c r="CF30" s="12"/>
       <c r="CG30" s="12"/>
-    </row>
-    <row r="31" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CH30" s="46"/>
+    </row>
+    <row r="31" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
         <v>1777</v>
       </c>
       <c r="B31" s="15" t="s">
+        <v>1874</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>1874</v>
+      </c>
+      <c r="D31" s="15" t="s">
         <v>1875</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>1880</v>
-      </c>
-      <c r="D31" s="15" t="s">
-        <v>1876</v>
       </c>
       <c r="E31" s="17" t="s">
         <v>1838</v>
       </c>
-      <c r="F31" s="12"/>
+      <c r="F31" s="30"/>
       <c r="G31" s="10" t="s">
         <v>31</v>
       </c>
@@ -68428,14 +68473,14 @@
       <c r="I31" s="12"/>
       <c r="J31" s="12"/>
       <c r="K31" s="12"/>
-      <c r="L31" s="12"/>
+      <c r="L31" s="54"/>
       <c r="M31" s="12"/>
       <c r="N31" s="12"/>
       <c r="O31" s="12"/>
       <c r="P31" s="12"/>
       <c r="Q31" s="12"/>
       <c r="R31" s="12"/>
-      <c r="S31" s="12"/>
+      <c r="S31" s="53"/>
       <c r="T31" s="12"/>
       <c r="U31" s="12"/>
       <c r="V31" s="12"/>
@@ -68502,24 +68547,25 @@
       <c r="CE31" s="12"/>
       <c r="CF31" s="12"/>
       <c r="CG31" s="12"/>
-    </row>
-    <row r="32" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CH31" s="48"/>
+    </row>
+    <row r="32" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
         <v>1777</v>
       </c>
-      <c r="B32" s="60" t="s">
-        <v>1875</v>
-      </c>
-      <c r="C32" s="60" t="s">
-        <v>1880</v>
+      <c r="B32" s="15" t="s">
+        <v>1874</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>1874</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>1877</v>
+        <v>1876</v>
       </c>
       <c r="E32" s="17" t="s">
         <v>1838</v>
       </c>
-      <c r="F32" s="12"/>
+      <c r="F32" s="30"/>
       <c r="G32" s="10" t="s">
         <v>31</v>
       </c>
@@ -68529,14 +68575,14 @@
       <c r="I32" s="12"/>
       <c r="J32" s="12"/>
       <c r="K32" s="12"/>
-      <c r="L32" s="12"/>
+      <c r="L32" s="54"/>
       <c r="M32" s="12"/>
       <c r="N32" s="12"/>
       <c r="O32" s="12"/>
       <c r="P32" s="12"/>
       <c r="Q32" s="12"/>
       <c r="R32" s="12"/>
-      <c r="S32" s="12"/>
+      <c r="S32" s="53"/>
       <c r="T32" s="12"/>
       <c r="U32" s="12"/>
       <c r="V32" s="12"/>
@@ -68603,24 +68649,25 @@
       <c r="CE32" s="12"/>
       <c r="CF32" s="12"/>
       <c r="CG32" s="12"/>
-    </row>
-    <row r="33" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CH32" s="12"/>
+    </row>
+    <row r="33" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>1777</v>
       </c>
       <c r="B33" s="60" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="C33" s="60" t="s">
-        <v>1880</v>
+        <v>1874</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>1878</v>
+        <v>1877</v>
       </c>
       <c r="E33" s="17" t="s">
         <v>1838</v>
       </c>
-      <c r="F33" s="12"/>
+      <c r="F33" s="30"/>
       <c r="G33" s="10" t="s">
         <v>31</v>
       </c>
@@ -68630,14 +68677,14 @@
       <c r="I33" s="12"/>
       <c r="J33" s="12"/>
       <c r="K33" s="12"/>
-      <c r="L33" s="12"/>
+      <c r="L33" s="54"/>
       <c r="M33" s="12"/>
       <c r="N33" s="12"/>
       <c r="O33" s="12"/>
       <c r="P33" s="12"/>
       <c r="Q33" s="12"/>
       <c r="R33" s="12"/>
-      <c r="S33" s="12"/>
+      <c r="S33" s="53"/>
       <c r="T33" s="12"/>
       <c r="U33" s="12"/>
       <c r="V33" s="12"/>
@@ -68704,24 +68751,25 @@
       <c r="CE33" s="12"/>
       <c r="CF33" s="12"/>
       <c r="CG33" s="12"/>
-    </row>
-    <row r="34" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CH33" s="12"/>
+    </row>
+    <row r="34" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
         <v>1777</v>
       </c>
       <c r="B34" s="60" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="C34" s="60" t="s">
-        <v>1880</v>
+        <v>1874</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>1879</v>
+        <v>1878</v>
       </c>
       <c r="E34" s="17" t="s">
         <v>1838</v>
       </c>
-      <c r="F34" s="12"/>
+      <c r="F34" s="30"/>
       <c r="G34" s="10" t="s">
         <v>31</v>
       </c>
@@ -68731,14 +68779,14 @@
       <c r="I34" s="12"/>
       <c r="J34" s="12"/>
       <c r="K34" s="12"/>
-      <c r="L34" s="12"/>
+      <c r="L34" s="54"/>
       <c r="M34" s="12"/>
       <c r="N34" s="12"/>
       <c r="O34" s="12"/>
       <c r="P34" s="12"/>
       <c r="Q34" s="12"/>
       <c r="R34" s="12"/>
-      <c r="S34" s="12"/>
+      <c r="S34" s="53"/>
       <c r="T34" s="12"/>
       <c r="U34" s="12"/>
       <c r="V34" s="12"/>
@@ -68805,41 +68853,40 @@
       <c r="CE34" s="12"/>
       <c r="CF34" s="12"/>
       <c r="CG34" s="12"/>
-    </row>
-    <row r="35" spans="1:85" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CH34" s="12"/>
+    </row>
+    <row r="35" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>1777</v>
       </c>
-      <c r="B35" s="60" t="s">
+      <c r="B35" s="67" t="s">
         <v>1873</v>
       </c>
-      <c r="C35" s="60" t="s">
+      <c r="C35" s="67" t="s">
         <v>1871</v>
       </c>
       <c r="D35" s="19" t="s">
         <v>1872</v>
       </c>
       <c r="E35" s="29" t="s">
-        <v>1874</v>
-      </c>
-      <c r="F35" s="12"/>
+        <v>1783</v>
+      </c>
+      <c r="F35" s="30"/>
       <c r="G35" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="H35" s="10" t="s">
-        <v>1060</v>
-      </c>
+      <c r="H35" s="10"/>
       <c r="I35" s="12"/>
       <c r="J35" s="12"/>
       <c r="K35" s="12"/>
-      <c r="L35" s="12"/>
+      <c r="L35" s="54"/>
       <c r="M35" s="12"/>
       <c r="N35" s="12"/>
       <c r="O35" s="12"/>
       <c r="P35" s="12"/>
       <c r="Q35" s="12"/>
       <c r="R35" s="12"/>
-      <c r="S35" s="12"/>
+      <c r="S35" s="53"/>
       <c r="T35" s="12"/>
       <c r="U35" s="12"/>
       <c r="V35" s="12"/>
@@ -68906,30 +68953,153 @@
       <c r="CE35" s="12"/>
       <c r="CF35" s="12"/>
       <c r="CG35" s="12"/>
+      <c r="CH35" s="12"/>
+    </row>
+    <row r="36" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="14"/>
+      <c r="B36" s="67"/>
+      <c r="C36" s="67" t="s">
+        <v>1879</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>1879</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>1879</v>
+      </c>
+      <c r="F36" s="15" t="s">
+        <v>1879</v>
+      </c>
+      <c r="G36" s="15" t="s">
+        <v>1879</v>
+      </c>
+      <c r="H36" s="15" t="s">
+        <v>1879</v>
+      </c>
+      <c r="I36" s="12">
+        <v>8</v>
+      </c>
+      <c r="J36" s="12"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="54"/>
+      <c r="M36" s="68"/>
+      <c r="N36" s="12">
+        <v>3</v>
+      </c>
+      <c r="O36" s="12" t="s">
+        <v>1864</v>
+      </c>
+      <c r="P36" s="12" t="s">
+        <v>1859</v>
+      </c>
+      <c r="Q36" s="72">
+        <v>45574</v>
+      </c>
+      <c r="R36" s="72">
+        <v>45576</v>
+      </c>
+      <c r="S36" s="53"/>
+      <c r="T36" s="12"/>
+      <c r="U36" s="12"/>
+      <c r="V36" s="12"/>
+      <c r="W36" s="12"/>
+      <c r="X36" s="59"/>
+      <c r="Y36" s="12"/>
+      <c r="Z36" s="12"/>
+      <c r="AA36" s="12"/>
+      <c r="AB36" s="12"/>
+      <c r="AC36" s="12"/>
+      <c r="AD36" s="12"/>
+      <c r="AE36" s="12"/>
+      <c r="AF36" s="12"/>
+      <c r="AG36" s="12"/>
+      <c r="AH36" s="12"/>
+      <c r="AI36" s="12"/>
+      <c r="AJ36" s="12"/>
+      <c r="AK36" s="12"/>
+      <c r="AL36" s="12"/>
+      <c r="AM36" s="12"/>
+      <c r="AN36" s="12"/>
+      <c r="AO36" s="12"/>
+      <c r="AP36" s="12"/>
+      <c r="AQ36" s="12"/>
+      <c r="AR36" s="12"/>
+      <c r="AS36" s="12"/>
+      <c r="AT36" s="12"/>
+      <c r="AU36" s="12"/>
+      <c r="AV36" s="12"/>
+      <c r="AW36" s="12"/>
+      <c r="AX36" s="12"/>
+      <c r="AY36" s="12"/>
+      <c r="AZ36" s="12"/>
+      <c r="BA36" s="12"/>
+      <c r="BB36" s="12"/>
+      <c r="BC36" s="12"/>
+      <c r="BD36" s="12"/>
+      <c r="BE36" s="12"/>
+      <c r="BF36" s="12"/>
+      <c r="BG36" s="12"/>
+      <c r="BH36" s="12"/>
+      <c r="BI36" s="12"/>
+      <c r="BJ36" s="12"/>
+      <c r="BK36" s="12"/>
+      <c r="BL36" s="12"/>
+      <c r="BM36" s="12"/>
+      <c r="BN36" s="12"/>
+      <c r="BO36" s="12"/>
+      <c r="BP36" s="12"/>
+      <c r="BQ36" s="12"/>
+      <c r="BR36" s="12"/>
+      <c r="BS36" s="12"/>
+      <c r="BT36" s="12"/>
+      <c r="BU36" s="12"/>
+      <c r="BV36" s="12"/>
+      <c r="BW36" s="12"/>
+      <c r="BX36" s="12"/>
+      <c r="BY36" s="12"/>
+      <c r="BZ36" s="12"/>
+      <c r="CA36" s="12"/>
+      <c r="CB36" s="12"/>
+      <c r="CC36" s="12"/>
+      <c r="CD36" s="12"/>
+      <c r="CE36" s="12"/>
+      <c r="CF36" s="12"/>
+      <c r="CG36" s="12"/>
+      <c r="CH36" s="12"/>
+    </row>
+    <row r="37" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="E37" s="69"/>
+      <c r="G37" s="70"/>
+    </row>
+    <row r="38" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="G38" s="70"/>
+    </row>
+    <row r="39" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="G39" s="70"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:CG31" xr:uid="{9585C0FF-65C5-4BD8-9936-5C9A63F7E604}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:CG35">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:CG36">
       <sortCondition ref="B2:B31"/>
     </sortState>
   </autoFilter>
   <mergeCells count="16">
-    <mergeCell ref="AO1:AR1"/>
-    <mergeCell ref="AS1:AV1"/>
-    <mergeCell ref="AW1:AZ1"/>
-    <mergeCell ref="BA1:BE1"/>
-    <mergeCell ref="BF1:BI1"/>
-    <mergeCell ref="S1:V1"/>
-    <mergeCell ref="W1:AA1"/>
-    <mergeCell ref="AB1:AE1"/>
-    <mergeCell ref="AF1:AI1"/>
-    <mergeCell ref="AJ1:AN1"/>
     <mergeCell ref="CF1:CG1"/>
     <mergeCell ref="BJ1:BN1"/>
     <mergeCell ref="BO1:BR1"/>
     <mergeCell ref="BS1:BV1"/>
     <mergeCell ref="BW1:BZ1"/>
     <mergeCell ref="CB1:CE1"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="W1:AA1"/>
+    <mergeCell ref="AB1:AE1"/>
+    <mergeCell ref="AF1:AI1"/>
+    <mergeCell ref="AJ1:AN1"/>
+    <mergeCell ref="AO1:AR1"/>
+    <mergeCell ref="AS1:AV1"/>
+    <mergeCell ref="AW1:AZ1"/>
+    <mergeCell ref="BA1:BE1"/>
+    <mergeCell ref="BF1:BI1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Se agrega el "Reporte de Talones (Texto-Excel)" al listado.
</commit_message>
<xml_diff>
--- a/00-Documentacion/Listado de reportes totales-TI.xlsx
+++ b/00-Documentacion/Listado de reportes totales-TI.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\source\repos\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B74622-26D9-4DE7-AB1D-D5686353CF95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7689B238-EA3A-44EC-89C3-91CE03D486AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{1498AA1A-1ACC-4329-A050-ACA05131B658}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13293" uniqueCount="1881">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13299" uniqueCount="1885">
   <si>
     <t xml:space="preserve">Reporte </t>
   </si>
@@ -5697,6 +5697,18 @@
   </si>
   <si>
     <t>Ajustes</t>
+  </si>
+  <si>
+    <t>Bajo demanda</t>
+  </si>
+  <si>
+    <t>Talones LTL (texto-excel)</t>
+  </si>
+  <si>
+    <t>correo, Excel, txt, zip</t>
+  </si>
+  <si>
+    <t>Pendiente</t>
   </si>
 </sst>
 </file>
@@ -5824,7 +5836,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5894,6 +5906,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00CC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6010,7 +6040,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6134,6 +6164,16 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6149,29 +6189,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF00CC99"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -64773,10 +64834,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9585C0FF-65C5-4BD8-9936-5C9A63F7E604}">
-  <dimension ref="A1:CH39"/>
+  <dimension ref="A1:CM40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BH1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CG11" sqref="CG11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64858,104 +64920,104 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:86" x14ac:dyDescent="0.25">
-      <c r="S1" s="64">
+      <c r="S1" s="68">
         <v>45536</v>
       </c>
-      <c r="T1" s="65"/>
-      <c r="U1" s="65"/>
-      <c r="V1" s="65"/>
-      <c r="W1" s="64">
+      <c r="T1" s="69"/>
+      <c r="U1" s="69"/>
+      <c r="V1" s="69"/>
+      <c r="W1" s="68">
         <v>45566</v>
       </c>
-      <c r="X1" s="64"/>
-      <c r="Y1" s="64"/>
-      <c r="Z1" s="64"/>
-      <c r="AA1" s="64"/>
-      <c r="AB1" s="61">
+      <c r="X1" s="68"/>
+      <c r="Y1" s="68"/>
+      <c r="Z1" s="68"/>
+      <c r="AA1" s="68"/>
+      <c r="AB1" s="65">
         <v>45597</v>
       </c>
-      <c r="AC1" s="62"/>
-      <c r="AD1" s="62"/>
-      <c r="AE1" s="63"/>
-      <c r="AF1" s="61">
+      <c r="AC1" s="66"/>
+      <c r="AD1" s="66"/>
+      <c r="AE1" s="67"/>
+      <c r="AF1" s="65">
         <v>45627</v>
       </c>
-      <c r="AG1" s="62"/>
-      <c r="AH1" s="62"/>
-      <c r="AI1" s="63"/>
-      <c r="AJ1" s="61">
+      <c r="AG1" s="66"/>
+      <c r="AH1" s="66"/>
+      <c r="AI1" s="67"/>
+      <c r="AJ1" s="65">
         <v>45658</v>
       </c>
-      <c r="AK1" s="62"/>
-      <c r="AL1" s="62"/>
-      <c r="AM1" s="62"/>
-      <c r="AN1" s="63"/>
-      <c r="AO1" s="61">
+      <c r="AK1" s="66"/>
+      <c r="AL1" s="66"/>
+      <c r="AM1" s="66"/>
+      <c r="AN1" s="67"/>
+      <c r="AO1" s="65">
         <v>45689</v>
       </c>
-      <c r="AP1" s="62"/>
-      <c r="AQ1" s="62"/>
-      <c r="AR1" s="63"/>
-      <c r="AS1" s="61">
+      <c r="AP1" s="66"/>
+      <c r="AQ1" s="66"/>
+      <c r="AR1" s="67"/>
+      <c r="AS1" s="65">
         <v>45717</v>
       </c>
-      <c r="AT1" s="62"/>
-      <c r="AU1" s="62"/>
-      <c r="AV1" s="63"/>
-      <c r="AW1" s="61">
+      <c r="AT1" s="66"/>
+      <c r="AU1" s="66"/>
+      <c r="AV1" s="67"/>
+      <c r="AW1" s="65">
         <v>45748</v>
       </c>
-      <c r="AX1" s="62"/>
-      <c r="AY1" s="62"/>
-      <c r="AZ1" s="63"/>
-      <c r="BA1" s="61">
+      <c r="AX1" s="66"/>
+      <c r="AY1" s="66"/>
+      <c r="AZ1" s="67"/>
+      <c r="BA1" s="65">
         <v>45778</v>
       </c>
-      <c r="BB1" s="62"/>
-      <c r="BC1" s="62"/>
-      <c r="BD1" s="62"/>
-      <c r="BE1" s="63"/>
-      <c r="BF1" s="61">
+      <c r="BB1" s="66"/>
+      <c r="BC1" s="66"/>
+      <c r="BD1" s="66"/>
+      <c r="BE1" s="67"/>
+      <c r="BF1" s="65">
         <v>45809</v>
       </c>
-      <c r="BG1" s="62"/>
-      <c r="BH1" s="62"/>
-      <c r="BI1" s="62"/>
-      <c r="BJ1" s="61">
+      <c r="BG1" s="66"/>
+      <c r="BH1" s="66"/>
+      <c r="BI1" s="66"/>
+      <c r="BJ1" s="65">
         <v>45839</v>
       </c>
-      <c r="BK1" s="62"/>
-      <c r="BL1" s="62"/>
-      <c r="BM1" s="62"/>
-      <c r="BN1" s="63"/>
-      <c r="BO1" s="61">
+      <c r="BK1" s="66"/>
+      <c r="BL1" s="66"/>
+      <c r="BM1" s="66"/>
+      <c r="BN1" s="67"/>
+      <c r="BO1" s="65">
         <v>45870</v>
       </c>
-      <c r="BP1" s="62"/>
-      <c r="BQ1" s="62"/>
-      <c r="BR1" s="62"/>
-      <c r="BS1" s="61">
+      <c r="BP1" s="66"/>
+      <c r="BQ1" s="66"/>
+      <c r="BR1" s="66"/>
+      <c r="BS1" s="65">
         <v>45901</v>
       </c>
-      <c r="BT1" s="62"/>
-      <c r="BU1" s="62"/>
-      <c r="BV1" s="62"/>
-      <c r="BW1" s="61">
+      <c r="BT1" s="66"/>
+      <c r="BU1" s="66"/>
+      <c r="BV1" s="66"/>
+      <c r="BW1" s="65">
         <v>45931</v>
       </c>
-      <c r="BX1" s="62"/>
-      <c r="BY1" s="62"/>
-      <c r="BZ1" s="62"/>
-      <c r="CB1" s="61">
+      <c r="BX1" s="66"/>
+      <c r="BY1" s="66"/>
+      <c r="BZ1" s="66"/>
+      <c r="CB1" s="65">
         <v>45962</v>
       </c>
-      <c r="CC1" s="62"/>
-      <c r="CD1" s="62"/>
-      <c r="CE1" s="62"/>
-      <c r="CF1" s="66" t="s">
+      <c r="CC1" s="66"/>
+      <c r="CD1" s="66"/>
+      <c r="CE1" s="66"/>
+      <c r="CF1" s="64" t="s">
         <v>1854</v>
       </c>
-      <c r="CG1" s="66"/>
+      <c r="CG1" s="64"/>
     </row>
     <row r="2" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
@@ -66192,7 +66254,7 @@
       <c r="E11" s="19" t="s">
         <v>1761</v>
       </c>
-      <c r="F11" s="71" t="s">
+      <c r="F11" s="62" t="s">
         <v>1762</v>
       </c>
       <c r="G11" s="12" t="s">
@@ -66460,7 +66522,6 @@
       <c r="T13" s="12"/>
       <c r="U13" s="12"/>
       <c r="V13" s="12"/>
-      <c r="W13" s="68"/>
       <c r="X13" s="12"/>
       <c r="Y13" s="12"/>
       <c r="Z13" s="12"/>
@@ -66928,7 +66989,6 @@
       <c r="X17" s="12"/>
       <c r="Y17" s="12"/>
       <c r="Z17" s="12"/>
-      <c r="AA17" s="68"/>
       <c r="AB17" s="12"/>
       <c r="AC17" s="12"/>
       <c r="AD17" s="12"/>
@@ -67741,10 +67801,6 @@
       <c r="AV24" s="12"/>
       <c r="AW24" s="12"/>
       <c r="AX24" s="12"/>
-      <c r="AY24" s="68"/>
-      <c r="AZ24" s="68"/>
-      <c r="BA24" s="68"/>
-      <c r="BB24" s="68"/>
       <c r="BC24" s="12"/>
       <c r="BD24" s="12"/>
       <c r="BE24" s="12"/>
@@ -67861,10 +67917,6 @@
       <c r="AZ25" s="12"/>
       <c r="BA25" s="12"/>
       <c r="BB25" s="12"/>
-      <c r="BC25" s="68"/>
-      <c r="BD25" s="68"/>
-      <c r="BE25" s="68"/>
-      <c r="BF25" s="68"/>
       <c r="BG25" s="12"/>
       <c r="BH25" s="12"/>
       <c r="BI25" s="12"/>
@@ -67961,7 +68013,6 @@
       <c r="AL26" s="12"/>
       <c r="AM26" s="12"/>
       <c r="AN26" s="12"/>
-      <c r="AO26" s="68"/>
       <c r="AP26" s="12"/>
       <c r="AQ26" s="12"/>
       <c r="AR26" s="12"/>
@@ -68201,7 +68252,6 @@
       <c r="BC28" s="12"/>
       <c r="BD28" s="12"/>
       <c r="BE28" s="12"/>
-      <c r="BF28" s="68"/>
       <c r="BG28" s="12"/>
       <c r="BH28" s="12"/>
       <c r="BI28" s="12"/>
@@ -68433,10 +68483,6 @@
       <c r="BS30" s="12"/>
       <c r="BT30" s="12"/>
       <c r="BU30" s="12"/>
-      <c r="BV30" s="68"/>
-      <c r="BW30" s="68"/>
-      <c r="BX30" s="68"/>
-      <c r="BY30" s="68"/>
       <c r="BZ30" s="12"/>
       <c r="CA30" s="12"/>
       <c r="CB30" s="12"/>
@@ -68651,7 +68697,7 @@
       <c r="CG32" s="12"/>
       <c r="CH32" s="12"/>
     </row>
-    <row r="33" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:91" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>1777</v>
       </c>
@@ -68753,7 +68799,7 @@
       <c r="CG33" s="12"/>
       <c r="CH33" s="12"/>
     </row>
-    <row r="34" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:91" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
         <v>1777</v>
       </c>
@@ -68855,14 +68901,14 @@
       <c r="CG34" s="12"/>
       <c r="CH34" s="12"/>
     </row>
-    <row r="35" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:91" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>1777</v>
       </c>
-      <c r="B35" s="67" t="s">
+      <c r="B35" s="60" t="s">
         <v>1873</v>
       </c>
-      <c r="C35" s="67" t="s">
+      <c r="C35" s="60" t="s">
         <v>1871</v>
       </c>
       <c r="D35" s="19" t="s">
@@ -68955,10 +69001,10 @@
       <c r="CG35" s="12"/>
       <c r="CH35" s="12"/>
     </row>
-    <row r="36" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:91" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="14"/>
-      <c r="B36" s="67"/>
-      <c r="C36" s="67" t="s">
+      <c r="B36" s="60"/>
+      <c r="C36" s="60" t="s">
         <v>1879</v>
       </c>
       <c r="D36" s="15" t="s">
@@ -68982,7 +69028,6 @@
       <c r="J36" s="12"/>
       <c r="K36" s="12"/>
       <c r="L36" s="54"/>
-      <c r="M36" s="68"/>
       <c r="N36" s="12">
         <v>3</v>
       </c>
@@ -68992,10 +69037,10 @@
       <c r="P36" s="12" t="s">
         <v>1859</v>
       </c>
-      <c r="Q36" s="72">
+      <c r="Q36" s="63">
         <v>45574</v>
       </c>
-      <c r="R36" s="72">
+      <c r="R36" s="63">
         <v>45576</v>
       </c>
       <c r="S36" s="53"/>
@@ -69067,15 +69112,295 @@
       <c r="CG36" s="12"/>
       <c r="CH36" s="12"/>
     </row>
-    <row r="37" spans="1:86" x14ac:dyDescent="0.25">
-      <c r="E37" s="69"/>
+    <row r="37" spans="1:91" s="74" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="70"/>
+      <c r="B37" s="71"/>
+      <c r="C37" s="71"/>
+      <c r="D37" s="70"/>
+      <c r="E37" s="72"/>
+      <c r="F37" s="72"/>
       <c r="G37" s="70"/>
-    </row>
-    <row r="38" spans="1:86" x14ac:dyDescent="0.25">
-      <c r="G38" s="70"/>
-    </row>
-    <row r="39" spans="1:86" x14ac:dyDescent="0.25">
-      <c r="G39" s="70"/>
+      <c r="H37" s="72"/>
+      <c r="I37" s="73"/>
+      <c r="J37" s="73"/>
+      <c r="K37" s="73"/>
+      <c r="L37" s="73"/>
+      <c r="N37" s="73"/>
+      <c r="O37" s="73"/>
+      <c r="P37" s="73"/>
+      <c r="Q37" s="75"/>
+      <c r="R37" s="75"/>
+      <c r="S37" s="73"/>
+      <c r="T37" s="73"/>
+      <c r="U37" s="73"/>
+      <c r="V37" s="73"/>
+      <c r="W37" s="73"/>
+      <c r="X37" s="73"/>
+      <c r="Y37" s="73"/>
+      <c r="Z37" s="73"/>
+      <c r="AA37" s="73"/>
+      <c r="AB37" s="73"/>
+      <c r="AC37" s="73"/>
+      <c r="AD37" s="73"/>
+      <c r="AE37" s="73"/>
+      <c r="AF37" s="73"/>
+      <c r="AG37" s="73"/>
+      <c r="AH37" s="73"/>
+      <c r="AI37" s="73"/>
+      <c r="AJ37" s="73"/>
+      <c r="AK37" s="73"/>
+      <c r="AL37" s="73"/>
+      <c r="AM37" s="73"/>
+      <c r="AN37" s="73"/>
+      <c r="AO37" s="73"/>
+      <c r="AP37" s="73"/>
+      <c r="AQ37" s="73"/>
+      <c r="AR37" s="73"/>
+      <c r="AS37" s="73"/>
+      <c r="AT37" s="73"/>
+      <c r="AU37" s="73"/>
+      <c r="AV37" s="73"/>
+      <c r="AW37" s="73"/>
+      <c r="AX37" s="73"/>
+      <c r="AY37" s="73"/>
+      <c r="AZ37" s="73"/>
+      <c r="BA37" s="73"/>
+      <c r="BB37" s="73"/>
+      <c r="BC37" s="73"/>
+      <c r="BD37" s="73"/>
+      <c r="BE37" s="73"/>
+      <c r="BF37" s="73"/>
+      <c r="BG37" s="73"/>
+      <c r="BH37" s="73"/>
+      <c r="BI37" s="73"/>
+      <c r="BJ37" s="73"/>
+      <c r="BK37" s="73"/>
+      <c r="BL37" s="73"/>
+      <c r="BM37" s="73"/>
+      <c r="BN37" s="73"/>
+      <c r="BO37" s="73"/>
+      <c r="BP37" s="73"/>
+      <c r="BQ37" s="73"/>
+      <c r="BR37" s="73"/>
+      <c r="BS37" s="73"/>
+      <c r="BT37" s="73"/>
+      <c r="BU37" s="73"/>
+      <c r="BV37" s="73"/>
+      <c r="BW37" s="73"/>
+      <c r="BX37" s="73"/>
+      <c r="BY37" s="73"/>
+      <c r="BZ37" s="73"/>
+      <c r="CA37" s="73"/>
+      <c r="CB37" s="73"/>
+      <c r="CC37" s="73"/>
+      <c r="CD37" s="73"/>
+      <c r="CE37" s="73"/>
+      <c r="CF37" s="73"/>
+      <c r="CG37" s="73"/>
+      <c r="CH37" s="73"/>
+    </row>
+    <row r="38" spans="1:91" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="82" t="s">
+        <v>1778</v>
+      </c>
+      <c r="B38" s="78"/>
+      <c r="C38" s="78"/>
+      <c r="D38" s="76" t="s">
+        <v>1882</v>
+      </c>
+      <c r="E38" s="77" t="s">
+        <v>1881</v>
+      </c>
+      <c r="F38" s="78"/>
+      <c r="G38" s="79" t="s">
+        <v>176</v>
+      </c>
+      <c r="H38" s="79" t="s">
+        <v>1883</v>
+      </c>
+      <c r="I38" s="78">
+        <v>23</v>
+      </c>
+      <c r="J38" s="78"/>
+      <c r="K38" s="78"/>
+      <c r="L38" s="78"/>
+      <c r="M38" s="78"/>
+      <c r="N38" s="78"/>
+      <c r="O38" s="78"/>
+      <c r="P38" s="78" t="s">
+        <v>1884</v>
+      </c>
+      <c r="Q38" s="78"/>
+      <c r="R38" s="78"/>
+      <c r="S38" s="78"/>
+      <c r="T38" s="78"/>
+      <c r="U38" s="78"/>
+      <c r="V38" s="78"/>
+      <c r="W38" s="78"/>
+      <c r="X38" s="78"/>
+      <c r="Y38" s="78"/>
+      <c r="Z38" s="78"/>
+      <c r="AA38" s="78"/>
+      <c r="AB38" s="78"/>
+      <c r="AC38" s="78"/>
+      <c r="AD38" s="78"/>
+      <c r="AE38" s="78"/>
+      <c r="AF38" s="78"/>
+      <c r="AG38" s="78"/>
+      <c r="AH38" s="78"/>
+      <c r="AI38" s="78"/>
+      <c r="AJ38" s="78"/>
+      <c r="AK38" s="78"/>
+      <c r="AL38" s="78"/>
+      <c r="AM38" s="78"/>
+      <c r="AN38" s="78"/>
+      <c r="AO38" s="78"/>
+      <c r="AP38" s="78"/>
+      <c r="AQ38" s="78"/>
+      <c r="AR38" s="78"/>
+      <c r="AS38" s="78"/>
+      <c r="AT38" s="78"/>
+      <c r="AU38" s="78"/>
+      <c r="AV38" s="78"/>
+      <c r="AW38" s="78"/>
+      <c r="AX38" s="78"/>
+      <c r="AY38" s="78"/>
+      <c r="AZ38" s="78"/>
+      <c r="BA38" s="78"/>
+      <c r="BB38" s="78"/>
+      <c r="BC38" s="78"/>
+      <c r="BD38" s="78"/>
+      <c r="BE38" s="78"/>
+      <c r="BF38" s="78"/>
+      <c r="BG38" s="78"/>
+      <c r="BH38" s="78"/>
+      <c r="BI38" s="78"/>
+      <c r="BJ38" s="78"/>
+      <c r="BK38" s="78"/>
+      <c r="BL38" s="78"/>
+      <c r="BM38" s="78"/>
+      <c r="BN38" s="78"/>
+      <c r="BO38" s="78"/>
+      <c r="BP38" s="78"/>
+      <c r="BQ38" s="78"/>
+      <c r="BR38" s="78"/>
+      <c r="BS38" s="78"/>
+      <c r="BT38" s="78"/>
+      <c r="BU38" s="78"/>
+      <c r="BV38" s="78"/>
+      <c r="BW38" s="78"/>
+      <c r="BX38" s="78"/>
+      <c r="BY38" s="78"/>
+      <c r="BZ38" s="78"/>
+      <c r="CA38" s="78"/>
+      <c r="CB38" s="78"/>
+      <c r="CC38" s="78"/>
+      <c r="CD38" s="78"/>
+      <c r="CE38" s="78"/>
+      <c r="CF38" s="78"/>
+      <c r="CG38" s="78"/>
+      <c r="CH38" s="78"/>
+      <c r="CI38" s="78"/>
+      <c r="CJ38" s="78"/>
+      <c r="CK38" s="78"/>
+      <c r="CL38" s="78"/>
+      <c r="CM38" s="78"/>
+    </row>
+    <row r="39" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="A39" s="80"/>
+      <c r="B39" s="80"/>
+      <c r="C39" s="80"/>
+      <c r="D39" s="80"/>
+      <c r="E39" s="80"/>
+      <c r="F39" s="80"/>
+      <c r="G39" s="81"/>
+      <c r="H39" s="80"/>
+      <c r="I39" s="80"/>
+      <c r="J39" s="80"/>
+      <c r="K39" s="80"/>
+      <c r="L39" s="80"/>
+      <c r="M39" s="80"/>
+      <c r="N39" s="80"/>
+      <c r="O39" s="80"/>
+      <c r="P39" s="80"/>
+      <c r="Q39" s="80"/>
+      <c r="R39" s="80"/>
+      <c r="S39" s="80"/>
+      <c r="T39" s="80"/>
+      <c r="U39" s="80"/>
+      <c r="V39" s="80"/>
+      <c r="W39" s="80"/>
+      <c r="X39" s="80"/>
+      <c r="Y39" s="80"/>
+      <c r="Z39" s="80"/>
+      <c r="AA39" s="80"/>
+      <c r="AB39" s="80"/>
+      <c r="AC39" s="80"/>
+      <c r="AD39" s="80"/>
+      <c r="AE39" s="80"/>
+      <c r="AF39" s="80"/>
+      <c r="AG39" s="80"/>
+      <c r="AH39" s="80"/>
+      <c r="AI39" s="80"/>
+      <c r="AJ39" s="80"/>
+      <c r="AK39" s="80"/>
+      <c r="AL39" s="80"/>
+      <c r="AM39" s="80"/>
+      <c r="AN39" s="80"/>
+      <c r="AO39" s="80"/>
+      <c r="AP39" s="80"/>
+      <c r="AQ39" s="80"/>
+      <c r="AR39" s="80"/>
+      <c r="AS39" s="80"/>
+      <c r="AT39" s="80"/>
+      <c r="AU39" s="80"/>
+      <c r="AV39" s="80"/>
+      <c r="AW39" s="80"/>
+      <c r="AX39" s="80"/>
+      <c r="AY39" s="80"/>
+      <c r="AZ39" s="80"/>
+      <c r="BA39" s="80"/>
+      <c r="BB39" s="80"/>
+      <c r="BC39" s="80"/>
+      <c r="BD39" s="80"/>
+      <c r="BE39" s="80"/>
+      <c r="BF39" s="80"/>
+      <c r="BG39" s="80"/>
+      <c r="BH39" s="80"/>
+      <c r="BI39" s="80"/>
+      <c r="BJ39" s="80"/>
+      <c r="BK39" s="80"/>
+      <c r="BL39" s="80"/>
+      <c r="BM39" s="80"/>
+      <c r="BN39" s="80"/>
+      <c r="BO39" s="80"/>
+      <c r="BP39" s="80"/>
+      <c r="BQ39" s="80"/>
+      <c r="BR39" s="80"/>
+      <c r="BS39" s="80"/>
+      <c r="BT39" s="80"/>
+      <c r="BU39" s="80"/>
+      <c r="BV39" s="80"/>
+      <c r="BW39" s="80"/>
+      <c r="BX39" s="80"/>
+      <c r="BY39" s="80"/>
+      <c r="BZ39" s="80"/>
+      <c r="CA39" s="80"/>
+      <c r="CB39" s="80"/>
+      <c r="CC39" s="80"/>
+      <c r="CD39" s="80"/>
+      <c r="CE39" s="80"/>
+      <c r="CF39" s="80"/>
+      <c r="CG39" s="80"/>
+      <c r="CH39" s="80"/>
+      <c r="CI39" s="80"/>
+      <c r="CJ39" s="80"/>
+      <c r="CK39" s="80"/>
+      <c r="CL39" s="80"/>
+      <c r="CM39" s="80"/>
+    </row>
+    <row r="40" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="G40" s="61"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:CG31" xr:uid="{9585C0FF-65C5-4BD8-9936-5C9A63F7E604}">
@@ -69084,22 +69409,22 @@
     </sortState>
   </autoFilter>
   <mergeCells count="16">
+    <mergeCell ref="AO1:AR1"/>
+    <mergeCell ref="AS1:AV1"/>
+    <mergeCell ref="AW1:AZ1"/>
+    <mergeCell ref="BA1:BE1"/>
+    <mergeCell ref="BF1:BI1"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="W1:AA1"/>
+    <mergeCell ref="AB1:AE1"/>
+    <mergeCell ref="AF1:AI1"/>
+    <mergeCell ref="AJ1:AN1"/>
     <mergeCell ref="CF1:CG1"/>
     <mergeCell ref="BJ1:BN1"/>
     <mergeCell ref="BO1:BR1"/>
     <mergeCell ref="BS1:BV1"/>
     <mergeCell ref="BW1:BZ1"/>
     <mergeCell ref="CB1:CE1"/>
-    <mergeCell ref="S1:V1"/>
-    <mergeCell ref="W1:AA1"/>
-    <mergeCell ref="AB1:AE1"/>
-    <mergeCell ref="AF1:AI1"/>
-    <mergeCell ref="AJ1:AN1"/>
-    <mergeCell ref="AO1:AR1"/>
-    <mergeCell ref="AS1:AV1"/>
-    <mergeCell ref="AW1:AZ1"/>
-    <mergeCell ref="BA1:BE1"/>
-    <mergeCell ref="BF1:BI1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Consumo de 2 de 2 procedimientos
actualizacion de listado de reportes
</commit_message>
<xml_diff>
--- a/00-Documentacion/Listado de reportes totales-TI.xlsx
+++ b/00-Documentacion/Listado de reportes totales-TI.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\source\repos\migracion_spooler\00-Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7689B238-EA3A-44EC-89C3-91CE03D486AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23BDB405-8ABB-4D5A-88EB-7699499BEA50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{1498AA1A-1ACC-4329-A050-ACA05131B658}"/>
   </bookViews>
@@ -6040,7 +6040,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6171,34 +6171,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6221,6 +6199,24 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -64836,9 +64832,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9585C0FF-65C5-4BD8-9936-5C9A63F7E604}">
   <dimension ref="A1:CM40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="X1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AO26" sqref="AO26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64920,104 +64916,104 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:86" x14ac:dyDescent="0.25">
-      <c r="S1" s="68">
+      <c r="S1" s="78">
         <v>45536</v>
       </c>
-      <c r="T1" s="69"/>
-      <c r="U1" s="69"/>
-      <c r="V1" s="69"/>
-      <c r="W1" s="68">
+      <c r="T1" s="79"/>
+      <c r="U1" s="79"/>
+      <c r="V1" s="79"/>
+      <c r="W1" s="78">
         <v>45566</v>
       </c>
-      <c r="X1" s="68"/>
-      <c r="Y1" s="68"/>
-      <c r="Z1" s="68"/>
-      <c r="AA1" s="68"/>
-      <c r="AB1" s="65">
+      <c r="X1" s="78"/>
+      <c r="Y1" s="78"/>
+      <c r="Z1" s="78"/>
+      <c r="AA1" s="78"/>
+      <c r="AB1" s="75">
         <v>45597</v>
       </c>
-      <c r="AC1" s="66"/>
-      <c r="AD1" s="66"/>
-      <c r="AE1" s="67"/>
-      <c r="AF1" s="65">
+      <c r="AC1" s="76"/>
+      <c r="AD1" s="76"/>
+      <c r="AE1" s="77"/>
+      <c r="AF1" s="75">
         <v>45627</v>
       </c>
-      <c r="AG1" s="66"/>
-      <c r="AH1" s="66"/>
-      <c r="AI1" s="67"/>
-      <c r="AJ1" s="65">
+      <c r="AG1" s="76"/>
+      <c r="AH1" s="76"/>
+      <c r="AI1" s="77"/>
+      <c r="AJ1" s="75">
         <v>45658</v>
       </c>
-      <c r="AK1" s="66"/>
-      <c r="AL1" s="66"/>
-      <c r="AM1" s="66"/>
-      <c r="AN1" s="67"/>
-      <c r="AO1" s="65">
+      <c r="AK1" s="76"/>
+      <c r="AL1" s="76"/>
+      <c r="AM1" s="76"/>
+      <c r="AN1" s="77"/>
+      <c r="AO1" s="75">
         <v>45689</v>
       </c>
-      <c r="AP1" s="66"/>
-      <c r="AQ1" s="66"/>
-      <c r="AR1" s="67"/>
-      <c r="AS1" s="65">
+      <c r="AP1" s="76"/>
+      <c r="AQ1" s="76"/>
+      <c r="AR1" s="77"/>
+      <c r="AS1" s="75">
         <v>45717</v>
       </c>
-      <c r="AT1" s="66"/>
-      <c r="AU1" s="66"/>
-      <c r="AV1" s="67"/>
-      <c r="AW1" s="65">
+      <c r="AT1" s="76"/>
+      <c r="AU1" s="76"/>
+      <c r="AV1" s="77"/>
+      <c r="AW1" s="75">
         <v>45748</v>
       </c>
-      <c r="AX1" s="66"/>
-      <c r="AY1" s="66"/>
-      <c r="AZ1" s="67"/>
-      <c r="BA1" s="65">
+      <c r="AX1" s="76"/>
+      <c r="AY1" s="76"/>
+      <c r="AZ1" s="77"/>
+      <c r="BA1" s="75">
         <v>45778</v>
       </c>
-      <c r="BB1" s="66"/>
-      <c r="BC1" s="66"/>
-      <c r="BD1" s="66"/>
-      <c r="BE1" s="67"/>
-      <c r="BF1" s="65">
+      <c r="BB1" s="76"/>
+      <c r="BC1" s="76"/>
+      <c r="BD1" s="76"/>
+      <c r="BE1" s="77"/>
+      <c r="BF1" s="75">
         <v>45809</v>
       </c>
-      <c r="BG1" s="66"/>
-      <c r="BH1" s="66"/>
-      <c r="BI1" s="66"/>
-      <c r="BJ1" s="65">
+      <c r="BG1" s="76"/>
+      <c r="BH1" s="76"/>
+      <c r="BI1" s="76"/>
+      <c r="BJ1" s="75">
         <v>45839</v>
       </c>
-      <c r="BK1" s="66"/>
-      <c r="BL1" s="66"/>
-      <c r="BM1" s="66"/>
-      <c r="BN1" s="67"/>
-      <c r="BO1" s="65">
+      <c r="BK1" s="76"/>
+      <c r="BL1" s="76"/>
+      <c r="BM1" s="76"/>
+      <c r="BN1" s="77"/>
+      <c r="BO1" s="75">
         <v>45870</v>
       </c>
-      <c r="BP1" s="66"/>
-      <c r="BQ1" s="66"/>
-      <c r="BR1" s="66"/>
-      <c r="BS1" s="65">
+      <c r="BP1" s="76"/>
+      <c r="BQ1" s="76"/>
+      <c r="BR1" s="76"/>
+      <c r="BS1" s="75">
         <v>45901</v>
       </c>
-      <c r="BT1" s="66"/>
-      <c r="BU1" s="66"/>
-      <c r="BV1" s="66"/>
-      <c r="BW1" s="65">
+      <c r="BT1" s="76"/>
+      <c r="BU1" s="76"/>
+      <c r="BV1" s="76"/>
+      <c r="BW1" s="75">
         <v>45931</v>
       </c>
-      <c r="BX1" s="66"/>
-      <c r="BY1" s="66"/>
-      <c r="BZ1" s="66"/>
-      <c r="CB1" s="65">
+      <c r="BX1" s="76"/>
+      <c r="BY1" s="76"/>
+      <c r="BZ1" s="76"/>
+      <c r="CB1" s="75">
         <v>45962</v>
       </c>
-      <c r="CC1" s="66"/>
-      <c r="CD1" s="66"/>
-      <c r="CE1" s="66"/>
-      <c r="CF1" s="64" t="s">
+      <c r="CC1" s="76"/>
+      <c r="CD1" s="76"/>
+      <c r="CE1" s="76"/>
+      <c r="CF1" s="80" t="s">
         <v>1854</v>
       </c>
-      <c r="CG1" s="64"/>
+      <c r="CG1" s="80"/>
     </row>
     <row r="2" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
@@ -67089,9 +67085,9 @@
       <c r="S18" s="53"/>
       <c r="T18" s="12"/>
       <c r="U18" s="12"/>
-      <c r="V18" s="59"/>
-      <c r="W18" s="59"/>
-      <c r="X18" s="59"/>
+      <c r="V18" s="12"/>
+      <c r="W18" s="12"/>
+      <c r="X18" s="12"/>
       <c r="Y18" s="12"/>
       <c r="Z18" s="12"/>
       <c r="AA18" s="12"/>
@@ -67210,9 +67206,9 @@
       <c r="V19" s="12"/>
       <c r="W19" s="12"/>
       <c r="X19" s="12"/>
-      <c r="Y19" s="48"/>
-      <c r="Z19" s="48"/>
-      <c r="AA19" s="48"/>
+      <c r="Y19" s="59"/>
+      <c r="Z19" s="59"/>
+      <c r="AA19" s="59"/>
       <c r="AB19" s="12"/>
       <c r="AC19" s="12"/>
       <c r="AD19" s="12"/>
@@ -69112,292 +69108,217 @@
       <c r="CG36" s="12"/>
       <c r="CH36" s="12"/>
     </row>
-    <row r="37" spans="1:91" s="74" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="70"/>
-      <c r="B37" s="71"/>
-      <c r="C37" s="71"/>
-      <c r="D37" s="70"/>
-      <c r="E37" s="72"/>
-      <c r="F37" s="72"/>
-      <c r="G37" s="70"/>
-      <c r="H37" s="72"/>
-      <c r="I37" s="73"/>
-      <c r="J37" s="73"/>
-      <c r="K37" s="73"/>
-      <c r="L37" s="73"/>
-      <c r="N37" s="73"/>
-      <c r="O37" s="73"/>
-      <c r="P37" s="73"/>
-      <c r="Q37" s="75"/>
-      <c r="R37" s="75"/>
-      <c r="S37" s="73"/>
-      <c r="T37" s="73"/>
-      <c r="U37" s="73"/>
-      <c r="V37" s="73"/>
-      <c r="W37" s="73"/>
-      <c r="X37" s="73"/>
-      <c r="Y37" s="73"/>
-      <c r="Z37" s="73"/>
-      <c r="AA37" s="73"/>
-      <c r="AB37" s="73"/>
-      <c r="AC37" s="73"/>
-      <c r="AD37" s="73"/>
-      <c r="AE37" s="73"/>
-      <c r="AF37" s="73"/>
-      <c r="AG37" s="73"/>
-      <c r="AH37" s="73"/>
-      <c r="AI37" s="73"/>
-      <c r="AJ37" s="73"/>
-      <c r="AK37" s="73"/>
-      <c r="AL37" s="73"/>
-      <c r="AM37" s="73"/>
-      <c r="AN37" s="73"/>
-      <c r="AO37" s="73"/>
-      <c r="AP37" s="73"/>
-      <c r="AQ37" s="73"/>
-      <c r="AR37" s="73"/>
-      <c r="AS37" s="73"/>
-      <c r="AT37" s="73"/>
-      <c r="AU37" s="73"/>
-      <c r="AV37" s="73"/>
-      <c r="AW37" s="73"/>
-      <c r="AX37" s="73"/>
-      <c r="AY37" s="73"/>
-      <c r="AZ37" s="73"/>
-      <c r="BA37" s="73"/>
-      <c r="BB37" s="73"/>
-      <c r="BC37" s="73"/>
-      <c r="BD37" s="73"/>
-      <c r="BE37" s="73"/>
-      <c r="BF37" s="73"/>
-      <c r="BG37" s="73"/>
-      <c r="BH37" s="73"/>
-      <c r="BI37" s="73"/>
-      <c r="BJ37" s="73"/>
-      <c r="BK37" s="73"/>
-      <c r="BL37" s="73"/>
-      <c r="BM37" s="73"/>
-      <c r="BN37" s="73"/>
-      <c r="BO37" s="73"/>
-      <c r="BP37" s="73"/>
-      <c r="BQ37" s="73"/>
-      <c r="BR37" s="73"/>
-      <c r="BS37" s="73"/>
-      <c r="BT37" s="73"/>
-      <c r="BU37" s="73"/>
-      <c r="BV37" s="73"/>
-      <c r="BW37" s="73"/>
-      <c r="BX37" s="73"/>
-      <c r="BY37" s="73"/>
-      <c r="BZ37" s="73"/>
-      <c r="CA37" s="73"/>
-      <c r="CB37" s="73"/>
-      <c r="CC37" s="73"/>
-      <c r="CD37" s="73"/>
-      <c r="CE37" s="73"/>
-      <c r="CF37" s="73"/>
-      <c r="CG37" s="73"/>
-      <c r="CH37" s="73"/>
+    <row r="37" spans="1:91" s="66" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="64"/>
+      <c r="B37" s="65"/>
+      <c r="C37" s="65"/>
+      <c r="D37" s="64"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="65"/>
+      <c r="G37" s="64"/>
+      <c r="H37" s="65"/>
+      <c r="Q37" s="67"/>
+      <c r="R37" s="67"/>
     </row>
     <row r="38" spans="1:91" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="82" t="s">
+      <c r="A38" s="74" t="s">
         <v>1778</v>
       </c>
-      <c r="B38" s="78"/>
-      <c r="C38" s="78"/>
-      <c r="D38" s="76" t="s">
+      <c r="B38" s="70"/>
+      <c r="C38" s="70"/>
+      <c r="D38" s="68" t="s">
         <v>1882</v>
       </c>
-      <c r="E38" s="77" t="s">
+      <c r="E38" s="69" t="s">
         <v>1881</v>
       </c>
-      <c r="F38" s="78"/>
-      <c r="G38" s="79" t="s">
+      <c r="F38" s="70"/>
+      <c r="G38" s="71" t="s">
         <v>176</v>
       </c>
-      <c r="H38" s="79" t="s">
+      <c r="H38" s="71" t="s">
         <v>1883</v>
       </c>
-      <c r="I38" s="78">
+      <c r="I38" s="70">
         <v>23</v>
       </c>
-      <c r="J38" s="78"/>
-      <c r="K38" s="78"/>
-      <c r="L38" s="78"/>
-      <c r="M38" s="78"/>
-      <c r="N38" s="78"/>
-      <c r="O38" s="78"/>
-      <c r="P38" s="78" t="s">
+      <c r="J38" s="70"/>
+      <c r="K38" s="70"/>
+      <c r="L38" s="70"/>
+      <c r="M38" s="70"/>
+      <c r="N38" s="70"/>
+      <c r="O38" s="70"/>
+      <c r="P38" s="70" t="s">
         <v>1884</v>
       </c>
-      <c r="Q38" s="78"/>
-      <c r="R38" s="78"/>
-      <c r="S38" s="78"/>
-      <c r="T38" s="78"/>
-      <c r="U38" s="78"/>
-      <c r="V38" s="78"/>
-      <c r="W38" s="78"/>
-      <c r="X38" s="78"/>
-      <c r="Y38" s="78"/>
-      <c r="Z38" s="78"/>
-      <c r="AA38" s="78"/>
-      <c r="AB38" s="78"/>
-      <c r="AC38" s="78"/>
-      <c r="AD38" s="78"/>
-      <c r="AE38" s="78"/>
-      <c r="AF38" s="78"/>
-      <c r="AG38" s="78"/>
-      <c r="AH38" s="78"/>
-      <c r="AI38" s="78"/>
-      <c r="AJ38" s="78"/>
-      <c r="AK38" s="78"/>
-      <c r="AL38" s="78"/>
-      <c r="AM38" s="78"/>
-      <c r="AN38" s="78"/>
-      <c r="AO38" s="78"/>
-      <c r="AP38" s="78"/>
-      <c r="AQ38" s="78"/>
-      <c r="AR38" s="78"/>
-      <c r="AS38" s="78"/>
-      <c r="AT38" s="78"/>
-      <c r="AU38" s="78"/>
-      <c r="AV38" s="78"/>
-      <c r="AW38" s="78"/>
-      <c r="AX38" s="78"/>
-      <c r="AY38" s="78"/>
-      <c r="AZ38" s="78"/>
-      <c r="BA38" s="78"/>
-      <c r="BB38" s="78"/>
-      <c r="BC38" s="78"/>
-      <c r="BD38" s="78"/>
-      <c r="BE38" s="78"/>
-      <c r="BF38" s="78"/>
-      <c r="BG38" s="78"/>
-      <c r="BH38" s="78"/>
-      <c r="BI38" s="78"/>
-      <c r="BJ38" s="78"/>
-      <c r="BK38" s="78"/>
-      <c r="BL38" s="78"/>
-      <c r="BM38" s="78"/>
-      <c r="BN38" s="78"/>
-      <c r="BO38" s="78"/>
-      <c r="BP38" s="78"/>
-      <c r="BQ38" s="78"/>
-      <c r="BR38" s="78"/>
-      <c r="BS38" s="78"/>
-      <c r="BT38" s="78"/>
-      <c r="BU38" s="78"/>
-      <c r="BV38" s="78"/>
-      <c r="BW38" s="78"/>
-      <c r="BX38" s="78"/>
-      <c r="BY38" s="78"/>
-      <c r="BZ38" s="78"/>
-      <c r="CA38" s="78"/>
-      <c r="CB38" s="78"/>
-      <c r="CC38" s="78"/>
-      <c r="CD38" s="78"/>
-      <c r="CE38" s="78"/>
-      <c r="CF38" s="78"/>
-      <c r="CG38" s="78"/>
-      <c r="CH38" s="78"/>
-      <c r="CI38" s="78"/>
-      <c r="CJ38" s="78"/>
-      <c r="CK38" s="78"/>
-      <c r="CL38" s="78"/>
-      <c r="CM38" s="78"/>
+      <c r="Q38" s="70"/>
+      <c r="R38" s="70"/>
+      <c r="S38" s="70"/>
+      <c r="T38" s="70"/>
+      <c r="U38" s="70"/>
+      <c r="V38" s="70"/>
+      <c r="W38" s="70"/>
+      <c r="X38" s="70"/>
+      <c r="Y38" s="70"/>
+      <c r="Z38" s="70"/>
+      <c r="AA38" s="70"/>
+      <c r="AB38" s="70"/>
+      <c r="AC38" s="70"/>
+      <c r="AD38" s="70"/>
+      <c r="AE38" s="70"/>
+      <c r="AF38" s="70"/>
+      <c r="AG38" s="70"/>
+      <c r="AH38" s="70"/>
+      <c r="AI38" s="70"/>
+      <c r="AJ38" s="70"/>
+      <c r="AK38" s="70"/>
+      <c r="AL38" s="70"/>
+      <c r="AM38" s="70"/>
+      <c r="AN38" s="70"/>
+      <c r="AO38" s="70"/>
+      <c r="AP38" s="70"/>
+      <c r="AQ38" s="70"/>
+      <c r="AR38" s="70"/>
+      <c r="AS38" s="70"/>
+      <c r="AT38" s="70"/>
+      <c r="AU38" s="70"/>
+      <c r="AV38" s="70"/>
+      <c r="AW38" s="70"/>
+      <c r="AX38" s="70"/>
+      <c r="AY38" s="70"/>
+      <c r="AZ38" s="70"/>
+      <c r="BA38" s="70"/>
+      <c r="BB38" s="70"/>
+      <c r="BC38" s="70"/>
+      <c r="BD38" s="70"/>
+      <c r="BE38" s="70"/>
+      <c r="BF38" s="70"/>
+      <c r="BG38" s="70"/>
+      <c r="BH38" s="70"/>
+      <c r="BI38" s="70"/>
+      <c r="BJ38" s="70"/>
+      <c r="BK38" s="70"/>
+      <c r="BL38" s="70"/>
+      <c r="BM38" s="70"/>
+      <c r="BN38" s="70"/>
+      <c r="BO38" s="70"/>
+      <c r="BP38" s="70"/>
+      <c r="BQ38" s="70"/>
+      <c r="BR38" s="70"/>
+      <c r="BS38" s="70"/>
+      <c r="BT38" s="70"/>
+      <c r="BU38" s="70"/>
+      <c r="BV38" s="70"/>
+      <c r="BW38" s="70"/>
+      <c r="BX38" s="70"/>
+      <c r="BY38" s="70"/>
+      <c r="BZ38" s="70"/>
+      <c r="CA38" s="70"/>
+      <c r="CB38" s="70"/>
+      <c r="CC38" s="70"/>
+      <c r="CD38" s="70"/>
+      <c r="CE38" s="70"/>
+      <c r="CF38" s="70"/>
+      <c r="CG38" s="70"/>
+      <c r="CH38" s="70"/>
+      <c r="CI38" s="70"/>
+      <c r="CJ38" s="70"/>
+      <c r="CK38" s="70"/>
+      <c r="CL38" s="70"/>
+      <c r="CM38" s="70"/>
     </row>
     <row r="39" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A39" s="80"/>
-      <c r="B39" s="80"/>
-      <c r="C39" s="80"/>
-      <c r="D39" s="80"/>
-      <c r="E39" s="80"/>
-      <c r="F39" s="80"/>
-      <c r="G39" s="81"/>
-      <c r="H39" s="80"/>
-      <c r="I39" s="80"/>
-      <c r="J39" s="80"/>
-      <c r="K39" s="80"/>
-      <c r="L39" s="80"/>
-      <c r="M39" s="80"/>
-      <c r="N39" s="80"/>
-      <c r="O39" s="80"/>
-      <c r="P39" s="80"/>
-      <c r="Q39" s="80"/>
-      <c r="R39" s="80"/>
-      <c r="S39" s="80"/>
-      <c r="T39" s="80"/>
-      <c r="U39" s="80"/>
-      <c r="V39" s="80"/>
-      <c r="W39" s="80"/>
-      <c r="X39" s="80"/>
-      <c r="Y39" s="80"/>
-      <c r="Z39" s="80"/>
-      <c r="AA39" s="80"/>
-      <c r="AB39" s="80"/>
-      <c r="AC39" s="80"/>
-      <c r="AD39" s="80"/>
-      <c r="AE39" s="80"/>
-      <c r="AF39" s="80"/>
-      <c r="AG39" s="80"/>
-      <c r="AH39" s="80"/>
-      <c r="AI39" s="80"/>
-      <c r="AJ39" s="80"/>
-      <c r="AK39" s="80"/>
-      <c r="AL39" s="80"/>
-      <c r="AM39" s="80"/>
-      <c r="AN39" s="80"/>
-      <c r="AO39" s="80"/>
-      <c r="AP39" s="80"/>
-      <c r="AQ39" s="80"/>
-      <c r="AR39" s="80"/>
-      <c r="AS39" s="80"/>
-      <c r="AT39" s="80"/>
-      <c r="AU39" s="80"/>
-      <c r="AV39" s="80"/>
-      <c r="AW39" s="80"/>
-      <c r="AX39" s="80"/>
-      <c r="AY39" s="80"/>
-      <c r="AZ39" s="80"/>
-      <c r="BA39" s="80"/>
-      <c r="BB39" s="80"/>
-      <c r="BC39" s="80"/>
-      <c r="BD39" s="80"/>
-      <c r="BE39" s="80"/>
-      <c r="BF39" s="80"/>
-      <c r="BG39" s="80"/>
-      <c r="BH39" s="80"/>
-      <c r="BI39" s="80"/>
-      <c r="BJ39" s="80"/>
-      <c r="BK39" s="80"/>
-      <c r="BL39" s="80"/>
-      <c r="BM39" s="80"/>
-      <c r="BN39" s="80"/>
-      <c r="BO39" s="80"/>
-      <c r="BP39" s="80"/>
-      <c r="BQ39" s="80"/>
-      <c r="BR39" s="80"/>
-      <c r="BS39" s="80"/>
-      <c r="BT39" s="80"/>
-      <c r="BU39" s="80"/>
-      <c r="BV39" s="80"/>
-      <c r="BW39" s="80"/>
-      <c r="BX39" s="80"/>
-      <c r="BY39" s="80"/>
-      <c r="BZ39" s="80"/>
-      <c r="CA39" s="80"/>
-      <c r="CB39" s="80"/>
-      <c r="CC39" s="80"/>
-      <c r="CD39" s="80"/>
-      <c r="CE39" s="80"/>
-      <c r="CF39" s="80"/>
-      <c r="CG39" s="80"/>
-      <c r="CH39" s="80"/>
-      <c r="CI39" s="80"/>
-      <c r="CJ39" s="80"/>
-      <c r="CK39" s="80"/>
-      <c r="CL39" s="80"/>
-      <c r="CM39" s="80"/>
+      <c r="A39" s="72"/>
+      <c r="B39" s="72"/>
+      <c r="C39" s="72"/>
+      <c r="D39" s="72"/>
+      <c r="E39" s="72"/>
+      <c r="F39" s="72"/>
+      <c r="G39" s="73"/>
+      <c r="H39" s="72"/>
+      <c r="I39" s="72"/>
+      <c r="J39" s="72"/>
+      <c r="K39" s="72"/>
+      <c r="L39" s="72"/>
+      <c r="M39" s="72"/>
+      <c r="N39" s="72"/>
+      <c r="O39" s="72"/>
+      <c r="P39" s="72"/>
+      <c r="Q39" s="72"/>
+      <c r="R39" s="72"/>
+      <c r="S39" s="72"/>
+      <c r="T39" s="72"/>
+      <c r="U39" s="72"/>
+      <c r="V39" s="72"/>
+      <c r="W39" s="72"/>
+      <c r="X39" s="72"/>
+      <c r="Y39" s="72"/>
+      <c r="Z39" s="72"/>
+      <c r="AA39" s="72"/>
+      <c r="AB39" s="72"/>
+      <c r="AC39" s="72"/>
+      <c r="AD39" s="72"/>
+      <c r="AE39" s="72"/>
+      <c r="AF39" s="72"/>
+      <c r="AG39" s="72"/>
+      <c r="AH39" s="72"/>
+      <c r="AI39" s="72"/>
+      <c r="AJ39" s="72"/>
+      <c r="AK39" s="72"/>
+      <c r="AL39" s="72"/>
+      <c r="AM39" s="72"/>
+      <c r="AN39" s="72"/>
+      <c r="AO39" s="72"/>
+      <c r="AP39" s="72"/>
+      <c r="AQ39" s="72"/>
+      <c r="AR39" s="72"/>
+      <c r="AS39" s="72"/>
+      <c r="AT39" s="72"/>
+      <c r="AU39" s="72"/>
+      <c r="AV39" s="72"/>
+      <c r="AW39" s="72"/>
+      <c r="AX39" s="72"/>
+      <c r="AY39" s="72"/>
+      <c r="AZ39" s="72"/>
+      <c r="BA39" s="72"/>
+      <c r="BB39" s="72"/>
+      <c r="BC39" s="72"/>
+      <c r="BD39" s="72"/>
+      <c r="BE39" s="72"/>
+      <c r="BF39" s="72"/>
+      <c r="BG39" s="72"/>
+      <c r="BH39" s="72"/>
+      <c r="BI39" s="72"/>
+      <c r="BJ39" s="72"/>
+      <c r="BK39" s="72"/>
+      <c r="BL39" s="72"/>
+      <c r="BM39" s="72"/>
+      <c r="BN39" s="72"/>
+      <c r="BO39" s="72"/>
+      <c r="BP39" s="72"/>
+      <c r="BQ39" s="72"/>
+      <c r="BR39" s="72"/>
+      <c r="BS39" s="72"/>
+      <c r="BT39" s="72"/>
+      <c r="BU39" s="72"/>
+      <c r="BV39" s="72"/>
+      <c r="BW39" s="72"/>
+      <c r="BX39" s="72"/>
+      <c r="BY39" s="72"/>
+      <c r="BZ39" s="72"/>
+      <c r="CA39" s="72"/>
+      <c r="CB39" s="72"/>
+      <c r="CC39" s="72"/>
+      <c r="CD39" s="72"/>
+      <c r="CE39" s="72"/>
+      <c r="CF39" s="72"/>
+      <c r="CG39" s="72"/>
+      <c r="CH39" s="72"/>
+      <c r="CI39" s="72"/>
+      <c r="CJ39" s="72"/>
+      <c r="CK39" s="72"/>
+      <c r="CL39" s="72"/>
+      <c r="CM39" s="72"/>
     </row>
     <row r="40" spans="1:91" x14ac:dyDescent="0.25">
       <c r="G40" s="61"/>
@@ -69409,22 +69330,22 @@
     </sortState>
   </autoFilter>
   <mergeCells count="16">
-    <mergeCell ref="AO1:AR1"/>
-    <mergeCell ref="AS1:AV1"/>
-    <mergeCell ref="AW1:AZ1"/>
-    <mergeCell ref="BA1:BE1"/>
-    <mergeCell ref="BF1:BI1"/>
-    <mergeCell ref="S1:V1"/>
-    <mergeCell ref="W1:AA1"/>
-    <mergeCell ref="AB1:AE1"/>
-    <mergeCell ref="AF1:AI1"/>
-    <mergeCell ref="AJ1:AN1"/>
     <mergeCell ref="CF1:CG1"/>
     <mergeCell ref="BJ1:BN1"/>
     <mergeCell ref="BO1:BR1"/>
     <mergeCell ref="BS1:BV1"/>
     <mergeCell ref="BW1:BZ1"/>
     <mergeCell ref="CB1:CE1"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="W1:AA1"/>
+    <mergeCell ref="AB1:AE1"/>
+    <mergeCell ref="AF1:AI1"/>
+    <mergeCell ref="AJ1:AN1"/>
+    <mergeCell ref="AO1:AR1"/>
+    <mergeCell ref="AS1:AV1"/>
+    <mergeCell ref="AW1:AZ1"/>
+    <mergeCell ref="BA1:BE1"/>
+    <mergeCell ref="BF1:BI1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Spooler - Procesos principales de Bosch - Interfaces SEG Automotive ( bosch_pedim3_xls)
análisis procesos
verificación de parámetros
generación de clase

actualizacion de plan de trabajo
</commit_message>
<xml_diff>
--- a/00-Documentacion/Listado de reportes totales-TI.xlsx
+++ b/00-Documentacion/Listado de reportes totales-TI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23BDB405-8ABB-4D5A-88EB-7699499BEA50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E225F2E9-3A54-4C4A-A738-583AC8A6BE86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{1498AA1A-1ACC-4329-A050-ACA05131B658}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13299" uniqueCount="1885">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13301" uniqueCount="1884">
   <si>
     <t xml:space="preserve">Reporte </t>
   </si>
@@ -5694,9 +5694,6 @@
   </si>
   <si>
     <t>Restrutura de Esquemas de Objetos</t>
-  </si>
-  <si>
-    <t>Ajustes</t>
   </si>
   <si>
     <t>Bajo demanda</t>
@@ -6200,6 +6197,9 @@
     <xf numFmtId="0" fontId="14" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6213,9 +6213,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -8782,7 +8779,7 @@
       </c>
       <c r="R54" s="8"/>
     </row>
-    <row r="55" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" ht="39" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>14</v>
       </c>
@@ -9310,7 +9307,7 @@
       </c>
       <c r="R66" s="8"/>
     </row>
-    <row r="67" spans="1:18" ht="39" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
         <v>14</v>
       </c>
@@ -16614,7 +16611,7 @@
       <c r="Q262" s="8"/>
       <c r="R262" s="8"/>
     </row>
-    <row r="263" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A263" s="5">
         <v>67</v>
       </c>
@@ -22026,7 +22023,7 @@
       </c>
       <c r="R403" s="8"/>
     </row>
-    <row r="404" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A404" s="5">
         <v>138</v>
       </c>
@@ -25042,7 +25039,7 @@
       </c>
       <c r="R479" s="8"/>
     </row>
-    <row r="480" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:18" ht="39" x14ac:dyDescent="0.25">
       <c r="A480" s="5">
         <v>173</v>
       </c>
@@ -26934,7 +26931,7 @@
       </c>
       <c r="R522" s="8"/>
     </row>
-    <row r="523" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="523" spans="1:18" ht="39" x14ac:dyDescent="0.25">
       <c r="A523" s="5">
         <v>173</v>
       </c>
@@ -37938,7 +37935,7 @@
       </c>
       <c r="R783" s="8"/>
     </row>
-    <row r="784" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="784" spans="1:18" ht="39" x14ac:dyDescent="0.25">
       <c r="A784" s="5">
         <v>174</v>
       </c>
@@ -51374,7 +51371,7 @@
       </c>
       <c r="R1118" s="8"/>
     </row>
-    <row r="1119" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1119" spans="1:18" ht="39" x14ac:dyDescent="0.25">
       <c r="A1119" s="10">
         <v>244</v>
       </c>
@@ -57034,7 +57031,7 @@
       <c r="Q1263" s="8"/>
       <c r="R1263" s="8"/>
     </row>
-    <row r="1264" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1264" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1264" s="10">
         <v>322</v>
       </c>
@@ -64832,9 +64829,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9585C0FF-65C5-4BD8-9936-5C9A63F7E604}">
   <dimension ref="A1:CM40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AO26" sqref="AO26"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AI20" sqref="AI20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64916,104 +64913,104 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:86" x14ac:dyDescent="0.25">
-      <c r="S1" s="78">
+      <c r="S1" s="79">
         <v>45536</v>
       </c>
-      <c r="T1" s="79"/>
-      <c r="U1" s="79"/>
-      <c r="V1" s="79"/>
-      <c r="W1" s="78">
+      <c r="T1" s="80"/>
+      <c r="U1" s="80"/>
+      <c r="V1" s="80"/>
+      <c r="W1" s="79">
         <v>45566</v>
       </c>
-      <c r="X1" s="78"/>
-      <c r="Y1" s="78"/>
-      <c r="Z1" s="78"/>
-      <c r="AA1" s="78"/>
-      <c r="AB1" s="75">
+      <c r="X1" s="79"/>
+      <c r="Y1" s="79"/>
+      <c r="Z1" s="79"/>
+      <c r="AA1" s="79"/>
+      <c r="AB1" s="76">
         <v>45597</v>
       </c>
-      <c r="AC1" s="76"/>
-      <c r="AD1" s="76"/>
-      <c r="AE1" s="77"/>
-      <c r="AF1" s="75">
+      <c r="AC1" s="77"/>
+      <c r="AD1" s="77"/>
+      <c r="AE1" s="78"/>
+      <c r="AF1" s="76">
         <v>45627</v>
       </c>
-      <c r="AG1" s="76"/>
-      <c r="AH1" s="76"/>
-      <c r="AI1" s="77"/>
-      <c r="AJ1" s="75">
+      <c r="AG1" s="77"/>
+      <c r="AH1" s="77"/>
+      <c r="AI1" s="78"/>
+      <c r="AJ1" s="76">
         <v>45658</v>
       </c>
-      <c r="AK1" s="76"/>
-      <c r="AL1" s="76"/>
-      <c r="AM1" s="76"/>
-      <c r="AN1" s="77"/>
-      <c r="AO1" s="75">
+      <c r="AK1" s="77"/>
+      <c r="AL1" s="77"/>
+      <c r="AM1" s="77"/>
+      <c r="AN1" s="78"/>
+      <c r="AO1" s="76">
         <v>45689</v>
       </c>
-      <c r="AP1" s="76"/>
-      <c r="AQ1" s="76"/>
-      <c r="AR1" s="77"/>
-      <c r="AS1" s="75">
+      <c r="AP1" s="77"/>
+      <c r="AQ1" s="77"/>
+      <c r="AR1" s="78"/>
+      <c r="AS1" s="76">
         <v>45717</v>
       </c>
-      <c r="AT1" s="76"/>
-      <c r="AU1" s="76"/>
-      <c r="AV1" s="77"/>
-      <c r="AW1" s="75">
+      <c r="AT1" s="77"/>
+      <c r="AU1" s="77"/>
+      <c r="AV1" s="78"/>
+      <c r="AW1" s="76">
         <v>45748</v>
       </c>
-      <c r="AX1" s="76"/>
-      <c r="AY1" s="76"/>
-      <c r="AZ1" s="77"/>
-      <c r="BA1" s="75">
+      <c r="AX1" s="77"/>
+      <c r="AY1" s="77"/>
+      <c r="AZ1" s="78"/>
+      <c r="BA1" s="76">
         <v>45778</v>
       </c>
-      <c r="BB1" s="76"/>
-      <c r="BC1" s="76"/>
-      <c r="BD1" s="76"/>
-      <c r="BE1" s="77"/>
-      <c r="BF1" s="75">
+      <c r="BB1" s="77"/>
+      <c r="BC1" s="77"/>
+      <c r="BD1" s="77"/>
+      <c r="BE1" s="78"/>
+      <c r="BF1" s="76">
         <v>45809</v>
       </c>
-      <c r="BG1" s="76"/>
-      <c r="BH1" s="76"/>
-      <c r="BI1" s="76"/>
-      <c r="BJ1" s="75">
+      <c r="BG1" s="77"/>
+      <c r="BH1" s="77"/>
+      <c r="BI1" s="77"/>
+      <c r="BJ1" s="76">
         <v>45839</v>
       </c>
-      <c r="BK1" s="76"/>
-      <c r="BL1" s="76"/>
-      <c r="BM1" s="76"/>
-      <c r="BN1" s="77"/>
-      <c r="BO1" s="75">
+      <c r="BK1" s="77"/>
+      <c r="BL1" s="77"/>
+      <c r="BM1" s="77"/>
+      <c r="BN1" s="78"/>
+      <c r="BO1" s="76">
         <v>45870</v>
       </c>
-      <c r="BP1" s="76"/>
-      <c r="BQ1" s="76"/>
-      <c r="BR1" s="76"/>
-      <c r="BS1" s="75">
+      <c r="BP1" s="77"/>
+      <c r="BQ1" s="77"/>
+      <c r="BR1" s="77"/>
+      <c r="BS1" s="76">
         <v>45901</v>
       </c>
-      <c r="BT1" s="76"/>
-      <c r="BU1" s="76"/>
-      <c r="BV1" s="76"/>
-      <c r="BW1" s="75">
+      <c r="BT1" s="77"/>
+      <c r="BU1" s="77"/>
+      <c r="BV1" s="77"/>
+      <c r="BW1" s="76">
         <v>45931</v>
       </c>
-      <c r="BX1" s="76"/>
-      <c r="BY1" s="76"/>
-      <c r="BZ1" s="76"/>
-      <c r="CB1" s="75">
+      <c r="BX1" s="77"/>
+      <c r="BY1" s="77"/>
+      <c r="BZ1" s="77"/>
+      <c r="CB1" s="76">
         <v>45962</v>
       </c>
-      <c r="CC1" s="76"/>
-      <c r="CD1" s="76"/>
-      <c r="CE1" s="76"/>
-      <c r="CF1" s="80" t="s">
+      <c r="CC1" s="77"/>
+      <c r="CD1" s="77"/>
+      <c r="CE1" s="77"/>
+      <c r="CF1" s="75" t="s">
         <v>1854</v>
       </c>
-      <c r="CG1" s="80"/>
+      <c r="CG1" s="75"/>
     </row>
     <row r="2" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
@@ -67074,7 +67071,7 @@
         <v>1864</v>
       </c>
       <c r="P18" s="12" t="s">
-        <v>1859</v>
+        <v>1865</v>
       </c>
       <c r="Q18" s="50">
         <v>45559</v>
@@ -67193,7 +67190,9 @@
       <c r="O19" s="12" t="s">
         <v>1864</v>
       </c>
-      <c r="P19" s="12"/>
+      <c r="P19" s="12" t="s">
+        <v>1865</v>
+      </c>
       <c r="Q19" s="50">
         <v>45579</v>
       </c>
@@ -67206,9 +67205,9 @@
       <c r="V19" s="12"/>
       <c r="W19" s="12"/>
       <c r="X19" s="12"/>
-      <c r="Y19" s="59"/>
-      <c r="Z19" s="59"/>
-      <c r="AA19" s="59"/>
+      <c r="Y19" s="12"/>
+      <c r="Z19" s="12"/>
+      <c r="AA19" s="12"/>
       <c r="AB19" s="12"/>
       <c r="AC19" s="12"/>
       <c r="AD19" s="12"/>
@@ -67295,9 +67294,11 @@
         <v>3</v>
       </c>
       <c r="O20" s="12" t="s">
-        <v>1880</v>
-      </c>
-      <c r="P20" s="12"/>
+        <v>1864</v>
+      </c>
+      <c r="P20" s="12" t="s">
+        <v>1859</v>
+      </c>
       <c r="Q20" s="50">
         <v>45590</v>
       </c>
@@ -67312,9 +67313,9 @@
       <c r="X20" s="12"/>
       <c r="Y20" s="12"/>
       <c r="Z20" s="12"/>
-      <c r="AA20" s="48"/>
-      <c r="AB20" s="48"/>
-      <c r="AC20" s="48"/>
+      <c r="AA20" s="59"/>
+      <c r="AB20" s="59"/>
+      <c r="AC20" s="59"/>
       <c r="AD20" s="12"/>
       <c r="AE20" s="12"/>
       <c r="AF20" s="12"/>
@@ -69031,20 +69032,20 @@
         <v>1864</v>
       </c>
       <c r="P36" s="12" t="s">
-        <v>1859</v>
+        <v>1865</v>
       </c>
       <c r="Q36" s="63">
         <v>45574</v>
       </c>
       <c r="R36" s="63">
-        <v>45576</v>
+        <v>45579</v>
       </c>
       <c r="S36" s="53"/>
       <c r="T36" s="12"/>
       <c r="U36" s="12"/>
       <c r="V36" s="12"/>
       <c r="W36" s="12"/>
-      <c r="X36" s="59"/>
+      <c r="X36" s="12"/>
       <c r="Y36" s="12"/>
       <c r="Z36" s="12"/>
       <c r="AA36" s="12"/>
@@ -69127,17 +69128,17 @@
       <c r="B38" s="70"/>
       <c r="C38" s="70"/>
       <c r="D38" s="68" t="s">
-        <v>1882</v>
+        <v>1881</v>
       </c>
       <c r="E38" s="69" t="s">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="F38" s="70"/>
       <c r="G38" s="71" t="s">
         <v>176</v>
       </c>
       <c r="H38" s="71" t="s">
-        <v>1883</v>
+        <v>1882</v>
       </c>
       <c r="I38" s="70">
         <v>23</v>
@@ -69149,7 +69150,7 @@
       <c r="N38" s="70"/>
       <c r="O38" s="70"/>
       <c r="P38" s="70" t="s">
-        <v>1884</v>
+        <v>1883</v>
       </c>
       <c r="Q38" s="70"/>
       <c r="R38" s="70"/>
@@ -69330,22 +69331,22 @@
     </sortState>
   </autoFilter>
   <mergeCells count="16">
+    <mergeCell ref="AO1:AR1"/>
+    <mergeCell ref="AS1:AV1"/>
+    <mergeCell ref="AW1:AZ1"/>
+    <mergeCell ref="BA1:BE1"/>
+    <mergeCell ref="BF1:BI1"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="W1:AA1"/>
+    <mergeCell ref="AB1:AE1"/>
+    <mergeCell ref="AF1:AI1"/>
+    <mergeCell ref="AJ1:AN1"/>
     <mergeCell ref="CF1:CG1"/>
     <mergeCell ref="BJ1:BN1"/>
     <mergeCell ref="BO1:BR1"/>
     <mergeCell ref="BS1:BV1"/>
     <mergeCell ref="BW1:BZ1"/>
     <mergeCell ref="CB1:CE1"/>
-    <mergeCell ref="S1:V1"/>
-    <mergeCell ref="W1:AA1"/>
-    <mergeCell ref="AB1:AE1"/>
-    <mergeCell ref="AF1:AI1"/>
-    <mergeCell ref="AJ1:AN1"/>
-    <mergeCell ref="AO1:AR1"/>
-    <mergeCell ref="AS1:AV1"/>
-    <mergeCell ref="AW1:AZ1"/>
-    <mergeCell ref="BA1:BE1"/>
-    <mergeCell ref="BF1:BI1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualizacion de plan de trabajo ajuste por analisis de la nva estrutura , ajuste de fechas
</commit_message>
<xml_diff>
--- a/00-Documentacion/Listado de reportes totales-TI.xlsx
+++ b/00-Documentacion/Listado de reportes totales-TI.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E225F2E9-3A54-4C4A-A738-583AC8A6BE86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7B58844-7338-47D8-92A3-083B59AE34F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{1498AA1A-1ACC-4329-A050-ACA05131B658}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Analisis Proceso con prioridad" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Analisis Proceso con prioridad'!$A$2:$CG$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Analisis Proceso con prioridad'!$A$2:$CG$32</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'General - Analisis'!$A$1:$R$1347</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'listado modulo sin area'!$A$1:$R$116</definedName>
   </definedNames>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13301" uniqueCount="1884">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13300" uniqueCount="1889">
   <si>
     <t xml:space="preserve">Reporte </t>
   </si>
@@ -5654,9 +5654,6 @@
     <t>Terminado</t>
   </si>
   <si>
-    <t>8-7</t>
-  </si>
-  <si>
     <t>|</t>
   </si>
   <si>
@@ -5706,6 +5703,24 @@
   </si>
   <si>
     <t>Pendiente</t>
+  </si>
+  <si>
+    <t>Estructura NV BD Spooler</t>
+  </si>
+  <si>
+    <t>BD Spooler</t>
+  </si>
+  <si>
+    <t>Analisis de estructura de NV spooler BD</t>
+  </si>
+  <si>
+    <t>8-12</t>
+  </si>
+  <si>
+    <t>15-19</t>
+  </si>
+  <si>
+    <t>22-27</t>
   </si>
 </sst>
 </file>
@@ -6037,7 +6052,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6158,16 +6173,9 @@
     <xf numFmtId="14" fontId="0" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6196,6 +6204,12 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -64827,18 +64841,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9585C0FF-65C5-4BD8-9936-5C9A63F7E604}">
-  <dimension ref="A1:CM40"/>
+  <dimension ref="A1:CM41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="BJ1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AI20" sqref="AI20"/>
+      <selection pane="bottomLeft" activeCell="CI7" sqref="CI7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.7109375" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="50.85546875" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="50.85546875" customWidth="1"/>
     <col min="4" max="4" width="50.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="55.42578125" customWidth="1"/>
     <col min="6" max="6" width="37.7109375" customWidth="1"/>
@@ -64861,9 +64875,9 @@
     <col min="24" max="24" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="7" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.140625" customWidth="1"/>
+    <col min="28" max="28" width="10.28515625" customWidth="1"/>
+    <col min="29" max="29" width="10.5703125" customWidth="1"/>
     <col min="30" max="30" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="8" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="7.5703125" bestFit="1" customWidth="1"/>
@@ -64909,110 +64923,111 @@
     <col min="81" max="82" width="7" bestFit="1" customWidth="1"/>
     <col min="83" max="83" width="8" bestFit="1" customWidth="1"/>
     <col min="84" max="84" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="6" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="86" max="87" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:86" x14ac:dyDescent="0.25">
-      <c r="S1" s="79">
+    <row r="1" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="S1" s="78">
         <v>45536</v>
       </c>
-      <c r="T1" s="80"/>
-      <c r="U1" s="80"/>
-      <c r="V1" s="80"/>
-      <c r="W1" s="79">
+      <c r="T1" s="79"/>
+      <c r="U1" s="79"/>
+      <c r="V1" s="79"/>
+      <c r="W1" s="78">
         <v>45566</v>
       </c>
-      <c r="X1" s="79"/>
-      <c r="Y1" s="79"/>
-      <c r="Z1" s="79"/>
-      <c r="AA1" s="79"/>
-      <c r="AB1" s="76">
+      <c r="X1" s="78"/>
+      <c r="Y1" s="78"/>
+      <c r="Z1" s="78"/>
+      <c r="AA1" s="78"/>
+      <c r="AB1" s="75">
         <v>45597</v>
       </c>
-      <c r="AC1" s="77"/>
-      <c r="AD1" s="77"/>
-      <c r="AE1" s="78"/>
-      <c r="AF1" s="76">
+      <c r="AC1" s="76"/>
+      <c r="AD1" s="76"/>
+      <c r="AE1" s="77"/>
+      <c r="AF1" s="75">
         <v>45627</v>
       </c>
-      <c r="AG1" s="77"/>
-      <c r="AH1" s="77"/>
-      <c r="AI1" s="78"/>
-      <c r="AJ1" s="76">
+      <c r="AG1" s="76"/>
+      <c r="AH1" s="76"/>
+      <c r="AI1" s="77"/>
+      <c r="AJ1" s="75">
         <v>45658</v>
       </c>
-      <c r="AK1" s="77"/>
-      <c r="AL1" s="77"/>
-      <c r="AM1" s="77"/>
-      <c r="AN1" s="78"/>
-      <c r="AO1" s="76">
+      <c r="AK1" s="76"/>
+      <c r="AL1" s="76"/>
+      <c r="AM1" s="76"/>
+      <c r="AN1" s="77"/>
+      <c r="AO1" s="75">
         <v>45689</v>
       </c>
-      <c r="AP1" s="77"/>
-      <c r="AQ1" s="77"/>
-      <c r="AR1" s="78"/>
-      <c r="AS1" s="76">
+      <c r="AP1" s="76"/>
+      <c r="AQ1" s="76"/>
+      <c r="AR1" s="77"/>
+      <c r="AS1" s="75">
         <v>45717</v>
       </c>
-      <c r="AT1" s="77"/>
-      <c r="AU1" s="77"/>
-      <c r="AV1" s="78"/>
-      <c r="AW1" s="76">
+      <c r="AT1" s="76"/>
+      <c r="AU1" s="76"/>
+      <c r="AV1" s="77"/>
+      <c r="AW1" s="75">
         <v>45748</v>
       </c>
-      <c r="AX1" s="77"/>
-      <c r="AY1" s="77"/>
-      <c r="AZ1" s="78"/>
-      <c r="BA1" s="76">
+      <c r="AX1" s="76"/>
+      <c r="AY1" s="76"/>
+      <c r="AZ1" s="77"/>
+      <c r="BA1" s="75">
         <v>45778</v>
       </c>
-      <c r="BB1" s="77"/>
-      <c r="BC1" s="77"/>
-      <c r="BD1" s="77"/>
-      <c r="BE1" s="78"/>
-      <c r="BF1" s="76">
+      <c r="BB1" s="76"/>
+      <c r="BC1" s="76"/>
+      <c r="BD1" s="76"/>
+      <c r="BE1" s="77"/>
+      <c r="BF1" s="75">
         <v>45809</v>
       </c>
-      <c r="BG1" s="77"/>
-      <c r="BH1" s="77"/>
-      <c r="BI1" s="77"/>
-      <c r="BJ1" s="76">
+      <c r="BG1" s="76"/>
+      <c r="BH1" s="76"/>
+      <c r="BI1" s="76"/>
+      <c r="BJ1" s="75">
         <v>45839</v>
       </c>
-      <c r="BK1" s="77"/>
-      <c r="BL1" s="77"/>
-      <c r="BM1" s="77"/>
-      <c r="BN1" s="78"/>
-      <c r="BO1" s="76">
+      <c r="BK1" s="76"/>
+      <c r="BL1" s="76"/>
+      <c r="BM1" s="76"/>
+      <c r="BN1" s="77"/>
+      <c r="BO1" s="75">
         <v>45870</v>
       </c>
-      <c r="BP1" s="77"/>
-      <c r="BQ1" s="77"/>
-      <c r="BR1" s="77"/>
-      <c r="BS1" s="76">
+      <c r="BP1" s="76"/>
+      <c r="BQ1" s="76"/>
+      <c r="BR1" s="76"/>
+      <c r="BS1" s="75">
         <v>45901</v>
       </c>
-      <c r="BT1" s="77"/>
-      <c r="BU1" s="77"/>
-      <c r="BV1" s="77"/>
-      <c r="BW1" s="76">
+      <c r="BT1" s="76"/>
+      <c r="BU1" s="76"/>
+      <c r="BV1" s="76"/>
+      <c r="BW1" s="75">
         <v>45931</v>
       </c>
-      <c r="BX1" s="77"/>
-      <c r="BY1" s="77"/>
-      <c r="BZ1" s="77"/>
-      <c r="CB1" s="76">
+      <c r="BX1" s="76"/>
+      <c r="BY1" s="76"/>
+      <c r="BZ1" s="76"/>
+      <c r="CB1" s="75">
         <v>45962</v>
       </c>
-      <c r="CC1" s="77"/>
-      <c r="CD1" s="77"/>
-      <c r="CE1" s="77"/>
-      <c r="CF1" s="75" t="s">
+      <c r="CC1" s="76"/>
+      <c r="CD1" s="76"/>
+      <c r="CE1" s="76"/>
+      <c r="CF1" s="74" t="s">
         <v>1854</v>
       </c>
-      <c r="CG1" s="75"/>
-    </row>
-    <row r="2" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CG1" s="74"/>
+    </row>
+    <row r="2" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>1780</v>
       </c>
@@ -65266,56 +65281,70 @@
         <v>1856</v>
       </c>
       <c r="CG2" s="46" t="s">
-        <v>1866</v>
-      </c>
-    </row>
-    <row r="3" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
+        <v>1886</v>
+      </c>
+      <c r="CH2" s="46" t="s">
+        <v>1887</v>
+      </c>
+      <c r="CI2" s="46" t="s">
+        <v>1888</v>
+      </c>
+    </row>
+    <row r="3" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="19" t="s">
-        <v>1773</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>1766</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>1768</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>15</v>
+      <c r="C3" s="15" t="s">
+        <v>1750</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>1750</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>1751</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>1744</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>1682</v>
+        <v>1684</v>
       </c>
       <c r="I3" s="12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J3" s="12">
         <v>2</v>
       </c>
       <c r="K3" s="12">
-        <f>2+1</f>
-        <v>3</v>
-      </c>
-      <c r="L3" s="54"/>
+        <f>3+1</f>
+        <v>4</v>
+      </c>
+      <c r="L3" s="54" t="s">
+        <v>1790</v>
+      </c>
       <c r="M3" s="12" t="s">
         <v>1787</v>
       </c>
-      <c r="N3" s="12"/>
+      <c r="N3" s="12">
+        <v>24</v>
+      </c>
       <c r="O3" s="12" t="s">
         <v>1864</v>
       </c>
       <c r="P3" s="12" t="s">
         <v>1865</v>
       </c>
-      <c r="Q3" s="12"/>
+      <c r="Q3" s="50">
+        <v>45485</v>
+      </c>
       <c r="R3" s="56">
-        <v>45453</v>
+        <v>45523</v>
       </c>
       <c r="S3" s="53"/>
       <c r="T3" s="12"/>
@@ -65384,46 +65413,52 @@
       <c r="CE3" s="12"/>
       <c r="CF3" s="12"/>
       <c r="CG3" s="12"/>
-    </row>
-    <row r="4" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CH3" s="12"/>
+      <c r="CI3" s="12"/>
+    </row>
+    <row r="4" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="21" t="s">
-        <v>1586</v>
-      </c>
-      <c r="E4" s="21" t="s">
-        <v>1763</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>1768</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>12</v>
+      <c r="C4" s="15" t="s">
+        <v>1752</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>1752</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>1751</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>1744</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>13</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>1682</v>
+        <v>1684</v>
       </c>
       <c r="I4" s="12">
+        <v>5</v>
+      </c>
+      <c r="J4" s="12">
         <v>2</v>
       </c>
-      <c r="J4" s="12">
-        <v>1</v>
-      </c>
       <c r="K4" s="12">
-        <f>2+1</f>
-        <v>3</v>
-      </c>
-      <c r="L4" s="54"/>
+        <f>4+1</f>
+        <v>5</v>
+      </c>
+      <c r="L4" s="54" t="s">
+        <v>1862</v>
+      </c>
       <c r="M4" s="12" t="s">
-        <v>1787</v>
+        <v>1861</v>
       </c>
       <c r="N4" s="12">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="O4" s="12" t="s">
         <v>1864</v>
@@ -65431,9 +65466,11 @@
       <c r="P4" s="12" t="s">
         <v>1865</v>
       </c>
-      <c r="Q4" s="12"/>
+      <c r="Q4" s="50">
+        <v>45537</v>
+      </c>
       <c r="R4" s="56">
-        <v>45468</v>
+        <v>45538</v>
       </c>
       <c r="S4" s="53"/>
       <c r="T4" s="12"/>
@@ -65502,8 +65539,10 @@
       <c r="CE4" s="12"/>
       <c r="CF4" s="12"/>
       <c r="CG4" s="12"/>
-    </row>
-    <row r="5" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CH4" s="12"/>
+      <c r="CI4" s="12"/>
+    </row>
+    <row r="5" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>1777</v>
       </c>
@@ -65622,8 +65661,10 @@
       <c r="CE5" s="12"/>
       <c r="CF5" s="12"/>
       <c r="CG5" s="12"/>
-    </row>
-    <row r="6" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CH5" s="12"/>
+      <c r="CI5" s="12"/>
+    </row>
+    <row r="6" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>1777</v>
       </c>
@@ -65631,41 +65672,41 @@
         <v>35</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>1750</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>1750</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>1751</v>
-      </c>
-      <c r="F6" s="24" t="s">
-        <v>1744</v>
+        <v>1739</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>1749</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>1747</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>1745</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>1684</v>
+        <v>16</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>1726</v>
       </c>
       <c r="I6" s="12">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J6" s="12">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K6" s="12">
-        <f>3+1</f>
-        <v>4</v>
+        <f>4+1</f>
+        <v>5</v>
       </c>
       <c r="L6" s="54" t="s">
-        <v>1790</v>
+        <v>1789</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>1787</v>
+        <v>1788</v>
       </c>
       <c r="N6" s="12">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="O6" s="12" t="s">
         <v>1864</v>
@@ -65674,10 +65715,10 @@
         <v>1865</v>
       </c>
       <c r="Q6" s="50">
-        <v>45485</v>
+        <v>45525</v>
       </c>
       <c r="R6" s="56">
-        <v>45523</v>
+        <v>45546</v>
       </c>
       <c r="S6" s="53"/>
       <c r="T6" s="12"/>
@@ -65746,8 +65787,10 @@
       <c r="CE6" s="12"/>
       <c r="CF6" s="12"/>
       <c r="CG6" s="12"/>
-    </row>
-    <row r="7" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CH6" s="12"/>
+      <c r="CI6" s="12"/>
+    </row>
+    <row r="7" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>1778</v>
       </c>
@@ -65756,50 +65799,44 @@
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="19" t="s">
-        <v>1771</v>
-      </c>
-      <c r="E7" s="21" t="s">
-        <v>1763</v>
+        <v>1773</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>1766</v>
       </c>
       <c r="F7" s="20" t="s">
         <v>1768</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>1684</v>
+        <v>1682</v>
       </c>
       <c r="I7" s="12">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J7" s="12">
         <v>2</v>
       </c>
       <c r="K7" s="12">
-        <f>4+1</f>
-        <v>5</v>
-      </c>
-      <c r="L7" s="54" t="s">
-        <v>1860</v>
-      </c>
+        <f>2+1</f>
+        <v>3</v>
+      </c>
+      <c r="L7" s="54"/>
       <c r="M7" s="12" t="s">
-        <v>1861</v>
-      </c>
-      <c r="N7" s="12">
-        <v>8</v>
-      </c>
+        <v>1787</v>
+      </c>
+      <c r="N7" s="12"/>
       <c r="O7" s="12" t="s">
         <v>1864</v>
       </c>
       <c r="P7" s="12" t="s">
         <v>1865</v>
       </c>
-      <c r="Q7" s="50">
-        <v>45514</v>
-      </c>
+      <c r="Q7" s="12"/>
       <c r="R7" s="56">
-        <v>45534</v>
+        <v>45453</v>
       </c>
       <c r="S7" s="53"/>
       <c r="T7" s="12"/>
@@ -65868,50 +65905,48 @@
       <c r="CE7" s="12"/>
       <c r="CF7" s="12"/>
       <c r="CG7" s="12"/>
-    </row>
-    <row r="8" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CH7" s="12"/>
+      <c r="CI7" s="12"/>
+    </row>
+    <row r="8" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>1777</v>
+        <v>1778</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="15" t="s">
-        <v>1752</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>1752</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>1751</v>
-      </c>
-      <c r="F8" s="24" t="s">
-        <v>1744</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>13</v>
+      <c r="C8" s="12"/>
+      <c r="D8" s="21" t="s">
+        <v>1586</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>1763</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>1768</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>1684</v>
+        <v>1682</v>
       </c>
       <c r="I8" s="12">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J8" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K8" s="12">
-        <f>4+1</f>
-        <v>5</v>
-      </c>
-      <c r="L8" s="54" t="s">
-        <v>1862</v>
-      </c>
+        <f>2+1</f>
+        <v>3</v>
+      </c>
+      <c r="L8" s="54"/>
       <c r="M8" s="12" t="s">
-        <v>1861</v>
+        <v>1787</v>
       </c>
       <c r="N8" s="12">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="O8" s="12" t="s">
         <v>1864</v>
@@ -65919,11 +65954,9 @@
       <c r="P8" s="12" t="s">
         <v>1865</v>
       </c>
-      <c r="Q8" s="50">
-        <v>45537</v>
-      </c>
+      <c r="Q8" s="12"/>
       <c r="R8" s="56">
-        <v>45538</v>
+        <v>45468</v>
       </c>
       <c r="S8" s="53"/>
       <c r="T8" s="12"/>
@@ -65992,50 +66025,50 @@
       <c r="CE8" s="12"/>
       <c r="CF8" s="12"/>
       <c r="CG8" s="12"/>
-    </row>
-    <row r="9" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CH8" s="12"/>
+      <c r="CI8" s="12"/>
+    </row>
+    <row r="9" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>1777</v>
+        <v>1778</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="15" t="s">
-        <v>1739</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>1749</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>1747</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>1745</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="12" t="s">
-        <v>1726</v>
+      <c r="C9" s="12"/>
+      <c r="D9" s="19" t="s">
+        <v>1771</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>1763</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>1768</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>1684</v>
       </c>
       <c r="I9" s="12">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J9" s="12">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K9" s="12">
         <f>4+1</f>
         <v>5</v>
       </c>
       <c r="L9" s="54" t="s">
-        <v>1789</v>
+        <v>1860</v>
       </c>
       <c r="M9" s="12" t="s">
-        <v>1788</v>
+        <v>1861</v>
       </c>
       <c r="N9" s="12">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="O9" s="12" t="s">
         <v>1864</v>
@@ -66044,10 +66077,10 @@
         <v>1865</v>
       </c>
       <c r="Q9" s="50">
-        <v>45525</v>
+        <v>45514</v>
       </c>
       <c r="R9" s="56">
-        <v>45546</v>
+        <v>45534</v>
       </c>
       <c r="S9" s="12"/>
       <c r="T9" s="12"/>
@@ -66116,8 +66149,10 @@
       <c r="CE9" s="12"/>
       <c r="CF9" s="12"/>
       <c r="CG9" s="12"/>
-    </row>
-    <row r="10" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CH9" s="12"/>
+      <c r="CI9" s="12"/>
+    </row>
+    <row r="10" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>1777</v>
       </c>
@@ -66160,10 +66195,10 @@
       <c r="O10" s="12"/>
       <c r="P10" s="12"/>
       <c r="Q10" s="50">
-        <v>45659</v>
+        <v>45664</v>
       </c>
       <c r="R10" s="56">
-        <v>45680</v>
+        <v>45681</v>
       </c>
       <c r="S10" s="53"/>
       <c r="T10" s="12"/>
@@ -66183,10 +66218,10 @@
       <c r="AH10" s="12"/>
       <c r="AI10" s="12"/>
       <c r="AJ10" s="12"/>
-      <c r="AK10" s="48"/>
+      <c r="AK10" s="12"/>
       <c r="AL10" s="48"/>
       <c r="AM10" s="48"/>
-      <c r="AN10" s="12"/>
+      <c r="AN10" s="48"/>
       <c r="AO10" s="12"/>
       <c r="AP10" s="12"/>
       <c r="AQ10" s="12"/>
@@ -66232,13 +66267,15 @@
       <c r="CE10" s="12"/>
       <c r="CF10" s="12"/>
       <c r="CG10" s="12"/>
-    </row>
-    <row r="11" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CH10" s="12"/>
+      <c r="CI10" s="12"/>
+    </row>
+    <row r="11" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>1778</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>1869</v>
+        <v>1868</v>
       </c>
       <c r="C11" s="12"/>
       <c r="D11" s="19" t="s">
@@ -66247,7 +66284,7 @@
       <c r="E11" s="19" t="s">
         <v>1761</v>
       </c>
-      <c r="F11" s="62" t="s">
+      <c r="F11" s="73" t="s">
         <v>1762</v>
       </c>
       <c r="G11" s="12" t="s">
@@ -66273,10 +66310,10 @@
       <c r="O11" s="12"/>
       <c r="P11" s="12"/>
       <c r="Q11" s="50">
-        <v>45844</v>
+        <v>45842</v>
       </c>
       <c r="R11" s="56">
-        <v>45866</v>
+        <v>45862</v>
       </c>
       <c r="S11" s="53"/>
       <c r="T11" s="12"/>
@@ -66324,11 +66361,11 @@
       <c r="BH11" s="12"/>
       <c r="BI11" s="12"/>
       <c r="BJ11" s="12"/>
-      <c r="BK11" s="48"/>
+      <c r="BK11" s="12"/>
       <c r="BL11" s="48"/>
       <c r="BM11" s="48"/>
       <c r="BN11" s="48"/>
-      <c r="BO11" s="12"/>
+      <c r="BO11" s="48"/>
       <c r="BP11" s="12"/>
       <c r="BQ11" s="12"/>
       <c r="BR11" s="12"/>
@@ -66347,53 +66384,43 @@
       <c r="CE11" s="12"/>
       <c r="CF11" s="12"/>
       <c r="CG11" s="12"/>
-    </row>
-    <row r="12" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
-        <v>1777</v>
-      </c>
+      <c r="CH11" s="12"/>
+      <c r="CI11" s="12"/>
+    </row>
+    <row r="12" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="14"/>
       <c r="B12" s="15" t="s">
-        <v>1757</v>
+        <v>1883</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>1757</v>
+        <v>1884</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>1757</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>1758</v>
-      </c>
-      <c r="F12" s="24" t="s">
-        <v>1744</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>1696</v>
-      </c>
+        <v>1884</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>1885</v>
+      </c>
+      <c r="F12" s="22"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="49"/>
       <c r="I12" s="12">
-        <v>20</v>
-      </c>
-      <c r="J12" s="12">
-        <v>12</v>
-      </c>
-      <c r="K12" s="12">
-        <v>16</v>
-      </c>
-      <c r="L12" s="54"/>
+        <v>8.01</v>
+      </c>
+      <c r="J12" s="49"/>
+      <c r="K12" s="49"/>
+      <c r="L12" s="55"/>
       <c r="M12" s="12"/>
-      <c r="N12" s="12">
-        <v>16</v>
-      </c>
-      <c r="O12" s="12"/>
-      <c r="P12" s="12"/>
-      <c r="Q12" s="50">
-        <v>45929</v>
-      </c>
-      <c r="R12" s="56">
-        <v>45953</v>
+      <c r="N12" s="49"/>
+      <c r="O12" s="49"/>
+      <c r="P12" s="12" t="s">
+        <v>1859</v>
+      </c>
+      <c r="Q12" s="51">
+        <v>45601</v>
+      </c>
+      <c r="R12" s="57">
+        <v>45608</v>
       </c>
       <c r="S12" s="53"/>
       <c r="T12" s="12"/>
@@ -66404,7 +66431,7 @@
       <c r="Y12" s="12"/>
       <c r="Z12" s="12"/>
       <c r="AA12" s="12"/>
-      <c r="AB12" s="12"/>
+      <c r="AB12" s="59"/>
       <c r="AC12" s="12"/>
       <c r="AD12" s="12"/>
       <c r="AE12" s="12"/>
@@ -66451,10 +66478,10 @@
       <c r="BT12" s="12"/>
       <c r="BU12" s="12"/>
       <c r="BV12" s="12"/>
-      <c r="BW12" s="48"/>
-      <c r="BX12" s="48"/>
-      <c r="BY12" s="48"/>
-      <c r="BZ12" s="48"/>
+      <c r="BW12" s="12"/>
+      <c r="BX12" s="12"/>
+      <c r="BY12" s="12"/>
+      <c r="BZ12" s="12"/>
       <c r="CA12" s="12"/>
       <c r="CB12" s="12"/>
       <c r="CC12" s="12"/>
@@ -66462,54 +66489,51 @@
       <c r="CE12" s="12"/>
       <c r="CF12" s="12"/>
       <c r="CG12" s="12"/>
-    </row>
-    <row r="13" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
-        <v>1777</v>
-      </c>
+      <c r="CH12" s="12"/>
+      <c r="CI12" s="12"/>
+    </row>
+    <row r="13" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
       <c r="B13" s="15" t="s">
-        <v>1756</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>1756</v>
-      </c>
+        <v>1883</v>
+      </c>
+      <c r="C13" s="15"/>
       <c r="D13" s="15" t="s">
-        <v>1756</v>
-      </c>
-      <c r="E13" s="23" t="s">
-        <v>1779</v>
-      </c>
-      <c r="F13" s="24" t="s">
-        <v>1745</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>1682</v>
+        <v>1878</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>1878</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>1878</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>1878</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>1878</v>
       </c>
       <c r="I13" s="12">
-        <v>10</v>
-      </c>
-      <c r="J13" s="12">
-        <v>9</v>
-      </c>
-      <c r="K13" s="12">
-        <f>4+1</f>
-        <v>5</v>
-      </c>
+        <v>7.9</v>
+      </c>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
       <c r="L13" s="54"/>
       <c r="M13" s="12"/>
       <c r="N13" s="12">
-        <v>14</v>
-      </c>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
+        <v>3</v>
+      </c>
+      <c r="O13" s="12" t="s">
+        <v>1864</v>
+      </c>
+      <c r="P13" s="12" t="s">
+        <v>1865</v>
+      </c>
       <c r="Q13" s="50">
-        <v>45681</v>
+        <v>45574</v>
       </c>
       <c r="R13" s="56">
-        <v>45702</v>
+        <v>45579</v>
       </c>
       <c r="S13" s="53"/>
       <c r="T13" s="12"/>
@@ -66531,9 +66555,9 @@
       <c r="AK13" s="12"/>
       <c r="AL13" s="12"/>
       <c r="AM13" s="12"/>
-      <c r="AN13" s="48"/>
-      <c r="AO13" s="48"/>
-      <c r="AP13" s="48"/>
+      <c r="AN13" s="12"/>
+      <c r="AO13" s="12"/>
+      <c r="AP13" s="12"/>
       <c r="AQ13" s="12"/>
       <c r="AR13" s="12"/>
       <c r="AS13" s="12"/>
@@ -66578,52 +66602,54 @@
       <c r="CF13" s="12"/>
       <c r="CG13" s="12"/>
       <c r="CH13" s="12"/>
-    </row>
-    <row r="14" spans="1:86" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
-        <v>1778</v>
+      <c r="CI13" s="12"/>
+    </row>
+    <row r="14" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>1777</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>1756</v>
-      </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="45" t="s">
-        <v>1767</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>1763</v>
-      </c>
-      <c r="F14" s="25" t="s">
-        <v>1764</v>
+        <v>1757</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>1757</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>1757</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>1758</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>1744</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>1682</v>
+        <v>1696</v>
       </c>
       <c r="I14" s="12">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="J14" s="12">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K14" s="12">
-        <f>6+7</f>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="L14" s="54"/>
       <c r="M14" s="12"/>
       <c r="N14" s="12">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="O14" s="12"/>
       <c r="P14" s="12"/>
       <c r="Q14" s="50">
-        <v>45705</v>
+        <v>45926</v>
       </c>
       <c r="R14" s="56">
-        <v>45725</v>
+        <v>45950</v>
       </c>
       <c r="S14" s="53"/>
       <c r="T14" s="12"/>
@@ -66649,9 +66675,9 @@
       <c r="AN14" s="12"/>
       <c r="AO14" s="12"/>
       <c r="AP14" s="12"/>
-      <c r="AQ14" s="48"/>
-      <c r="AR14" s="48"/>
-      <c r="AS14" s="48"/>
+      <c r="AQ14" s="12"/>
+      <c r="AR14" s="12"/>
+      <c r="AS14" s="12"/>
       <c r="AT14" s="12"/>
       <c r="AU14" s="12"/>
       <c r="AV14" s="12"/>
@@ -66682,10 +66708,10 @@
       <c r="BU14" s="12"/>
       <c r="BV14" s="12"/>
       <c r="BW14" s="12"/>
-      <c r="BX14" s="12"/>
-      <c r="BY14" s="12"/>
-      <c r="BZ14" s="12"/>
-      <c r="CA14" s="12"/>
+      <c r="BX14" s="48"/>
+      <c r="BY14" s="48"/>
+      <c r="BZ14" s="48"/>
+      <c r="CA14" s="48"/>
       <c r="CB14" s="12"/>
       <c r="CC14" s="12"/>
       <c r="CD14" s="12"/>
@@ -66693,39 +66719,42 @@
       <c r="CF14" s="12"/>
       <c r="CG14" s="12"/>
       <c r="CH14" s="12"/>
-    </row>
-    <row r="15" spans="1:86" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
-        <v>1778</v>
+      <c r="CI14" s="12"/>
+    </row>
+    <row r="15" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>1777</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>1756</v>
       </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="19" t="s">
-        <v>1643</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>1763</v>
-      </c>
-      <c r="F15" s="25" t="s">
-        <v>1764</v>
+      <c r="C15" s="15" t="s">
+        <v>1756</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>1756</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>1779</v>
+      </c>
+      <c r="F15" s="24" t="s">
+        <v>1745</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="H15" s="10" t="s">
-        <v>1681</v>
+        <v>29</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>1682</v>
       </c>
       <c r="I15" s="12">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="J15" s="12">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="K15" s="12">
-        <f>9+2</f>
-        <v>11</v>
+        <f>4+1</f>
+        <v>5</v>
       </c>
       <c r="L15" s="54"/>
       <c r="M15" s="12"/>
@@ -66735,10 +66764,10 @@
       <c r="O15" s="12"/>
       <c r="P15" s="12"/>
       <c r="Q15" s="50">
-        <v>45820</v>
+        <v>45684</v>
       </c>
       <c r="R15" s="56">
-        <v>45841</v>
+        <v>45702</v>
       </c>
       <c r="S15" s="53"/>
       <c r="T15" s="12"/>
@@ -66750,7 +66779,6 @@
       <c r="Z15" s="12"/>
       <c r="AA15" s="12"/>
       <c r="AB15" s="12"/>
-      <c r="AC15" s="12"/>
       <c r="AD15" s="12"/>
       <c r="AE15" s="12"/>
       <c r="AF15" s="12"/>
@@ -66762,9 +66790,9 @@
       <c r="AL15" s="12"/>
       <c r="AM15" s="12"/>
       <c r="AN15" s="12"/>
-      <c r="AO15" s="12"/>
-      <c r="AP15" s="12"/>
-      <c r="AQ15" s="12"/>
+      <c r="AO15" s="48"/>
+      <c r="AP15" s="48"/>
+      <c r="AQ15" s="48"/>
       <c r="AR15" s="12"/>
       <c r="AS15" s="12"/>
       <c r="AT15" s="12"/>
@@ -66781,9 +66809,9 @@
       <c r="BE15" s="12"/>
       <c r="BF15" s="12"/>
       <c r="BG15" s="12"/>
-      <c r="BH15" s="48"/>
-      <c r="BI15" s="48"/>
-      <c r="BJ15" s="48"/>
+      <c r="BH15" s="12"/>
+      <c r="BI15" s="12"/>
+      <c r="BJ15" s="12"/>
       <c r="BK15" s="12"/>
       <c r="BL15" s="12"/>
       <c r="BM15" s="12"/>
@@ -66808,8 +66836,9 @@
       <c r="CF15" s="12"/>
       <c r="CG15" s="12"/>
       <c r="CH15" s="12"/>
-    </row>
-    <row r="16" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI15" s="12"/>
+    </row>
+    <row r="16" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>1778</v>
       </c>
@@ -66817,42 +66846,43 @@
         <v>1756</v>
       </c>
       <c r="C16" s="12"/>
-      <c r="D16" s="19" t="s">
-        <v>1622</v>
+      <c r="D16" s="45" t="s">
+        <v>1767</v>
       </c>
       <c r="E16" s="21" t="s">
         <v>1763</v>
       </c>
-      <c r="F16" s="20" t="s">
-        <v>1768</v>
-      </c>
-      <c r="G16" s="10" t="s">
+      <c r="F16" s="25" t="s">
+        <v>1764</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>1682</v>
+      </c>
+      <c r="I16" s="12">
         <v>11</v>
       </c>
-      <c r="H16" s="10" t="s">
-        <v>1706</v>
-      </c>
-      <c r="I16" s="12">
-        <v>21</v>
-      </c>
       <c r="J16" s="12">
-        <v>76</v>
+        <v>13</v>
       </c>
       <c r="K16" s="12">
-        <v>8</v>
+        <f>6+7</f>
+        <v>13</v>
       </c>
       <c r="L16" s="54"/>
       <c r="M16" s="12"/>
       <c r="N16" s="12">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="O16" s="12"/>
       <c r="P16" s="12"/>
       <c r="Q16" s="50">
-        <v>45956</v>
+        <v>45705</v>
       </c>
       <c r="R16" s="56">
-        <v>45979</v>
+        <v>45723</v>
       </c>
       <c r="S16" s="53"/>
       <c r="T16" s="12"/>
@@ -66879,9 +66909,9 @@
       <c r="AO16" s="12"/>
       <c r="AP16" s="12"/>
       <c r="AQ16" s="12"/>
-      <c r="AR16" s="12"/>
-      <c r="AS16" s="12"/>
-      <c r="AT16" s="12"/>
+      <c r="AR16" s="48"/>
+      <c r="AS16" s="48"/>
+      <c r="AT16" s="48"/>
       <c r="AU16" s="12"/>
       <c r="AV16" s="12"/>
       <c r="AW16" s="12"/>
@@ -66914,65 +66944,61 @@
       <c r="BX16" s="12"/>
       <c r="BY16" s="12"/>
       <c r="BZ16" s="12"/>
-      <c r="CA16" s="48"/>
-      <c r="CB16" s="48"/>
-      <c r="CC16" s="48"/>
-      <c r="CD16" s="48"/>
+      <c r="CA16" s="12"/>
+      <c r="CB16" s="12"/>
+      <c r="CC16" s="12"/>
+      <c r="CD16" s="12"/>
       <c r="CE16" s="12"/>
       <c r="CF16" s="12"/>
-      <c r="CG16" s="46"/>
+      <c r="CG16" s="12"/>
       <c r="CH16" s="12"/>
-    </row>
-    <row r="17" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
-        <v>1777</v>
+      <c r="CI16" s="12"/>
+    </row>
+    <row r="17" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>1778</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>1739</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>1739</v>
-      </c>
-      <c r="D17" s="16"/>
-      <c r="E17" s="17" t="s">
-        <v>1784</v>
-      </c>
-      <c r="F17" s="22" t="s">
-        <v>1745</v>
+        <v>1756</v>
+      </c>
+      <c r="C17" s="12"/>
+      <c r="D17" s="19" t="s">
+        <v>1643</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>1763</v>
+      </c>
+      <c r="F17" s="25" t="s">
+        <v>1764</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>1218</v>
-      </c>
-      <c r="H17" s="12" t="s">
-        <v>1716</v>
+        <v>7</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>1681</v>
       </c>
       <c r="I17" s="12">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="J17" s="12">
-        <v>10</v>
+        <v>61</v>
       </c>
       <c r="K17" s="12">
-        <v>3</v>
-      </c>
-      <c r="L17" s="54" t="s">
-        <v>1791</v>
-      </c>
+        <f>9+2</f>
+        <v>11</v>
+      </c>
+      <c r="L17" s="54"/>
       <c r="M17" s="12"/>
       <c r="N17" s="12">
-        <v>6</v>
-      </c>
-      <c r="O17" s="12" t="s">
-        <v>1864</v>
-      </c>
-      <c r="P17" s="12" t="s">
-        <v>1865</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
       <c r="Q17" s="50">
-        <v>45547</v>
+        <v>45820</v>
       </c>
       <c r="R17" s="56">
-        <v>45558</v>
+        <v>45841</v>
       </c>
       <c r="S17" s="53"/>
       <c r="T17" s="12"/>
@@ -66982,6 +67008,7 @@
       <c r="X17" s="12"/>
       <c r="Y17" s="12"/>
       <c r="Z17" s="12"/>
+      <c r="AA17" s="12"/>
       <c r="AB17" s="12"/>
       <c r="AC17" s="12"/>
       <c r="AD17" s="12"/>
@@ -67015,9 +67042,9 @@
       <c r="BF17" s="12"/>
       <c r="BG17" s="12"/>
       <c r="BH17" s="12"/>
-      <c r="BI17" s="12"/>
-      <c r="BJ17" s="12"/>
-      <c r="BK17" s="12"/>
+      <c r="BI17" s="48"/>
+      <c r="BJ17" s="48"/>
+      <c r="BK17" s="48"/>
       <c r="BL17" s="12"/>
       <c r="BM17" s="12"/>
       <c r="BN17" s="12"/>
@@ -67041,43 +67068,52 @@
       <c r="CF17" s="12"/>
       <c r="CG17" s="12"/>
       <c r="CH17" s="12"/>
-    </row>
-    <row r="18" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
+      <c r="CI17" s="12"/>
+    </row>
+    <row r="18" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>1778</v>
+      </c>
       <c r="B18" s="15" t="s">
-        <v>1739</v>
-      </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12" t="s">
-        <v>1868</v>
-      </c>
-      <c r="H18" s="12" t="s">
-        <v>1716</v>
+        <v>1756</v>
+      </c>
+      <c r="C18" s="12"/>
+      <c r="D18" s="19" t="s">
+        <v>1622</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>1763</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>1768</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>1706</v>
       </c>
       <c r="I18" s="12">
+        <v>21</v>
+      </c>
+      <c r="J18" s="12">
+        <v>76</v>
+      </c>
+      <c r="K18" s="12">
         <v>8</v>
       </c>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
       <c r="L18" s="54"/>
       <c r="M18" s="12"/>
       <c r="N18" s="12">
-        <v>6</v>
-      </c>
-      <c r="O18" s="12" t="s">
-        <v>1864</v>
-      </c>
-      <c r="P18" s="12" t="s">
-        <v>1865</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
       <c r="Q18" s="50">
-        <v>45559</v>
+        <v>45953</v>
       </c>
       <c r="R18" s="56">
-        <v>45573</v>
+        <v>45978</v>
       </c>
       <c r="S18" s="53"/>
       <c r="T18" s="12"/>
@@ -67140,15 +67176,16 @@
       <c r="BY18" s="12"/>
       <c r="BZ18" s="12"/>
       <c r="CA18" s="12"/>
-      <c r="CB18" s="12"/>
-      <c r="CC18" s="12"/>
-      <c r="CD18" s="12"/>
-      <c r="CE18" s="12"/>
+      <c r="CB18" s="48"/>
+      <c r="CC18" s="48"/>
+      <c r="CD18" s="48"/>
+      <c r="CE18" s="48"/>
       <c r="CF18" s="12"/>
       <c r="CG18" s="12"/>
       <c r="CH18" s="12"/>
-    </row>
-    <row r="19" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CI18" s="12"/>
+    </row>
+    <row r="19" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>1777</v>
       </c>
@@ -67158,17 +67195,15 @@
       <c r="C19" s="15" t="s">
         <v>1739</v>
       </c>
-      <c r="D19" s="15" t="s">
-        <v>1746</v>
-      </c>
-      <c r="E19" s="15" t="s">
+      <c r="D19" s="16"/>
+      <c r="E19" s="17" t="s">
         <v>1784</v>
       </c>
       <c r="F19" s="22" t="s">
         <v>1745</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>187</v>
+        <v>1218</v>
       </c>
       <c r="H19" s="12" t="s">
         <v>1716</v>
@@ -67182,10 +67217,12 @@
       <c r="K19" s="12">
         <v>3</v>
       </c>
-      <c r="L19" s="54"/>
+      <c r="L19" s="54" t="s">
+        <v>1791</v>
+      </c>
       <c r="M19" s="12"/>
       <c r="N19" s="12">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="O19" s="12" t="s">
         <v>1864</v>
@@ -67194,10 +67231,10 @@
         <v>1865</v>
       </c>
       <c r="Q19" s="50">
-        <v>45579</v>
+        <v>45547</v>
       </c>
       <c r="R19" s="56">
-        <v>45589</v>
+        <v>45558</v>
       </c>
       <c r="S19" s="53"/>
       <c r="T19" s="12"/>
@@ -67267,18 +67304,27 @@
       <c r="CF19" s="12"/>
       <c r="CG19" s="12"/>
       <c r="CH19" s="12"/>
-    </row>
-    <row r="20" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
+      <c r="CI19" s="12"/>
+    </row>
+    <row r="20" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>1777</v>
+      </c>
       <c r="B20" s="15" t="s">
         <v>1739</v>
       </c>
       <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="22"/>
+      <c r="D20" s="15" t="s">
+        <v>1746</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>1784</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>1745</v>
+      </c>
       <c r="G20" s="12" t="s">
-        <v>777</v>
+        <v>187</v>
       </c>
       <c r="H20" s="12" t="s">
         <v>1716</v>
@@ -67286,24 +67332,28 @@
       <c r="I20" s="12">
         <v>8</v>
       </c>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
+      <c r="J20" s="12">
+        <v>10</v>
+      </c>
+      <c r="K20" s="12">
+        <v>3</v>
+      </c>
       <c r="L20" s="54"/>
-      <c r="M20" s="49"/>
+      <c r="M20" s="12"/>
       <c r="N20" s="12">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="O20" s="12" t="s">
         <v>1864</v>
       </c>
       <c r="P20" s="12" t="s">
-        <v>1859</v>
+        <v>1865</v>
       </c>
       <c r="Q20" s="50">
-        <v>45590</v>
+        <v>45579</v>
       </c>
       <c r="R20" s="56">
-        <v>45604</v>
+        <v>45589</v>
       </c>
       <c r="S20" s="53"/>
       <c r="T20" s="12"/>
@@ -67313,9 +67363,9 @@
       <c r="X20" s="12"/>
       <c r="Y20" s="12"/>
       <c r="Z20" s="12"/>
-      <c r="AA20" s="59"/>
-      <c r="AB20" s="59"/>
-      <c r="AC20" s="59"/>
+      <c r="AA20" s="12"/>
+      <c r="AB20" s="12"/>
+      <c r="AC20" s="12"/>
       <c r="AD20" s="12"/>
       <c r="AE20" s="12"/>
       <c r="AF20" s="12"/>
@@ -67373,17 +67423,16 @@
       <c r="CF20" s="12"/>
       <c r="CG20" s="12"/>
       <c r="CH20" s="12"/>
-    </row>
-    <row r="21" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CI20" s="12"/>
+    </row>
+    <row r="21" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>1777</v>
       </c>
       <c r="B21" s="15" t="s">
         <v>1739</v>
       </c>
-      <c r="C21" s="15" t="s">
-        <v>1739</v>
-      </c>
+      <c r="C21" s="15"/>
       <c r="D21" s="16" t="s">
         <v>1352</v>
       </c>
@@ -67419,7 +67468,7 @@
         <v>45726</v>
       </c>
       <c r="R21" s="56">
-        <v>45748</v>
+        <v>45747</v>
       </c>
       <c r="S21" s="53"/>
       <c r="T21" s="12"/>
@@ -67431,6 +67480,7 @@
       <c r="Z21" s="12"/>
       <c r="AA21" s="12"/>
       <c r="AB21" s="12"/>
+      <c r="AC21" s="12"/>
       <c r="AD21" s="12"/>
       <c r="AE21" s="12"/>
       <c r="AF21" s="12"/>
@@ -67447,10 +67497,10 @@
       <c r="AQ21" s="12"/>
       <c r="AR21" s="12"/>
       <c r="AS21" s="12"/>
-      <c r="AT21" s="48"/>
+      <c r="AT21" s="12"/>
       <c r="AU21" s="48"/>
       <c r="AV21" s="48"/>
-      <c r="AW21" s="12"/>
+      <c r="AW21" s="48"/>
       <c r="AX21" s="12"/>
       <c r="AY21" s="12"/>
       <c r="AZ21" s="12"/>
@@ -67488,39 +67538,40 @@
       <c r="CF21" s="12"/>
       <c r="CG21" s="12"/>
       <c r="CH21" s="12"/>
-    </row>
-    <row r="22" spans="1:86" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
-        <v>1778</v>
+      <c r="CI21" s="12"/>
+    </row>
+    <row r="22" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
+        <v>1777</v>
       </c>
       <c r="B22" s="15" t="s">
         <v>1739</v>
       </c>
-      <c r="C22" s="12"/>
-      <c r="D22" s="19" t="s">
-        <v>1765</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>1766</v>
-      </c>
-      <c r="F22" s="25" t="s">
-        <v>1764</v>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15" t="s">
+        <v>1742</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>1743</v>
+      </c>
+      <c r="F22" s="28" t="s">
+        <v>1744</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>1249</v>
+        <v>18</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
       <c r="I22" s="12">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J22" s="12">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="K22" s="12">
-        <f>15+5</f>
-        <v>20</v>
+        <f>3+8</f>
+        <v>11</v>
       </c>
       <c r="L22" s="54"/>
       <c r="M22" s="12"/>
@@ -67530,10 +67581,10 @@
       <c r="O22" s="12"/>
       <c r="P22" s="12"/>
       <c r="Q22" s="50">
-        <v>45749</v>
+        <v>45770</v>
       </c>
       <c r="R22" s="56">
-        <v>45769</v>
+        <v>45790</v>
       </c>
       <c r="S22" s="53"/>
       <c r="T22" s="12"/>
@@ -67546,7 +67597,6 @@
       <c r="AA22" s="12"/>
       <c r="AB22" s="12"/>
       <c r="AC22" s="12"/>
-      <c r="AD22" s="12"/>
       <c r="AE22" s="12"/>
       <c r="AF22" s="12"/>
       <c r="AG22" s="12"/>
@@ -67556,6 +67606,7 @@
       <c r="AK22" s="12"/>
       <c r="AL22" s="12"/>
       <c r="AM22" s="12"/>
+      <c r="AN22" s="12"/>
       <c r="AO22" s="12"/>
       <c r="AP22" s="12"/>
       <c r="AQ22" s="12"/>
@@ -67564,13 +67615,15 @@
       <c r="AT22" s="12"/>
       <c r="AU22" s="12"/>
       <c r="AV22" s="12"/>
-      <c r="AW22" s="48"/>
-      <c r="AX22" s="48"/>
-      <c r="AY22" s="48"/>
+      <c r="AW22" s="12"/>
+      <c r="AX22" s="12"/>
+      <c r="AY22" s="12"/>
       <c r="AZ22" s="12"/>
-      <c r="BA22" s="12"/>
-      <c r="BB22" s="12"/>
-      <c r="BC22" s="12"/>
+      <c r="BA22" s="48"/>
+      <c r="BB22" s="48"/>
+      <c r="BC22" s="48" t="s">
+        <v>1866</v>
+      </c>
       <c r="BD22" s="12"/>
       <c r="BE22" s="12"/>
       <c r="BF22" s="12"/>
@@ -67602,54 +67655,52 @@
       <c r="CF22" s="12"/>
       <c r="CG22" s="12"/>
       <c r="CH22" s="12"/>
-    </row>
-    <row r="23" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CI22" s="12"/>
+    </row>
+    <row r="23" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>1777</v>
       </c>
       <c r="B23" s="15" t="s">
         <v>1739</v>
       </c>
-      <c r="C23" s="15" t="s">
-        <v>1739</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>1742</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>1743</v>
-      </c>
-      <c r="F23" s="28" t="s">
-        <v>1744</v>
+      <c r="C23" s="15"/>
+      <c r="D23" s="19" t="s">
+        <v>1740</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>1783</v>
+      </c>
+      <c r="F23" s="30" t="s">
+        <v>1741</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>1681</v>
+        <v>17</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>1759</v>
       </c>
       <c r="I23" s="12">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="J23" s="12">
-        <v>35</v>
+        <v>78</v>
       </c>
       <c r="K23" s="12">
-        <f>3+8</f>
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="L23" s="54"/>
       <c r="M23" s="12"/>
       <c r="N23" s="12">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="O23" s="12"/>
       <c r="P23" s="12"/>
       <c r="Q23" s="50">
-        <v>45770</v>
+        <v>45979</v>
       </c>
       <c r="R23" s="56">
-        <v>45790</v>
+        <v>46010</v>
       </c>
       <c r="S23" s="53"/>
       <c r="T23" s="12"/>
@@ -67666,13 +67717,13 @@
       <c r="AE23" s="12"/>
       <c r="AF23" s="12"/>
       <c r="AG23" s="12"/>
+      <c r="AH23" s="12"/>
       <c r="AI23" s="12"/>
       <c r="AJ23" s="12"/>
       <c r="AK23" s="12"/>
       <c r="AL23" s="12"/>
       <c r="AM23" s="12"/>
       <c r="AN23" s="12"/>
-      <c r="AO23" s="12"/>
       <c r="AP23" s="12"/>
       <c r="AQ23" s="12"/>
       <c r="AR23" s="12"/>
@@ -67683,11 +67734,9 @@
       <c r="AW23" s="12"/>
       <c r="AX23" s="12"/>
       <c r="AY23" s="12"/>
-      <c r="AZ23" s="48"/>
-      <c r="BA23" s="48"/>
-      <c r="BB23" s="48" t="s">
-        <v>1867</v>
-      </c>
+      <c r="AZ23" s="12"/>
+      <c r="BA23" s="12"/>
+      <c r="BB23" s="12"/>
       <c r="BC23" s="12"/>
       <c r="BD23" s="12"/>
       <c r="BE23" s="12"/>
@@ -67717,54 +67766,47 @@
       <c r="CC23" s="12"/>
       <c r="CD23" s="12"/>
       <c r="CE23" s="12"/>
-      <c r="CF23" s="12"/>
-      <c r="CG23" s="12"/>
+      <c r="CF23" s="48"/>
+      <c r="CG23" s="48"/>
       <c r="CH23" s="12"/>
-    </row>
-    <row r="24" spans="1:86" x14ac:dyDescent="0.25">
-      <c r="A24" s="12" t="s">
-        <v>1778</v>
-      </c>
+      <c r="CI23" s="12"/>
+    </row>
+    <row r="24" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="14"/>
       <c r="B24" s="15" t="s">
         <v>1739</v>
       </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="19" t="s">
-        <v>1769</v>
-      </c>
-      <c r="E24" s="21" t="s">
-        <v>1763</v>
-      </c>
-      <c r="F24" s="20" t="s">
-        <v>1770</v>
-      </c>
-      <c r="G24" s="10" t="s">
+      <c r="C24" s="15"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12" t="s">
+        <v>1867</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>1716</v>
+      </c>
+      <c r="I24" s="12">
         <v>8</v>
       </c>
-      <c r="H24" s="10" t="s">
-        <v>1707</v>
-      </c>
-      <c r="I24" s="12">
-        <v>18</v>
-      </c>
-      <c r="J24" s="12">
-        <v>5</v>
-      </c>
-      <c r="K24" s="12">
-        <v>4</v>
-      </c>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
       <c r="L24" s="54"/>
       <c r="M24" s="12"/>
       <c r="N24" s="12">
-        <v>20</v>
-      </c>
-      <c r="O24" s="12"/>
-      <c r="P24" s="12"/>
+        <v>6</v>
+      </c>
+      <c r="O24" s="12" t="s">
+        <v>1864</v>
+      </c>
+      <c r="P24" s="12" t="s">
+        <v>1865</v>
+      </c>
       <c r="Q24" s="50">
-        <v>45867</v>
+        <v>45559</v>
       </c>
       <c r="R24" s="56">
-        <v>45903</v>
+        <v>45573</v>
       </c>
       <c r="S24" s="53"/>
       <c r="T24" s="12"/>
@@ -67782,7 +67824,6 @@
       <c r="AF24" s="12"/>
       <c r="AG24" s="12"/>
       <c r="AH24" s="12"/>
-      <c r="AI24" s="12"/>
       <c r="AJ24" s="12"/>
       <c r="AK24" s="12"/>
       <c r="AL24" s="12"/>
@@ -67798,6 +67839,10 @@
       <c r="AV24" s="12"/>
       <c r="AW24" s="12"/>
       <c r="AX24" s="12"/>
+      <c r="AY24" s="12"/>
+      <c r="AZ24" s="12"/>
+      <c r="BA24" s="12"/>
+      <c r="BB24" s="12"/>
       <c r="BC24" s="12"/>
       <c r="BD24" s="12"/>
       <c r="BE24" s="12"/>
@@ -67811,10 +67856,10 @@
       <c r="BM24" s="12"/>
       <c r="BN24" s="12"/>
       <c r="BO24" s="12"/>
-      <c r="BP24" s="48"/>
-      <c r="BQ24" s="48"/>
-      <c r="BR24" s="48"/>
-      <c r="BS24" s="48"/>
+      <c r="BP24" s="12"/>
+      <c r="BQ24" s="12"/>
+      <c r="BR24" s="12"/>
+      <c r="BS24" s="12"/>
       <c r="BT24" s="12"/>
       <c r="BU24" s="12"/>
       <c r="BV24" s="12"/>
@@ -67830,53 +67875,44 @@
       <c r="CF24" s="12"/>
       <c r="CG24" s="12"/>
       <c r="CH24" s="12"/>
-    </row>
-    <row r="25" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
-        <v>1777</v>
-      </c>
+      <c r="CI24" s="12"/>
+    </row>
+    <row r="25" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
       <c r="B25" s="15" t="s">
         <v>1739</v>
       </c>
-      <c r="C25" s="15" t="s">
-        <v>1739</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>1740</v>
-      </c>
-      <c r="E25" s="29" t="s">
-        <v>1783</v>
-      </c>
-      <c r="F25" s="30" t="s">
-        <v>1741</v>
-      </c>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="22"/>
       <c r="G25" s="12" t="s">
-        <v>17</v>
+        <v>777</v>
       </c>
       <c r="H25" s="12" t="s">
-        <v>1759</v>
+        <v>1716</v>
       </c>
       <c r="I25" s="12">
-        <v>22</v>
-      </c>
-      <c r="J25" s="12">
-        <v>78</v>
-      </c>
-      <c r="K25" s="12">
-        <v>25</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
       <c r="L25" s="54"/>
-      <c r="M25" s="12"/>
+      <c r="M25" s="49"/>
       <c r="N25" s="12">
-        <v>20</v>
-      </c>
-      <c r="O25" s="12"/>
-      <c r="P25" s="12"/>
-      <c r="Q25" s="12">
-        <v>45980</v>
-      </c>
-      <c r="R25" s="54">
-        <v>46009</v>
+        <v>3</v>
+      </c>
+      <c r="O25" s="12" t="s">
+        <v>1864</v>
+      </c>
+      <c r="P25" s="12" t="s">
+        <v>1859</v>
+      </c>
+      <c r="Q25" s="50">
+        <v>45590</v>
+      </c>
+      <c r="R25" s="56">
+        <v>45611</v>
       </c>
       <c r="S25" s="53"/>
       <c r="T25" s="12"/>
@@ -67886,9 +67922,9 @@
       <c r="X25" s="12"/>
       <c r="Y25" s="12"/>
       <c r="Z25" s="12"/>
-      <c r="AA25" s="12"/>
+      <c r="AA25" s="59"/>
       <c r="AB25" s="12"/>
-      <c r="AC25" s="12"/>
+      <c r="AC25" s="59"/>
       <c r="AD25" s="12"/>
       <c r="AE25" s="12"/>
       <c r="AF25" s="12"/>
@@ -67911,9 +67947,9 @@
       <c r="AW25" s="12"/>
       <c r="AX25" s="12"/>
       <c r="AY25" s="12"/>
-      <c r="AZ25" s="12"/>
-      <c r="BA25" s="12"/>
-      <c r="BB25" s="12"/>
+      <c r="BD25" s="12"/>
+      <c r="BE25" s="12"/>
+      <c r="BF25" s="12"/>
       <c r="BG25" s="12"/>
       <c r="BH25" s="12"/>
       <c r="BI25" s="12"/>
@@ -67938,55 +67974,57 @@
       <c r="CB25" s="12"/>
       <c r="CC25" s="12"/>
       <c r="CD25" s="12"/>
-      <c r="CE25" s="48"/>
-      <c r="CF25" s="48"/>
-      <c r="CG25" s="48"/>
+      <c r="CE25" s="12"/>
+      <c r="CF25" s="12"/>
+      <c r="CG25" s="12"/>
       <c r="CH25" s="12"/>
-    </row>
-    <row r="26" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI25" s="12"/>
+    </row>
+    <row r="26" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>1778</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>1870</v>
+        <v>1739</v>
       </c>
       <c r="C26" s="12"/>
       <c r="D26" s="19" t="s">
-        <v>1774</v>
+        <v>1765</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>1763</v>
+        <v>1766</v>
       </c>
       <c r="F26" s="25" t="s">
         <v>1764</v>
       </c>
-      <c r="G26" s="10" t="s">
-        <v>227</v>
-      </c>
-      <c r="H26" s="10" t="s">
-        <v>1690</v>
+      <c r="G26" s="12" t="s">
+        <v>1249</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>1682</v>
       </c>
       <c r="I26" s="12">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J26" s="12">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="K26" s="12">
-        <v>5</v>
+        <f>15+5</f>
+        <v>20</v>
       </c>
       <c r="L26" s="54"/>
       <c r="M26" s="12"/>
       <c r="N26" s="12">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="O26" s="12"/>
       <c r="P26" s="12"/>
       <c r="Q26" s="50">
-        <v>45791</v>
+        <v>45748</v>
       </c>
       <c r="R26" s="56">
-        <v>45819</v>
+        <v>45769</v>
       </c>
       <c r="S26" s="53"/>
       <c r="T26" s="12"/>
@@ -68010,6 +68048,7 @@
       <c r="AL26" s="12"/>
       <c r="AM26" s="12"/>
       <c r="AN26" s="12"/>
+      <c r="AO26" s="12"/>
       <c r="AP26" s="12"/>
       <c r="AQ26" s="12"/>
       <c r="AR26" s="12"/>
@@ -68018,15 +68057,12 @@
       <c r="AU26" s="12"/>
       <c r="AV26" s="12"/>
       <c r="AW26" s="12"/>
-      <c r="AX26" s="12"/>
-      <c r="AZ26" s="12"/>
+      <c r="AX26" s="48"/>
+      <c r="AY26" s="48"/>
+      <c r="AZ26" s="48"/>
       <c r="BA26" s="12"/>
       <c r="BB26" s="12"/>
-      <c r="BC26" s="48"/>
-      <c r="BD26" s="48"/>
-      <c r="BE26" s="48"/>
-      <c r="BF26" s="48"/>
-      <c r="BG26" s="48"/>
+      <c r="BC26" s="12"/>
       <c r="BH26" s="12"/>
       <c r="BI26" s="12"/>
       <c r="BJ26" s="12"/>
@@ -68054,51 +68090,52 @@
       <c r="CF26" s="12"/>
       <c r="CG26" s="12"/>
       <c r="CH26" s="12"/>
-    </row>
-    <row r="27" spans="1:86" x14ac:dyDescent="0.25">
+      <c r="CI26" s="12"/>
+    </row>
+    <row r="27" spans="1:87" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>1778</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>1870</v>
+        <v>1739</v>
       </c>
       <c r="C27" s="12"/>
       <c r="D27" s="19" t="s">
-        <v>1562</v>
+        <v>1769</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>1772</v>
+        <v>1763</v>
       </c>
       <c r="F27" s="20" t="s">
-        <v>1768</v>
+        <v>1770</v>
       </c>
       <c r="G27" s="10" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="H27" s="10" t="s">
-        <v>1101</v>
+        <v>1707</v>
       </c>
       <c r="I27" s="12">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J27" s="12">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K27" s="12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L27" s="54"/>
       <c r="M27" s="12"/>
       <c r="N27" s="12">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="O27" s="12"/>
       <c r="P27" s="12"/>
       <c r="Q27" s="50">
-        <v>45904</v>
+        <v>45863</v>
       </c>
       <c r="R27" s="56">
-        <v>45928</v>
+        <v>45901</v>
       </c>
       <c r="S27" s="53"/>
       <c r="T27" s="12"/>
@@ -68123,7 +68160,6 @@
       <c r="AM27" s="12"/>
       <c r="AN27" s="12"/>
       <c r="AO27" s="12"/>
-      <c r="AP27" s="12"/>
       <c r="AQ27" s="12"/>
       <c r="AR27" s="12"/>
       <c r="AS27" s="12"/>
@@ -68133,7 +68169,6 @@
       <c r="AW27" s="12"/>
       <c r="AX27" s="12"/>
       <c r="AY27" s="12"/>
-      <c r="AZ27" s="12"/>
       <c r="BA27" s="12"/>
       <c r="BB27" s="12"/>
       <c r="BC27" s="12"/>
@@ -68150,12 +68185,12 @@
       <c r="BN27" s="12"/>
       <c r="BO27" s="12"/>
       <c r="BP27" s="12"/>
-      <c r="BQ27" s="12"/>
-      <c r="BR27" s="12"/>
-      <c r="BS27" s="12"/>
+      <c r="BQ27" s="48"/>
+      <c r="BR27" s="48"/>
+      <c r="BS27" s="48"/>
       <c r="BT27" s="48"/>
-      <c r="BU27" s="48"/>
-      <c r="BV27" s="48"/>
+      <c r="BU27" s="12"/>
+      <c r="BV27" s="12"/>
       <c r="BW27" s="12"/>
       <c r="BX27" s="12"/>
       <c r="BY27" s="12"/>
@@ -68168,47 +68203,52 @@
       <c r="CF27" s="12"/>
       <c r="CG27" s="12"/>
       <c r="CH27" s="12"/>
-    </row>
-    <row r="28" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
+      <c r="CI27" s="12"/>
+    </row>
+    <row r="28" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="A28" s="12" t="s">
         <v>1778</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>1836</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>1836</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>1837</v>
-      </c>
-      <c r="E28" s="17" t="s">
-        <v>1838</v>
-      </c>
-      <c r="F28" s="22"/>
-      <c r="G28" s="49" t="s">
-        <v>1839</v>
-      </c>
-      <c r="H28" s="49" t="s">
-        <v>1730</v>
-      </c>
-      <c r="I28" s="49">
-        <v>8.1</v>
-      </c>
-      <c r="J28" s="49"/>
-      <c r="K28" s="49"/>
-      <c r="L28" s="55"/>
-      <c r="M28" s="49"/>
-      <c r="N28" s="49">
-        <v>10</v>
-      </c>
-      <c r="O28" s="49"/>
-      <c r="P28" s="49"/>
-      <c r="Q28" s="51">
-        <v>45607</v>
-      </c>
-      <c r="R28" s="57">
-        <v>45624</v>
+        <v>1869</v>
+      </c>
+      <c r="C28" s="12"/>
+      <c r="D28" s="19" t="s">
+        <v>1774</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>1763</v>
+      </c>
+      <c r="F28" s="25" t="s">
+        <v>1764</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="H28" s="10" t="s">
+        <v>1690</v>
+      </c>
+      <c r="I28" s="12">
+        <v>15</v>
+      </c>
+      <c r="J28" s="12">
+        <v>11</v>
+      </c>
+      <c r="K28" s="12">
+        <v>5</v>
+      </c>
+      <c r="L28" s="54"/>
+      <c r="M28" s="12"/>
+      <c r="N28" s="12">
+        <v>20</v>
+      </c>
+      <c r="O28" s="12"/>
+      <c r="P28" s="12"/>
+      <c r="Q28" s="50">
+        <v>45791</v>
+      </c>
+      <c r="R28" s="56">
+        <v>45819</v>
       </c>
       <c r="S28" s="53"/>
       <c r="T28" s="12"/>
@@ -68221,9 +68261,9 @@
       <c r="AA28" s="12"/>
       <c r="AB28" s="12"/>
       <c r="AC28" s="12"/>
-      <c r="AD28" s="48"/>
-      <c r="AE28" s="48"/>
-      <c r="AF28" s="48"/>
+      <c r="AD28" s="12"/>
+      <c r="AE28" s="12"/>
+      <c r="AF28" s="12"/>
       <c r="AG28" s="12"/>
       <c r="AH28" s="12"/>
       <c r="AI28" s="12"/>
@@ -68247,10 +68287,11 @@
       <c r="BA28" s="12"/>
       <c r="BB28" s="12"/>
       <c r="BC28" s="12"/>
-      <c r="BD28" s="12"/>
-      <c r="BE28" s="12"/>
-      <c r="BG28" s="12"/>
-      <c r="BH28" s="12"/>
+      <c r="BD28" s="48"/>
+      <c r="BE28" s="48"/>
+      <c r="BF28" s="48"/>
+      <c r="BG28" s="48"/>
+      <c r="BH28" s="48"/>
       <c r="BI28" s="12"/>
       <c r="BJ28" s="12"/>
       <c r="BK28" s="12"/>
@@ -68277,45 +68318,52 @@
       <c r="CF28" s="12"/>
       <c r="CG28" s="12"/>
       <c r="CH28" s="12"/>
-    </row>
-    <row r="29" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
+      <c r="CI28" s="12"/>
+    </row>
+    <row r="29" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="A29" s="12" t="s">
         <v>1778</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>1836</v>
+        <v>1869</v>
       </c>
       <c r="C29" s="12"/>
-      <c r="D29" s="15" t="s">
-        <v>1840</v>
-      </c>
-      <c r="E29" s="17" t="s">
-        <v>1838</v>
-      </c>
-      <c r="F29" s="22"/>
-      <c r="G29" s="49" t="s">
-        <v>1841</v>
-      </c>
-      <c r="H29" s="49" t="s">
-        <v>1716</v>
-      </c>
-      <c r="I29" s="49">
-        <v>8.1</v>
-      </c>
-      <c r="J29" s="49"/>
-      <c r="K29" s="49"/>
-      <c r="L29" s="55"/>
-      <c r="M29" s="49"/>
-      <c r="N29" s="49">
-        <v>10</v>
-      </c>
-      <c r="O29" s="49"/>
-      <c r="P29" s="49"/>
-      <c r="Q29" s="51">
-        <v>45625</v>
-      </c>
-      <c r="R29" s="57">
-        <v>45639</v>
+      <c r="D29" s="19" t="s">
+        <v>1562</v>
+      </c>
+      <c r="E29" s="21" t="s">
+        <v>1772</v>
+      </c>
+      <c r="F29" s="20" t="s">
+        <v>1768</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>1101</v>
+      </c>
+      <c r="I29" s="12">
+        <v>19</v>
+      </c>
+      <c r="J29" s="12">
+        <v>4</v>
+      </c>
+      <c r="K29" s="12">
+        <v>3</v>
+      </c>
+      <c r="L29" s="54"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12">
+        <v>16</v>
+      </c>
+      <c r="O29" s="12"/>
+      <c r="P29" s="12"/>
+      <c r="Q29" s="50">
+        <v>45902</v>
+      </c>
+      <c r="R29" s="56">
+        <v>45925</v>
       </c>
       <c r="S29" s="53"/>
       <c r="T29" s="12"/>
@@ -68330,9 +68378,9 @@
       <c r="AC29" s="12"/>
       <c r="AD29" s="12"/>
       <c r="AE29" s="12"/>
-      <c r="AF29" s="48"/>
-      <c r="AG29" s="48"/>
-      <c r="AH29" s="48"/>
+      <c r="AF29" s="12"/>
+      <c r="AG29" s="12"/>
+      <c r="AH29" s="12"/>
       <c r="AI29" s="12"/>
       <c r="AJ29" s="12"/>
       <c r="AK29" s="12"/>
@@ -68357,7 +68405,6 @@
       <c r="BD29" s="12"/>
       <c r="BE29" s="12"/>
       <c r="BF29" s="12"/>
-      <c r="BG29" s="12"/>
       <c r="BH29" s="12"/>
       <c r="BI29" s="12"/>
       <c r="BJ29" s="12"/>
@@ -68371,9 +68418,9 @@
       <c r="BR29" s="12"/>
       <c r="BS29" s="12"/>
       <c r="BT29" s="12"/>
-      <c r="BU29" s="12"/>
-      <c r="BV29" s="12"/>
-      <c r="BW29" s="12"/>
+      <c r="BU29" s="48"/>
+      <c r="BV29" s="48"/>
+      <c r="BW29" s="48"/>
       <c r="BX29" s="12"/>
       <c r="BY29" s="12"/>
       <c r="BZ29" s="12"/>
@@ -68385,27 +68432,30 @@
       <c r="CF29" s="12"/>
       <c r="CG29" s="12"/>
       <c r="CH29" s="12"/>
-    </row>
-    <row r="30" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CI29" s="12"/>
+    </row>
+    <row r="30" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>1778</v>
       </c>
       <c r="B30" s="15" t="s">
         <v>1836</v>
       </c>
-      <c r="C30" s="12"/>
+      <c r="C30" s="15" t="s">
+        <v>1836</v>
+      </c>
       <c r="D30" s="15" t="s">
-        <v>1842</v>
+        <v>1837</v>
       </c>
       <c r="E30" s="17" t="s">
         <v>1838</v>
       </c>
       <c r="F30" s="22"/>
       <c r="G30" s="49" t="s">
-        <v>1843</v>
+        <v>1839</v>
       </c>
       <c r="H30" s="49" t="s">
-        <v>1716</v>
+        <v>1730</v>
       </c>
       <c r="I30" s="49">
         <v>8.1</v>
@@ -68413,17 +68463,17 @@
       <c r="J30" s="49"/>
       <c r="K30" s="49"/>
       <c r="L30" s="55"/>
-      <c r="M30" s="12"/>
+      <c r="M30" s="49"/>
       <c r="N30" s="49">
         <v>10</v>
       </c>
       <c r="O30" s="49"/>
       <c r="P30" s="49"/>
       <c r="Q30" s="51">
-        <v>45642</v>
+        <v>45614</v>
       </c>
       <c r="R30" s="57">
-        <v>45657</v>
+        <v>45629</v>
       </c>
       <c r="S30" s="53"/>
       <c r="T30" s="12"/>
@@ -68436,13 +68486,13 @@
       <c r="AA30" s="12"/>
       <c r="AB30" s="12"/>
       <c r="AC30" s="12"/>
-      <c r="AD30" s="12"/>
-      <c r="AE30" s="12"/>
-      <c r="AF30" s="12"/>
+      <c r="AD30" s="48"/>
+      <c r="AE30" s="48"/>
+      <c r="AF30" s="48"/>
       <c r="AG30" s="12"/>
-      <c r="AH30" s="48"/>
-      <c r="AI30" s="48"/>
-      <c r="AJ30" s="48"/>
+      <c r="AH30" s="12"/>
+      <c r="AI30" s="12"/>
+      <c r="AJ30" s="12"/>
       <c r="AK30" s="12"/>
       <c r="AL30" s="12"/>
       <c r="AM30" s="12"/>
@@ -68480,6 +68530,10 @@
       <c r="BS30" s="12"/>
       <c r="BT30" s="12"/>
       <c r="BU30" s="12"/>
+      <c r="BV30" s="12"/>
+      <c r="BW30" s="12"/>
+      <c r="BX30" s="12"/>
+      <c r="BY30" s="12"/>
       <c r="BZ30" s="12"/>
       <c r="CA30" s="12"/>
       <c r="CB30" s="12"/>
@@ -68488,41 +68542,48 @@
       <c r="CE30" s="12"/>
       <c r="CF30" s="12"/>
       <c r="CG30" s="12"/>
-      <c r="CH30" s="46"/>
-    </row>
-    <row r="31" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CH30" s="12"/>
+      <c r="CI30" s="12"/>
+    </row>
+    <row r="31" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
-        <v>1777</v>
+        <v>1778</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>1874</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>1874</v>
-      </c>
+        <v>1836</v>
+      </c>
+      <c r="C31" s="12"/>
       <c r="D31" s="15" t="s">
-        <v>1875</v>
+        <v>1840</v>
       </c>
       <c r="E31" s="17" t="s">
         <v>1838</v>
       </c>
-      <c r="F31" s="30"/>
-      <c r="G31" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="H31" s="10" t="s">
-        <v>1075</v>
-      </c>
-      <c r="I31" s="12"/>
-      <c r="J31" s="12"/>
-      <c r="K31" s="12"/>
-      <c r="L31" s="54"/>
-      <c r="M31" s="12"/>
-      <c r="N31" s="12"/>
-      <c r="O31" s="12"/>
-      <c r="P31" s="12"/>
-      <c r="Q31" s="12"/>
-      <c r="R31" s="12"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="49" t="s">
+        <v>1841</v>
+      </c>
+      <c r="H31" s="49" t="s">
+        <v>1716</v>
+      </c>
+      <c r="I31" s="49">
+        <v>8.1</v>
+      </c>
+      <c r="J31" s="49"/>
+      <c r="K31" s="49"/>
+      <c r="L31" s="55"/>
+      <c r="M31" s="49"/>
+      <c r="N31" s="49">
+        <v>10</v>
+      </c>
+      <c r="O31" s="49"/>
+      <c r="P31" s="49"/>
+      <c r="Q31" s="51">
+        <v>45630</v>
+      </c>
+      <c r="R31" s="57">
+        <v>45644</v>
+      </c>
       <c r="S31" s="53"/>
       <c r="T31" s="12"/>
       <c r="U31" s="12"/>
@@ -68537,9 +68598,9 @@
       <c r="AD31" s="12"/>
       <c r="AE31" s="12"/>
       <c r="AF31" s="12"/>
-      <c r="AG31" s="12"/>
-      <c r="AH31" s="12"/>
-      <c r="AI31" s="12"/>
+      <c r="AG31" s="48"/>
+      <c r="AH31" s="48"/>
+      <c r="AI31" s="48"/>
       <c r="AJ31" s="12"/>
       <c r="AK31" s="12"/>
       <c r="AL31" s="12"/>
@@ -68579,10 +68640,6 @@
       <c r="BT31" s="12"/>
       <c r="BU31" s="12"/>
       <c r="BV31" s="12"/>
-      <c r="BW31" s="12"/>
-      <c r="BX31" s="12"/>
-      <c r="BY31" s="12"/>
-      <c r="BZ31" s="12"/>
       <c r="CA31" s="12"/>
       <c r="CB31" s="12"/>
       <c r="CC31" s="12"/>
@@ -68590,41 +68647,48 @@
       <c r="CE31" s="12"/>
       <c r="CF31" s="12"/>
       <c r="CG31" s="12"/>
-      <c r="CH31" s="48"/>
-    </row>
-    <row r="32" spans="1:86" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CH31" s="46"/>
+      <c r="CI31" s="46"/>
+    </row>
+    <row r="32" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
-        <v>1777</v>
+        <v>1778</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>1874</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>1874</v>
-      </c>
+        <v>1836</v>
+      </c>
+      <c r="C32" s="12"/>
       <c r="D32" s="15" t="s">
-        <v>1876</v>
+        <v>1842</v>
       </c>
       <c r="E32" s="17" t="s">
         <v>1838</v>
       </c>
-      <c r="F32" s="30"/>
-      <c r="G32" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="H32" s="10" t="s">
-        <v>1075</v>
-      </c>
-      <c r="I32" s="12"/>
-      <c r="J32" s="12"/>
-      <c r="K32" s="12"/>
-      <c r="L32" s="54"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="49" t="s">
+        <v>1843</v>
+      </c>
+      <c r="H32" s="49" t="s">
+        <v>1716</v>
+      </c>
+      <c r="I32" s="49">
+        <v>8.1</v>
+      </c>
+      <c r="J32" s="49"/>
+      <c r="K32" s="49"/>
+      <c r="L32" s="55"/>
       <c r="M32" s="12"/>
-      <c r="N32" s="12"/>
-      <c r="O32" s="12"/>
-      <c r="P32" s="12"/>
-      <c r="Q32" s="12"/>
-      <c r="R32" s="12"/>
+      <c r="N32" s="49">
+        <v>10</v>
+      </c>
+      <c r="O32" s="49"/>
+      <c r="P32" s="49"/>
+      <c r="Q32" s="51">
+        <v>45645</v>
+      </c>
+      <c r="R32" s="57">
+        <v>45663</v>
+      </c>
       <c r="S32" s="53"/>
       <c r="T32" s="12"/>
       <c r="U32" s="12"/>
@@ -68641,9 +68705,9 @@
       <c r="AF32" s="12"/>
       <c r="AG32" s="12"/>
       <c r="AH32" s="12"/>
-      <c r="AI32" s="12"/>
-      <c r="AJ32" s="12"/>
-      <c r="AK32" s="12"/>
+      <c r="AI32" s="48"/>
+      <c r="AJ32" s="48"/>
+      <c r="AK32" s="48"/>
       <c r="AL32" s="12"/>
       <c r="AM32" s="12"/>
       <c r="AN32" s="12"/>
@@ -68692,20 +68756,19 @@
       <c r="CE32" s="12"/>
       <c r="CF32" s="12"/>
       <c r="CG32" s="12"/>
-      <c r="CH32" s="12"/>
+      <c r="CH32" s="48"/>
+      <c r="CI32" s="48"/>
     </row>
     <row r="33" spans="1:91" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>1777</v>
       </c>
-      <c r="B33" s="60" t="s">
+      <c r="B33" s="15" t="s">
+        <v>1873</v>
+      </c>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15" t="s">
         <v>1874</v>
-      </c>
-      <c r="C33" s="60" t="s">
-        <v>1874</v>
-      </c>
-      <c r="D33" s="15" t="s">
-        <v>1877</v>
       </c>
       <c r="E33" s="17" t="s">
         <v>1838</v>
@@ -68735,49 +68798,49 @@
       <c r="X33" s="12"/>
       <c r="Y33" s="12"/>
       <c r="Z33" s="12"/>
-      <c r="AA33" s="12"/>
-      <c r="AB33" s="12"/>
-      <c r="AC33" s="12"/>
-      <c r="AD33" s="12"/>
-      <c r="AE33" s="12"/>
-      <c r="AF33" s="12"/>
-      <c r="AG33" s="12"/>
-      <c r="AH33" s="12"/>
-      <c r="AI33" s="12"/>
-      <c r="AJ33" s="12"/>
-      <c r="AK33" s="12"/>
-      <c r="AL33" s="12"/>
-      <c r="AM33" s="12"/>
-      <c r="AN33" s="12"/>
-      <c r="AO33" s="12"/>
-      <c r="AP33" s="12"/>
-      <c r="AQ33" s="12"/>
-      <c r="AR33" s="12"/>
-      <c r="AS33" s="12"/>
-      <c r="AT33" s="12"/>
-      <c r="AU33" s="12"/>
-      <c r="AV33" s="12"/>
-      <c r="AW33" s="12"/>
-      <c r="AX33" s="12"/>
-      <c r="AY33" s="12"/>
-      <c r="AZ33" s="12"/>
-      <c r="BA33" s="12"/>
-      <c r="BB33" s="12"/>
-      <c r="BC33" s="12"/>
-      <c r="BD33" s="12"/>
-      <c r="BE33" s="12"/>
-      <c r="BF33" s="12"/>
-      <c r="BG33" s="12"/>
-      <c r="BH33" s="12"/>
-      <c r="BI33" s="12"/>
-      <c r="BJ33" s="12"/>
-      <c r="BK33" s="12"/>
-      <c r="BL33" s="12"/>
-      <c r="BM33" s="12"/>
-      <c r="BN33" s="12"/>
-      <c r="BO33" s="12"/>
-      <c r="BP33" s="12"/>
-      <c r="BQ33" s="12"/>
+      <c r="AA33" s="67"/>
+      <c r="AB33" s="67"/>
+      <c r="AC33" s="67"/>
+      <c r="AD33" s="67"/>
+      <c r="AE33" s="67"/>
+      <c r="AF33" s="67"/>
+      <c r="AG33" s="67"/>
+      <c r="AH33" s="67"/>
+      <c r="AI33" s="67"/>
+      <c r="AJ33" s="67"/>
+      <c r="AK33" s="67"/>
+      <c r="AL33" s="67"/>
+      <c r="AM33" s="67"/>
+      <c r="AN33" s="67"/>
+      <c r="AO33" s="67"/>
+      <c r="AP33" s="67"/>
+      <c r="AQ33" s="67"/>
+      <c r="AR33" s="67"/>
+      <c r="AS33" s="67"/>
+      <c r="AT33" s="67"/>
+      <c r="AU33" s="67"/>
+      <c r="AV33" s="67"/>
+      <c r="AW33" s="67"/>
+      <c r="AX33" s="67"/>
+      <c r="AY33" s="67"/>
+      <c r="AZ33" s="67"/>
+      <c r="BA33" s="67"/>
+      <c r="BB33" s="67"/>
+      <c r="BC33" s="67"/>
+      <c r="BD33" s="67"/>
+      <c r="BE33" s="67"/>
+      <c r="BF33" s="67"/>
+      <c r="BG33" s="67"/>
+      <c r="BH33" s="67"/>
+      <c r="BI33" s="67"/>
+      <c r="BJ33" s="67"/>
+      <c r="BK33" s="67"/>
+      <c r="BL33" s="67"/>
+      <c r="BM33" s="67"/>
+      <c r="BN33" s="67"/>
+      <c r="BO33" s="67"/>
+      <c r="BP33" s="67"/>
+      <c r="BQ33" s="67"/>
       <c r="BR33" s="12"/>
       <c r="BS33" s="12"/>
       <c r="BT33" s="12"/>
@@ -68795,19 +68858,18 @@
       <c r="CF33" s="12"/>
       <c r="CG33" s="12"/>
       <c r="CH33" s="12"/>
+      <c r="CI33" s="12"/>
     </row>
     <row r="34" spans="1:91" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
         <v>1777</v>
       </c>
-      <c r="B34" s="60" t="s">
-        <v>1874</v>
-      </c>
-      <c r="C34" s="60" t="s">
-        <v>1874</v>
-      </c>
+      <c r="B34" s="72" t="s">
+        <v>1873</v>
+      </c>
+      <c r="C34" s="72"/>
       <c r="D34" s="15" t="s">
-        <v>1878</v>
+        <v>1875</v>
       </c>
       <c r="E34" s="17" t="s">
         <v>1838</v>
@@ -68897,28 +68959,29 @@
       <c r="CF34" s="12"/>
       <c r="CG34" s="12"/>
       <c r="CH34" s="12"/>
+      <c r="CI34" s="12"/>
     </row>
     <row r="35" spans="1:91" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>1777</v>
       </c>
-      <c r="B35" s="60" t="s">
+      <c r="B35" s="72" t="s">
         <v>1873</v>
       </c>
-      <c r="C35" s="60" t="s">
-        <v>1871</v>
-      </c>
-      <c r="D35" s="19" t="s">
-        <v>1872</v>
-      </c>
-      <c r="E35" s="29" t="s">
-        <v>1783</v>
+      <c r="C35" s="72"/>
+      <c r="D35" s="15" t="s">
+        <v>1876</v>
+      </c>
+      <c r="E35" s="17" t="s">
+        <v>1838</v>
       </c>
       <c r="F35" s="30"/>
       <c r="G35" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="H35" s="10"/>
+        <v>31</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>1075</v>
+      </c>
       <c r="I35" s="12"/>
       <c r="J35" s="12"/>
       <c r="K35" s="12"/>
@@ -68997,49 +69060,39 @@
       <c r="CF35" s="12"/>
       <c r="CG35" s="12"/>
       <c r="CH35" s="12"/>
+      <c r="CI35" s="12"/>
     </row>
     <row r="36" spans="1:91" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="14"/>
-      <c r="B36" s="60"/>
-      <c r="C36" s="60" t="s">
-        <v>1879</v>
-      </c>
+      <c r="A36" s="14" t="s">
+        <v>1777</v>
+      </c>
+      <c r="B36" s="72" t="s">
+        <v>1873</v>
+      </c>
+      <c r="C36" s="72"/>
       <c r="D36" s="15" t="s">
-        <v>1879</v>
-      </c>
-      <c r="E36" s="15" t="s">
-        <v>1879</v>
-      </c>
-      <c r="F36" s="15" t="s">
-        <v>1879</v>
-      </c>
-      <c r="G36" s="15" t="s">
-        <v>1879</v>
-      </c>
-      <c r="H36" s="15" t="s">
-        <v>1879</v>
-      </c>
-      <c r="I36" s="12">
-        <v>8</v>
-      </c>
+        <v>1877</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>1838</v>
+      </c>
+      <c r="F36" s="30"/>
+      <c r="G36" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H36" s="10" t="s">
+        <v>1075</v>
+      </c>
+      <c r="I36" s="12"/>
       <c r="J36" s="12"/>
       <c r="K36" s="12"/>
       <c r="L36" s="54"/>
-      <c r="N36" s="12">
-        <v>3</v>
-      </c>
-      <c r="O36" s="12" t="s">
-        <v>1864</v>
-      </c>
-      <c r="P36" s="12" t="s">
-        <v>1865</v>
-      </c>
-      <c r="Q36" s="63">
-        <v>45574</v>
-      </c>
-      <c r="R36" s="63">
-        <v>45579</v>
-      </c>
+      <c r="M36" s="12"/>
+      <c r="N36" s="12"/>
+      <c r="O36" s="12"/>
+      <c r="P36" s="12"/>
+      <c r="Q36" s="12"/>
+      <c r="R36" s="12"/>
       <c r="S36" s="53"/>
       <c r="T36" s="12"/>
       <c r="U36" s="12"/>
@@ -69108,228 +69161,322 @@
       <c r="CF36" s="12"/>
       <c r="CG36" s="12"/>
       <c r="CH36" s="12"/>
-    </row>
-    <row r="37" spans="1:91" s="66" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="64"/>
-      <c r="B37" s="65"/>
-      <c r="C37" s="65"/>
-      <c r="D37" s="64"/>
-      <c r="E37" s="65"/>
-      <c r="F37" s="65"/>
-      <c r="G37" s="64"/>
-      <c r="H37" s="65"/>
-      <c r="Q37" s="67"/>
-      <c r="R37" s="67"/>
-    </row>
-    <row r="38" spans="1:91" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="74" t="s">
+      <c r="CI36" s="12"/>
+    </row>
+    <row r="37" spans="1:91" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="14" t="s">
+        <v>1777</v>
+      </c>
+      <c r="B37" s="72" t="s">
+        <v>1872</v>
+      </c>
+      <c r="C37" s="72" t="s">
+        <v>1870</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>1871</v>
+      </c>
+      <c r="E37" s="29" t="s">
+        <v>1783</v>
+      </c>
+      <c r="F37" s="30"/>
+      <c r="G37" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H37" s="10"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="12"/>
+      <c r="K37" s="12"/>
+      <c r="L37" s="54"/>
+      <c r="N37" s="12"/>
+      <c r="O37" s="12"/>
+      <c r="P37" s="12"/>
+      <c r="S37" s="53"/>
+      <c r="T37" s="12"/>
+      <c r="U37" s="12"/>
+      <c r="V37" s="12"/>
+      <c r="W37" s="12"/>
+      <c r="X37" s="12"/>
+      <c r="Y37" s="12"/>
+      <c r="Z37" s="12"/>
+      <c r="AA37" s="12"/>
+      <c r="AB37" s="12"/>
+      <c r="AC37" s="12"/>
+      <c r="AD37" s="12"/>
+      <c r="AE37" s="12"/>
+      <c r="AF37" s="12"/>
+      <c r="AG37" s="12"/>
+      <c r="AH37" s="12"/>
+      <c r="AI37" s="12"/>
+      <c r="AJ37" s="12"/>
+      <c r="AK37" s="12"/>
+      <c r="AL37" s="12"/>
+      <c r="AM37" s="12"/>
+      <c r="AN37" s="12"/>
+      <c r="AO37" s="12"/>
+      <c r="AP37" s="12"/>
+      <c r="AQ37" s="12"/>
+      <c r="AR37" s="12"/>
+      <c r="AS37" s="12"/>
+      <c r="AT37" s="12"/>
+      <c r="AU37" s="12"/>
+      <c r="AV37" s="12"/>
+      <c r="AW37" s="12"/>
+      <c r="AX37" s="12"/>
+      <c r="AY37" s="12"/>
+      <c r="AZ37" s="12"/>
+      <c r="BA37" s="12"/>
+      <c r="BB37" s="12"/>
+      <c r="BC37" s="12"/>
+      <c r="BD37" s="12"/>
+      <c r="BE37" s="12"/>
+      <c r="BF37" s="12"/>
+      <c r="BG37" s="12"/>
+      <c r="BH37" s="12"/>
+      <c r="BI37" s="12"/>
+      <c r="BJ37" s="12"/>
+      <c r="BK37" s="12"/>
+      <c r="BL37" s="12"/>
+      <c r="BM37" s="12"/>
+      <c r="BN37" s="12"/>
+      <c r="BO37" s="12"/>
+      <c r="BP37" s="12"/>
+      <c r="BQ37" s="12"/>
+      <c r="BR37" s="12"/>
+      <c r="BS37" s="12"/>
+      <c r="BT37" s="12"/>
+      <c r="BU37" s="12"/>
+      <c r="BV37" s="12"/>
+      <c r="BW37" s="12"/>
+      <c r="BX37" s="12"/>
+      <c r="BY37" s="12"/>
+      <c r="BZ37" s="12"/>
+      <c r="CA37" s="12"/>
+      <c r="CB37" s="12"/>
+      <c r="CC37" s="12"/>
+      <c r="CD37" s="12"/>
+      <c r="CE37" s="12"/>
+      <c r="CF37" s="12"/>
+      <c r="CG37" s="12"/>
+      <c r="CH37" s="12"/>
+      <c r="CI37" s="12"/>
+    </row>
+    <row r="38" spans="1:91" s="63" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="61"/>
+      <c r="B38" s="62"/>
+      <c r="C38" s="62"/>
+      <c r="D38" s="61"/>
+      <c r="E38" s="62"/>
+      <c r="F38" s="62"/>
+      <c r="G38" s="61"/>
+      <c r="H38" s="62"/>
+      <c r="Q38" s="64"/>
+      <c r="R38" s="64"/>
+    </row>
+    <row r="39" spans="1:91" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="71" t="s">
         <v>1778</v>
       </c>
-      <c r="B38" s="70"/>
-      <c r="C38" s="70"/>
-      <c r="D38" s="68" t="s">
+      <c r="B39" s="67"/>
+      <c r="C39" s="67"/>
+      <c r="D39" s="65" t="s">
+        <v>1880</v>
+      </c>
+      <c r="E39" s="66" t="s">
+        <v>1879</v>
+      </c>
+      <c r="F39" s="67"/>
+      <c r="G39" s="68" t="s">
+        <v>176</v>
+      </c>
+      <c r="H39" s="68" t="s">
         <v>1881</v>
       </c>
-      <c r="E38" s="69" t="s">
-        <v>1880</v>
-      </c>
-      <c r="F38" s="70"/>
-      <c r="G38" s="71" t="s">
-        <v>176</v>
-      </c>
-      <c r="H38" s="71" t="s">
+      <c r="I39" s="67">
+        <v>23</v>
+      </c>
+      <c r="J39" s="67"/>
+      <c r="K39" s="67"/>
+      <c r="L39" s="67"/>
+      <c r="M39" s="67"/>
+      <c r="N39" s="67"/>
+      <c r="O39" s="67"/>
+      <c r="P39" s="67" t="s">
         <v>1882</v>
       </c>
-      <c r="I38" s="70">
-        <v>23</v>
-      </c>
-      <c r="J38" s="70"/>
-      <c r="K38" s="70"/>
-      <c r="L38" s="70"/>
-      <c r="M38" s="70"/>
-      <c r="N38" s="70"/>
-      <c r="O38" s="70"/>
-      <c r="P38" s="70" t="s">
-        <v>1883</v>
-      </c>
-      <c r="Q38" s="70"/>
-      <c r="R38" s="70"/>
-      <c r="S38" s="70"/>
-      <c r="T38" s="70"/>
-      <c r="U38" s="70"/>
-      <c r="V38" s="70"/>
-      <c r="W38" s="70"/>
-      <c r="X38" s="70"/>
-      <c r="Y38" s="70"/>
-      <c r="Z38" s="70"/>
-      <c r="AA38" s="70"/>
-      <c r="AB38" s="70"/>
-      <c r="AC38" s="70"/>
-      <c r="AD38" s="70"/>
-      <c r="AE38" s="70"/>
-      <c r="AF38" s="70"/>
-      <c r="AG38" s="70"/>
-      <c r="AH38" s="70"/>
-      <c r="AI38" s="70"/>
-      <c r="AJ38" s="70"/>
-      <c r="AK38" s="70"/>
-      <c r="AL38" s="70"/>
-      <c r="AM38" s="70"/>
-      <c r="AN38" s="70"/>
-      <c r="AO38" s="70"/>
-      <c r="AP38" s="70"/>
-      <c r="AQ38" s="70"/>
-      <c r="AR38" s="70"/>
-      <c r="AS38" s="70"/>
-      <c r="AT38" s="70"/>
-      <c r="AU38" s="70"/>
-      <c r="AV38" s="70"/>
-      <c r="AW38" s="70"/>
-      <c r="AX38" s="70"/>
-      <c r="AY38" s="70"/>
-      <c r="AZ38" s="70"/>
-      <c r="BA38" s="70"/>
-      <c r="BB38" s="70"/>
-      <c r="BC38" s="70"/>
-      <c r="BD38" s="70"/>
-      <c r="BE38" s="70"/>
-      <c r="BF38" s="70"/>
-      <c r="BG38" s="70"/>
-      <c r="BH38" s="70"/>
-      <c r="BI38" s="70"/>
-      <c r="BJ38" s="70"/>
-      <c r="BK38" s="70"/>
-      <c r="BL38" s="70"/>
-      <c r="BM38" s="70"/>
-      <c r="BN38" s="70"/>
-      <c r="BO38" s="70"/>
-      <c r="BP38" s="70"/>
-      <c r="BQ38" s="70"/>
-      <c r="BR38" s="70"/>
-      <c r="BS38" s="70"/>
-      <c r="BT38" s="70"/>
-      <c r="BU38" s="70"/>
-      <c r="BV38" s="70"/>
-      <c r="BW38" s="70"/>
-      <c r="BX38" s="70"/>
-      <c r="BY38" s="70"/>
-      <c r="BZ38" s="70"/>
-      <c r="CA38" s="70"/>
-      <c r="CB38" s="70"/>
-      <c r="CC38" s="70"/>
-      <c r="CD38" s="70"/>
-      <c r="CE38" s="70"/>
-      <c r="CF38" s="70"/>
-      <c r="CG38" s="70"/>
-      <c r="CH38" s="70"/>
-      <c r="CI38" s="70"/>
-      <c r="CJ38" s="70"/>
-      <c r="CK38" s="70"/>
-      <c r="CL38" s="70"/>
-      <c r="CM38" s="70"/>
-    </row>
-    <row r="39" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A39" s="72"/>
-      <c r="B39" s="72"/>
-      <c r="C39" s="72"/>
-      <c r="D39" s="72"/>
-      <c r="E39" s="72"/>
-      <c r="F39" s="72"/>
-      <c r="G39" s="73"/>
-      <c r="H39" s="72"/>
-      <c r="I39" s="72"/>
-      <c r="J39" s="72"/>
-      <c r="K39" s="72"/>
-      <c r="L39" s="72"/>
-      <c r="M39" s="72"/>
-      <c r="N39" s="72"/>
-      <c r="O39" s="72"/>
-      <c r="P39" s="72"/>
-      <c r="Q39" s="72"/>
-      <c r="R39" s="72"/>
-      <c r="S39" s="72"/>
-      <c r="T39" s="72"/>
-      <c r="U39" s="72"/>
-      <c r="V39" s="72"/>
-      <c r="W39" s="72"/>
-      <c r="X39" s="72"/>
-      <c r="Y39" s="72"/>
-      <c r="Z39" s="72"/>
-      <c r="AA39" s="72"/>
-      <c r="AB39" s="72"/>
-      <c r="AC39" s="72"/>
-      <c r="AD39" s="72"/>
-      <c r="AE39" s="72"/>
-      <c r="AF39" s="72"/>
-      <c r="AG39" s="72"/>
-      <c r="AH39" s="72"/>
-      <c r="AI39" s="72"/>
-      <c r="AJ39" s="72"/>
-      <c r="AK39" s="72"/>
-      <c r="AL39" s="72"/>
-      <c r="AM39" s="72"/>
-      <c r="AN39" s="72"/>
-      <c r="AO39" s="72"/>
-      <c r="AP39" s="72"/>
-      <c r="AQ39" s="72"/>
-      <c r="AR39" s="72"/>
-      <c r="AS39" s="72"/>
-      <c r="AT39" s="72"/>
-      <c r="AU39" s="72"/>
-      <c r="AV39" s="72"/>
-      <c r="AW39" s="72"/>
-      <c r="AX39" s="72"/>
-      <c r="AY39" s="72"/>
-      <c r="AZ39" s="72"/>
-      <c r="BA39" s="72"/>
-      <c r="BB39" s="72"/>
-      <c r="BC39" s="72"/>
-      <c r="BD39" s="72"/>
-      <c r="BE39" s="72"/>
-      <c r="BF39" s="72"/>
-      <c r="BG39" s="72"/>
-      <c r="BH39" s="72"/>
-      <c r="BI39" s="72"/>
-      <c r="BJ39" s="72"/>
-      <c r="BK39" s="72"/>
-      <c r="BL39" s="72"/>
-      <c r="BM39" s="72"/>
-      <c r="BN39" s="72"/>
-      <c r="BO39" s="72"/>
-      <c r="BP39" s="72"/>
-      <c r="BQ39" s="72"/>
-      <c r="BR39" s="72"/>
-      <c r="BS39" s="72"/>
-      <c r="BT39" s="72"/>
-      <c r="BU39" s="72"/>
-      <c r="BV39" s="72"/>
-      <c r="BW39" s="72"/>
-      <c r="BX39" s="72"/>
-      <c r="BY39" s="72"/>
-      <c r="BZ39" s="72"/>
-      <c r="CA39" s="72"/>
-      <c r="CB39" s="72"/>
-      <c r="CC39" s="72"/>
-      <c r="CD39" s="72"/>
-      <c r="CE39" s="72"/>
-      <c r="CF39" s="72"/>
-      <c r="CG39" s="72"/>
-      <c r="CH39" s="72"/>
-      <c r="CI39" s="72"/>
-      <c r="CJ39" s="72"/>
-      <c r="CK39" s="72"/>
-      <c r="CL39" s="72"/>
-      <c r="CM39" s="72"/>
+      <c r="Q39" s="67"/>
+      <c r="R39" s="67"/>
+      <c r="S39" s="67"/>
+      <c r="T39" s="67"/>
+      <c r="U39" s="67"/>
+      <c r="V39" s="67"/>
+      <c r="W39" s="67"/>
+      <c r="X39" s="67"/>
+      <c r="Y39" s="67"/>
+      <c r="Z39" s="67"/>
+      <c r="AA39" s="67"/>
+      <c r="AB39" s="67"/>
+      <c r="AC39" s="67"/>
+      <c r="AD39" s="67"/>
+      <c r="AE39" s="67"/>
+      <c r="AF39" s="67"/>
+      <c r="AG39" s="67"/>
+      <c r="AH39" s="67"/>
+      <c r="AI39" s="67"/>
+      <c r="AJ39" s="67"/>
+      <c r="AK39" s="67"/>
+      <c r="AL39" s="67"/>
+      <c r="AM39" s="67"/>
+      <c r="AN39" s="67"/>
+      <c r="AO39" s="67"/>
+      <c r="AP39" s="67"/>
+      <c r="AQ39" s="67"/>
+      <c r="AR39" s="67"/>
+      <c r="AS39" s="67"/>
+      <c r="AT39" s="67"/>
+      <c r="AU39" s="67"/>
+      <c r="AV39" s="67"/>
+      <c r="AW39" s="67"/>
+      <c r="AX39" s="67"/>
+      <c r="AY39" s="67"/>
+      <c r="AZ39" s="67"/>
+      <c r="BA39" s="67"/>
+      <c r="BB39" s="67"/>
+      <c r="BC39" s="67"/>
+      <c r="BD39" s="67"/>
+      <c r="BE39" s="67"/>
+      <c r="BF39" s="67"/>
+      <c r="BG39" s="67"/>
+      <c r="BH39" s="67"/>
+      <c r="BI39" s="67"/>
+      <c r="BJ39" s="67"/>
+      <c r="BK39" s="67"/>
+      <c r="BL39" s="67"/>
+      <c r="BM39" s="67"/>
+      <c r="BN39" s="67"/>
+      <c r="BO39" s="67"/>
+      <c r="BP39" s="67"/>
+      <c r="BQ39" s="67"/>
+      <c r="BR39" s="67"/>
+      <c r="BS39" s="67"/>
+      <c r="BT39" s="67"/>
+      <c r="BU39" s="67"/>
+      <c r="BV39" s="67"/>
+      <c r="BW39" s="67"/>
+      <c r="BX39" s="67"/>
+      <c r="BY39" s="67"/>
+      <c r="BZ39" s="67"/>
+      <c r="CA39" s="67"/>
+      <c r="CB39" s="67"/>
+      <c r="CC39" s="67"/>
+      <c r="CD39" s="67"/>
+      <c r="CE39" s="67"/>
+      <c r="CF39" s="67"/>
+      <c r="CG39" s="67"/>
+      <c r="CH39" s="67"/>
+      <c r="CI39" s="67"/>
+      <c r="CJ39" s="67"/>
+      <c r="CK39" s="67"/>
+      <c r="CL39" s="67"/>
+      <c r="CM39" s="67"/>
     </row>
     <row r="40" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="G40" s="61"/>
+      <c r="A40" s="69"/>
+      <c r="B40" s="69"/>
+      <c r="C40" s="69"/>
+      <c r="D40" s="69"/>
+      <c r="E40" s="69"/>
+      <c r="F40" s="69"/>
+      <c r="G40" s="70"/>
+      <c r="H40" s="69"/>
+      <c r="I40" s="69"/>
+      <c r="J40" s="69"/>
+      <c r="K40" s="69"/>
+      <c r="L40" s="69"/>
+      <c r="M40" s="69"/>
+      <c r="N40" s="69"/>
+      <c r="O40" s="69"/>
+      <c r="P40" s="69"/>
+      <c r="Q40" s="69"/>
+      <c r="R40" s="69"/>
+      <c r="S40" s="69"/>
+      <c r="T40" s="69"/>
+      <c r="U40" s="69"/>
+      <c r="V40" s="69"/>
+      <c r="W40" s="69"/>
+      <c r="X40" s="69"/>
+      <c r="Y40" s="69"/>
+      <c r="Z40" s="69"/>
+      <c r="AA40" s="69"/>
+      <c r="AB40" s="69"/>
+      <c r="AC40" s="69"/>
+      <c r="AD40" s="69"/>
+      <c r="AE40" s="69"/>
+      <c r="AF40" s="69"/>
+      <c r="AG40" s="69"/>
+      <c r="AH40" s="69"/>
+      <c r="AI40" s="69"/>
+      <c r="AJ40" s="69"/>
+      <c r="AK40" s="69"/>
+      <c r="AL40" s="69"/>
+      <c r="AM40" s="69"/>
+      <c r="AN40" s="69"/>
+      <c r="AO40" s="69"/>
+      <c r="AP40" s="69"/>
+      <c r="AQ40" s="69"/>
+      <c r="AR40" s="69"/>
+      <c r="AS40" s="69"/>
+      <c r="AT40" s="69"/>
+      <c r="AU40" s="69"/>
+      <c r="AV40" s="69"/>
+      <c r="AW40" s="69"/>
+      <c r="AX40" s="69"/>
+      <c r="AY40" s="69"/>
+      <c r="AZ40" s="69"/>
+      <c r="BA40" s="69"/>
+      <c r="BB40" s="69"/>
+      <c r="BC40" s="69"/>
+      <c r="BD40" s="69"/>
+      <c r="BE40" s="69"/>
+      <c r="BF40" s="69"/>
+      <c r="BG40" s="69"/>
+      <c r="BH40" s="69"/>
+      <c r="BI40" s="69"/>
+      <c r="BJ40" s="69"/>
+      <c r="BK40" s="69"/>
+      <c r="BL40" s="69"/>
+      <c r="BM40" s="69"/>
+      <c r="BN40" s="69"/>
+      <c r="BO40" s="69"/>
+      <c r="BP40" s="69"/>
+      <c r="BQ40" s="69"/>
+      <c r="BR40" s="69"/>
+      <c r="BS40" s="69"/>
+      <c r="BT40" s="69"/>
+      <c r="BU40" s="69"/>
+      <c r="BV40" s="69"/>
+      <c r="BW40" s="69"/>
+      <c r="BX40" s="69"/>
+      <c r="BY40" s="69"/>
+      <c r="BZ40" s="69"/>
+      <c r="CA40" s="69"/>
+      <c r="CB40" s="69"/>
+      <c r="CC40" s="69"/>
+      <c r="CD40" s="69"/>
+      <c r="CE40" s="69"/>
+      <c r="CF40" s="69"/>
+      <c r="CG40" s="69"/>
+      <c r="CH40" s="69"/>
+      <c r="CI40" s="69"/>
+      <c r="CJ40" s="69"/>
+      <c r="CK40" s="69"/>
+      <c r="CL40" s="69"/>
+      <c r="CM40" s="69"/>
+    </row>
+    <row r="41" spans="1:91" x14ac:dyDescent="0.25">
+      <c r="G41" s="60"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:CG31" xr:uid="{9585C0FF-65C5-4BD8-9936-5C9A63F7E604}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:CG36">
-      <sortCondition ref="B2:B31"/>
-    </sortState>
-  </autoFilter>
   <mergeCells count="16">
     <mergeCell ref="AO1:AR1"/>
     <mergeCell ref="AS1:AV1"/>

</xml_diff>

<commit_message>
Actualizacion de plan de trabajo controldigit3
</commit_message>
<xml_diff>
--- a/00-Documentacion/Listado de reportes totales-TI.xlsx
+++ b/00-Documentacion/Listado de reportes totales-TI.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A50E21D0-5F7C-4A7E-A036-265AD72CAF3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF91E91F-6660-4C9D-A74F-72F1632E1310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{1498AA1A-1ACC-4329-A050-ACA05131B658}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Analisis Proceso con prioridad" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Analisis Proceso con prioridad'!$A$2:$CI$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Analisis Proceso con prioridad'!$A$2:$CN$39</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'General - Analisis'!$A$1:$R$1347</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'listado modulo sin area'!$A$1:$R$116</definedName>
   </definedNames>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13301" uniqueCount="1890">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13314" uniqueCount="1893">
   <si>
     <t xml:space="preserve">Reporte </t>
   </si>
@@ -5267,21 +5267,6 @@
     <t>Expediente aduanal</t>
   </si>
   <si>
-    <r>
-      <t>CORRECTO</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (18 CLIENTES)</t>
-    </r>
-  </si>
-  <si>
     <t>Anexo 24 Integration Point</t>
   </si>
   <si>
@@ -5702,9 +5687,6 @@
     <t>correo, Excel, txt, zip</t>
   </si>
   <si>
-    <t>Pendiente</t>
-  </si>
-  <si>
     <t>Estructura NV BD Spooler</t>
   </si>
   <si>
@@ -5720,17 +5702,32 @@
     <t>15-19</t>
   </si>
   <si>
-    <t>22-27</t>
-  </si>
-  <si>
-    <t>Generación diagrama flujo de Spooler manual y bajo demanda dos dia adicionales</t>
+    <t>Complejida</t>
+  </si>
+  <si>
+    <t>Agregar 2 dias diagrama solicitados</t>
+  </si>
+  <si>
+    <t>CORRECTO (18 CLIENTES)</t>
+  </si>
+  <si>
+    <t>ZxDocumentacion</t>
+  </si>
+  <si>
+    <t>ZEDocumentacion</t>
+  </si>
+  <si>
+    <t>Enero</t>
+  </si>
+  <si>
+    <t>22-26</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5769,13 +5766,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -6055,7 +6045,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6085,56 +6075,56 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -6157,16 +6147,16 @@
     <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="15" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -6175,22 +6165,17 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6205,17 +6190,17 @@
     <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6231,9 +6216,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -54726,7 +54740,7 @@
         <v>4</v>
       </c>
       <c r="E1208" s="8" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="F1208" s="8"/>
       <c r="G1208" s="8" t="s">
@@ -54768,7 +54782,7 @@
         <v>4</v>
       </c>
       <c r="E1209" s="8" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="F1209" s="8"/>
       <c r="G1209" s="8" t="s">
@@ -54810,7 +54824,7 @@
         <v>4</v>
       </c>
       <c r="E1210" s="8" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="F1210" s="10"/>
       <c r="G1210" s="10" t="s">
@@ -54852,7 +54866,7 @@
         <v>4</v>
       </c>
       <c r="E1211" s="8" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="F1211" s="8"/>
       <c r="G1211" s="8" t="s">
@@ -54894,7 +54908,7 @@
         <v>4</v>
       </c>
       <c r="E1212" s="8" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="F1212" s="10"/>
       <c r="G1212" s="10" t="s">
@@ -54936,7 +54950,7 @@
         <v>4</v>
       </c>
       <c r="E1213" s="8" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="F1213" s="10"/>
       <c r="G1213" s="10" t="s">
@@ -54978,7 +54992,7 @@
         <v>4</v>
       </c>
       <c r="E1214" s="8" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="F1214" s="8"/>
       <c r="G1214" s="8" t="s">
@@ -55020,7 +55034,7 @@
         <v>4</v>
       </c>
       <c r="E1215" s="8" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="F1215" s="8"/>
       <c r="G1215" s="8" t="s">
@@ -55062,7 +55076,7 @@
         <v>4</v>
       </c>
       <c r="E1216" s="8" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="F1216" s="8"/>
       <c r="G1216" s="8" t="s">
@@ -55104,7 +55118,7 @@
         <v>4</v>
       </c>
       <c r="E1217" s="8" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="F1217" s="10"/>
       <c r="G1217" s="10" t="s">
@@ -55146,7 +55160,7 @@
         <v>4</v>
       </c>
       <c r="E1218" s="8" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="F1218" s="10"/>
       <c r="G1218" s="10" t="s">
@@ -55188,7 +55202,7 @@
         <v>4</v>
       </c>
       <c r="E1219" s="8" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="F1219" s="10"/>
       <c r="G1219" s="10" t="s">
@@ -55230,7 +55244,7 @@
         <v>4</v>
       </c>
       <c r="E1220" s="8" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="F1220" s="10"/>
       <c r="G1220" s="10" t="s">
@@ -55272,7 +55286,7 @@
         <v>4</v>
       </c>
       <c r="E1221" s="8" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="F1221" s="10"/>
       <c r="G1221" s="10" t="s">
@@ -55314,7 +55328,7 @@
         <v>4</v>
       </c>
       <c r="E1222" s="8" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="F1222" s="10"/>
       <c r="G1222" s="10" t="s">
@@ -55356,7 +55370,7 @@
         <v>4</v>
       </c>
       <c r="E1223" s="8" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="F1223" s="10"/>
       <c r="G1223" s="10"/>
@@ -55396,7 +55410,7 @@
         <v>4</v>
       </c>
       <c r="E1224" s="8" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="F1224" s="10"/>
       <c r="G1224" s="10" t="s">
@@ -55438,7 +55452,7 @@
         <v>4</v>
       </c>
       <c r="E1225" s="8" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="F1225" s="10"/>
       <c r="G1225" s="10" t="s">
@@ -55480,7 +55494,7 @@
         <v>4</v>
       </c>
       <c r="E1226" s="8" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="F1226" s="10"/>
       <c r="G1226" s="10" t="s">
@@ -64846,11 +64860,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9585C0FF-65C5-4BD8-9936-5C9A63F7E604}">
-  <dimension ref="A1:CM41"/>
+  <dimension ref="A1:CN41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" topLeftCell="AU1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="BP31" sqref="BP31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64932,115 +64946,121 @@
     <col min="86" max="87" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="S1" s="79">
+    <row r="1" spans="1:92" x14ac:dyDescent="0.25">
+      <c r="B1" s="71"/>
+      <c r="M1" s="71"/>
+      <c r="S1" s="76">
         <v>45536</v>
       </c>
-      <c r="T1" s="80"/>
-      <c r="U1" s="80"/>
-      <c r="V1" s="80"/>
-      <c r="W1" s="79">
+      <c r="T1" s="77"/>
+      <c r="U1" s="77"/>
+      <c r="V1" s="77"/>
+      <c r="W1" s="76">
         <v>45566</v>
       </c>
-      <c r="X1" s="79"/>
-      <c r="Y1" s="79"/>
-      <c r="Z1" s="79"/>
-      <c r="AA1" s="79"/>
-      <c r="AB1" s="76">
+      <c r="X1" s="76"/>
+      <c r="Y1" s="76"/>
+      <c r="Z1" s="76"/>
+      <c r="AA1" s="76"/>
+      <c r="AB1" s="73">
         <v>45597</v>
       </c>
-      <c r="AC1" s="77"/>
-      <c r="AD1" s="77"/>
-      <c r="AE1" s="78"/>
-      <c r="AF1" s="76">
+      <c r="AC1" s="74"/>
+      <c r="AD1" s="74"/>
+      <c r="AE1" s="75"/>
+      <c r="AF1" s="73">
         <v>45627</v>
       </c>
-      <c r="AG1" s="77"/>
-      <c r="AH1" s="77"/>
-      <c r="AI1" s="78"/>
-      <c r="AJ1" s="76">
+      <c r="AG1" s="74"/>
+      <c r="AH1" s="74"/>
+      <c r="AI1" s="75"/>
+      <c r="AJ1" s="73">
         <v>45658</v>
       </c>
-      <c r="AK1" s="77"/>
-      <c r="AL1" s="77"/>
-      <c r="AM1" s="77"/>
-      <c r="AN1" s="78"/>
-      <c r="AO1" s="76">
+      <c r="AK1" s="74"/>
+      <c r="AL1" s="74"/>
+      <c r="AM1" s="74"/>
+      <c r="AN1" s="75"/>
+      <c r="AO1" s="73">
         <v>45689</v>
       </c>
-      <c r="AP1" s="77"/>
-      <c r="AQ1" s="77"/>
-      <c r="AR1" s="78"/>
-      <c r="AS1" s="76">
+      <c r="AP1" s="74"/>
+      <c r="AQ1" s="74"/>
+      <c r="AR1" s="75"/>
+      <c r="AS1" s="73">
         <v>45717</v>
       </c>
-      <c r="AT1" s="77"/>
-      <c r="AU1" s="77"/>
-      <c r="AV1" s="78"/>
-      <c r="AW1" s="76">
+      <c r="AT1" s="74"/>
+      <c r="AU1" s="74"/>
+      <c r="AV1" s="75"/>
+      <c r="AW1" s="73">
         <v>45748</v>
       </c>
-      <c r="AX1" s="77"/>
-      <c r="AY1" s="77"/>
-      <c r="AZ1" s="78"/>
-      <c r="BA1" s="76">
+      <c r="AX1" s="74"/>
+      <c r="AY1" s="74"/>
+      <c r="AZ1" s="75"/>
+      <c r="BA1" s="73">
         <v>45778</v>
       </c>
-      <c r="BB1" s="77"/>
-      <c r="BC1" s="77"/>
-      <c r="BD1" s="77"/>
-      <c r="BE1" s="78"/>
-      <c r="BF1" s="76">
+      <c r="BB1" s="74"/>
+      <c r="BC1" s="74"/>
+      <c r="BD1" s="74"/>
+      <c r="BE1" s="75"/>
+      <c r="BF1" s="73">
         <v>45809</v>
       </c>
-      <c r="BG1" s="77"/>
-      <c r="BH1" s="77"/>
-      <c r="BI1" s="77"/>
-      <c r="BJ1" s="76">
+      <c r="BG1" s="74"/>
+      <c r="BH1" s="74"/>
+      <c r="BI1" s="74"/>
+      <c r="BJ1" s="73">
         <v>45839</v>
       </c>
-      <c r="BK1" s="77"/>
-      <c r="BL1" s="77"/>
-      <c r="BM1" s="77"/>
-      <c r="BN1" s="78"/>
-      <c r="BO1" s="76">
+      <c r="BK1" s="74"/>
+      <c r="BL1" s="74"/>
+      <c r="BM1" s="74"/>
+      <c r="BN1" s="75"/>
+      <c r="BO1" s="73">
         <v>45870</v>
       </c>
-      <c r="BP1" s="77"/>
-      <c r="BQ1" s="77"/>
-      <c r="BR1" s="77"/>
-      <c r="BS1" s="76">
+      <c r="BP1" s="74"/>
+      <c r="BQ1" s="74"/>
+      <c r="BR1" s="74"/>
+      <c r="BS1" s="73">
         <v>45901</v>
       </c>
-      <c r="BT1" s="77"/>
-      <c r="BU1" s="77"/>
-      <c r="BV1" s="77"/>
-      <c r="BW1" s="76">
+      <c r="BT1" s="74"/>
+      <c r="BU1" s="74"/>
+      <c r="BV1" s="74"/>
+      <c r="BW1" s="73">
         <v>45931</v>
       </c>
-      <c r="BX1" s="77"/>
-      <c r="BY1" s="77"/>
-      <c r="BZ1" s="77"/>
-      <c r="CB1" s="76">
+      <c r="BX1" s="74"/>
+      <c r="BY1" s="74"/>
+      <c r="BZ1" s="74"/>
+      <c r="CB1" s="73">
         <v>45962</v>
       </c>
-      <c r="CC1" s="77"/>
-      <c r="CD1" s="77"/>
-      <c r="CE1" s="77"/>
-      <c r="CF1" s="81" t="s">
-        <v>1854</v>
-      </c>
-      <c r="CG1" s="81"/>
-    </row>
-    <row r="2" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CC1" s="74"/>
+      <c r="CD1" s="74"/>
+      <c r="CE1" s="74"/>
+      <c r="CF1" s="72" t="s">
+        <v>1853</v>
+      </c>
+      <c r="CG1" s="72"/>
+      <c r="CK1" s="72" t="s">
+        <v>1891</v>
+      </c>
+      <c r="CL1" s="72"/>
+    </row>
+    <row r="2" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
+        <v>1779</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>1856</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>1780</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>1857</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>1781</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>1737</v>
@@ -65052,265 +65072,280 @@
         <v>37</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>1782</v>
+        <v>1781</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>36</v>
+        <v>1886</v>
       </c>
       <c r="J2" s="13" t="s">
+        <v>1774</v>
+      </c>
+      <c r="K2" s="13" t="s">
         <v>1775</v>
       </c>
-      <c r="K2" s="13" t="s">
-        <v>1776</v>
-      </c>
       <c r="L2" s="52" t="s">
-        <v>1786</v>
+        <v>1785</v>
       </c>
       <c r="M2" s="52" t="s">
-        <v>1785</v>
+        <v>1784</v>
       </c>
       <c r="N2" s="52" t="s">
-        <v>1858</v>
+        <v>1857</v>
       </c>
       <c r="O2" s="52" t="s">
-        <v>1863</v>
+        <v>1862</v>
       </c>
       <c r="P2" s="52" t="s">
         <v>37</v>
       </c>
       <c r="Q2" s="52" t="s">
+        <v>1791</v>
+      </c>
+      <c r="R2" s="52" t="s">
         <v>1792</v>
       </c>
-      <c r="R2" s="52" t="s">
+      <c r="S2" s="58" t="s">
         <v>1793</v>
       </c>
-      <c r="S2" s="58" t="s">
+      <c r="T2" s="46" t="s">
         <v>1794</v>
       </c>
-      <c r="T2" s="46" t="s">
+      <c r="U2" s="47" t="s">
+        <v>1854</v>
+      </c>
+      <c r="V2" s="46" t="s">
         <v>1795</v>
       </c>
-      <c r="U2" s="47" t="s">
+      <c r="W2" s="46" t="s">
+        <v>1796</v>
+      </c>
+      <c r="X2" s="46" t="s">
+        <v>1797</v>
+      </c>
+      <c r="Y2" s="46" t="s">
+        <v>1798</v>
+      </c>
+      <c r="Z2" s="46" t="s">
+        <v>1799</v>
+      </c>
+      <c r="AA2" s="46" t="s">
+        <v>1800</v>
+      </c>
+      <c r="AB2" s="46" t="s">
+        <v>1801</v>
+      </c>
+      <c r="AC2" s="46" t="s">
+        <v>1802</v>
+      </c>
+      <c r="AD2" s="47" t="s">
+        <v>1803</v>
+      </c>
+      <c r="AE2" s="46" t="s">
+        <v>1804</v>
+      </c>
+      <c r="AF2" s="46" t="s">
+        <v>1805</v>
+      </c>
+      <c r="AG2" s="46" t="s">
+        <v>1806</v>
+      </c>
+      <c r="AH2" s="46" t="s">
+        <v>1807</v>
+      </c>
+      <c r="AI2" s="47" t="s">
+        <v>1808</v>
+      </c>
+      <c r="AJ2" s="47" t="s">
+        <v>1809</v>
+      </c>
+      <c r="AK2" s="46" t="s">
+        <v>1810</v>
+      </c>
+      <c r="AL2" s="46" t="s">
+        <v>1811</v>
+      </c>
+      <c r="AM2" s="46" t="s">
+        <v>1812</v>
+      </c>
+      <c r="AN2" s="46" t="s">
+        <v>1813</v>
+      </c>
+      <c r="AO2" s="47" t="s">
+        <v>1814</v>
+      </c>
+      <c r="AP2" s="46" t="s">
+        <v>1815</v>
+      </c>
+      <c r="AQ2" s="47" t="s">
+        <v>1816</v>
+      </c>
+      <c r="AR2" s="46" t="s">
+        <v>1817</v>
+      </c>
+      <c r="AS2" s="46" t="s">
+        <v>1818</v>
+      </c>
+      <c r="AT2" s="46" t="s">
+        <v>1815</v>
+      </c>
+      <c r="AU2" s="47" t="s">
+        <v>1819</v>
+      </c>
+      <c r="AV2" s="46" t="s">
+        <v>1817</v>
+      </c>
+      <c r="AW2" s="46" t="s">
+        <v>1820</v>
+      </c>
+      <c r="AX2" s="46" t="s">
+        <v>1821</v>
+      </c>
+      <c r="AY2" s="46" t="s">
+        <v>1798</v>
+      </c>
+      <c r="AZ2" s="46" t="s">
+        <v>1799</v>
+      </c>
+      <c r="BA2" s="47" t="s">
+        <v>1822</v>
+      </c>
+      <c r="BB2" s="46" t="s">
+        <v>1823</v>
+      </c>
+      <c r="BC2" s="46" t="s">
+        <v>1824</v>
+      </c>
+      <c r="BD2" s="46" t="s">
+        <v>1825</v>
+      </c>
+      <c r="BE2" s="46" t="s">
+        <v>1826</v>
+      </c>
+      <c r="BF2" s="47" t="s">
+        <v>1827</v>
+      </c>
+      <c r="BG2" s="46" t="s">
+        <v>1806</v>
+      </c>
+      <c r="BH2" s="46" t="s">
+        <v>1807</v>
+      </c>
+      <c r="BI2" s="46" t="s">
+        <v>1828</v>
+      </c>
+      <c r="BJ2" s="47" t="s">
+        <v>1829</v>
+      </c>
+      <c r="BK2" s="46" t="s">
+        <v>1830</v>
+      </c>
+      <c r="BL2" s="46" t="s">
+        <v>1831</v>
+      </c>
+      <c r="BM2" s="46" t="s">
+        <v>1799</v>
+      </c>
+      <c r="BN2" s="46" t="s">
+        <v>1800</v>
+      </c>
+      <c r="BO2" s="46" t="s">
+        <v>1832</v>
+      </c>
+      <c r="BP2" s="46" t="s">
+        <v>1802</v>
+      </c>
+      <c r="BQ2" s="46" t="s">
+        <v>1833</v>
+      </c>
+      <c r="BR2" s="46" t="s">
+        <v>1804</v>
+      </c>
+      <c r="BS2" s="46" t="s">
+        <v>1843</v>
+      </c>
+      <c r="BT2" s="46" t="s">
+        <v>1844</v>
+      </c>
+      <c r="BU2" s="46" t="s">
+        <v>1845</v>
+      </c>
+      <c r="BV2" s="46" t="s">
+        <v>1846</v>
+      </c>
+      <c r="BW2" s="46" t="s">
+        <v>1847</v>
+      </c>
+      <c r="BX2" s="46" t="s">
+        <v>1848</v>
+      </c>
+      <c r="BY2" s="46" t="s">
+        <v>1849</v>
+      </c>
+      <c r="BZ2" s="46" t="s">
+        <v>1812</v>
+      </c>
+      <c r="CA2" s="46" t="s">
+        <v>1813</v>
+      </c>
+      <c r="CB2" s="46" t="s">
+        <v>1850</v>
+      </c>
+      <c r="CC2" s="46" t="s">
+        <v>1851</v>
+      </c>
+      <c r="CD2" s="46" t="s">
+        <v>1852</v>
+      </c>
+      <c r="CE2" s="46" t="s">
+        <v>1817</v>
+      </c>
+      <c r="CF2" s="46" t="s">
         <v>1855</v>
       </c>
-      <c r="V2" s="46" t="s">
-        <v>1796</v>
-      </c>
-      <c r="W2" s="46" t="s">
-        <v>1797</v>
-      </c>
-      <c r="X2" s="46" t="s">
-        <v>1798</v>
-      </c>
-      <c r="Y2" s="46" t="s">
-        <v>1799</v>
-      </c>
-      <c r="Z2" s="46" t="s">
-        <v>1800</v>
-      </c>
-      <c r="AA2" s="46" t="s">
-        <v>1801</v>
-      </c>
-      <c r="AB2" s="46" t="s">
-        <v>1802</v>
-      </c>
-      <c r="AC2" s="46" t="s">
-        <v>1803</v>
-      </c>
-      <c r="AD2" s="47" t="s">
-        <v>1804</v>
-      </c>
-      <c r="AE2" s="46" t="s">
-        <v>1805</v>
-      </c>
-      <c r="AF2" s="46" t="s">
-        <v>1806</v>
-      </c>
-      <c r="AG2" s="46" t="s">
-        <v>1807</v>
-      </c>
-      <c r="AH2" s="46" t="s">
-        <v>1808</v>
-      </c>
-      <c r="AI2" s="47" t="s">
-        <v>1809</v>
-      </c>
-      <c r="AJ2" s="47" t="s">
-        <v>1810</v>
-      </c>
-      <c r="AK2" s="46" t="s">
-        <v>1811</v>
-      </c>
-      <c r="AL2" s="46" t="s">
-        <v>1812</v>
-      </c>
-      <c r="AM2" s="46" t="s">
-        <v>1813</v>
-      </c>
-      <c r="AN2" s="46" t="s">
-        <v>1814</v>
-      </c>
-      <c r="AO2" s="47" t="s">
-        <v>1815</v>
-      </c>
-      <c r="AP2" s="46" t="s">
-        <v>1816</v>
-      </c>
-      <c r="AQ2" s="47" t="s">
+      <c r="CG2" s="46" t="s">
+        <v>1884</v>
+      </c>
+      <c r="CH2" s="46" t="s">
+        <v>1885</v>
+      </c>
+      <c r="CI2" s="46" t="s">
+        <v>1892</v>
+      </c>
+      <c r="CJ2" s="46" t="s">
         <v>1817</v>
       </c>
-      <c r="AR2" s="46" t="s">
-        <v>1818</v>
-      </c>
-      <c r="AS2" s="46" t="s">
-        <v>1819</v>
-      </c>
-      <c r="AT2" s="46" t="s">
-        <v>1816</v>
-      </c>
-      <c r="AU2" s="47" t="s">
-        <v>1820</v>
-      </c>
-      <c r="AV2" s="46" t="s">
-        <v>1818</v>
-      </c>
-      <c r="AW2" s="46" t="s">
-        <v>1821</v>
-      </c>
-      <c r="AX2" s="46" t="s">
-        <v>1822</v>
-      </c>
-      <c r="AY2" s="46" t="s">
-        <v>1799</v>
-      </c>
-      <c r="AZ2" s="46" t="s">
-        <v>1800</v>
-      </c>
-      <c r="BA2" s="47" t="s">
-        <v>1823</v>
-      </c>
-      <c r="BB2" s="46" t="s">
-        <v>1824</v>
-      </c>
-      <c r="BC2" s="46" t="s">
-        <v>1825</v>
-      </c>
-      <c r="BD2" s="46" t="s">
-        <v>1826</v>
-      </c>
-      <c r="BE2" s="46" t="s">
-        <v>1827</v>
-      </c>
-      <c r="BF2" s="47" t="s">
-        <v>1828</v>
-      </c>
-      <c r="BG2" s="46" t="s">
-        <v>1807</v>
-      </c>
-      <c r="BH2" s="46" t="s">
-        <v>1808</v>
-      </c>
-      <c r="BI2" s="46" t="s">
-        <v>1829</v>
-      </c>
-      <c r="BJ2" s="47" t="s">
-        <v>1830</v>
-      </c>
-      <c r="BK2" s="46" t="s">
-        <v>1831</v>
-      </c>
-      <c r="BL2" s="46" t="s">
-        <v>1832</v>
-      </c>
-      <c r="BM2" s="46" t="s">
-        <v>1800</v>
-      </c>
-      <c r="BN2" s="46" t="s">
-        <v>1801</v>
-      </c>
-      <c r="BO2" s="46" t="s">
-        <v>1833</v>
-      </c>
-      <c r="BP2" s="46" t="s">
-        <v>1803</v>
-      </c>
-      <c r="BQ2" s="46" t="s">
-        <v>1834</v>
-      </c>
-      <c r="BR2" s="46" t="s">
-        <v>1805</v>
-      </c>
-      <c r="BS2" s="46" t="s">
-        <v>1844</v>
-      </c>
-      <c r="BT2" s="46" t="s">
-        <v>1845</v>
-      </c>
-      <c r="BU2" s="46" t="s">
-        <v>1846</v>
-      </c>
-      <c r="BV2" s="46" t="s">
-        <v>1847</v>
-      </c>
-      <c r="BW2" s="46" t="s">
-        <v>1848</v>
-      </c>
-      <c r="BX2" s="46" t="s">
-        <v>1849</v>
-      </c>
-      <c r="BY2" s="46" t="s">
-        <v>1850</v>
-      </c>
-      <c r="BZ2" s="46" t="s">
-        <v>1813</v>
-      </c>
-      <c r="CA2" s="46" t="s">
-        <v>1814</v>
-      </c>
-      <c r="CB2" s="46" t="s">
-        <v>1851</v>
-      </c>
-      <c r="CC2" s="46" t="s">
-        <v>1852</v>
-      </c>
-      <c r="CD2" s="46" t="s">
-        <v>1853</v>
-      </c>
-      <c r="CE2" s="46" t="s">
-        <v>1818</v>
-      </c>
-      <c r="CF2" s="46" t="s">
-        <v>1856</v>
-      </c>
-      <c r="CG2" s="46" t="s">
-        <v>1886</v>
-      </c>
-      <c r="CH2" s="46" t="s">
-        <v>1887</v>
-      </c>
-      <c r="CI2" s="46" t="s">
-        <v>1888</v>
-      </c>
-    </row>
-    <row r="3" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CK2" s="46" t="s">
+        <v>1855</v>
+      </c>
+      <c r="CL2" s="46" t="s">
+        <v>1884</v>
+      </c>
+      <c r="CM2" s="46" t="s">
+        <v>1885</v>
+      </c>
+      <c r="CN2" s="46" t="s">
+        <v>1892</v>
+      </c>
+    </row>
+    <row r="3" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="19" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
       <c r="G3" s="10" t="s">
         <v>15</v>
@@ -65325,19 +65360,18 @@
         <v>2</v>
       </c>
       <c r="K3" s="12">
-        <f>2+1</f>
         <v>3</v>
       </c>
       <c r="L3" s="54"/>
       <c r="M3" s="12" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="N3" s="12"/>
       <c r="O3" s="12" t="s">
+        <v>1863</v>
+      </c>
+      <c r="P3" s="12" t="s">
         <v>1864</v>
-      </c>
-      <c r="P3" s="12" t="s">
-        <v>1865</v>
       </c>
       <c r="Q3" s="12"/>
       <c r="R3" s="56">
@@ -65412,10 +65446,15 @@
       <c r="CG3" s="12"/>
       <c r="CH3" s="12"/>
       <c r="CI3" s="12"/>
-    </row>
-    <row r="4" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CJ3" s="12"/>
+      <c r="CK3" s="12"/>
+      <c r="CL3" s="12"/>
+      <c r="CM3" s="12"/>
+      <c r="CN3" s="12"/>
+    </row>
+    <row r="4" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>35</v>
@@ -65425,10 +65464,10 @@
         <v>1586</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>1763</v>
+        <v>1762</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>12</v>
@@ -65443,21 +65482,20 @@
         <v>1</v>
       </c>
       <c r="K4" s="12">
-        <f>2+1</f>
         <v>3</v>
       </c>
       <c r="L4" s="54"/>
       <c r="M4" s="12" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="N4" s="12">
         <v>12</v>
       </c>
       <c r="O4" s="12" t="s">
+        <v>1863</v>
+      </c>
+      <c r="P4" s="12" t="s">
         <v>1864</v>
-      </c>
-      <c r="P4" s="12" t="s">
-        <v>1865</v>
       </c>
       <c r="Q4" s="12"/>
       <c r="R4" s="56">
@@ -65532,10 +65570,15 @@
       <c r="CG4" s="12"/>
       <c r="CH4" s="12"/>
       <c r="CI4" s="12"/>
-    </row>
-    <row r="5" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CJ4" s="12"/>
+      <c r="CK4" s="12"/>
+      <c r="CL4" s="12"/>
+      <c r="CM4" s="12"/>
+      <c r="CN4" s="12"/>
+    </row>
+    <row r="5" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>35</v>
@@ -65544,13 +65587,13 @@
         <v>1739</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>19</v>
@@ -65565,21 +65608,20 @@
         <v>3</v>
       </c>
       <c r="K5" s="12">
-        <f>2+1</f>
         <v>3</v>
       </c>
       <c r="L5" s="54"/>
       <c r="M5" s="12" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="N5" s="12">
         <v>15</v>
       </c>
       <c r="O5" s="12" t="s">
+        <v>1863</v>
+      </c>
+      <c r="P5" s="12" t="s">
         <v>1864</v>
-      </c>
-      <c r="P5" s="12" t="s">
-        <v>1865</v>
       </c>
       <c r="Q5" s="50"/>
       <c r="R5" s="56">
@@ -65654,25 +65696,30 @@
       <c r="CG5" s="12"/>
       <c r="CH5" s="12"/>
       <c r="CI5" s="12"/>
-    </row>
-    <row r="6" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CJ5" s="12"/>
+      <c r="CK5" s="12"/>
+      <c r="CL5" s="12"/>
+      <c r="CM5" s="12"/>
+      <c r="CN5" s="12"/>
+    </row>
+    <row r="6" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C6" s="15" t="s">
+        <v>1749</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>1749</v>
+      </c>
+      <c r="E6" s="23" t="s">
         <v>1750</v>
       </c>
-      <c r="D6" s="15" t="s">
-        <v>1750</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>1751</v>
-      </c>
       <c r="F6" s="24" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>20</v>
@@ -65687,23 +65734,22 @@
         <v>2</v>
       </c>
       <c r="K6" s="12">
-        <f>3+1</f>
         <v>4</v>
       </c>
       <c r="L6" s="54" t="s">
-        <v>1790</v>
+        <v>1789</v>
       </c>
       <c r="M6" s="12" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="N6" s="12">
         <v>24</v>
       </c>
       <c r="O6" s="12" t="s">
+        <v>1863</v>
+      </c>
+      <c r="P6" s="12" t="s">
         <v>1864</v>
-      </c>
-      <c r="P6" s="12" t="s">
-        <v>1865</v>
       </c>
       <c r="Q6" s="50">
         <v>45485</v>
@@ -65780,23 +65826,28 @@
       <c r="CG6" s="12"/>
       <c r="CH6" s="12"/>
       <c r="CI6" s="12"/>
-    </row>
-    <row r="7" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CJ6" s="12"/>
+      <c r="CK6" s="12"/>
+      <c r="CL6" s="12"/>
+      <c r="CM6" s="12"/>
+      <c r="CN6" s="12"/>
+    </row>
+    <row r="7" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="19" t="s">
-        <v>1771</v>
+        <v>1770</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>1763</v>
+        <v>1762</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
       <c r="G7" s="10" t="s">
         <v>13</v>
@@ -65811,23 +65862,22 @@
         <v>2</v>
       </c>
       <c r="K7" s="12">
-        <f>4+1</f>
         <v>5</v>
       </c>
       <c r="L7" s="54" t="s">
+        <v>1859</v>
+      </c>
+      <c r="M7" s="12" t="s">
         <v>1860</v>
-      </c>
-      <c r="M7" s="12" t="s">
-        <v>1861</v>
       </c>
       <c r="N7" s="12">
         <v>8</v>
       </c>
       <c r="O7" s="12" t="s">
+        <v>1863</v>
+      </c>
+      <c r="P7" s="12" t="s">
         <v>1864</v>
-      </c>
-      <c r="P7" s="12" t="s">
-        <v>1865</v>
       </c>
       <c r="Q7" s="50">
         <v>45514</v>
@@ -65904,25 +65954,30 @@
       <c r="CG7" s="12"/>
       <c r="CH7" s="12"/>
       <c r="CI7" s="12"/>
-    </row>
-    <row r="8" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CJ7" s="12"/>
+      <c r="CK7" s="12"/>
+      <c r="CL7" s="12"/>
+      <c r="CM7" s="12"/>
+      <c r="CN7" s="12"/>
+    </row>
+    <row r="8" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>35</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
       <c r="G8" s="12" t="s">
         <v>13</v>
@@ -65937,23 +65992,22 @@
         <v>2</v>
       </c>
       <c r="K8" s="12">
-        <f>4+1</f>
         <v>5</v>
       </c>
       <c r="L8" s="54" t="s">
-        <v>1862</v>
+        <v>1861</v>
       </c>
       <c r="M8" s="12" t="s">
-        <v>1861</v>
+        <v>1860</v>
       </c>
       <c r="N8" s="12">
         <v>2</v>
       </c>
       <c r="O8" s="12" t="s">
+        <v>1863</v>
+      </c>
+      <c r="P8" s="12" t="s">
         <v>1864</v>
-      </c>
-      <c r="P8" s="12" t="s">
-        <v>1865</v>
       </c>
       <c r="Q8" s="50">
         <v>45537</v>
@@ -66030,10 +66084,15 @@
       <c r="CG8" s="12"/>
       <c r="CH8" s="12"/>
       <c r="CI8" s="12"/>
-    </row>
-    <row r="9" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CJ8" s="12"/>
+      <c r="CK8" s="12"/>
+      <c r="CL8" s="12"/>
+      <c r="CM8" s="12"/>
+      <c r="CN8" s="12"/>
+    </row>
+    <row r="9" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>35</v>
@@ -66042,13 +66101,13 @@
         <v>1739</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
       <c r="G9" s="12" t="s">
         <v>16</v>
@@ -66063,23 +66122,22 @@
         <v>5</v>
       </c>
       <c r="K9" s="12">
-        <f>4+1</f>
         <v>5</v>
       </c>
       <c r="L9" s="54" t="s">
-        <v>1789</v>
+        <v>1788</v>
       </c>
       <c r="M9" s="12" t="s">
-        <v>1788</v>
+        <v>1787</v>
       </c>
       <c r="N9" s="12">
         <v>15</v>
       </c>
       <c r="O9" s="12" t="s">
+        <v>1863</v>
+      </c>
+      <c r="P9" s="12" t="s">
         <v>1864</v>
-      </c>
-      <c r="P9" s="12" t="s">
-        <v>1865</v>
       </c>
       <c r="Q9" s="50">
         <v>45525</v>
@@ -66156,30 +66214,35 @@
       <c r="CG9" s="12"/>
       <c r="CH9" s="12"/>
       <c r="CI9" s="12"/>
-    </row>
-    <row r="10" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CJ9" s="12"/>
+      <c r="CK9" s="12"/>
+      <c r="CL9" s="12"/>
+      <c r="CM9" s="12"/>
+      <c r="CN9" s="12"/>
+    </row>
+    <row r="10" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="B10" s="15" t="s">
+        <v>1752</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>1752</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>1752</v>
+      </c>
+      <c r="E10" s="17" t="s">
         <v>1753</v>
       </c>
-      <c r="C10" s="15" t="s">
-        <v>1753</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>1753</v>
-      </c>
-      <c r="E10" s="23" t="s">
+      <c r="F10" s="22" t="s">
         <v>1754</v>
-      </c>
-      <c r="F10" s="26" t="s">
-        <v>1755</v>
       </c>
       <c r="G10" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H10" s="12" t="s">
         <v>1684</v>
       </c>
       <c r="I10" s="12">
@@ -66188,8 +66251,7 @@
       <c r="J10" s="12">
         <v>32</v>
       </c>
-      <c r="K10" s="27">
-        <f>5+2</f>
+      <c r="K10" s="12">
         <v>7</v>
       </c>
       <c r="L10" s="54"/>
@@ -66274,32 +66336,37 @@
       <c r="CG10" s="12"/>
       <c r="CH10" s="12"/>
       <c r="CI10" s="12"/>
-    </row>
-    <row r="11" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
-        <v>1778</v>
+      <c r="CJ10" s="12"/>
+      <c r="CK10" s="12"/>
+      <c r="CL10" s="12"/>
+      <c r="CM10" s="12"/>
+      <c r="CN10" s="12"/>
+    </row>
+    <row r="11" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>1777</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>1868</v>
-      </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="19" t="s">
+        <v>1867</v>
+      </c>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15" t="s">
+        <v>1759</v>
+      </c>
+      <c r="E11" s="15" t="s">
         <v>1760</v>
       </c>
-      <c r="E11" s="19" t="s">
+      <c r="F11" s="86" t="s">
         <v>1761</v>
-      </c>
-      <c r="F11" s="74" t="s">
-        <v>1762</v>
       </c>
       <c r="G11" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="12" t="s">
         <v>1725</v>
       </c>
       <c r="I11" s="12">
-        <v>17</v>
+        <v>9.1</v>
       </c>
       <c r="J11" s="12">
         <v>12</v>
@@ -66310,15 +66377,15 @@
       <c r="L11" s="54"/>
       <c r="M11" s="12"/>
       <c r="N11" s="12">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="O11" s="12"/>
       <c r="P11" s="12"/>
       <c r="Q11" s="50">
-        <v>45845</v>
+        <v>45688</v>
       </c>
       <c r="R11" s="56">
-        <v>45866</v>
+        <v>45713</v>
       </c>
       <c r="S11" s="53"/>
       <c r="T11" s="12"/>
@@ -66329,7 +66396,7 @@
       <c r="Y11" s="12"/>
       <c r="Z11" s="12"/>
       <c r="AA11" s="12" t="s">
-        <v>1835</v>
+        <v>1834</v>
       </c>
       <c r="AB11" s="12"/>
       <c r="AC11" s="12"/>
@@ -66344,9 +66411,9 @@
       <c r="AL11" s="12"/>
       <c r="AM11" s="12"/>
       <c r="AN11" s="12"/>
-      <c r="AO11" s="12"/>
-      <c r="AP11" s="12"/>
-      <c r="AQ11" s="12"/>
+      <c r="AO11" s="48"/>
+      <c r="AP11" s="48"/>
+      <c r="AQ11" s="48"/>
       <c r="AR11" s="12"/>
       <c r="AS11" s="12"/>
       <c r="AT11" s="12"/>
@@ -66367,10 +66434,10 @@
       <c r="BI11" s="12"/>
       <c r="BJ11" s="12"/>
       <c r="BK11" s="12"/>
-      <c r="BL11" s="48"/>
-      <c r="BM11" s="48"/>
-      <c r="BN11" s="48"/>
-      <c r="BO11" s="48"/>
+      <c r="BL11" s="12"/>
+      <c r="BM11" s="12"/>
+      <c r="BN11" s="12"/>
+      <c r="BO11" s="12"/>
       <c r="BP11" s="12"/>
       <c r="BQ11" s="12"/>
       <c r="BR11" s="12"/>
@@ -66391,30 +66458,37 @@
       <c r="CG11" s="12"/>
       <c r="CH11" s="12"/>
       <c r="CI11" s="12"/>
-    </row>
-    <row r="12" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CJ11" s="12"/>
+      <c r="CK11" s="12"/>
+      <c r="CL11" s="12"/>
+      <c r="CM11" s="12"/>
+      <c r="CN11" s="12"/>
+    </row>
+    <row r="12" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
       <c r="B12" s="15" t="s">
-        <v>1883</v>
-      </c>
-      <c r="C12" s="15"/>
+        <v>1881</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>1877</v>
+      </c>
       <c r="D12" s="15" t="s">
-        <v>1878</v>
+        <v>1877</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>1878</v>
+        <v>1877</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>1878</v>
+        <v>1877</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>1878</v>
+        <v>1877</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>1878</v>
+        <v>1877</v>
       </c>
       <c r="I12" s="12">
-        <v>7.9</v>
+        <v>8</v>
       </c>
       <c r="J12" s="12"/>
       <c r="K12" s="12"/>
@@ -66424,16 +66498,16 @@
         <v>3</v>
       </c>
       <c r="O12" s="12" t="s">
+        <v>1863</v>
+      </c>
+      <c r="P12" s="12" t="s">
         <v>1864</v>
-      </c>
-      <c r="P12" s="12" t="s">
-        <v>1865</v>
       </c>
       <c r="Q12" s="50">
         <v>45574</v>
       </c>
       <c r="R12" s="56">
-        <v>45579</v>
+        <v>45576</v>
       </c>
       <c r="S12" s="53"/>
       <c r="T12" s="12"/>
@@ -66441,7 +66515,6 @@
       <c r="V12" s="12"/>
       <c r="W12" s="12"/>
       <c r="X12" s="12"/>
-      <c r="Y12" s="12"/>
       <c r="Z12" s="12"/>
       <c r="AA12" s="12"/>
       <c r="AB12" s="12"/>
@@ -66504,161 +66577,170 @@
       <c r="CG12" s="12"/>
       <c r="CH12" s="12"/>
       <c r="CI12" s="12"/>
-    </row>
-    <row r="13" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CJ12" s="12"/>
+      <c r="CK12" s="12"/>
+      <c r="CL12" s="12"/>
+      <c r="CM12" s="12"/>
+      <c r="CN12" s="12"/>
+    </row>
+    <row r="13" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="15" t="s">
+        <v>1881</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>1882</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>1882</v>
+      </c>
+      <c r="E13" s="23" t="s">
         <v>1883</v>
       </c>
-      <c r="C13" s="15" t="s">
-        <v>1884</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>1884</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>1885</v>
-      </c>
-      <c r="F13" s="22"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="49"/>
+      <c r="F13" s="24" t="s">
+        <v>1887</v>
+      </c>
+      <c r="G13" s="12"/>
+      <c r="H13" s="8"/>
       <c r="I13" s="12">
         <v>8.01</v>
       </c>
-      <c r="J13" s="49"/>
-      <c r="K13" s="49"/>
-      <c r="L13" s="55" t="s">
-        <v>1889</v>
-      </c>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="54"/>
       <c r="M13" s="12"/>
-      <c r="N13" s="49">
-        <v>7</v>
-      </c>
-      <c r="O13" s="49"/>
-      <c r="P13" s="12" t="s">
-        <v>1859</v>
-      </c>
-      <c r="Q13" s="51">
-        <v>45601</v>
-      </c>
-      <c r="R13" s="57">
-        <v>45610</v>
-      </c>
-      <c r="S13" s="53"/>
-      <c r="T13" s="12"/>
-      <c r="U13" s="12"/>
-      <c r="V13" s="12"/>
-      <c r="X13" s="12"/>
-      <c r="Y13" s="12"/>
-      <c r="Z13" s="12"/>
-      <c r="AA13" s="12"/>
-      <c r="AB13" s="59"/>
-      <c r="AC13" s="12"/>
-      <c r="AD13" s="12"/>
-      <c r="AE13" s="12"/>
-      <c r="AF13" s="12"/>
-      <c r="AG13" s="12"/>
-      <c r="AH13" s="12"/>
-      <c r="AI13" s="12"/>
-      <c r="AJ13" s="12"/>
-      <c r="AK13" s="12"/>
-      <c r="AL13" s="12"/>
-      <c r="AM13" s="12"/>
-      <c r="AN13" s="12"/>
-      <c r="AO13" s="12"/>
-      <c r="AP13" s="12"/>
-      <c r="AQ13" s="12"/>
-      <c r="AR13" s="12"/>
-      <c r="AS13" s="12"/>
-      <c r="AT13" s="12"/>
-      <c r="AU13" s="12"/>
-      <c r="AV13" s="12"/>
-      <c r="AW13" s="12"/>
-      <c r="AX13" s="12"/>
-      <c r="AY13" s="12"/>
-      <c r="AZ13" s="12"/>
-      <c r="BA13" s="12"/>
-      <c r="BB13" s="12"/>
-      <c r="BC13" s="12"/>
-      <c r="BD13" s="12"/>
-      <c r="BE13" s="12"/>
-      <c r="BF13" s="12"/>
-      <c r="BG13" s="12"/>
-      <c r="BH13" s="12"/>
-      <c r="BI13" s="12"/>
-      <c r="BJ13" s="12"/>
-      <c r="BK13" s="12"/>
-      <c r="BL13" s="12"/>
-      <c r="BM13" s="12"/>
-      <c r="BN13" s="12"/>
-      <c r="BO13" s="12"/>
-      <c r="BP13" s="12"/>
-      <c r="BQ13" s="12"/>
-      <c r="BR13" s="12"/>
-      <c r="BS13" s="12"/>
-      <c r="BT13" s="12"/>
-      <c r="BU13" s="12"/>
-      <c r="BV13" s="12"/>
-      <c r="BW13" s="12"/>
-      <c r="BX13" s="12"/>
-      <c r="BY13" s="12"/>
-      <c r="BZ13" s="12"/>
-      <c r="CA13" s="12"/>
-      <c r="CB13" s="12"/>
-      <c r="CC13" s="12"/>
-      <c r="CD13" s="12"/>
-      <c r="CE13" s="12"/>
-      <c r="CF13" s="12"/>
-      <c r="CG13" s="12"/>
-      <c r="CH13" s="12"/>
-      <c r="CI13" s="12"/>
-    </row>
-    <row r="14" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="N13" s="12">
+        <v>5</v>
+      </c>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="50">
+        <v>45605</v>
+      </c>
+      <c r="R13" s="56">
+        <v>45615</v>
+      </c>
+      <c r="S13" s="80"/>
+      <c r="T13" s="78"/>
+      <c r="U13" s="78"/>
+      <c r="V13" s="78"/>
+      <c r="W13" s="93"/>
+      <c r="X13" s="78"/>
+      <c r="Y13" s="78"/>
+      <c r="Z13" s="78"/>
+      <c r="AA13" s="78"/>
+      <c r="AB13" s="78"/>
+      <c r="AC13" s="78"/>
+      <c r="AD13" s="78"/>
+      <c r="AE13" s="78"/>
+      <c r="AF13" s="78"/>
+      <c r="AG13" s="78"/>
+      <c r="AH13" s="78"/>
+      <c r="AI13" s="78"/>
+      <c r="AJ13" s="78"/>
+      <c r="AK13" s="78"/>
+      <c r="AL13" s="78"/>
+      <c r="AM13" s="78"/>
+      <c r="AN13" s="78"/>
+      <c r="AO13" s="78"/>
+      <c r="AP13" s="78"/>
+      <c r="AQ13" s="78"/>
+      <c r="AR13" s="78"/>
+      <c r="AS13" s="78"/>
+      <c r="AT13" s="78"/>
+      <c r="AU13" s="78"/>
+      <c r="AV13" s="78"/>
+      <c r="AW13" s="78"/>
+      <c r="AX13" s="78"/>
+      <c r="AY13" s="78"/>
+      <c r="AZ13" s="78"/>
+      <c r="BA13" s="78"/>
+      <c r="BB13" s="78"/>
+      <c r="BC13" s="78"/>
+      <c r="BD13" s="78"/>
+      <c r="BE13" s="78"/>
+      <c r="BF13" s="78"/>
+      <c r="BG13" s="78"/>
+      <c r="BH13" s="78"/>
+      <c r="BI13" s="78"/>
+      <c r="BJ13" s="78"/>
+      <c r="BK13" s="78"/>
+      <c r="BL13" s="78"/>
+      <c r="BM13" s="78"/>
+      <c r="BN13" s="78"/>
+      <c r="BO13" s="78"/>
+      <c r="BP13" s="78"/>
+      <c r="BQ13" s="78"/>
+      <c r="BR13" s="78"/>
+      <c r="BS13" s="78"/>
+      <c r="BT13" s="78"/>
+      <c r="BU13" s="78"/>
+      <c r="BV13" s="78"/>
+      <c r="BW13" s="78"/>
+      <c r="BX13" s="78"/>
+      <c r="BY13" s="78"/>
+      <c r="BZ13" s="78"/>
+      <c r="CA13" s="78"/>
+      <c r="CB13" s="78"/>
+      <c r="CC13" s="78"/>
+      <c r="CD13" s="78"/>
+      <c r="CE13" s="78"/>
+      <c r="CF13" s="78"/>
+      <c r="CG13" s="78"/>
+      <c r="CH13" s="78"/>
+      <c r="CI13" s="78"/>
+      <c r="CJ13" s="78"/>
+      <c r="CK13" s="78"/>
+      <c r="CL13" s="78"/>
+      <c r="CM13" s="78"/>
+      <c r="CN13" s="78"/>
+    </row>
+    <row r="14" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="B14" s="15" t="s">
+        <v>1756</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>1756</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>1756</v>
+      </c>
+      <c r="E14" s="17" t="s">
         <v>1757</v>
       </c>
-      <c r="C14" s="15" t="s">
-        <v>1757</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>1757</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>1758</v>
-      </c>
-      <c r="F14" s="24" t="s">
-        <v>1744</v>
-      </c>
-      <c r="G14" s="12" t="s">
+      <c r="F14" s="22" t="s">
+        <v>1743</v>
+      </c>
+      <c r="G14" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="H14" s="10" t="s">
+      <c r="H14" s="49" t="s">
         <v>1696</v>
       </c>
-      <c r="I14" s="12">
+      <c r="I14" s="49">
         <v>20</v>
       </c>
-      <c r="J14" s="12">
+      <c r="J14" s="49">
         <v>12</v>
       </c>
-      <c r="K14" s="12">
+      <c r="K14" s="49">
         <v>16</v>
       </c>
-      <c r="L14" s="54"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12">
-        <v>16</v>
-      </c>
-      <c r="O14" s="12"/>
-      <c r="P14" s="12"/>
-      <c r="Q14" s="50">
-        <v>45932</v>
-      </c>
-      <c r="R14" s="56">
-        <v>45957</v>
+      <c r="L14" s="55"/>
+      <c r="M14" s="49"/>
+      <c r="N14" s="49">
+        <v>18</v>
+      </c>
+      <c r="O14" s="49"/>
+      <c r="P14" s="49"/>
+      <c r="Q14" s="51">
+        <v>45951</v>
+      </c>
+      <c r="R14" s="57">
+        <v>45979</v>
       </c>
       <c r="S14" s="53"/>
       <c r="T14" s="12"/>
@@ -66717,42 +66799,47 @@
       <c r="BU14" s="12"/>
       <c r="BV14" s="12"/>
       <c r="BW14" s="12"/>
-      <c r="BX14" s="48"/>
-      <c r="BY14" s="48"/>
+      <c r="BX14" s="12"/>
+      <c r="BY14" s="12"/>
       <c r="BZ14" s="48"/>
       <c r="CA14" s="48"/>
-      <c r="CB14" s="12"/>
-      <c r="CC14" s="12"/>
+      <c r="CB14" s="48"/>
+      <c r="CC14" s="48"/>
       <c r="CD14" s="12"/>
       <c r="CE14" s="12"/>
       <c r="CF14" s="12"/>
       <c r="CG14" s="12"/>
       <c r="CH14" s="12"/>
       <c r="CI14" s="12"/>
-    </row>
-    <row r="15" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CJ14" s="12"/>
+      <c r="CK14" s="12"/>
+      <c r="CL14" s="12"/>
+      <c r="CM14" s="12"/>
+      <c r="CN14" s="12"/>
+    </row>
+    <row r="15" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>1756</v>
+        <v>1755</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>1756</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>1756</v>
-      </c>
-      <c r="E15" s="23" t="s">
-        <v>1779</v>
-      </c>
-      <c r="F15" s="24" t="s">
-        <v>1745</v>
+        <v>1755</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>1755</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>1778</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>1744</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="H15" s="8" t="s">
+      <c r="H15" s="12" t="s">
         <v>1682</v>
       </c>
       <c r="I15" s="12">
@@ -66762,21 +66849,20 @@
         <v>9</v>
       </c>
       <c r="K15" s="12">
-        <f>4+1</f>
         <v>5</v>
       </c>
       <c r="L15" s="54"/>
       <c r="M15" s="12"/>
       <c r="N15" s="12">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="O15" s="12"/>
       <c r="P15" s="12"/>
       <c r="Q15" s="50">
-        <v>45688</v>
+        <v>45714</v>
       </c>
       <c r="R15" s="56">
-        <v>45706</v>
+        <v>45739</v>
       </c>
       <c r="S15" s="53"/>
       <c r="T15" s="12"/>
@@ -66788,6 +66874,7 @@
       <c r="Z15" s="12"/>
       <c r="AA15" s="12"/>
       <c r="AB15" s="12"/>
+      <c r="AC15" s="12"/>
       <c r="AD15" s="12"/>
       <c r="AE15" s="12"/>
       <c r="AF15" s="12"/>
@@ -66799,13 +66886,13 @@
       <c r="AL15" s="12"/>
       <c r="AM15" s="12"/>
       <c r="AN15" s="12"/>
-      <c r="AO15" s="48"/>
-      <c r="AP15" s="48"/>
-      <c r="AQ15" s="48"/>
-      <c r="AR15" s="12"/>
-      <c r="AS15" s="12"/>
-      <c r="AT15" s="12"/>
-      <c r="AU15" s="12"/>
+      <c r="AO15" s="12"/>
+      <c r="AP15" s="12"/>
+      <c r="AQ15" s="12"/>
+      <c r="AR15" s="48"/>
+      <c r="AS15" s="48"/>
+      <c r="AT15" s="48"/>
+      <c r="AU15" s="48"/>
       <c r="AV15" s="12"/>
       <c r="AW15" s="12"/>
       <c r="AX15" s="12"/>
@@ -66845,29 +66932,34 @@
       <c r="CF15" s="12"/>
       <c r="CG15" s="12"/>
       <c r="CH15" s="12"/>
-      <c r="CI15" s="12"/>
-    </row>
-    <row r="16" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
-        <v>1778</v>
+      <c r="CI15" s="89"/>
+      <c r="CJ15" s="12"/>
+      <c r="CK15" s="12"/>
+      <c r="CL15" s="12"/>
+      <c r="CM15" s="12"/>
+      <c r="CN15" s="89"/>
+    </row>
+    <row r="16" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>1777</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>1756</v>
-      </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="45" t="s">
-        <v>1767</v>
-      </c>
-      <c r="E16" s="21" t="s">
+        <v>1755</v>
+      </c>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15" t="s">
+        <v>1766</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>1762</v>
+      </c>
+      <c r="F16" s="22" t="s">
         <v>1763</v>
-      </c>
-      <c r="F16" s="25" t="s">
-        <v>1764</v>
       </c>
       <c r="G16" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="H16" s="12" t="s">
         <v>1682</v>
       </c>
       <c r="I16" s="12">
@@ -66877,21 +66969,20 @@
         <v>13</v>
       </c>
       <c r="K16" s="12">
-        <f>6+7</f>
         <v>13</v>
       </c>
       <c r="L16" s="54"/>
-      <c r="M16" s="12"/>
+      <c r="M16" s="49"/>
       <c r="N16" s="12">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="O16" s="12"/>
       <c r="P16" s="12"/>
       <c r="Q16" s="50">
-        <v>45707</v>
+        <v>45740</v>
       </c>
       <c r="R16" s="56">
-        <v>45726</v>
+        <v>45766</v>
       </c>
       <c r="S16" s="53"/>
       <c r="T16" s="12"/>
@@ -66918,14 +67009,14 @@
       <c r="AO16" s="12"/>
       <c r="AP16" s="12"/>
       <c r="AQ16" s="12"/>
-      <c r="AR16" s="48"/>
-      <c r="AS16" s="48"/>
-      <c r="AT16" s="48"/>
+      <c r="AR16" s="12"/>
+      <c r="AS16" s="12"/>
+      <c r="AT16" s="12"/>
       <c r="AU16" s="12"/>
-      <c r="AV16" s="12"/>
-      <c r="AW16" s="12"/>
-      <c r="AX16" s="12"/>
-      <c r="AY16" s="12"/>
+      <c r="AV16" s="48"/>
+      <c r="AW16" s="48"/>
+      <c r="AX16" s="48"/>
+      <c r="AY16" s="48"/>
       <c r="AZ16" s="12"/>
       <c r="BA16" s="12"/>
       <c r="BB16" s="12"/>
@@ -66962,28 +67053,33 @@
       <c r="CG16" s="12"/>
       <c r="CH16" s="12"/>
       <c r="CI16" s="12"/>
-    </row>
-    <row r="17" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
-        <v>1778</v>
+      <c r="CJ16" s="12"/>
+      <c r="CK16" s="12"/>
+      <c r="CL16" s="12"/>
+      <c r="CM16" s="12"/>
+      <c r="CN16" s="12"/>
+    </row>
+    <row r="17" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>1777</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>1756</v>
-      </c>
-      <c r="C17" s="12"/>
+        <v>1755</v>
+      </c>
+      <c r="C17" s="15"/>
       <c r="D17" s="19" t="s">
         <v>1643</v>
       </c>
-      <c r="E17" s="21" t="s">
+      <c r="E17" s="29" t="s">
+        <v>1762</v>
+      </c>
+      <c r="F17" s="30" t="s">
         <v>1763</v>
-      </c>
-      <c r="F17" s="25" t="s">
-        <v>1764</v>
       </c>
       <c r="G17" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="H17" s="10" t="s">
+      <c r="H17" s="12" t="s">
         <v>1681</v>
       </c>
       <c r="I17" s="12">
@@ -66993,21 +67089,20 @@
         <v>61</v>
       </c>
       <c r="K17" s="12">
-        <f>9+2</f>
         <v>11</v>
       </c>
       <c r="L17" s="54"/>
       <c r="M17" s="12"/>
       <c r="N17" s="12">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="O17" s="12"/>
       <c r="P17" s="12"/>
       <c r="Q17" s="50">
-        <v>45821</v>
+        <v>45870</v>
       </c>
       <c r="R17" s="56">
-        <v>45842</v>
+        <v>45894</v>
       </c>
       <c r="S17" s="53"/>
       <c r="T17" s="12"/>
@@ -67051,15 +67146,15 @@
       <c r="BF17" s="12"/>
       <c r="BG17" s="12"/>
       <c r="BH17" s="12"/>
-      <c r="BI17" s="48"/>
-      <c r="BJ17" s="48"/>
-      <c r="BK17" s="48"/>
+      <c r="BI17" s="12"/>
+      <c r="BJ17" s="12"/>
+      <c r="BK17" s="12"/>
       <c r="BL17" s="12"/>
       <c r="BM17" s="12"/>
       <c r="BN17" s="12"/>
-      <c r="BO17" s="12"/>
-      <c r="BP17" s="12"/>
-      <c r="BQ17" s="12"/>
+      <c r="BO17" s="48"/>
+      <c r="BP17" s="48"/>
+      <c r="BQ17" s="48"/>
       <c r="BR17" s="12"/>
       <c r="BS17" s="12"/>
       <c r="BT17" s="12"/>
@@ -67078,51 +67173,56 @@
       <c r="CG17" s="12"/>
       <c r="CH17" s="12"/>
       <c r="CI17" s="12"/>
-    </row>
-    <row r="18" spans="1:87" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
-        <v>1778</v>
+      <c r="CJ17" s="12"/>
+      <c r="CK17" s="12"/>
+      <c r="CL17" s="12"/>
+      <c r="CM17" s="12"/>
+      <c r="CN17" s="12"/>
+    </row>
+    <row r="18" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
+        <v>1777</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>1756</v>
+        <v>1755</v>
       </c>
       <c r="C18" s="12"/>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="15" t="s">
         <v>1622</v>
       </c>
-      <c r="E18" s="21" t="s">
-        <v>1763</v>
-      </c>
-      <c r="F18" s="20" t="s">
-        <v>1768</v>
-      </c>
-      <c r="G18" s="10" t="s">
+      <c r="E18" s="17" t="s">
+        <v>1762</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>1767</v>
+      </c>
+      <c r="G18" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="H18" s="49" t="s">
         <v>1706</v>
       </c>
-      <c r="I18" s="12">
+      <c r="I18" s="49">
         <v>21</v>
       </c>
-      <c r="J18" s="12">
+      <c r="J18" s="49">
         <v>76</v>
       </c>
-      <c r="K18" s="12">
+      <c r="K18" s="49">
         <v>8</v>
       </c>
-      <c r="L18" s="54"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="12">
-        <v>17</v>
-      </c>
-      <c r="O18" s="12"/>
-      <c r="P18" s="12"/>
-      <c r="Q18" s="50">
-        <v>45958</v>
-      </c>
-      <c r="R18" s="56">
-        <v>45985</v>
+      <c r="L18" s="55"/>
+      <c r="M18" s="49"/>
+      <c r="N18" s="49">
+        <v>20</v>
+      </c>
+      <c r="O18" s="49"/>
+      <c r="P18" s="49"/>
+      <c r="Q18" s="51">
+        <v>45980</v>
+      </c>
+      <c r="R18" s="57">
+        <v>46009</v>
       </c>
       <c r="S18" s="53"/>
       <c r="T18" s="12"/>
@@ -67185,18 +67285,23 @@
       <c r="BY18" s="12"/>
       <c r="BZ18" s="12"/>
       <c r="CA18" s="12"/>
-      <c r="CB18" s="48"/>
-      <c r="CC18" s="48"/>
+      <c r="CB18" s="12"/>
+      <c r="CC18" s="12"/>
       <c r="CD18" s="48"/>
       <c r="CE18" s="48"/>
-      <c r="CF18" s="12"/>
-      <c r="CG18" s="12"/>
-      <c r="CH18" s="12"/>
+      <c r="CF18" s="48"/>
+      <c r="CG18" s="48"/>
+      <c r="CH18" s="48"/>
       <c r="CI18" s="12"/>
-    </row>
-    <row r="19" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CJ18" s="12"/>
+      <c r="CK18" s="12"/>
+      <c r="CL18" s="12"/>
+      <c r="CM18" s="12"/>
+      <c r="CN18" s="46"/>
+    </row>
+    <row r="19" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>1739</v>
@@ -67204,17 +67309,17 @@
       <c r="C19" s="15" t="s">
         <v>1739</v>
       </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="17" t="s">
-        <v>1784</v>
-      </c>
-      <c r="F19" s="22" t="s">
-        <v>1745</v>
+      <c r="D19" s="15"/>
+      <c r="E19" s="23" t="s">
+        <v>1783</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>1744</v>
       </c>
       <c r="G19" s="12" t="s">
         <v>1218</v>
       </c>
-      <c r="H19" s="12" t="s">
+      <c r="H19" s="10" t="s">
         <v>1716</v>
       </c>
       <c r="I19" s="12">
@@ -67223,21 +67328,23 @@
       <c r="J19" s="12">
         <v>10</v>
       </c>
-      <c r="K19" s="12">
+      <c r="K19" s="27">
         <v>3</v>
       </c>
       <c r="L19" s="54" t="s">
-        <v>1791</v>
-      </c>
-      <c r="M19" s="12"/>
+        <v>1790</v>
+      </c>
+      <c r="M19" s="12" t="s">
+        <v>1787</v>
+      </c>
       <c r="N19" s="12">
         <v>6</v>
       </c>
       <c r="O19" s="12" t="s">
+        <v>1863</v>
+      </c>
+      <c r="P19" s="12" t="s">
         <v>1864</v>
-      </c>
-      <c r="P19" s="12" t="s">
-        <v>1865</v>
       </c>
       <c r="Q19" s="50">
         <v>45547</v>
@@ -67314,55 +67421,48 @@
       <c r="CG19" s="12"/>
       <c r="CH19" s="12"/>
       <c r="CI19" s="12"/>
-    </row>
-    <row r="20" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
-        <v>1777</v>
-      </c>
+      <c r="CJ19" s="12"/>
+      <c r="CK19" s="12"/>
+      <c r="CL19" s="12"/>
+      <c r="CM19" s="12"/>
+      <c r="CN19" s="12"/>
+    </row>
+    <row r="20" spans="1:92" x14ac:dyDescent="0.25">
+      <c r="A20" s="12"/>
       <c r="B20" s="15" t="s">
         <v>1739</v>
       </c>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15" t="s">
-        <v>1746</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>1784</v>
-      </c>
-      <c r="F20" s="22" t="s">
-        <v>1745</v>
-      </c>
+      <c r="C20" s="12"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="25"/>
       <c r="G20" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="H20" s="12" t="s">
+        <v>1866</v>
+      </c>
+      <c r="H20" s="10" t="s">
         <v>1716</v>
       </c>
       <c r="I20" s="12">
         <v>8</v>
       </c>
-      <c r="J20" s="12">
-        <v>10</v>
-      </c>
-      <c r="K20" s="12">
-        <v>3</v>
-      </c>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
       <c r="L20" s="54"/>
       <c r="M20" s="12"/>
       <c r="N20" s="12">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="O20" s="12" t="s">
+        <v>1863</v>
+      </c>
+      <c r="P20" s="12" t="s">
         <v>1864</v>
       </c>
-      <c r="P20" s="12" t="s">
-        <v>1865</v>
-      </c>
       <c r="Q20" s="50">
-        <v>45579</v>
+        <v>45559</v>
       </c>
       <c r="R20" s="56">
-        <v>45589</v>
+        <v>45573</v>
       </c>
       <c r="S20" s="53"/>
       <c r="T20" s="12"/>
@@ -67433,43 +67533,62 @@
       <c r="CG20" s="12"/>
       <c r="CH20" s="12"/>
       <c r="CI20" s="12"/>
-    </row>
-    <row r="21" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
+      <c r="CJ20" s="12"/>
+      <c r="CK20" s="12"/>
+      <c r="CL20" s="12"/>
+      <c r="CM20" s="12"/>
+      <c r="CN20" s="12"/>
+    </row>
+    <row r="21" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>1776</v>
+      </c>
       <c r="B21" s="15" t="s">
         <v>1739</v>
       </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12" t="s">
-        <v>1867</v>
-      </c>
-      <c r="H21" s="12" t="s">
+      <c r="C21" s="15" t="s">
+        <v>1739</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>1745</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>1783</v>
+      </c>
+      <c r="F21" s="22" t="s">
+        <v>1744</v>
+      </c>
+      <c r="G21" s="49" t="s">
+        <v>187</v>
+      </c>
+      <c r="H21" s="49" t="s">
         <v>1716</v>
       </c>
       <c r="I21" s="12">
         <v>8</v>
       </c>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="54"/>
+      <c r="J21" s="49">
+        <v>10</v>
+      </c>
+      <c r="K21" s="49">
+        <v>3</v>
+      </c>
+      <c r="L21" s="55"/>
       <c r="M21" s="12"/>
-      <c r="N21" s="12">
-        <v>6</v>
-      </c>
-      <c r="O21" s="12" t="s">
+      <c r="N21" s="49">
+        <v>8</v>
+      </c>
+      <c r="O21" s="49" t="s">
+        <v>1863</v>
+      </c>
+      <c r="P21" s="12" t="s">
         <v>1864</v>
       </c>
-      <c r="P21" s="12" t="s">
-        <v>1865</v>
-      </c>
-      <c r="Q21" s="50">
-        <v>45559</v>
-      </c>
-      <c r="R21" s="56">
-        <v>45573</v>
+      <c r="Q21" s="51">
+        <v>45579</v>
+      </c>
+      <c r="R21" s="57">
+        <v>45589</v>
       </c>
       <c r="S21" s="53"/>
       <c r="T21" s="12"/>
@@ -67540,20 +67659,25 @@
       <c r="CG21" s="12"/>
       <c r="CH21" s="12"/>
       <c r="CI21" s="12"/>
-    </row>
-    <row r="22" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CJ21" s="12"/>
+      <c r="CK21" s="12"/>
+      <c r="CL21" s="12"/>
+      <c r="CM21" s="12"/>
+      <c r="CN21" s="12"/>
+    </row>
+    <row r="22" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="14"/>
       <c r="B22" s="15" t="s">
         <v>1739</v>
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="22"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="24"/>
       <c r="G22" s="12" t="s">
         <v>777</v>
       </c>
-      <c r="H22" s="12" t="s">
+      <c r="H22" s="10" t="s">
         <v>1716</v>
       </c>
       <c r="I22" s="12">
@@ -67562,21 +67686,21 @@
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
       <c r="L22" s="54"/>
-      <c r="M22" s="49"/>
+      <c r="M22" s="12"/>
       <c r="N22" s="12">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="O22" s="12" t="s">
-        <v>1864</v>
+        <v>1863</v>
       </c>
       <c r="P22" s="12" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
       <c r="Q22" s="50">
         <v>45590</v>
       </c>
       <c r="R22" s="56">
-        <v>45615</v>
+        <v>45604</v>
       </c>
       <c r="S22" s="53"/>
       <c r="T22" s="12"/>
@@ -67586,10 +67710,10 @@
       <c r="X22" s="12"/>
       <c r="Y22" s="12"/>
       <c r="Z22" s="12"/>
-      <c r="AA22" s="59"/>
+      <c r="AA22" s="12"/>
       <c r="AB22" s="12"/>
-      <c r="AC22" s="59"/>
-      <c r="AD22" s="75"/>
+      <c r="AC22" s="12"/>
+      <c r="AD22" s="89"/>
       <c r="AE22" s="12"/>
       <c r="AF22" s="12"/>
       <c r="AG22" s="12"/>
@@ -67647,10 +67771,15 @@
       <c r="CG22" s="12"/>
       <c r="CH22" s="12"/>
       <c r="CI22" s="12"/>
-    </row>
-    <row r="23" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CJ22" s="12"/>
+      <c r="CK22" s="12"/>
+      <c r="CL22" s="12"/>
+      <c r="CM22" s="12"/>
+      <c r="CN22" s="12"/>
+    </row>
+    <row r="23" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="B23" s="15" t="s">
         <v>1739</v>
@@ -67660,10 +67789,10 @@
         <v>1352</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
       <c r="F23" s="18" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
       <c r="G23" s="12" t="s">
         <v>24</v>
@@ -67688,10 +67817,10 @@
       <c r="O23" s="12"/>
       <c r="P23" s="12"/>
       <c r="Q23" s="50">
-        <v>45727</v>
+        <v>45767</v>
       </c>
       <c r="R23" s="56">
-        <v>45748</v>
+        <v>45788</v>
       </c>
       <c r="S23" s="53"/>
       <c r="T23" s="12"/>
@@ -67720,14 +67849,14 @@
       <c r="AR23" s="12"/>
       <c r="AS23" s="12"/>
       <c r="AT23" s="12"/>
-      <c r="AU23" s="48"/>
-      <c r="AV23" s="48"/>
-      <c r="AW23" s="48"/>
+      <c r="AU23" s="12"/>
+      <c r="AV23" s="12"/>
+      <c r="AW23" s="12"/>
       <c r="AX23" s="12"/>
       <c r="AY23" s="12"/>
-      <c r="AZ23" s="12"/>
-      <c r="BA23" s="12"/>
-      <c r="BB23" s="12"/>
+      <c r="AZ23" s="48"/>
+      <c r="BA23" s="48"/>
+      <c r="BB23" s="48"/>
       <c r="BC23" s="12"/>
       <c r="BD23" s="12"/>
       <c r="BE23" s="12"/>
@@ -67761,23 +67890,28 @@
       <c r="CG23" s="12"/>
       <c r="CH23" s="12"/>
       <c r="CI23" s="12"/>
-    </row>
-    <row r="24" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ23" s="12"/>
+      <c r="CK23" s="12"/>
+      <c r="CL23" s="12"/>
+      <c r="CM23" s="12"/>
+      <c r="CN23" s="12"/>
+    </row>
+    <row r="24" spans="1:92" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="B24" s="15" t="s">
         <v>1739</v>
       </c>
       <c r="C24" s="12"/>
       <c r="D24" s="19" t="s">
+        <v>1764</v>
+      </c>
+      <c r="E24" s="19" t="s">
         <v>1765</v>
       </c>
-      <c r="E24" s="19" t="s">
-        <v>1766</v>
-      </c>
       <c r="F24" s="25" t="s">
-        <v>1764</v>
+        <v>1763</v>
       </c>
       <c r="G24" s="12" t="s">
         <v>1249</v>
@@ -67792,21 +67926,20 @@
         <v>29</v>
       </c>
       <c r="K24" s="12">
-        <f>15+5</f>
         <v>20</v>
       </c>
       <c r="L24" s="54"/>
       <c r="M24" s="12"/>
       <c r="N24" s="12">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="O24" s="12"/>
       <c r="P24" s="12"/>
       <c r="Q24" s="50">
-        <v>45749</v>
+        <v>45789</v>
       </c>
       <c r="R24" s="56">
-        <v>45770</v>
+        <v>45810</v>
       </c>
       <c r="S24" s="53"/>
       <c r="T24" s="12"/>
@@ -67838,14 +67971,13 @@
       <c r="AU24" s="12"/>
       <c r="AV24" s="12"/>
       <c r="AW24" s="12"/>
-      <c r="AX24" s="48"/>
-      <c r="AY24" s="48"/>
-      <c r="AZ24" s="48"/>
       <c r="BA24" s="12"/>
       <c r="BB24" s="12"/>
-      <c r="BC24" s="12"/>
-      <c r="BD24" s="12"/>
-      <c r="BE24" s="12"/>
+      <c r="BC24" s="70"/>
+      <c r="BD24" s="70"/>
+      <c r="BE24" s="70" t="s">
+        <v>1865</v>
+      </c>
       <c r="BF24" s="12"/>
       <c r="BG24" s="12"/>
       <c r="BH24" s="12"/>
@@ -67876,23 +68008,28 @@
       <c r="CG24" s="12"/>
       <c r="CH24" s="12"/>
       <c r="CI24" s="12"/>
-    </row>
-    <row r="25" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CJ24" s="12"/>
+      <c r="CK24" s="12"/>
+      <c r="CL24" s="12"/>
+      <c r="CM24" s="12"/>
+      <c r="CN24" s="12"/>
+    </row>
+    <row r="25" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="B25" s="15" t="s">
         <v>1739</v>
       </c>
       <c r="C25" s="15"/>
       <c r="D25" s="15" t="s">
+        <v>1741</v>
+      </c>
+      <c r="E25" s="15" t="s">
         <v>1742</v>
       </c>
-      <c r="E25" s="15" t="s">
+      <c r="F25" s="28" t="s">
         <v>1743</v>
-      </c>
-      <c r="F25" s="28" t="s">
-        <v>1744</v>
       </c>
       <c r="G25" s="12" t="s">
         <v>18</v>
@@ -67907,21 +68044,20 @@
         <v>35</v>
       </c>
       <c r="K25" s="12">
-        <f>3+8</f>
         <v>11</v>
       </c>
       <c r="L25" s="54"/>
       <c r="M25" s="12"/>
       <c r="N25" s="12">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="O25" s="12"/>
       <c r="P25" s="12"/>
       <c r="Q25" s="50">
-        <v>45771</v>
+        <v>45811</v>
       </c>
       <c r="R25" s="56">
-        <v>45791</v>
+        <v>45832</v>
       </c>
       <c r="S25" s="53"/>
       <c r="T25" s="12"/>
@@ -67956,19 +68092,17 @@
       <c r="AW25" s="12"/>
       <c r="AX25" s="12"/>
       <c r="AY25" s="12"/>
-      <c r="BA25" s="73"/>
-      <c r="BB25" s="73"/>
-      <c r="BC25" s="73" t="s">
-        <v>1866</v>
-      </c>
+      <c r="AZ25" s="12"/>
+      <c r="BA25" s="12"/>
+      <c r="BB25" s="12"/>
+      <c r="BC25" s="12"/>
       <c r="BD25" s="12"/>
       <c r="BE25" s="12"/>
-      <c r="BF25" s="12"/>
-      <c r="BG25" s="12"/>
-      <c r="BH25" s="12"/>
-      <c r="BI25" s="12"/>
+      <c r="BF25" s="70"/>
+      <c r="BG25" s="70"/>
+      <c r="BH25" s="70"/>
+      <c r="BI25" s="70"/>
       <c r="BJ25" s="12"/>
-      <c r="BK25" s="12"/>
       <c r="BL25" s="12"/>
       <c r="BM25" s="12"/>
       <c r="BN25" s="12"/>
@@ -67993,23 +68127,28 @@
       <c r="CG25" s="12"/>
       <c r="CH25" s="12"/>
       <c r="CI25" s="12"/>
-    </row>
-    <row r="26" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ25" s="12"/>
+      <c r="CK25" s="12"/>
+      <c r="CL25" s="12"/>
+      <c r="CM25" s="12"/>
+      <c r="CN25" s="12"/>
+    </row>
+    <row r="26" spans="1:92" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="B26" s="15" t="s">
         <v>1739</v>
       </c>
       <c r="C26" s="12"/>
       <c r="D26" s="19" t="s">
+        <v>1768</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>1762</v>
+      </c>
+      <c r="F26" s="25" t="s">
         <v>1769</v>
-      </c>
-      <c r="E26" s="21" t="s">
-        <v>1763</v>
-      </c>
-      <c r="F26" s="20" t="s">
-        <v>1770</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>8</v>
@@ -68034,10 +68173,10 @@
       <c r="O26" s="12"/>
       <c r="P26" s="12"/>
       <c r="Q26" s="50">
-        <v>45867</v>
+        <v>45895</v>
       </c>
       <c r="R26" s="56">
-        <v>45905</v>
+        <v>45924</v>
       </c>
       <c r="S26" s="53"/>
       <c r="T26" s="12"/>
@@ -68075,8 +68214,12 @@
       <c r="AZ26" s="12"/>
       <c r="BA26" s="12"/>
       <c r="BB26" s="12"/>
-      <c r="BC26" s="12"/>
-      <c r="BH26" s="12"/>
+      <c r="BC26" s="89"/>
+      <c r="BD26" s="89"/>
+      <c r="BE26" s="89"/>
+      <c r="BF26" s="89"/>
+      <c r="BG26" s="89"/>
+      <c r="BH26" s="89"/>
       <c r="BI26" s="12"/>
       <c r="BJ26" s="12"/>
       <c r="BK26" s="12"/>
@@ -68085,11 +68228,11 @@
       <c r="BN26" s="12"/>
       <c r="BO26" s="12"/>
       <c r="BP26" s="12"/>
-      <c r="BQ26" s="48"/>
+      <c r="BQ26" s="12"/>
       <c r="BR26" s="48"/>
       <c r="BS26" s="48"/>
       <c r="BT26" s="48"/>
-      <c r="BU26" s="12"/>
+      <c r="BU26" s="48"/>
       <c r="BV26" s="12"/>
       <c r="BW26" s="12"/>
       <c r="BX26" s="12"/>
@@ -68104,51 +68247,56 @@
       <c r="CG26" s="12"/>
       <c r="CH26" s="12"/>
       <c r="CI26" s="12"/>
-    </row>
-    <row r="27" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CJ26" s="12"/>
+      <c r="CK26" s="12"/>
+      <c r="CL26" s="12"/>
+      <c r="CM26" s="12"/>
+      <c r="CN26" s="12"/>
+    </row>
+    <row r="27" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="B27" s="15" t="s">
         <v>1739</v>
       </c>
-      <c r="C27" s="15"/>
-      <c r="D27" s="19" t="s">
+      <c r="C27" s="12"/>
+      <c r="D27" s="15" t="s">
         <v>1740</v>
       </c>
-      <c r="E27" s="29" t="s">
-        <v>1783</v>
-      </c>
-      <c r="F27" s="30" t="s">
-        <v>1741</v>
-      </c>
-      <c r="G27" s="12" t="s">
+      <c r="E27" s="17" t="s">
+        <v>1782</v>
+      </c>
+      <c r="F27" s="22" t="s">
+        <v>1888</v>
+      </c>
+      <c r="G27" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="H27" s="12" t="s">
-        <v>1759</v>
-      </c>
-      <c r="I27" s="12">
+      <c r="H27" s="49" t="s">
+        <v>1758</v>
+      </c>
+      <c r="I27" s="49">
         <v>22</v>
       </c>
-      <c r="J27" s="12">
+      <c r="J27" s="49">
         <v>78</v>
       </c>
-      <c r="K27" s="12">
+      <c r="K27" s="49">
         <v>25</v>
       </c>
-      <c r="L27" s="54"/>
+      <c r="L27" s="55"/>
       <c r="M27" s="12"/>
-      <c r="N27" s="12">
+      <c r="N27" s="49">
         <v>20</v>
       </c>
-      <c r="O27" s="12"/>
-      <c r="P27" s="12"/>
-      <c r="Q27" s="50">
-        <v>45986</v>
-      </c>
-      <c r="R27" s="56">
-        <v>46017</v>
+      <c r="O27" s="49"/>
+      <c r="P27" s="49"/>
+      <c r="Q27" s="51">
+        <v>46010</v>
+      </c>
+      <c r="R27" s="57">
+        <v>46040</v>
       </c>
       <c r="S27" s="53"/>
       <c r="T27" s="12"/>
@@ -68173,6 +68321,7 @@
       <c r="AM27" s="12"/>
       <c r="AN27" s="12"/>
       <c r="AO27" s="12"/>
+      <c r="AP27" s="89"/>
       <c r="AQ27" s="12"/>
       <c r="AR27" s="12"/>
       <c r="AS27" s="12"/>
@@ -68182,6 +68331,7 @@
       <c r="AW27" s="12"/>
       <c r="AX27" s="12"/>
       <c r="AY27" s="12"/>
+      <c r="AZ27" s="89"/>
       <c r="BA27" s="12"/>
       <c r="BB27" s="12"/>
       <c r="BC27" s="12"/>
@@ -68190,16 +68340,16 @@
       <c r="BF27" s="12"/>
       <c r="BG27" s="12"/>
       <c r="BH27" s="12"/>
-      <c r="BI27" s="12"/>
-      <c r="BJ27" s="12"/>
-      <c r="BK27" s="12"/>
+      <c r="BI27" s="89"/>
+      <c r="BJ27" s="89"/>
+      <c r="BK27" s="89"/>
       <c r="BL27" s="12"/>
       <c r="BM27" s="12"/>
       <c r="BN27" s="12"/>
       <c r="BO27" s="12"/>
       <c r="BP27" s="12"/>
       <c r="BQ27" s="12"/>
-      <c r="BR27" s="12"/>
+      <c r="BR27" s="89"/>
       <c r="BS27" s="12"/>
       <c r="BT27" s="12"/>
       <c r="BU27" s="12"/>
@@ -68213,27 +68363,32 @@
       <c r="CC27" s="12"/>
       <c r="CD27" s="12"/>
       <c r="CE27" s="12"/>
-      <c r="CF27" s="48"/>
-      <c r="CG27" s="48"/>
+      <c r="CF27" s="12"/>
+      <c r="CG27" s="12"/>
       <c r="CH27" s="12"/>
-      <c r="CI27" s="12"/>
-    </row>
-    <row r="28" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CI27" s="48"/>
+      <c r="CJ27" s="48"/>
+      <c r="CK27" s="48"/>
+      <c r="CL27" s="48"/>
+      <c r="CM27" s="12"/>
+      <c r="CN27" s="12"/>
+    </row>
+    <row r="28" spans="1:92" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>1869</v>
+        <v>1868</v>
       </c>
       <c r="C28" s="12"/>
       <c r="D28" s="19" t="s">
-        <v>1774</v>
-      </c>
-      <c r="E28" s="19" t="s">
+        <v>1773</v>
+      </c>
+      <c r="E28" s="21" t="s">
+        <v>1762</v>
+      </c>
+      <c r="F28" s="20" t="s">
         <v>1763</v>
-      </c>
-      <c r="F28" s="25" t="s">
-        <v>1764</v>
       </c>
       <c r="G28" s="10" t="s">
         <v>227</v>
@@ -68258,10 +68413,10 @@
       <c r="O28" s="12"/>
       <c r="P28" s="12"/>
       <c r="Q28" s="50">
-        <v>45792</v>
+        <v>45833</v>
       </c>
       <c r="R28" s="56">
-        <v>45820</v>
+        <v>45861</v>
       </c>
       <c r="S28" s="53"/>
       <c r="T28" s="12"/>
@@ -68300,20 +68455,20 @@
       <c r="BA28" s="12"/>
       <c r="BB28" s="12"/>
       <c r="BC28" s="12"/>
-      <c r="BD28" s="48"/>
-      <c r="BE28" s="48"/>
-      <c r="BF28" s="48"/>
-      <c r="BG28" s="48"/>
-      <c r="BH28" s="48"/>
+      <c r="BD28" s="12"/>
+      <c r="BE28" s="12"/>
+      <c r="BF28" s="12"/>
+      <c r="BG28" s="12"/>
+      <c r="BH28" s="12"/>
       <c r="BI28" s="12"/>
-      <c r="BJ28" s="12"/>
-      <c r="BK28" s="12"/>
-      <c r="BL28" s="12"/>
-      <c r="BM28" s="12"/>
+      <c r="BJ28" s="48"/>
+      <c r="BK28" s="48"/>
+      <c r="BL28" s="48"/>
+      <c r="BM28" s="48"/>
       <c r="BN28" s="12"/>
       <c r="BO28" s="12"/>
       <c r="BP28" s="12"/>
-      <c r="BQ28" s="12"/>
+      <c r="BQ28" s="89"/>
       <c r="BR28" s="12"/>
       <c r="BS28" s="12"/>
       <c r="BT28" s="12"/>
@@ -68332,23 +68487,28 @@
       <c r="CG28" s="12"/>
       <c r="CH28" s="12"/>
       <c r="CI28" s="12"/>
-    </row>
-    <row r="29" spans="1:87" x14ac:dyDescent="0.25">
+      <c r="CJ28" s="12"/>
+      <c r="CK28" s="12"/>
+      <c r="CL28" s="12"/>
+      <c r="CM28" s="12"/>
+      <c r="CN28" s="12"/>
+    </row>
+    <row r="29" spans="1:92" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>1869</v>
+        <v>1868</v>
       </c>
       <c r="C29" s="12"/>
       <c r="D29" s="19" t="s">
         <v>1562</v>
       </c>
       <c r="E29" s="21" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="F29" s="20" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
       <c r="G29" s="10" t="s">
         <v>14</v>
@@ -68368,15 +68528,15 @@
       <c r="L29" s="54"/>
       <c r="M29" s="12"/>
       <c r="N29" s="12">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="O29" s="12"/>
       <c r="P29" s="12"/>
       <c r="Q29" s="50">
-        <v>45908</v>
+        <v>45924</v>
       </c>
       <c r="R29" s="56">
-        <v>45931</v>
+        <v>45950</v>
       </c>
       <c r="S29" s="53"/>
       <c r="T29" s="12"/>
@@ -68431,11 +68591,11 @@
       <c r="BR29" s="12"/>
       <c r="BS29" s="12"/>
       <c r="BT29" s="12"/>
-      <c r="BU29" s="48"/>
+      <c r="BU29" s="12"/>
       <c r="BV29" s="48"/>
       <c r="BW29" s="48"/>
-      <c r="BX29" s="12"/>
-      <c r="BY29" s="12"/>
+      <c r="BX29" s="48"/>
+      <c r="BY29" s="48"/>
       <c r="BZ29" s="12"/>
       <c r="CA29" s="12"/>
       <c r="CB29" s="12"/>
@@ -68446,46 +68606,53 @@
       <c r="CG29" s="12"/>
       <c r="CH29" s="12"/>
       <c r="CI29" s="12"/>
-    </row>
-    <row r="30" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="14" t="s">
-        <v>1778</v>
+      <c r="CJ29" s="12"/>
+      <c r="CK29" s="12"/>
+      <c r="CL29" s="12"/>
+      <c r="CM29" s="12"/>
+      <c r="CN29" s="12"/>
+    </row>
+    <row r="30" spans="1:92" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
+        <v>1777</v>
       </c>
       <c r="B30" s="15" t="s">
+        <v>1835</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>1835</v>
+      </c>
+      <c r="D30" s="45" t="s">
         <v>1836</v>
       </c>
-      <c r="C30" s="15" t="s">
-        <v>1836</v>
-      </c>
-      <c r="D30" s="15" t="s">
+      <c r="E30" s="21" t="s">
         <v>1837</v>
       </c>
-      <c r="E30" s="17" t="s">
+      <c r="F30" s="25"/>
+      <c r="G30" s="12" t="s">
         <v>1838</v>
       </c>
-      <c r="F30" s="22"/>
-      <c r="G30" s="49" t="s">
-        <v>1839</v>
-      </c>
-      <c r="H30" s="49" t="s">
+      <c r="H30" s="10" t="s">
         <v>1730</v>
       </c>
-      <c r="I30" s="49">
+      <c r="I30" s="12">
         <v>8.1</v>
       </c>
-      <c r="J30" s="49"/>
-      <c r="K30" s="49"/>
-      <c r="L30" s="55"/>
-      <c r="M30" s="49"/>
-      <c r="N30" s="49">
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="54"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="12">
         <v>10</v>
       </c>
-      <c r="O30" s="49"/>
-      <c r="P30" s="49"/>
-      <c r="Q30" s="51">
+      <c r="O30" s="12" t="s">
+        <v>1863</v>
+      </c>
+      <c r="P30" s="12"/>
+      <c r="Q30" s="50">
         <v>45616</v>
       </c>
-      <c r="R30" s="57">
+      <c r="R30" s="56">
         <v>45631</v>
       </c>
       <c r="S30" s="53"/>
@@ -68499,9 +68666,9 @@
       <c r="AA30" s="12"/>
       <c r="AB30" s="12"/>
       <c r="AC30" s="12"/>
-      <c r="AD30" s="48"/>
-      <c r="AE30" s="48"/>
-      <c r="AF30" s="48"/>
+      <c r="AD30" s="78"/>
+      <c r="AE30" s="78"/>
+      <c r="AF30" s="78"/>
       <c r="AG30" s="12"/>
       <c r="AH30" s="12"/>
       <c r="AI30" s="12"/>
@@ -68545,8 +68712,8 @@
       <c r="BU30" s="12"/>
       <c r="BV30" s="12"/>
       <c r="BW30" s="12"/>
-      <c r="BX30" s="12"/>
-      <c r="BY30" s="12"/>
+      <c r="BX30" s="89"/>
+      <c r="BY30" s="89"/>
       <c r="BZ30" s="12"/>
       <c r="CA30" s="12"/>
       <c r="CB30" s="12"/>
@@ -68557,44 +68724,51 @@
       <c r="CG30" s="12"/>
       <c r="CH30" s="12"/>
       <c r="CI30" s="12"/>
-    </row>
-    <row r="31" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
-        <v>1778</v>
+      <c r="CJ30" s="12"/>
+      <c r="CK30" s="12"/>
+      <c r="CL30" s="12"/>
+      <c r="CM30" s="12"/>
+      <c r="CN30" s="12"/>
+    </row>
+    <row r="31" spans="1:92" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
+        <v>1777</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>1836</v>
+        <v>1835</v>
       </c>
       <c r="C31" s="12"/>
-      <c r="D31" s="15" t="s">
+      <c r="D31" s="19" t="s">
+        <v>1839</v>
+      </c>
+      <c r="E31" s="21" t="s">
+        <v>1837</v>
+      </c>
+      <c r="F31" s="25"/>
+      <c r="G31" s="12" t="s">
         <v>1840</v>
       </c>
-      <c r="E31" s="17" t="s">
-        <v>1838</v>
-      </c>
-      <c r="F31" s="22"/>
-      <c r="G31" s="49" t="s">
-        <v>1841</v>
-      </c>
-      <c r="H31" s="49" t="s">
+      <c r="H31" s="10" t="s">
         <v>1716</v>
       </c>
-      <c r="I31" s="49">
+      <c r="I31" s="12">
         <v>8.1</v>
       </c>
-      <c r="J31" s="49"/>
-      <c r="K31" s="49"/>
-      <c r="L31" s="55"/>
-      <c r="M31" s="49"/>
-      <c r="N31" s="49">
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="54"/>
+      <c r="M31" s="12"/>
+      <c r="N31" s="12">
         <v>10</v>
       </c>
-      <c r="O31" s="49"/>
-      <c r="P31" s="49"/>
-      <c r="Q31" s="51">
+      <c r="O31" s="12" t="s">
+        <v>1863</v>
+      </c>
+      <c r="P31" s="12"/>
+      <c r="Q31" s="50">
         <v>45632</v>
       </c>
-      <c r="R31" s="57">
+      <c r="R31" s="56">
         <v>45646</v>
       </c>
       <c r="S31" s="53"/>
@@ -68653,6 +68827,10 @@
       <c r="BT31" s="12"/>
       <c r="BU31" s="12"/>
       <c r="BV31" s="12"/>
+      <c r="BW31" s="89"/>
+      <c r="BX31" s="89"/>
+      <c r="BY31" s="89"/>
+      <c r="BZ31" s="89"/>
       <c r="CA31" s="12"/>
       <c r="CB31" s="12"/>
       <c r="CC31" s="12"/>
@@ -68660,46 +68838,53 @@
       <c r="CE31" s="12"/>
       <c r="CF31" s="12"/>
       <c r="CG31" s="12"/>
-      <c r="CH31" s="46"/>
-      <c r="CI31" s="46"/>
-    </row>
-    <row r="32" spans="1:87" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
-        <v>1778</v>
+      <c r="CH31" s="12"/>
+      <c r="CI31" s="12"/>
+      <c r="CJ31" s="12"/>
+      <c r="CK31" s="12"/>
+      <c r="CL31" s="12"/>
+      <c r="CM31" s="12"/>
+      <c r="CN31" s="12"/>
+    </row>
+    <row r="32" spans="1:92" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
+        <v>1777</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>1836</v>
+        <v>1835</v>
       </c>
       <c r="C32" s="12"/>
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="19" t="s">
+        <v>1841</v>
+      </c>
+      <c r="E32" s="21" t="s">
+        <v>1837</v>
+      </c>
+      <c r="F32" s="20"/>
+      <c r="G32" s="10" t="s">
         <v>1842</v>
       </c>
-      <c r="E32" s="17" t="s">
-        <v>1838</v>
-      </c>
-      <c r="F32" s="22"/>
-      <c r="G32" s="49" t="s">
-        <v>1843</v>
-      </c>
-      <c r="H32" s="49" t="s">
+      <c r="H32" s="10" t="s">
         <v>1716</v>
       </c>
-      <c r="I32" s="49">
+      <c r="I32" s="12">
         <v>8.1</v>
       </c>
-      <c r="J32" s="49"/>
-      <c r="K32" s="49"/>
-      <c r="L32" s="55"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="54"/>
       <c r="M32" s="12"/>
-      <c r="N32" s="49">
+      <c r="N32" s="12">
         <v>10</v>
       </c>
-      <c r="O32" s="49"/>
-      <c r="P32" s="49"/>
-      <c r="Q32" s="51">
+      <c r="O32" s="12" t="s">
+        <v>1863</v>
+      </c>
+      <c r="P32" s="12"/>
+      <c r="Q32" s="50">
         <v>45649</v>
       </c>
-      <c r="R32" s="57">
+      <c r="R32" s="56">
         <v>45667</v>
       </c>
       <c r="S32" s="53"/>
@@ -68769,22 +68954,27 @@
       <c r="CE32" s="12"/>
       <c r="CF32" s="12"/>
       <c r="CG32" s="12"/>
-      <c r="CH32" s="48"/>
-      <c r="CI32" s="48"/>
-    </row>
-    <row r="33" spans="1:91" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CH32" s="12"/>
+      <c r="CI32" s="12"/>
+      <c r="CJ32" s="12"/>
+      <c r="CK32" s="12"/>
+      <c r="CL32" s="12"/>
+      <c r="CM32" s="89"/>
+      <c r="CN32" s="12"/>
+    </row>
+    <row r="33" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>1873</v>
+        <v>1872</v>
       </c>
       <c r="C33" s="15"/>
       <c r="D33" s="15" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
       <c r="F33" s="30"/>
       <c r="G33" s="10" t="s">
@@ -68811,49 +69001,49 @@
       <c r="X33" s="12"/>
       <c r="Y33" s="12"/>
       <c r="Z33" s="12"/>
-      <c r="AA33" s="67"/>
-      <c r="AB33" s="67"/>
-      <c r="AC33" s="67"/>
-      <c r="AD33" s="67"/>
-      <c r="AE33" s="67"/>
-      <c r="AF33" s="67"/>
-      <c r="AG33" s="67"/>
-      <c r="AH33" s="67"/>
-      <c r="AI33" s="67"/>
-      <c r="AJ33" s="67"/>
-      <c r="AK33" s="67"/>
-      <c r="AL33" s="67"/>
-      <c r="AM33" s="67"/>
-      <c r="AN33" s="67"/>
-      <c r="AO33" s="67"/>
-      <c r="AP33" s="67"/>
-      <c r="AQ33" s="67"/>
-      <c r="AR33" s="67"/>
-      <c r="AS33" s="67"/>
-      <c r="AT33" s="67"/>
-      <c r="AU33" s="67"/>
-      <c r="AV33" s="67"/>
-      <c r="AW33" s="67"/>
-      <c r="AX33" s="67"/>
-      <c r="AY33" s="67"/>
-      <c r="AZ33" s="67"/>
-      <c r="BA33" s="67"/>
-      <c r="BB33" s="67"/>
-      <c r="BC33" s="67"/>
-      <c r="BD33" s="67"/>
-      <c r="BE33" s="67"/>
-      <c r="BF33" s="67"/>
-      <c r="BG33" s="67"/>
-      <c r="BH33" s="67"/>
-      <c r="BI33" s="67"/>
-      <c r="BJ33" s="67"/>
-      <c r="BK33" s="67"/>
-      <c r="BL33" s="67"/>
-      <c r="BM33" s="67"/>
-      <c r="BN33" s="67"/>
-      <c r="BO33" s="67"/>
-      <c r="BP33" s="67"/>
-      <c r="BQ33" s="67"/>
+      <c r="AA33" s="12"/>
+      <c r="AB33" s="12"/>
+      <c r="AC33" s="12"/>
+      <c r="AD33" s="12"/>
+      <c r="AE33" s="12"/>
+      <c r="AF33" s="12"/>
+      <c r="AG33" s="12"/>
+      <c r="AH33" s="12"/>
+      <c r="AI33" s="12"/>
+      <c r="AJ33" s="12"/>
+      <c r="AK33" s="12"/>
+      <c r="AL33" s="12"/>
+      <c r="AM33" s="12"/>
+      <c r="AN33" s="12"/>
+      <c r="AO33" s="12"/>
+      <c r="AP33" s="12"/>
+      <c r="AQ33" s="12"/>
+      <c r="AR33" s="12"/>
+      <c r="AS33" s="12"/>
+      <c r="AT33" s="12"/>
+      <c r="AU33" s="12"/>
+      <c r="AV33" s="12"/>
+      <c r="AW33" s="12"/>
+      <c r="AX33" s="12"/>
+      <c r="AY33" s="12"/>
+      <c r="AZ33" s="12"/>
+      <c r="BA33" s="12"/>
+      <c r="BB33" s="12"/>
+      <c r="BC33" s="12"/>
+      <c r="BD33" s="12"/>
+      <c r="BE33" s="12"/>
+      <c r="BF33" s="12"/>
+      <c r="BG33" s="12"/>
+      <c r="BH33" s="12"/>
+      <c r="BI33" s="12"/>
+      <c r="BJ33" s="12"/>
+      <c r="BK33" s="12"/>
+      <c r="BL33" s="12"/>
+      <c r="BM33" s="12"/>
+      <c r="BN33" s="12"/>
+      <c r="BO33" s="12"/>
+      <c r="BP33" s="12"/>
+      <c r="BQ33" s="12"/>
       <c r="BR33" s="12"/>
       <c r="BS33" s="12"/>
       <c r="BT33" s="12"/>
@@ -68872,20 +69062,25 @@
       <c r="CG33" s="12"/>
       <c r="CH33" s="12"/>
       <c r="CI33" s="12"/>
-    </row>
-    <row r="34" spans="1:91" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CJ33" s="12"/>
+      <c r="CK33" s="12"/>
+      <c r="CL33" s="12"/>
+      <c r="CM33" s="12"/>
+      <c r="CN33" s="12"/>
+    </row>
+    <row r="34" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
-        <v>1777</v>
-      </c>
-      <c r="B34" s="72" t="s">
-        <v>1873</v>
-      </c>
-      <c r="C34" s="72"/>
+        <v>1776</v>
+      </c>
+      <c r="B34" s="69" t="s">
+        <v>1872</v>
+      </c>
+      <c r="C34" s="69"/>
       <c r="D34" s="15" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
       <c r="F34" s="30"/>
       <c r="G34" s="10" t="s">
@@ -68973,20 +69168,25 @@
       <c r="CG34" s="12"/>
       <c r="CH34" s="12"/>
       <c r="CI34" s="12"/>
-    </row>
-    <row r="35" spans="1:91" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CJ34" s="12"/>
+      <c r="CK34" s="12"/>
+      <c r="CL34" s="12"/>
+      <c r="CM34" s="12"/>
+      <c r="CN34" s="12"/>
+    </row>
+    <row r="35" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
-        <v>1777</v>
-      </c>
-      <c r="B35" s="72" t="s">
-        <v>1873</v>
-      </c>
-      <c r="C35" s="72"/>
-      <c r="D35" s="15" t="s">
-        <v>1876</v>
-      </c>
-      <c r="E35" s="17" t="s">
-        <v>1838</v>
+        <v>1776</v>
+      </c>
+      <c r="B35" s="69" t="s">
+        <v>1872</v>
+      </c>
+      <c r="C35" s="69"/>
+      <c r="D35" s="19" t="s">
+        <v>1875</v>
+      </c>
+      <c r="E35" s="29" t="s">
+        <v>1837</v>
       </c>
       <c r="F35" s="30"/>
       <c r="G35" s="10" t="s">
@@ -69074,38 +69274,43 @@
       <c r="CG35" s="12"/>
       <c r="CH35" s="12"/>
       <c r="CI35" s="12"/>
-    </row>
-    <row r="36" spans="1:91" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="s">
-        <v>1777</v>
-      </c>
-      <c r="B36" s="72" t="s">
-        <v>1873</v>
-      </c>
-      <c r="C36" s="72"/>
-      <c r="D36" s="15" t="s">
-        <v>1877</v>
-      </c>
-      <c r="E36" s="17" t="s">
-        <v>1838</v>
-      </c>
-      <c r="F36" s="30"/>
-      <c r="G36" s="10" t="s">
+      <c r="CJ35" s="12"/>
+      <c r="CK35" s="12"/>
+      <c r="CL35" s="12"/>
+      <c r="CM35" s="12"/>
+      <c r="CN35" s="12"/>
+    </row>
+    <row r="36" spans="1:92" x14ac:dyDescent="0.25">
+      <c r="A36" s="81" t="s">
+        <v>1776</v>
+      </c>
+      <c r="B36" s="60" t="s">
+        <v>1872</v>
+      </c>
+      <c r="C36" s="60"/>
+      <c r="D36" s="81" t="s">
+        <v>1876</v>
+      </c>
+      <c r="E36" s="81" t="s">
+        <v>1837</v>
+      </c>
+      <c r="F36" s="81"/>
+      <c r="G36" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="H36" s="10" t="s">
+      <c r="H36" s="81" t="s">
         <v>1075</v>
       </c>
-      <c r="I36" s="12"/>
-      <c r="J36" s="12"/>
-      <c r="K36" s="12"/>
-      <c r="L36" s="54"/>
-      <c r="M36" s="12"/>
-      <c r="N36" s="12"/>
-      <c r="O36" s="12"/>
-      <c r="P36" s="12"/>
-      <c r="Q36" s="12"/>
-      <c r="R36" s="12"/>
+      <c r="I36" s="79"/>
+      <c r="J36" s="79"/>
+      <c r="K36" s="79"/>
+      <c r="L36" s="90"/>
+      <c r="M36" s="79"/>
+      <c r="N36" s="79"/>
+      <c r="O36" s="79"/>
+      <c r="P36" s="79"/>
+      <c r="Q36" s="91"/>
+      <c r="R36" s="91"/>
       <c r="S36" s="53"/>
       <c r="T36" s="12"/>
       <c r="U36" s="12"/>
@@ -69175,22 +69380,27 @@
       <c r="CG36" s="12"/>
       <c r="CH36" s="12"/>
       <c r="CI36" s="12"/>
-    </row>
-    <row r="37" spans="1:91" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="CJ36" s="12"/>
+      <c r="CK36" s="12"/>
+      <c r="CL36" s="12"/>
+      <c r="CM36" s="12"/>
+      <c r="CN36" s="12"/>
+    </row>
+    <row r="37" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
-        <v>1777</v>
-      </c>
-      <c r="B37" s="72" t="s">
-        <v>1872</v>
-      </c>
-      <c r="C37" s="72" t="s">
+        <v>1776</v>
+      </c>
+      <c r="B37" s="69" t="s">
+        <v>1871</v>
+      </c>
+      <c r="C37" s="69" t="s">
+        <v>1869</v>
+      </c>
+      <c r="D37" s="15" t="s">
         <v>1870</v>
       </c>
-      <c r="D37" s="19" t="s">
-        <v>1871</v>
-      </c>
-      <c r="E37" s="29" t="s">
-        <v>1783</v>
+      <c r="E37" s="17" t="s">
+        <v>1782</v>
       </c>
       <c r="F37" s="30"/>
       <c r="G37" s="10" t="s">
@@ -69201,9 +69411,12 @@
       <c r="J37" s="12"/>
       <c r="K37" s="12"/>
       <c r="L37" s="54"/>
+      <c r="M37" s="89"/>
       <c r="N37" s="12"/>
       <c r="O37" s="12"/>
       <c r="P37" s="12"/>
+      <c r="Q37" s="89"/>
+      <c r="R37" s="89"/>
       <c r="S37" s="53"/>
       <c r="T37" s="12"/>
       <c r="U37" s="12"/>
@@ -69273,245 +69486,337 @@
       <c r="CG37" s="12"/>
       <c r="CH37" s="12"/>
       <c r="CI37" s="12"/>
-    </row>
-    <row r="38" spans="1:91" s="63" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="61"/>
-      <c r="B38" s="62"/>
-      <c r="C38" s="62"/>
-      <c r="D38" s="61"/>
-      <c r="E38" s="62"/>
-      <c r="F38" s="62"/>
-      <c r="G38" s="61"/>
-      <c r="H38" s="62"/>
-      <c r="Q38" s="64"/>
-      <c r="R38" s="64"/>
-    </row>
-    <row r="39" spans="1:91" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="71" t="s">
-        <v>1778</v>
-      </c>
-      <c r="B39" s="67"/>
-      <c r="C39" s="67"/>
-      <c r="D39" s="65" t="s">
+      <c r="CJ37" s="12"/>
+      <c r="CK37" s="12"/>
+      <c r="CL37" s="12"/>
+      <c r="CM37" s="12"/>
+      <c r="CN37" s="12"/>
+    </row>
+    <row r="38" spans="1:92" s="61" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="82" t="s">
+        <v>1777</v>
+      </c>
+      <c r="B38" s="83" t="s">
+        <v>1889</v>
+      </c>
+      <c r="C38" s="83" t="s">
+        <v>1890</v>
+      </c>
+      <c r="D38" s="84" t="s">
+        <v>1879</v>
+      </c>
+      <c r="E38" s="85" t="s">
+        <v>1878</v>
+      </c>
+      <c r="F38" s="87"/>
+      <c r="G38" s="59" t="s">
+        <v>176</v>
+      </c>
+      <c r="H38" s="88" t="s">
         <v>1880</v>
       </c>
-      <c r="E39" s="66" t="s">
-        <v>1879</v>
-      </c>
-      <c r="F39" s="67"/>
-      <c r="G39" s="68" t="s">
-        <v>176</v>
-      </c>
-      <c r="H39" s="68" t="s">
-        <v>1881</v>
-      </c>
-      <c r="I39" s="67">
+      <c r="I38" s="89">
         <v>23</v>
       </c>
-      <c r="J39" s="67"/>
-      <c r="K39" s="67"/>
-      <c r="L39" s="67"/>
-      <c r="M39" s="67"/>
-      <c r="N39" s="67"/>
-      <c r="O39" s="67"/>
-      <c r="P39" s="67" t="s">
-        <v>1882</v>
-      </c>
-      <c r="Q39" s="67"/>
-      <c r="R39" s="67"/>
-      <c r="S39" s="67"/>
-      <c r="T39" s="67"/>
-      <c r="U39" s="67"/>
-      <c r="V39" s="67"/>
-      <c r="W39" s="67"/>
-      <c r="X39" s="67"/>
-      <c r="Y39" s="67"/>
-      <c r="Z39" s="67"/>
-      <c r="AA39" s="67"/>
-      <c r="AB39" s="67"/>
-      <c r="AC39" s="67"/>
-      <c r="AD39" s="67"/>
-      <c r="AE39" s="67"/>
-      <c r="AF39" s="67"/>
-      <c r="AG39" s="67"/>
-      <c r="AH39" s="67"/>
-      <c r="AI39" s="67"/>
-      <c r="AJ39" s="67"/>
-      <c r="AK39" s="67"/>
-      <c r="AL39" s="67"/>
-      <c r="AM39" s="67"/>
-      <c r="AN39" s="67"/>
-      <c r="AO39" s="67"/>
-      <c r="AP39" s="67"/>
-      <c r="AQ39" s="67"/>
-      <c r="AR39" s="67"/>
-      <c r="AS39" s="67"/>
-      <c r="AT39" s="67"/>
-      <c r="AU39" s="67"/>
-      <c r="AV39" s="67"/>
-      <c r="AW39" s="67"/>
-      <c r="AX39" s="67"/>
-      <c r="AY39" s="67"/>
-      <c r="AZ39" s="67"/>
-      <c r="BA39" s="67"/>
-      <c r="BB39" s="67"/>
-      <c r="BC39" s="67"/>
-      <c r="BD39" s="67"/>
-      <c r="BE39" s="67"/>
-      <c r="BF39" s="67"/>
-      <c r="BG39" s="67"/>
-      <c r="BH39" s="67"/>
-      <c r="BI39" s="67"/>
-      <c r="BJ39" s="67"/>
-      <c r="BK39" s="67"/>
-      <c r="BL39" s="67"/>
-      <c r="BM39" s="67"/>
-      <c r="BN39" s="67"/>
-      <c r="BO39" s="67"/>
-      <c r="BP39" s="67"/>
-      <c r="BQ39" s="67"/>
-      <c r="BR39" s="67"/>
-      <c r="BS39" s="67"/>
-      <c r="BT39" s="67"/>
-      <c r="BU39" s="67"/>
-      <c r="BV39" s="67"/>
-      <c r="BW39" s="67"/>
-      <c r="BX39" s="67"/>
-      <c r="BY39" s="67"/>
-      <c r="BZ39" s="67"/>
-      <c r="CA39" s="67"/>
-      <c r="CB39" s="67"/>
-      <c r="CC39" s="67"/>
-      <c r="CD39" s="67"/>
-      <c r="CE39" s="67"/>
-      <c r="CF39" s="67"/>
-      <c r="CG39" s="67"/>
-      <c r="CH39" s="67"/>
-      <c r="CI39" s="67"/>
-      <c r="CJ39" s="67"/>
-      <c r="CK39" s="67"/>
-      <c r="CL39" s="67"/>
-      <c r="CM39" s="67"/>
-    </row>
-    <row r="40" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="A40" s="69"/>
-      <c r="B40" s="69"/>
-      <c r="C40" s="69"/>
-      <c r="D40" s="69"/>
-      <c r="E40" s="69"/>
-      <c r="F40" s="69"/>
-      <c r="G40" s="70"/>
-      <c r="H40" s="69"/>
-      <c r="I40" s="69"/>
-      <c r="J40" s="69"/>
-      <c r="K40" s="69"/>
-      <c r="L40" s="69"/>
-      <c r="M40" s="69"/>
-      <c r="N40" s="69"/>
-      <c r="O40" s="69"/>
-      <c r="P40" s="69"/>
-      <c r="Q40" s="69"/>
-      <c r="R40" s="69"/>
-      <c r="S40" s="69"/>
-      <c r="T40" s="69"/>
-      <c r="U40" s="69"/>
-      <c r="V40" s="69"/>
-      <c r="W40" s="69"/>
-      <c r="X40" s="69"/>
-      <c r="Y40" s="69"/>
-      <c r="Z40" s="69"/>
-      <c r="AA40" s="69"/>
-      <c r="AB40" s="69"/>
-      <c r="AC40" s="69"/>
-      <c r="AD40" s="69"/>
-      <c r="AE40" s="69"/>
-      <c r="AF40" s="69"/>
-      <c r="AG40" s="69"/>
-      <c r="AH40" s="69"/>
-      <c r="AI40" s="69"/>
-      <c r="AJ40" s="69"/>
-      <c r="AK40" s="69"/>
-      <c r="AL40" s="69"/>
-      <c r="AM40" s="69"/>
-      <c r="AN40" s="69"/>
-      <c r="AO40" s="69"/>
-      <c r="AP40" s="69"/>
-      <c r="AQ40" s="69"/>
-      <c r="AR40" s="69"/>
-      <c r="AS40" s="69"/>
-      <c r="AT40" s="69"/>
-      <c r="AU40" s="69"/>
-      <c r="AV40" s="69"/>
-      <c r="AW40" s="69"/>
-      <c r="AX40" s="69"/>
-      <c r="AY40" s="69"/>
-      <c r="AZ40" s="69"/>
-      <c r="BA40" s="69"/>
-      <c r="BB40" s="69"/>
-      <c r="BC40" s="69"/>
-      <c r="BD40" s="69"/>
-      <c r="BE40" s="69"/>
-      <c r="BF40" s="69"/>
-      <c r="BG40" s="69"/>
-      <c r="BH40" s="69"/>
-      <c r="BI40" s="69"/>
-      <c r="BJ40" s="69"/>
-      <c r="BK40" s="69"/>
-      <c r="BL40" s="69"/>
-      <c r="BM40" s="69"/>
-      <c r="BN40" s="69"/>
-      <c r="BO40" s="69"/>
-      <c r="BP40" s="69"/>
-      <c r="BQ40" s="69"/>
-      <c r="BR40" s="69"/>
-      <c r="BS40" s="69"/>
-      <c r="BT40" s="69"/>
-      <c r="BU40" s="69"/>
-      <c r="BV40" s="69"/>
-      <c r="BW40" s="69"/>
-      <c r="BX40" s="69"/>
-      <c r="BY40" s="69"/>
-      <c r="BZ40" s="69"/>
-      <c r="CA40" s="69"/>
-      <c r="CB40" s="69"/>
-      <c r="CC40" s="69"/>
-      <c r="CD40" s="69"/>
-      <c r="CE40" s="69"/>
-      <c r="CF40" s="69"/>
-      <c r="CG40" s="69"/>
-      <c r="CH40" s="69"/>
-      <c r="CI40" s="69"/>
-      <c r="CJ40" s="69"/>
-      <c r="CK40" s="69"/>
-      <c r="CL40" s="69"/>
-      <c r="CM40" s="69"/>
-    </row>
-    <row r="41" spans="1:91" x14ac:dyDescent="0.25">
-      <c r="G41" s="60"/>
+      <c r="J38" s="89"/>
+      <c r="K38" s="89"/>
+      <c r="L38" s="89"/>
+      <c r="M38" s="89"/>
+      <c r="N38" s="89"/>
+      <c r="O38" s="89"/>
+      <c r="P38" s="89"/>
+      <c r="Q38" s="89"/>
+      <c r="R38" s="89"/>
+      <c r="S38" s="92"/>
+      <c r="T38" s="92"/>
+      <c r="U38" s="92"/>
+      <c r="V38" s="92"/>
+      <c r="W38" s="92"/>
+      <c r="X38" s="92"/>
+      <c r="Y38" s="92"/>
+      <c r="Z38" s="92"/>
+      <c r="AA38" s="92"/>
+      <c r="AB38" s="92"/>
+      <c r="AC38" s="92"/>
+      <c r="AD38" s="92"/>
+      <c r="AE38" s="92"/>
+      <c r="AF38" s="92"/>
+      <c r="AG38" s="92"/>
+      <c r="AH38" s="92"/>
+      <c r="AI38" s="92"/>
+      <c r="AJ38" s="92"/>
+      <c r="AK38" s="92"/>
+      <c r="AL38" s="92"/>
+      <c r="AM38" s="92"/>
+      <c r="AN38" s="92"/>
+      <c r="AO38" s="92"/>
+      <c r="AP38" s="92"/>
+      <c r="AQ38" s="92"/>
+      <c r="AR38" s="92"/>
+      <c r="AS38" s="92"/>
+      <c r="AT38" s="92"/>
+      <c r="AU38" s="92"/>
+      <c r="AV38" s="92"/>
+      <c r="AW38" s="92"/>
+      <c r="AX38" s="92"/>
+      <c r="AY38" s="92"/>
+      <c r="AZ38" s="92"/>
+      <c r="BA38" s="92"/>
+      <c r="BB38" s="92"/>
+      <c r="BC38" s="92"/>
+      <c r="BD38" s="92"/>
+      <c r="BE38" s="92"/>
+      <c r="BF38" s="92"/>
+      <c r="BG38" s="92"/>
+      <c r="BH38" s="92"/>
+      <c r="BI38" s="92"/>
+      <c r="BJ38" s="92"/>
+      <c r="BK38" s="92"/>
+      <c r="BL38" s="92"/>
+      <c r="BM38" s="92"/>
+      <c r="BN38" s="92"/>
+      <c r="BO38" s="92"/>
+      <c r="BP38" s="92"/>
+      <c r="BQ38" s="92"/>
+      <c r="BR38" s="89"/>
+      <c r="BS38" s="89"/>
+      <c r="BT38" s="89"/>
+      <c r="BU38" s="89"/>
+      <c r="BV38" s="89"/>
+      <c r="BW38" s="89"/>
+      <c r="BX38" s="89"/>
+      <c r="BY38" s="89"/>
+      <c r="BZ38" s="89"/>
+      <c r="CA38" s="89"/>
+      <c r="CB38" s="89"/>
+      <c r="CC38" s="89"/>
+      <c r="CD38" s="89"/>
+      <c r="CE38" s="89"/>
+      <c r="CF38" s="89"/>
+      <c r="CG38" s="89"/>
+      <c r="CH38" s="89"/>
+      <c r="CI38" s="89"/>
+      <c r="CJ38" s="89"/>
+      <c r="CK38" s="89"/>
+      <c r="CL38" s="89"/>
+      <c r="CM38" s="89"/>
+      <c r="CN38" s="89"/>
+    </row>
+    <row r="39" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="68"/>
+      <c r="B39" s="64" t="s">
+        <v>1889</v>
+      </c>
+      <c r="C39" s="64"/>
+      <c r="D39" s="62"/>
+      <c r="E39" s="63"/>
+      <c r="F39" s="64"/>
+      <c r="G39" s="65"/>
+      <c r="H39" s="65"/>
+      <c r="I39" s="64"/>
+      <c r="J39" s="64"/>
+      <c r="K39" s="64"/>
+      <c r="L39" s="64"/>
+      <c r="M39" s="64"/>
+      <c r="N39" s="64"/>
+      <c r="O39" s="64"/>
+      <c r="P39" s="64"/>
+      <c r="Q39" s="64"/>
+      <c r="R39" s="64"/>
+      <c r="S39" s="79"/>
+      <c r="T39" s="79"/>
+      <c r="U39" s="79"/>
+      <c r="V39" s="79"/>
+      <c r="W39" s="79"/>
+      <c r="X39" s="79"/>
+      <c r="Y39" s="79"/>
+      <c r="Z39" s="79"/>
+      <c r="AA39" s="79"/>
+      <c r="AB39" s="79"/>
+      <c r="AC39" s="79"/>
+      <c r="AD39" s="79"/>
+      <c r="AE39" s="79"/>
+      <c r="AF39" s="79"/>
+      <c r="AG39" s="79"/>
+      <c r="AH39" s="79"/>
+      <c r="AI39" s="79"/>
+      <c r="AJ39" s="79"/>
+      <c r="AK39" s="79"/>
+      <c r="AL39" s="79"/>
+      <c r="AM39" s="79"/>
+      <c r="AN39" s="79"/>
+      <c r="AO39" s="79"/>
+      <c r="AP39" s="79"/>
+      <c r="AQ39" s="79"/>
+      <c r="AR39" s="79"/>
+      <c r="AS39" s="79"/>
+      <c r="AT39" s="79"/>
+      <c r="AU39" s="79"/>
+      <c r="AV39" s="79"/>
+      <c r="AW39" s="79"/>
+      <c r="AX39" s="79"/>
+      <c r="AY39" s="79"/>
+      <c r="AZ39" s="79"/>
+      <c r="BA39" s="79"/>
+      <c r="BB39" s="79"/>
+      <c r="BC39" s="79"/>
+      <c r="BD39" s="79"/>
+      <c r="BE39" s="79"/>
+      <c r="BF39" s="79"/>
+      <c r="BG39" s="79"/>
+      <c r="BH39" s="79"/>
+      <c r="BI39" s="79"/>
+      <c r="BJ39" s="79"/>
+      <c r="BK39" s="79"/>
+      <c r="BL39" s="79"/>
+      <c r="BM39" s="79"/>
+      <c r="BN39" s="79"/>
+      <c r="BO39" s="79"/>
+      <c r="BP39" s="79"/>
+      <c r="BQ39" s="61"/>
+      <c r="BR39" s="61"/>
+      <c r="BS39" s="61"/>
+      <c r="BT39" s="61"/>
+      <c r="BU39" s="61"/>
+      <c r="BV39" s="61"/>
+      <c r="BW39" s="61"/>
+      <c r="BX39" s="61"/>
+      <c r="BY39" s="61"/>
+      <c r="BZ39" s="61"/>
+      <c r="CA39" s="61"/>
+      <c r="CB39" s="61"/>
+      <c r="CC39" s="61"/>
+      <c r="CD39" s="61"/>
+      <c r="CE39" s="61"/>
+      <c r="CF39" s="61"/>
+      <c r="CG39" s="61"/>
+      <c r="CH39" s="61"/>
+      <c r="CI39" s="61"/>
+      <c r="CJ39" s="61"/>
+      <c r="CK39" s="61"/>
+      <c r="CL39" s="61"/>
+      <c r="CM39" s="61"/>
+    </row>
+    <row r="40" spans="1:92" x14ac:dyDescent="0.25">
+      <c r="A40" s="66"/>
+      <c r="B40" s="66"/>
+      <c r="C40" s="66"/>
+      <c r="D40" s="66"/>
+      <c r="E40" s="66"/>
+      <c r="F40" s="66"/>
+      <c r="G40" s="67"/>
+      <c r="H40" s="66"/>
+      <c r="I40" s="66"/>
+      <c r="J40" s="66"/>
+      <c r="K40" s="66"/>
+      <c r="L40" s="66"/>
+      <c r="M40" s="66"/>
+      <c r="N40" s="66"/>
+      <c r="O40" s="66"/>
+      <c r="P40" s="66"/>
+      <c r="Q40" s="66"/>
+      <c r="R40" s="66"/>
+      <c r="S40" s="66"/>
+      <c r="T40" s="66"/>
+      <c r="U40" s="66"/>
+      <c r="V40" s="66"/>
+      <c r="W40" s="66"/>
+      <c r="X40" s="66"/>
+      <c r="Y40" s="66"/>
+      <c r="Z40" s="66"/>
+      <c r="AA40" s="66"/>
+      <c r="AB40" s="66"/>
+      <c r="AC40" s="66"/>
+      <c r="AD40" s="66"/>
+      <c r="AE40" s="66"/>
+      <c r="AF40" s="66"/>
+      <c r="AG40" s="66"/>
+      <c r="AH40" s="66"/>
+      <c r="AI40" s="66"/>
+      <c r="AJ40" s="66"/>
+      <c r="AK40" s="66"/>
+      <c r="AL40" s="66"/>
+      <c r="AM40" s="66"/>
+      <c r="AN40" s="66"/>
+      <c r="AO40" s="66"/>
+      <c r="AP40" s="66"/>
+      <c r="AQ40" s="66"/>
+      <c r="AR40" s="66"/>
+      <c r="AS40" s="66"/>
+      <c r="AT40" s="66"/>
+      <c r="AU40" s="66"/>
+      <c r="AV40" s="66"/>
+      <c r="AW40" s="66"/>
+      <c r="AX40" s="66"/>
+      <c r="AY40" s="66"/>
+      <c r="AZ40" s="66"/>
+      <c r="BA40" s="66"/>
+      <c r="BB40" s="66"/>
+      <c r="BC40" s="66"/>
+      <c r="BD40" s="66"/>
+      <c r="BE40" s="66"/>
+      <c r="BF40" s="66"/>
+      <c r="BG40" s="66"/>
+      <c r="BH40" s="66"/>
+      <c r="BI40" s="66"/>
+      <c r="BJ40" s="66"/>
+      <c r="BK40" s="66"/>
+      <c r="BL40" s="66"/>
+      <c r="BM40" s="66"/>
+      <c r="BN40" s="66"/>
+      <c r="BO40" s="66"/>
+      <c r="BP40" s="66"/>
+      <c r="BQ40" s="66"/>
+      <c r="BR40" s="66"/>
+      <c r="BS40" s="66"/>
+      <c r="BT40" s="66"/>
+      <c r="BU40" s="66"/>
+      <c r="BV40" s="66"/>
+      <c r="BW40" s="66"/>
+      <c r="BX40" s="66"/>
+      <c r="BY40" s="66"/>
+      <c r="BZ40" s="66"/>
+      <c r="CA40" s="66"/>
+      <c r="CB40" s="66"/>
+      <c r="CC40" s="66"/>
+      <c r="CD40" s="66"/>
+      <c r="CE40" s="66"/>
+      <c r="CF40" s="66"/>
+      <c r="CG40" s="66"/>
+      <c r="CH40" s="66"/>
+      <c r="CI40" s="66"/>
+      <c r="CJ40" s="66"/>
+      <c r="CK40" s="66"/>
+      <c r="CL40" s="66"/>
+      <c r="CM40" s="66"/>
+    </row>
+    <row r="41" spans="1:92" x14ac:dyDescent="0.25">
+      <c r="G41" s="59"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:CI37" xr:uid="{9585C0FF-65C5-4BD8-9936-5C9A63F7E604}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:CI37">
-      <sortCondition ref="B2:B37"/>
+  <autoFilter ref="A2:CN39" xr:uid="{9585C0FF-65C5-4BD8-9936-5C9A63F7E604}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:CN39">
+      <sortCondition ref="B2:B39"/>
     </sortState>
   </autoFilter>
-  <mergeCells count="16">
+  <mergeCells count="17">
+    <mergeCell ref="CK1:CL1"/>
+    <mergeCell ref="AO1:AR1"/>
+    <mergeCell ref="AS1:AV1"/>
+    <mergeCell ref="AW1:AZ1"/>
+    <mergeCell ref="BA1:BE1"/>
+    <mergeCell ref="BF1:BI1"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="W1:AA1"/>
+    <mergeCell ref="AB1:AE1"/>
+    <mergeCell ref="AF1:AI1"/>
+    <mergeCell ref="AJ1:AN1"/>
     <mergeCell ref="CF1:CG1"/>
     <mergeCell ref="BJ1:BN1"/>
     <mergeCell ref="BO1:BR1"/>
     <mergeCell ref="BS1:BV1"/>
     <mergeCell ref="BW1:BZ1"/>
     <mergeCell ref="CB1:CE1"/>
-    <mergeCell ref="S1:V1"/>
-    <mergeCell ref="W1:AA1"/>
-    <mergeCell ref="AB1:AE1"/>
-    <mergeCell ref="AF1:AI1"/>
-    <mergeCell ref="AJ1:AN1"/>
-    <mergeCell ref="AO1:AR1"/>
-    <mergeCell ref="AS1:AV1"/>
-    <mergeCell ref="AW1:AZ1"/>
-    <mergeCell ref="BA1:BE1"/>
-    <mergeCell ref="BF1:BI1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
actualization de avance gral
</commit_message>
<xml_diff>
--- a/00-Documentacion/Listado de reportes totales-TI.xlsx
+++ b/00-Documentacion/Listado de reportes totales-TI.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF91E91F-6660-4C9D-A74F-72F1632E1310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3579DB9-21A1-4186-8A38-F7A24AF64137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{1498AA1A-1ACC-4329-A050-ACA05131B658}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="4" xr2:uid="{1498AA1A-1ACC-4329-A050-ACA05131B658}"/>
   </bookViews>
   <sheets>
     <sheet name="General - Analisis" sheetId="4" r:id="rId1"/>
     <sheet name="listado modulo sin area" sheetId="6" r:id="rId2"/>
     <sheet name="Analisis Proceso con prioridad" sheetId="5" r:id="rId3"/>
+    <sheet name="Hoja1" sheetId="7" r:id="rId4"/>
+    <sheet name="Avance General" sheetId="8" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Analisis Proceso con prioridad'!$A$2:$CN$39</definedName>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13314" uniqueCount="1893">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13353" uniqueCount="1910">
   <si>
     <t xml:space="preserve">Reporte </t>
   </si>
@@ -5721,13 +5723,64 @@
   </si>
   <si>
     <t>22-26</t>
+  </si>
+  <si>
+    <t>MIGRACION SPOOLER</t>
+  </si>
+  <si>
+    <t>PROCESO</t>
+  </si>
+  <si>
+    <t>SUBPROCESO</t>
+  </si>
+  <si>
+    <t>AVANCE</t>
+  </si>
+  <si>
+    <t>COMENTARIOS</t>
+  </si>
+  <si>
+    <t>BD</t>
+  </si>
+  <si>
+    <t>Diseño</t>
+  </si>
+  <si>
+    <t>Carga Información</t>
+  </si>
+  <si>
+    <t>Cuentas</t>
+  </si>
+  <si>
+    <t>Generación de Procedimientos</t>
+  </si>
+  <si>
+    <t>Servidores</t>
+  </si>
+  <si>
+    <t>Configuración librerías (instancian aplicación)</t>
+  </si>
+  <si>
+    <t>Cuentas (correo, carpetas)</t>
+  </si>
+  <si>
+    <t>Sitios</t>
+  </si>
+  <si>
+    <t>Desarrollo</t>
+  </si>
+  <si>
+    <t>Reportes 10 de 33</t>
+  </si>
+  <si>
+    <t>El Diseño BD afectaría el avance, versión no validada con usuario</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5840,8 +5893,47 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <color theme="7" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5932,8 +6024,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -6041,11 +6139,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6198,6 +6346,31 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -6216,41 +6389,70 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="9" fontId="20" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="17" fillId="0" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -8812,7 +9014,7 @@
       </c>
       <c r="R54" s="8"/>
     </row>
-    <row r="55" spans="1:18" ht="39" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>14</v>
       </c>
@@ -9340,7 +9542,7 @@
       </c>
       <c r="R66" s="8"/>
     </row>
-    <row r="67" spans="1:18" ht="51.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" ht="39" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
         <v>14</v>
       </c>
@@ -16644,7 +16846,7 @@
       <c r="Q262" s="8"/>
       <c r="R262" s="8"/>
     </row>
-    <row r="263" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A263" s="5">
         <v>67</v>
       </c>
@@ -22056,7 +22258,7 @@
       </c>
       <c r="R403" s="8"/>
     </row>
-    <row r="404" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A404" s="5">
         <v>138</v>
       </c>
@@ -25072,7 +25274,7 @@
       </c>
       <c r="R479" s="8"/>
     </row>
-    <row r="480" spans="1:18" ht="39" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A480" s="5">
         <v>173</v>
       </c>
@@ -26964,7 +27166,7 @@
       </c>
       <c r="R522" s="8"/>
     </row>
-    <row r="523" spans="1:18" ht="39" x14ac:dyDescent="0.25">
+    <row r="523" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A523" s="5">
         <v>173</v>
       </c>
@@ -37968,7 +38170,7 @@
       </c>
       <c r="R783" s="8"/>
     </row>
-    <row r="784" spans="1:18" ht="39" x14ac:dyDescent="0.25">
+    <row r="784" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A784" s="5">
         <v>174</v>
       </c>
@@ -51404,7 +51606,7 @@
       </c>
       <c r="R1118" s="8"/>
     </row>
-    <row r="1119" spans="1:18" ht="39" x14ac:dyDescent="0.25">
+    <row r="1119" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1119" s="10">
         <v>244</v>
       </c>
@@ -57064,7 +57266,7 @@
       <c r="Q1263" s="8"/>
       <c r="R1263" s="8"/>
     </row>
-    <row r="1264" spans="1:18" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1264" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1264" s="10">
         <v>322</v>
       </c>
@@ -60275,7 +60477,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF9BE15D-6351-44F9-8E43-517339B371DC}">
   <dimension ref="A1:R124"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:R124"/>
     </sheetView>
   </sheetViews>
@@ -64860,11 +65062,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9585C0FF-65C5-4BD8-9936-5C9A63F7E604}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:CN41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AU1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BP31" sqref="BP31"/>
+    <sheetView topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G22" sqref="D2:G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64949,108 +65152,108 @@
     <row r="1" spans="1:92" x14ac:dyDescent="0.25">
       <c r="B1" s="71"/>
       <c r="M1" s="71"/>
-      <c r="S1" s="76">
+      <c r="S1" s="89">
         <v>45536</v>
       </c>
-      <c r="T1" s="77"/>
-      <c r="U1" s="77"/>
-      <c r="V1" s="77"/>
-      <c r="W1" s="76">
+      <c r="T1" s="90"/>
+      <c r="U1" s="90"/>
+      <c r="V1" s="90"/>
+      <c r="W1" s="89">
         <v>45566</v>
       </c>
-      <c r="X1" s="76"/>
-      <c r="Y1" s="76"/>
-      <c r="Z1" s="76"/>
-      <c r="AA1" s="76"/>
-      <c r="AB1" s="73">
+      <c r="X1" s="89"/>
+      <c r="Y1" s="89"/>
+      <c r="Z1" s="89"/>
+      <c r="AA1" s="89"/>
+      <c r="AB1" s="86">
         <v>45597</v>
       </c>
-      <c r="AC1" s="74"/>
-      <c r="AD1" s="74"/>
-      <c r="AE1" s="75"/>
-      <c r="AF1" s="73">
+      <c r="AC1" s="87"/>
+      <c r="AD1" s="87"/>
+      <c r="AE1" s="88"/>
+      <c r="AF1" s="86">
         <v>45627</v>
       </c>
-      <c r="AG1" s="74"/>
-      <c r="AH1" s="74"/>
-      <c r="AI1" s="75"/>
-      <c r="AJ1" s="73">
+      <c r="AG1" s="87"/>
+      <c r="AH1" s="87"/>
+      <c r="AI1" s="88"/>
+      <c r="AJ1" s="86">
         <v>45658</v>
       </c>
-      <c r="AK1" s="74"/>
-      <c r="AL1" s="74"/>
-      <c r="AM1" s="74"/>
-      <c r="AN1" s="75"/>
-      <c r="AO1" s="73">
+      <c r="AK1" s="87"/>
+      <c r="AL1" s="87"/>
+      <c r="AM1" s="87"/>
+      <c r="AN1" s="88"/>
+      <c r="AO1" s="86">
         <v>45689</v>
       </c>
-      <c r="AP1" s="74"/>
-      <c r="AQ1" s="74"/>
-      <c r="AR1" s="75"/>
-      <c r="AS1" s="73">
+      <c r="AP1" s="87"/>
+      <c r="AQ1" s="87"/>
+      <c r="AR1" s="88"/>
+      <c r="AS1" s="86">
         <v>45717</v>
       </c>
-      <c r="AT1" s="74"/>
-      <c r="AU1" s="74"/>
-      <c r="AV1" s="75"/>
-      <c r="AW1" s="73">
+      <c r="AT1" s="87"/>
+      <c r="AU1" s="87"/>
+      <c r="AV1" s="88"/>
+      <c r="AW1" s="86">
         <v>45748</v>
       </c>
-      <c r="AX1" s="74"/>
-      <c r="AY1" s="74"/>
-      <c r="AZ1" s="75"/>
-      <c r="BA1" s="73">
+      <c r="AX1" s="87"/>
+      <c r="AY1" s="87"/>
+      <c r="AZ1" s="88"/>
+      <c r="BA1" s="86">
         <v>45778</v>
       </c>
-      <c r="BB1" s="74"/>
-      <c r="BC1" s="74"/>
-      <c r="BD1" s="74"/>
-      <c r="BE1" s="75"/>
-      <c r="BF1" s="73">
+      <c r="BB1" s="87"/>
+      <c r="BC1" s="87"/>
+      <c r="BD1" s="87"/>
+      <c r="BE1" s="88"/>
+      <c r="BF1" s="86">
         <v>45809</v>
       </c>
-      <c r="BG1" s="74"/>
-      <c r="BH1" s="74"/>
-      <c r="BI1" s="74"/>
-      <c r="BJ1" s="73">
+      <c r="BG1" s="87"/>
+      <c r="BH1" s="87"/>
+      <c r="BI1" s="87"/>
+      <c r="BJ1" s="86">
         <v>45839</v>
       </c>
-      <c r="BK1" s="74"/>
-      <c r="BL1" s="74"/>
-      <c r="BM1" s="74"/>
-      <c r="BN1" s="75"/>
-      <c r="BO1" s="73">
+      <c r="BK1" s="87"/>
+      <c r="BL1" s="87"/>
+      <c r="BM1" s="87"/>
+      <c r="BN1" s="88"/>
+      <c r="BO1" s="86">
         <v>45870</v>
       </c>
-      <c r="BP1" s="74"/>
-      <c r="BQ1" s="74"/>
-      <c r="BR1" s="74"/>
-      <c r="BS1" s="73">
+      <c r="BP1" s="87"/>
+      <c r="BQ1" s="87"/>
+      <c r="BR1" s="87"/>
+      <c r="BS1" s="86">
         <v>45901</v>
       </c>
-      <c r="BT1" s="74"/>
-      <c r="BU1" s="74"/>
-      <c r="BV1" s="74"/>
-      <c r="BW1" s="73">
+      <c r="BT1" s="87"/>
+      <c r="BU1" s="87"/>
+      <c r="BV1" s="87"/>
+      <c r="BW1" s="86">
         <v>45931</v>
       </c>
-      <c r="BX1" s="74"/>
-      <c r="BY1" s="74"/>
-      <c r="BZ1" s="74"/>
-      <c r="CB1" s="73">
+      <c r="BX1" s="87"/>
+      <c r="BY1" s="87"/>
+      <c r="BZ1" s="87"/>
+      <c r="CB1" s="86">
         <v>45962</v>
       </c>
-      <c r="CC1" s="74"/>
-      <c r="CD1" s="74"/>
-      <c r="CE1" s="74"/>
-      <c r="CF1" s="72" t="s">
+      <c r="CC1" s="87"/>
+      <c r="CD1" s="87"/>
+      <c r="CE1" s="87"/>
+      <c r="CF1" s="85" t="s">
         <v>1853</v>
       </c>
-      <c r="CG1" s="72"/>
-      <c r="CK1" s="72" t="s">
+      <c r="CG1" s="85"/>
+      <c r="CK1" s="85" t="s">
         <v>1891</v>
       </c>
-      <c r="CL1" s="72"/>
+      <c r="CL1" s="85"/>
     </row>
     <row r="2" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
@@ -66220,7 +66423,7 @@
       <c r="CM9" s="12"/>
       <c r="CN9" s="12"/>
     </row>
-    <row r="10" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:92" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>1776</v>
       </c>
@@ -66342,7 +66545,7 @@
       <c r="CM10" s="12"/>
       <c r="CN10" s="12"/>
     </row>
-    <row r="11" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:92" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>1777</v>
       </c>
@@ -66356,7 +66559,7 @@
       <c r="E11" s="15" t="s">
         <v>1760</v>
       </c>
-      <c r="F11" s="86" t="s">
+      <c r="F11" s="79" t="s">
         <v>1761</v>
       </c>
       <c r="G11" s="12" t="s">
@@ -66583,7 +66786,7 @@
       <c r="CM12" s="12"/>
       <c r="CN12" s="12"/>
     </row>
-    <row r="13" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:92" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="15" t="s">
         <v>1881</v>
@@ -66620,82 +66823,82 @@
       <c r="R13" s="56">
         <v>45615</v>
       </c>
-      <c r="S13" s="80"/>
-      <c r="T13" s="78"/>
-      <c r="U13" s="78"/>
-      <c r="V13" s="78"/>
-      <c r="W13" s="93"/>
-      <c r="X13" s="78"/>
-      <c r="Y13" s="78"/>
-      <c r="Z13" s="78"/>
-      <c r="AA13" s="78"/>
-      <c r="AB13" s="78"/>
-      <c r="AC13" s="78"/>
-      <c r="AD13" s="78"/>
-      <c r="AE13" s="78"/>
-      <c r="AF13" s="78"/>
-      <c r="AG13" s="78"/>
-      <c r="AH13" s="78"/>
-      <c r="AI13" s="78"/>
-      <c r="AJ13" s="78"/>
-      <c r="AK13" s="78"/>
-      <c r="AL13" s="78"/>
-      <c r="AM13" s="78"/>
-      <c r="AN13" s="78"/>
-      <c r="AO13" s="78"/>
-      <c r="AP13" s="78"/>
-      <c r="AQ13" s="78"/>
-      <c r="AR13" s="78"/>
-      <c r="AS13" s="78"/>
-      <c r="AT13" s="78"/>
-      <c r="AU13" s="78"/>
-      <c r="AV13" s="78"/>
-      <c r="AW13" s="78"/>
-      <c r="AX13" s="78"/>
-      <c r="AY13" s="78"/>
-      <c r="AZ13" s="78"/>
-      <c r="BA13" s="78"/>
-      <c r="BB13" s="78"/>
-      <c r="BC13" s="78"/>
-      <c r="BD13" s="78"/>
-      <c r="BE13" s="78"/>
-      <c r="BF13" s="78"/>
-      <c r="BG13" s="78"/>
-      <c r="BH13" s="78"/>
-      <c r="BI13" s="78"/>
-      <c r="BJ13" s="78"/>
-      <c r="BK13" s="78"/>
-      <c r="BL13" s="78"/>
-      <c r="BM13" s="78"/>
-      <c r="BN13" s="78"/>
-      <c r="BO13" s="78"/>
-      <c r="BP13" s="78"/>
-      <c r="BQ13" s="78"/>
-      <c r="BR13" s="78"/>
-      <c r="BS13" s="78"/>
-      <c r="BT13" s="78"/>
-      <c r="BU13" s="78"/>
-      <c r="BV13" s="78"/>
-      <c r="BW13" s="78"/>
-      <c r="BX13" s="78"/>
-      <c r="BY13" s="78"/>
-      <c r="BZ13" s="78"/>
-      <c r="CA13" s="78"/>
-      <c r="CB13" s="78"/>
-      <c r="CC13" s="78"/>
-      <c r="CD13" s="78"/>
-      <c r="CE13" s="78"/>
-      <c r="CF13" s="78"/>
-      <c r="CG13" s="78"/>
-      <c r="CH13" s="78"/>
-      <c r="CI13" s="78"/>
-      <c r="CJ13" s="78"/>
-      <c r="CK13" s="78"/>
-      <c r="CL13" s="78"/>
-      <c r="CM13" s="78"/>
-      <c r="CN13" s="78"/>
-    </row>
-    <row r="14" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="S13" s="74"/>
+      <c r="T13" s="72"/>
+      <c r="U13" s="72"/>
+      <c r="V13" s="72"/>
+      <c r="W13" s="84"/>
+      <c r="X13" s="72"/>
+      <c r="Y13" s="72"/>
+      <c r="Z13" s="72"/>
+      <c r="AA13" s="72"/>
+      <c r="AB13" s="72"/>
+      <c r="AC13" s="72"/>
+      <c r="AD13" s="72"/>
+      <c r="AE13" s="72"/>
+      <c r="AF13" s="72"/>
+      <c r="AG13" s="72"/>
+      <c r="AH13" s="72"/>
+      <c r="AI13" s="72"/>
+      <c r="AJ13" s="72"/>
+      <c r="AK13" s="72"/>
+      <c r="AL13" s="72"/>
+      <c r="AM13" s="72"/>
+      <c r="AN13" s="72"/>
+      <c r="AO13" s="72"/>
+      <c r="AP13" s="72"/>
+      <c r="AQ13" s="72"/>
+      <c r="AR13" s="72"/>
+      <c r="AS13" s="72"/>
+      <c r="AT13" s="72"/>
+      <c r="AU13" s="72"/>
+      <c r="AV13" s="72"/>
+      <c r="AW13" s="72"/>
+      <c r="AX13" s="72"/>
+      <c r="AY13" s="72"/>
+      <c r="AZ13" s="72"/>
+      <c r="BA13" s="72"/>
+      <c r="BB13" s="72"/>
+      <c r="BC13" s="72"/>
+      <c r="BD13" s="72"/>
+      <c r="BE13" s="72"/>
+      <c r="BF13" s="72"/>
+      <c r="BG13" s="72"/>
+      <c r="BH13" s="72"/>
+      <c r="BI13" s="72"/>
+      <c r="BJ13" s="72"/>
+      <c r="BK13" s="72"/>
+      <c r="BL13" s="72"/>
+      <c r="BM13" s="72"/>
+      <c r="BN13" s="72"/>
+      <c r="BO13" s="72"/>
+      <c r="BP13" s="72"/>
+      <c r="BQ13" s="72"/>
+      <c r="BR13" s="72"/>
+      <c r="BS13" s="72"/>
+      <c r="BT13" s="72"/>
+      <c r="BU13" s="72"/>
+      <c r="BV13" s="72"/>
+      <c r="BW13" s="72"/>
+      <c r="BX13" s="72"/>
+      <c r="BY13" s="72"/>
+      <c r="BZ13" s="72"/>
+      <c r="CA13" s="72"/>
+      <c r="CB13" s="72"/>
+      <c r="CC13" s="72"/>
+      <c r="CD13" s="72"/>
+      <c r="CE13" s="72"/>
+      <c r="CF13" s="72"/>
+      <c r="CG13" s="72"/>
+      <c r="CH13" s="72"/>
+      <c r="CI13" s="72"/>
+      <c r="CJ13" s="72"/>
+      <c r="CK13" s="72"/>
+      <c r="CL13" s="72"/>
+      <c r="CM13" s="72"/>
+      <c r="CN13" s="72"/>
+    </row>
+    <row r="14" spans="1:92" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>1776</v>
       </c>
@@ -66817,7 +67020,7 @@
       <c r="CM14" s="12"/>
       <c r="CN14" s="12"/>
     </row>
-    <row r="15" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:92" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>1776</v>
       </c>
@@ -66932,14 +67135,12 @@
       <c r="CF15" s="12"/>
       <c r="CG15" s="12"/>
       <c r="CH15" s="12"/>
-      <c r="CI15" s="89"/>
       <c r="CJ15" s="12"/>
       <c r="CK15" s="12"/>
       <c r="CL15" s="12"/>
       <c r="CM15" s="12"/>
-      <c r="CN15" s="89"/>
-    </row>
-    <row r="16" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:92" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>1777</v>
       </c>
@@ -67059,7 +67260,7 @@
       <c r="CM16" s="12"/>
       <c r="CN16" s="12"/>
     </row>
-    <row r="17" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:92" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>1777</v>
       </c>
@@ -67179,7 +67380,7 @@
       <c r="CM17" s="12"/>
       <c r="CN17" s="12"/>
     </row>
-    <row r="18" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:92" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>1777</v>
       </c>
@@ -67694,7 +67895,7 @@
         <v>1863</v>
       </c>
       <c r="P22" s="12" t="s">
-        <v>1858</v>
+        <v>1864</v>
       </c>
       <c r="Q22" s="50">
         <v>45590</v>
@@ -67713,7 +67914,6 @@
       <c r="AA22" s="12"/>
       <c r="AB22" s="12"/>
       <c r="AC22" s="12"/>
-      <c r="AD22" s="89"/>
       <c r="AE22" s="12"/>
       <c r="AF22" s="12"/>
       <c r="AG22" s="12"/>
@@ -67777,7 +67977,7 @@
       <c r="CM22" s="12"/>
       <c r="CN22" s="12"/>
     </row>
-    <row r="23" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:92" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>1776</v>
       </c>
@@ -67896,7 +68096,7 @@
       <c r="CM23" s="12"/>
       <c r="CN23" s="12"/>
     </row>
-    <row r="24" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:92" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>1777</v>
       </c>
@@ -68014,7 +68214,7 @@
       <c r="CM24" s="12"/>
       <c r="CN24" s="12"/>
     </row>
-    <row r="25" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:92" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>1776</v>
       </c>
@@ -68133,7 +68333,7 @@
       <c r="CM25" s="12"/>
       <c r="CN25" s="12"/>
     </row>
-    <row r="26" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:92" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>1777</v>
       </c>
@@ -68214,12 +68414,6 @@
       <c r="AZ26" s="12"/>
       <c r="BA26" s="12"/>
       <c r="BB26" s="12"/>
-      <c r="BC26" s="89"/>
-      <c r="BD26" s="89"/>
-      <c r="BE26" s="89"/>
-      <c r="BF26" s="89"/>
-      <c r="BG26" s="89"/>
-      <c r="BH26" s="89"/>
       <c r="BI26" s="12"/>
       <c r="BJ26" s="12"/>
       <c r="BK26" s="12"/>
@@ -68253,7 +68447,7 @@
       <c r="CM26" s="12"/>
       <c r="CN26" s="12"/>
     </row>
-    <row r="27" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:92" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14" t="s">
         <v>1776</v>
       </c>
@@ -68321,7 +68515,6 @@
       <c r="AM27" s="12"/>
       <c r="AN27" s="12"/>
       <c r="AO27" s="12"/>
-      <c r="AP27" s="89"/>
       <c r="AQ27" s="12"/>
       <c r="AR27" s="12"/>
       <c r="AS27" s="12"/>
@@ -68331,7 +68524,6 @@
       <c r="AW27" s="12"/>
       <c r="AX27" s="12"/>
       <c r="AY27" s="12"/>
-      <c r="AZ27" s="89"/>
       <c r="BA27" s="12"/>
       <c r="BB27" s="12"/>
       <c r="BC27" s="12"/>
@@ -68340,16 +68532,12 @@
       <c r="BF27" s="12"/>
       <c r="BG27" s="12"/>
       <c r="BH27" s="12"/>
-      <c r="BI27" s="89"/>
-      <c r="BJ27" s="89"/>
-      <c r="BK27" s="89"/>
       <c r="BL27" s="12"/>
       <c r="BM27" s="12"/>
       <c r="BN27" s="12"/>
       <c r="BO27" s="12"/>
       <c r="BP27" s="12"/>
       <c r="BQ27" s="12"/>
-      <c r="BR27" s="89"/>
       <c r="BS27" s="12"/>
       <c r="BT27" s="12"/>
       <c r="BU27" s="12"/>
@@ -68373,7 +68561,7 @@
       <c r="CM27" s="12"/>
       <c r="CN27" s="12"/>
     </row>
-    <row r="28" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:92" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>1777</v>
       </c>
@@ -68468,7 +68656,6 @@
       <c r="BN28" s="12"/>
       <c r="BO28" s="12"/>
       <c r="BP28" s="12"/>
-      <c r="BQ28" s="89"/>
       <c r="BR28" s="12"/>
       <c r="BS28" s="12"/>
       <c r="BT28" s="12"/>
@@ -68493,7 +68680,7 @@
       <c r="CM28" s="12"/>
       <c r="CN28" s="12"/>
     </row>
-    <row r="29" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:92" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>1777</v>
       </c>
@@ -68612,7 +68799,7 @@
       <c r="CM29" s="12"/>
       <c r="CN29" s="12"/>
     </row>
-    <row r="30" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:92" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
         <v>1777</v>
       </c>
@@ -68666,9 +68853,9 @@
       <c r="AA30" s="12"/>
       <c r="AB30" s="12"/>
       <c r="AC30" s="12"/>
-      <c r="AD30" s="78"/>
-      <c r="AE30" s="78"/>
-      <c r="AF30" s="78"/>
+      <c r="AD30" s="72"/>
+      <c r="AE30" s="72"/>
+      <c r="AF30" s="72"/>
       <c r="AG30" s="12"/>
       <c r="AH30" s="12"/>
       <c r="AI30" s="12"/>
@@ -68712,8 +68899,6 @@
       <c r="BU30" s="12"/>
       <c r="BV30" s="12"/>
       <c r="BW30" s="12"/>
-      <c r="BX30" s="89"/>
-      <c r="BY30" s="89"/>
       <c r="BZ30" s="12"/>
       <c r="CA30" s="12"/>
       <c r="CB30" s="12"/>
@@ -68730,7 +68915,7 @@
       <c r="CM30" s="12"/>
       <c r="CN30" s="12"/>
     </row>
-    <row r="31" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:92" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>1777</v>
       </c>
@@ -68827,10 +69012,6 @@
       <c r="BT31" s="12"/>
       <c r="BU31" s="12"/>
       <c r="BV31" s="12"/>
-      <c r="BW31" s="89"/>
-      <c r="BX31" s="89"/>
-      <c r="BY31" s="89"/>
-      <c r="BZ31" s="89"/>
       <c r="CA31" s="12"/>
       <c r="CB31" s="12"/>
       <c r="CC31" s="12"/>
@@ -68846,7 +69027,7 @@
       <c r="CM31" s="12"/>
       <c r="CN31" s="12"/>
     </row>
-    <row r="32" spans="1:92" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:92" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
         <v>1777</v>
       </c>
@@ -68959,10 +69140,9 @@
       <c r="CJ32" s="12"/>
       <c r="CK32" s="12"/>
       <c r="CL32" s="12"/>
-      <c r="CM32" s="89"/>
       <c r="CN32" s="12"/>
     </row>
-    <row r="33" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:92" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>1776</v>
       </c>
@@ -69068,7 +69248,7 @@
       <c r="CM33" s="12"/>
       <c r="CN33" s="12"/>
     </row>
-    <row r="34" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:92" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
         <v>1776</v>
       </c>
@@ -69174,7 +69354,7 @@
       <c r="CM34" s="12"/>
       <c r="CN34" s="12"/>
     </row>
-    <row r="35" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:92" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>1776</v>
       </c>
@@ -69280,37 +69460,37 @@
       <c r="CM35" s="12"/>
       <c r="CN35" s="12"/>
     </row>
-    <row r="36" spans="1:92" x14ac:dyDescent="0.25">
-      <c r="A36" s="81" t="s">
+    <row r="36" spans="1:92" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="75" t="s">
         <v>1776</v>
       </c>
       <c r="B36" s="60" t="s">
         <v>1872</v>
       </c>
       <c r="C36" s="60"/>
-      <c r="D36" s="81" t="s">
+      <c r="D36" s="75" t="s">
         <v>1876</v>
       </c>
-      <c r="E36" s="81" t="s">
+      <c r="E36" s="75" t="s">
         <v>1837</v>
       </c>
-      <c r="F36" s="81"/>
-      <c r="G36" s="81" t="s">
+      <c r="F36" s="75"/>
+      <c r="G36" s="75" t="s">
         <v>31</v>
       </c>
-      <c r="H36" s="81" t="s">
+      <c r="H36" s="75" t="s">
         <v>1075</v>
       </c>
-      <c r="I36" s="79"/>
-      <c r="J36" s="79"/>
-      <c r="K36" s="79"/>
-      <c r="L36" s="90"/>
-      <c r="M36" s="79"/>
-      <c r="N36" s="79"/>
-      <c r="O36" s="79"/>
-      <c r="P36" s="79"/>
-      <c r="Q36" s="91"/>
-      <c r="R36" s="91"/>
+      <c r="I36" s="73"/>
+      <c r="J36" s="73"/>
+      <c r="K36" s="73"/>
+      <c r="L36" s="81"/>
+      <c r="M36" s="73"/>
+      <c r="N36" s="73"/>
+      <c r="O36" s="73"/>
+      <c r="P36" s="73"/>
+      <c r="Q36" s="82"/>
+      <c r="R36" s="82"/>
       <c r="S36" s="53"/>
       <c r="T36" s="12"/>
       <c r="U36" s="12"/>
@@ -69386,7 +69566,7 @@
       <c r="CM36" s="12"/>
       <c r="CN36" s="12"/>
     </row>
-    <row r="37" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:92" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
         <v>1776</v>
       </c>
@@ -69411,12 +69591,9 @@
       <c r="J37" s="12"/>
       <c r="K37" s="12"/>
       <c r="L37" s="54"/>
-      <c r="M37" s="89"/>
       <c r="N37" s="12"/>
       <c r="O37" s="12"/>
       <c r="P37" s="12"/>
-      <c r="Q37" s="89"/>
-      <c r="R37" s="89"/>
       <c r="S37" s="53"/>
       <c r="T37" s="12"/>
       <c r="U37" s="12"/>
@@ -69492,117 +69669,117 @@
       <c r="CM37" s="12"/>
       <c r="CN37" s="12"/>
     </row>
-    <row r="38" spans="1:92" s="61" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="82" t="s">
+    <row r="38" spans="1:92" s="61" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="76" t="s">
         <v>1777</v>
       </c>
-      <c r="B38" s="83" t="s">
+      <c r="B38" s="69" t="s">
         <v>1889</v>
       </c>
-      <c r="C38" s="83" t="s">
+      <c r="C38" s="69" t="s">
         <v>1890</v>
       </c>
-      <c r="D38" s="84" t="s">
+      <c r="D38" s="77" t="s">
         <v>1879</v>
       </c>
-      <c r="E38" s="85" t="s">
+      <c r="E38" s="78" t="s">
         <v>1878</v>
       </c>
-      <c r="F38" s="87"/>
+      <c r="F38" s="80"/>
       <c r="G38" s="59" t="s">
         <v>176</v>
       </c>
-      <c r="H38" s="88" t="s">
+      <c r="H38" s="6" t="s">
         <v>1880</v>
       </c>
-      <c r="I38" s="89">
+      <c r="I38">
         <v>23</v>
       </c>
-      <c r="J38" s="89"/>
-      <c r="K38" s="89"/>
-      <c r="L38" s="89"/>
-      <c r="M38" s="89"/>
-      <c r="N38" s="89"/>
-      <c r="O38" s="89"/>
-      <c r="P38" s="89"/>
-      <c r="Q38" s="89"/>
-      <c r="R38" s="89"/>
-      <c r="S38" s="92"/>
-      <c r="T38" s="92"/>
-      <c r="U38" s="92"/>
-      <c r="V38" s="92"/>
-      <c r="W38" s="92"/>
-      <c r="X38" s="92"/>
-      <c r="Y38" s="92"/>
-      <c r="Z38" s="92"/>
-      <c r="AA38" s="92"/>
-      <c r="AB38" s="92"/>
-      <c r="AC38" s="92"/>
-      <c r="AD38" s="92"/>
-      <c r="AE38" s="92"/>
-      <c r="AF38" s="92"/>
-      <c r="AG38" s="92"/>
-      <c r="AH38" s="92"/>
-      <c r="AI38" s="92"/>
-      <c r="AJ38" s="92"/>
-      <c r="AK38" s="92"/>
-      <c r="AL38" s="92"/>
-      <c r="AM38" s="92"/>
-      <c r="AN38" s="92"/>
-      <c r="AO38" s="92"/>
-      <c r="AP38" s="92"/>
-      <c r="AQ38" s="92"/>
-      <c r="AR38" s="92"/>
-      <c r="AS38" s="92"/>
-      <c r="AT38" s="92"/>
-      <c r="AU38" s="92"/>
-      <c r="AV38" s="92"/>
-      <c r="AW38" s="92"/>
-      <c r="AX38" s="92"/>
-      <c r="AY38" s="92"/>
-      <c r="AZ38" s="92"/>
-      <c r="BA38" s="92"/>
-      <c r="BB38" s="92"/>
-      <c r="BC38" s="92"/>
-      <c r="BD38" s="92"/>
-      <c r="BE38" s="92"/>
-      <c r="BF38" s="92"/>
-      <c r="BG38" s="92"/>
-      <c r="BH38" s="92"/>
-      <c r="BI38" s="92"/>
-      <c r="BJ38" s="92"/>
-      <c r="BK38" s="92"/>
-      <c r="BL38" s="92"/>
-      <c r="BM38" s="92"/>
-      <c r="BN38" s="92"/>
-      <c r="BO38" s="92"/>
-      <c r="BP38" s="92"/>
-      <c r="BQ38" s="92"/>
-      <c r="BR38" s="89"/>
-      <c r="BS38" s="89"/>
-      <c r="BT38" s="89"/>
-      <c r="BU38" s="89"/>
-      <c r="BV38" s="89"/>
-      <c r="BW38" s="89"/>
-      <c r="BX38" s="89"/>
-      <c r="BY38" s="89"/>
-      <c r="BZ38" s="89"/>
-      <c r="CA38" s="89"/>
-      <c r="CB38" s="89"/>
-      <c r="CC38" s="89"/>
-      <c r="CD38" s="89"/>
-      <c r="CE38" s="89"/>
-      <c r="CF38" s="89"/>
-      <c r="CG38" s="89"/>
-      <c r="CH38" s="89"/>
-      <c r="CI38" s="89"/>
-      <c r="CJ38" s="89"/>
-      <c r="CK38" s="89"/>
-      <c r="CL38" s="89"/>
-      <c r="CM38" s="89"/>
-      <c r="CN38" s="89"/>
-    </row>
-    <row r="39" spans="1:92" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J38"/>
+      <c r="K38"/>
+      <c r="L38"/>
+      <c r="M38"/>
+      <c r="N38"/>
+      <c r="O38"/>
+      <c r="P38"/>
+      <c r="Q38"/>
+      <c r="R38"/>
+      <c r="S38" s="83"/>
+      <c r="T38" s="83"/>
+      <c r="U38" s="83"/>
+      <c r="V38" s="83"/>
+      <c r="W38" s="83"/>
+      <c r="X38" s="83"/>
+      <c r="Y38" s="83"/>
+      <c r="Z38" s="83"/>
+      <c r="AA38" s="83"/>
+      <c r="AB38" s="83"/>
+      <c r="AC38" s="83"/>
+      <c r="AD38" s="83"/>
+      <c r="AE38" s="83"/>
+      <c r="AF38" s="83"/>
+      <c r="AG38" s="83"/>
+      <c r="AH38" s="83"/>
+      <c r="AI38" s="83"/>
+      <c r="AJ38" s="83"/>
+      <c r="AK38" s="83"/>
+      <c r="AL38" s="83"/>
+      <c r="AM38" s="83"/>
+      <c r="AN38" s="83"/>
+      <c r="AO38" s="83"/>
+      <c r="AP38" s="83"/>
+      <c r="AQ38" s="83"/>
+      <c r="AR38" s="83"/>
+      <c r="AS38" s="83"/>
+      <c r="AT38" s="83"/>
+      <c r="AU38" s="83"/>
+      <c r="AV38" s="83"/>
+      <c r="AW38" s="83"/>
+      <c r="AX38" s="83"/>
+      <c r="AY38" s="83"/>
+      <c r="AZ38" s="83"/>
+      <c r="BA38" s="83"/>
+      <c r="BB38" s="83"/>
+      <c r="BC38" s="83"/>
+      <c r="BD38" s="83"/>
+      <c r="BE38" s="83"/>
+      <c r="BF38" s="83"/>
+      <c r="BG38" s="83"/>
+      <c r="BH38" s="83"/>
+      <c r="BI38" s="83"/>
+      <c r="BJ38" s="83"/>
+      <c r="BK38" s="83"/>
+      <c r="BL38" s="83"/>
+      <c r="BM38" s="83"/>
+      <c r="BN38" s="83"/>
+      <c r="BO38" s="83"/>
+      <c r="BP38" s="83"/>
+      <c r="BQ38" s="83"/>
+      <c r="BR38"/>
+      <c r="BS38"/>
+      <c r="BT38"/>
+      <c r="BU38"/>
+      <c r="BV38"/>
+      <c r="BW38"/>
+      <c r="BX38"/>
+      <c r="BY38"/>
+      <c r="BZ38"/>
+      <c r="CA38"/>
+      <c r="CB38"/>
+      <c r="CC38"/>
+      <c r="CD38"/>
+      <c r="CE38"/>
+      <c r="CF38"/>
+      <c r="CG38"/>
+      <c r="CH38"/>
+      <c r="CI38"/>
+      <c r="CJ38"/>
+      <c r="CK38"/>
+      <c r="CL38"/>
+      <c r="CM38"/>
+      <c r="CN38"/>
+    </row>
+    <row r="39" spans="1:92" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="68"/>
       <c r="B39" s="64" t="s">
         <v>1889</v>
@@ -69623,56 +69800,56 @@
       <c r="P39" s="64"/>
       <c r="Q39" s="64"/>
       <c r="R39" s="64"/>
-      <c r="S39" s="79"/>
-      <c r="T39" s="79"/>
-      <c r="U39" s="79"/>
-      <c r="V39" s="79"/>
-      <c r="W39" s="79"/>
-      <c r="X39" s="79"/>
-      <c r="Y39" s="79"/>
-      <c r="Z39" s="79"/>
-      <c r="AA39" s="79"/>
-      <c r="AB39" s="79"/>
-      <c r="AC39" s="79"/>
-      <c r="AD39" s="79"/>
-      <c r="AE39" s="79"/>
-      <c r="AF39" s="79"/>
-      <c r="AG39" s="79"/>
-      <c r="AH39" s="79"/>
-      <c r="AI39" s="79"/>
-      <c r="AJ39" s="79"/>
-      <c r="AK39" s="79"/>
-      <c r="AL39" s="79"/>
-      <c r="AM39" s="79"/>
-      <c r="AN39" s="79"/>
-      <c r="AO39" s="79"/>
-      <c r="AP39" s="79"/>
-      <c r="AQ39" s="79"/>
-      <c r="AR39" s="79"/>
-      <c r="AS39" s="79"/>
-      <c r="AT39" s="79"/>
-      <c r="AU39" s="79"/>
-      <c r="AV39" s="79"/>
-      <c r="AW39" s="79"/>
-      <c r="AX39" s="79"/>
-      <c r="AY39" s="79"/>
-      <c r="AZ39" s="79"/>
-      <c r="BA39" s="79"/>
-      <c r="BB39" s="79"/>
-      <c r="BC39" s="79"/>
-      <c r="BD39" s="79"/>
-      <c r="BE39" s="79"/>
-      <c r="BF39" s="79"/>
-      <c r="BG39" s="79"/>
-      <c r="BH39" s="79"/>
-      <c r="BI39" s="79"/>
-      <c r="BJ39" s="79"/>
-      <c r="BK39" s="79"/>
-      <c r="BL39" s="79"/>
-      <c r="BM39" s="79"/>
-      <c r="BN39" s="79"/>
-      <c r="BO39" s="79"/>
-      <c r="BP39" s="79"/>
+      <c r="S39" s="73"/>
+      <c r="T39" s="73"/>
+      <c r="U39" s="73"/>
+      <c r="V39" s="73"/>
+      <c r="W39" s="73"/>
+      <c r="X39" s="73"/>
+      <c r="Y39" s="73"/>
+      <c r="Z39" s="73"/>
+      <c r="AA39" s="73"/>
+      <c r="AB39" s="73"/>
+      <c r="AC39" s="73"/>
+      <c r="AD39" s="73"/>
+      <c r="AE39" s="73"/>
+      <c r="AF39" s="73"/>
+      <c r="AG39" s="73"/>
+      <c r="AH39" s="73"/>
+      <c r="AI39" s="73"/>
+      <c r="AJ39" s="73"/>
+      <c r="AK39" s="73"/>
+      <c r="AL39" s="73"/>
+      <c r="AM39" s="73"/>
+      <c r="AN39" s="73"/>
+      <c r="AO39" s="73"/>
+      <c r="AP39" s="73"/>
+      <c r="AQ39" s="73"/>
+      <c r="AR39" s="73"/>
+      <c r="AS39" s="73"/>
+      <c r="AT39" s="73"/>
+      <c r="AU39" s="73"/>
+      <c r="AV39" s="73"/>
+      <c r="AW39" s="73"/>
+      <c r="AX39" s="73"/>
+      <c r="AY39" s="73"/>
+      <c r="AZ39" s="73"/>
+      <c r="BA39" s="73"/>
+      <c r="BB39" s="73"/>
+      <c r="BC39" s="73"/>
+      <c r="BD39" s="73"/>
+      <c r="BE39" s="73"/>
+      <c r="BF39" s="73"/>
+      <c r="BG39" s="73"/>
+      <c r="BH39" s="73"/>
+      <c r="BI39" s="73"/>
+      <c r="BJ39" s="73"/>
+      <c r="BK39" s="73"/>
+      <c r="BL39" s="73"/>
+      <c r="BM39" s="73"/>
+      <c r="BN39" s="73"/>
+      <c r="BO39" s="73"/>
+      <c r="BP39" s="73"/>
       <c r="BQ39" s="61"/>
       <c r="BR39" s="61"/>
       <c r="BS39" s="61"/>
@@ -69795,22 +69972,27 @@
     </row>
   </sheetData>
   <autoFilter ref="A2:CN39" xr:uid="{9585C0FF-65C5-4BD8-9936-5C9A63F7E604}">
+    <filterColumn colId="15">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:CN39">
       <sortCondition ref="B2:B39"/>
     </sortState>
   </autoFilter>
   <mergeCells count="17">
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="W1:AA1"/>
+    <mergeCell ref="AB1:AE1"/>
+    <mergeCell ref="AF1:AI1"/>
+    <mergeCell ref="AJ1:AN1"/>
     <mergeCell ref="CK1:CL1"/>
     <mergeCell ref="AO1:AR1"/>
     <mergeCell ref="AS1:AV1"/>
     <mergeCell ref="AW1:AZ1"/>
     <mergeCell ref="BA1:BE1"/>
     <mergeCell ref="BF1:BI1"/>
-    <mergeCell ref="S1:V1"/>
-    <mergeCell ref="W1:AA1"/>
-    <mergeCell ref="AB1:AE1"/>
-    <mergeCell ref="AF1:AI1"/>
-    <mergeCell ref="AJ1:AN1"/>
     <mergeCell ref="CF1:CG1"/>
     <mergeCell ref="BJ1:BN1"/>
     <mergeCell ref="BO1:BR1"/>
@@ -69820,4 +70002,247 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A37070B-603E-4598-8F3E-8F89C39581A8}">
+  <dimension ref="B1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B1" s="13" t="s">
+        <v>1737</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>1781</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="12" t="s">
+        <v>1772</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="12" t="s">
+        <v>1586</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="s">
+        <v>1747</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="12" t="s">
+        <v>1749</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="12" t="s">
+        <v>1770</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="12" t="s">
+        <v>1751</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="12" t="s">
+        <v>1748</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="12" t="s">
+        <v>1877</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>1877</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="12" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="12" t="s">
+        <v>1745</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>777</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4466A9F8-7313-47F5-A50A-ED409D20B744}">
+  <dimension ref="B1:E11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="91" t="s">
+        <v>1893</v>
+      </c>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="92" t="s">
+        <v>1894</v>
+      </c>
+      <c r="C3" s="93" t="s">
+        <v>1895</v>
+      </c>
+      <c r="D3" s="94" t="s">
+        <v>1896</v>
+      </c>
+      <c r="E3" s="94" t="s">
+        <v>1897</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="95" t="s">
+        <v>1898</v>
+      </c>
+      <c r="C4" s="96" t="s">
+        <v>1899</v>
+      </c>
+      <c r="D4" s="97">
+        <v>0</v>
+      </c>
+      <c r="E4" s="98"/>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="95"/>
+      <c r="C5" s="96" t="s">
+        <v>1900</v>
+      </c>
+      <c r="D5" s="99">
+        <v>0</v>
+      </c>
+      <c r="E5" s="100"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="95"/>
+      <c r="C6" s="96" t="s">
+        <v>1901</v>
+      </c>
+      <c r="D6" s="101">
+        <v>1</v>
+      </c>
+      <c r="E6" s="100"/>
+    </row>
+    <row r="7" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="102"/>
+      <c r="C7" s="103" t="s">
+        <v>1902</v>
+      </c>
+      <c r="D7" s="104">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E7" s="105"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="95" t="s">
+        <v>1903</v>
+      </c>
+      <c r="C8" s="96" t="s">
+        <v>1904</v>
+      </c>
+      <c r="D8" s="106">
+        <v>1</v>
+      </c>
+      <c r="E8" s="98"/>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="95"/>
+      <c r="C9" s="96" t="s">
+        <v>1905</v>
+      </c>
+      <c r="D9" s="99">
+        <v>0</v>
+      </c>
+      <c r="E9" s="100"/>
+    </row>
+    <row r="10" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="102"/>
+      <c r="C10" s="103" t="s">
+        <v>1906</v>
+      </c>
+      <c r="D10" s="107">
+        <v>0</v>
+      </c>
+      <c r="E10" s="105"/>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="108" t="s">
+        <v>1907</v>
+      </c>
+      <c r="C11" s="109" t="s">
+        <v>1908</v>
+      </c>
+      <c r="D11" s="104">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E11" s="110" t="s">
+        <v>1909</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="B8:B10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Actualizacion de Avances en modulos migrados
</commit_message>
<xml_diff>
--- a/00-Documentacion/Listado de reportes totales-TI.xlsx
+++ b/00-Documentacion/Listado de reportes totales-TI.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D170E1-38E5-491A-A452-79742EBD9E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A57653-D882-43E1-859B-2E130F0298EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="834" activeTab="2" xr2:uid="{1498AA1A-1ACC-4329-A050-ACA05131B658}"/>
   </bookViews>
@@ -29,7 +29,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId8"/>
+    <pivotCache cacheId="1" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15972" uniqueCount="1930">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15974" uniqueCount="1930">
   <si>
     <t xml:space="preserve">Reporte </t>
   </si>
@@ -6546,7 +6546,17 @@
     <xf numFmtId="0" fontId="8" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -6558,10 +6568,7 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -6573,13 +6580,6 @@
     <xf numFmtId="0" fontId="17" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
@@ -11684,7 +11684,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{94ADBEE8-D536-427C-89A0-0A0A6F573128}" name="TablaDinámica2" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{94ADBEE8-D536-427C-89A0-0A0A6F573128}" name="TablaDinámica2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:A58" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="18">
     <pivotField showAll="0"/>
@@ -70580,9 +70580,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9585C0FF-65C5-4BD8-9936-5C9A63F7E604}">
   <dimension ref="A1:CP43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -70672,108 +70672,108 @@
     <row r="1" spans="1:94" x14ac:dyDescent="0.25">
       <c r="B1" s="64"/>
       <c r="M1" s="64"/>
-      <c r="S1" s="110">
+      <c r="S1" s="111">
         <v>45536</v>
       </c>
-      <c r="T1" s="111"/>
-      <c r="U1" s="111"/>
-      <c r="V1" s="111"/>
-      <c r="W1" s="110">
+      <c r="T1" s="112"/>
+      <c r="U1" s="112"/>
+      <c r="V1" s="112"/>
+      <c r="W1" s="111">
         <v>45566</v>
       </c>
-      <c r="X1" s="110"/>
-      <c r="Y1" s="110"/>
-      <c r="Z1" s="110"/>
-      <c r="AA1" s="110"/>
-      <c r="AB1" s="107">
+      <c r="X1" s="111"/>
+      <c r="Y1" s="111"/>
+      <c r="Z1" s="111"/>
+      <c r="AA1" s="111"/>
+      <c r="AB1" s="113">
         <v>45597</v>
       </c>
-      <c r="AC1" s="108"/>
-      <c r="AD1" s="108"/>
-      <c r="AE1" s="109"/>
-      <c r="AF1" s="107">
+      <c r="AC1" s="114"/>
+      <c r="AD1" s="114"/>
+      <c r="AE1" s="115"/>
+      <c r="AF1" s="113">
         <v>45627</v>
       </c>
-      <c r="AG1" s="108"/>
-      <c r="AH1" s="108"/>
-      <c r="AI1" s="109"/>
-      <c r="AJ1" s="107">
+      <c r="AG1" s="114"/>
+      <c r="AH1" s="114"/>
+      <c r="AI1" s="115"/>
+      <c r="AJ1" s="113">
         <v>45658</v>
       </c>
-      <c r="AK1" s="108"/>
-      <c r="AL1" s="108"/>
-      <c r="AM1" s="108"/>
-      <c r="AN1" s="109"/>
-      <c r="AO1" s="107">
+      <c r="AK1" s="114"/>
+      <c r="AL1" s="114"/>
+      <c r="AM1" s="114"/>
+      <c r="AN1" s="115"/>
+      <c r="AO1" s="113">
         <v>45689</v>
       </c>
-      <c r="AP1" s="108"/>
-      <c r="AQ1" s="108"/>
-      <c r="AR1" s="109"/>
-      <c r="AS1" s="107">
+      <c r="AP1" s="114"/>
+      <c r="AQ1" s="114"/>
+      <c r="AR1" s="115"/>
+      <c r="AS1" s="113">
         <v>45717</v>
       </c>
-      <c r="AT1" s="108"/>
-      <c r="AU1" s="108"/>
-      <c r="AV1" s="109"/>
-      <c r="AW1" s="107">
+      <c r="AT1" s="114"/>
+      <c r="AU1" s="114"/>
+      <c r="AV1" s="115"/>
+      <c r="AW1" s="113">
         <v>45748</v>
       </c>
-      <c r="AX1" s="108"/>
-      <c r="AY1" s="108"/>
-      <c r="AZ1" s="109"/>
-      <c r="BA1" s="107">
+      <c r="AX1" s="114"/>
+      <c r="AY1" s="114"/>
+      <c r="AZ1" s="115"/>
+      <c r="BA1" s="113">
         <v>45778</v>
       </c>
-      <c r="BB1" s="108"/>
-      <c r="BC1" s="108"/>
-      <c r="BD1" s="108"/>
-      <c r="BE1" s="109"/>
-      <c r="BF1" s="107">
+      <c r="BB1" s="114"/>
+      <c r="BC1" s="114"/>
+      <c r="BD1" s="114"/>
+      <c r="BE1" s="115"/>
+      <c r="BF1" s="113">
         <v>45809</v>
       </c>
-      <c r="BG1" s="108"/>
-      <c r="BH1" s="108"/>
-      <c r="BI1" s="108"/>
-      <c r="BJ1" s="107">
+      <c r="BG1" s="114"/>
+      <c r="BH1" s="114"/>
+      <c r="BI1" s="114"/>
+      <c r="BJ1" s="113">
         <v>45839</v>
       </c>
-      <c r="BK1" s="108"/>
-      <c r="BL1" s="108"/>
-      <c r="BM1" s="108"/>
-      <c r="BN1" s="109"/>
-      <c r="BO1" s="107">
+      <c r="BK1" s="114"/>
+      <c r="BL1" s="114"/>
+      <c r="BM1" s="114"/>
+      <c r="BN1" s="115"/>
+      <c r="BO1" s="113">
         <v>45870</v>
       </c>
-      <c r="BP1" s="108"/>
-      <c r="BQ1" s="108"/>
-      <c r="BR1" s="108"/>
-      <c r="BS1" s="107">
+      <c r="BP1" s="114"/>
+      <c r="BQ1" s="114"/>
+      <c r="BR1" s="114"/>
+      <c r="BS1" s="113">
         <v>45901</v>
       </c>
-      <c r="BT1" s="108"/>
-      <c r="BU1" s="108"/>
-      <c r="BV1" s="108"/>
-      <c r="BW1" s="107">
+      <c r="BT1" s="114"/>
+      <c r="BU1" s="114"/>
+      <c r="BV1" s="114"/>
+      <c r="BW1" s="113">
         <v>45931</v>
       </c>
-      <c r="BX1" s="108"/>
-      <c r="BY1" s="108"/>
-      <c r="BZ1" s="108"/>
-      <c r="CB1" s="107">
+      <c r="BX1" s="114"/>
+      <c r="BY1" s="114"/>
+      <c r="BZ1" s="114"/>
+      <c r="CB1" s="113">
         <v>45962</v>
       </c>
-      <c r="CC1" s="108"/>
-      <c r="CD1" s="108"/>
-      <c r="CE1" s="108"/>
-      <c r="CF1" s="106" t="s">
+      <c r="CC1" s="114"/>
+      <c r="CD1" s="114"/>
+      <c r="CE1" s="114"/>
+      <c r="CF1" s="116" t="s">
         <v>1853</v>
       </c>
-      <c r="CG1" s="106"/>
-      <c r="CK1" s="106" t="s">
+      <c r="CG1" s="116"/>
+      <c r="CK1" s="116" t="s">
         <v>1890</v>
       </c>
-      <c r="CL1" s="106"/>
+      <c r="CL1" s="116"/>
     </row>
     <row r="2" spans="1:94" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
@@ -71993,7 +71993,9 @@
         <v>14</v>
       </c>
       <c r="O10" s="12"/>
-      <c r="P10" s="12"/>
+      <c r="P10" s="12" t="s">
+        <v>1858</v>
+      </c>
       <c r="Q10" s="50">
         <v>45701</v>
       </c>
@@ -72089,7 +72091,7 @@
       <c r="E11" s="19" t="s">
         <v>1760</v>
       </c>
-      <c r="F11" s="118" t="s">
+      <c r="F11" s="109" t="s">
         <v>1761</v>
       </c>
       <c r="G11" s="12" t="s">
@@ -72248,7 +72250,7 @@
       <c r="V12" s="12"/>
       <c r="W12" s="12"/>
       <c r="X12" s="12"/>
-      <c r="Y12" s="115"/>
+      <c r="Y12" s="106"/>
       <c r="Z12" s="12"/>
       <c r="AA12" s="12"/>
       <c r="AB12" s="12"/>
@@ -72360,7 +72362,7 @@
       <c r="T13" s="65"/>
       <c r="U13" s="65"/>
       <c r="V13" s="65"/>
-      <c r="W13" s="116"/>
+      <c r="W13" s="107"/>
       <c r="X13" s="65"/>
       <c r="Y13" s="65"/>
       <c r="Z13" s="65"/>
@@ -72666,12 +72668,12 @@
       <c r="CF15" s="12"/>
       <c r="CG15" s="12"/>
       <c r="CH15" s="12"/>
-      <c r="CI15" s="115"/>
+      <c r="CI15" s="106"/>
       <c r="CJ15" s="12"/>
       <c r="CK15" s="12"/>
       <c r="CL15" s="12"/>
       <c r="CM15" s="12"/>
-      <c r="CN15" s="119"/>
+      <c r="CN15" s="110"/>
       <c r="CO15" s="71"/>
       <c r="CP15" s="71"/>
     </row>
@@ -73380,10 +73382,10 @@
       <c r="BO21" s="12"/>
       <c r="BP21" s="12"/>
       <c r="BQ21" s="12"/>
-      <c r="BR21" s="115"/>
-      <c r="BS21" s="115"/>
-      <c r="BT21" s="115"/>
-      <c r="BU21" s="115"/>
+      <c r="BR21" s="106"/>
+      <c r="BS21" s="106"/>
+      <c r="BT21" s="106"/>
+      <c r="BU21" s="106"/>
       <c r="BV21" s="12"/>
       <c r="BW21" s="12"/>
       <c r="BX21" s="12"/>
@@ -73452,7 +73454,7 @@
       <c r="AA22" s="12"/>
       <c r="AB22" s="12"/>
       <c r="AC22" s="12"/>
-      <c r="AD22" s="115"/>
+      <c r="AD22" s="106"/>
       <c r="AE22" s="12"/>
       <c r="AF22" s="12"/>
       <c r="AG22" s="12"/>
@@ -73480,10 +73482,10 @@
       <c r="BC22" s="12"/>
       <c r="BD22" s="12"/>
       <c r="BE22" s="12"/>
-      <c r="BF22" s="115"/>
-      <c r="BG22" s="115"/>
-      <c r="BH22" s="115"/>
-      <c r="BI22" s="115"/>
+      <c r="BF22" s="106"/>
+      <c r="BG22" s="106"/>
+      <c r="BH22" s="106"/>
+      <c r="BI22" s="106"/>
       <c r="BJ22" s="12"/>
       <c r="BK22" s="12"/>
       <c r="BL22" s="12"/>
@@ -73583,7 +73585,7 @@
       <c r="AL23" s="12"/>
       <c r="AM23" s="12"/>
       <c r="AN23" s="12"/>
-      <c r="AO23" s="115"/>
+      <c r="AO23" s="106"/>
       <c r="AP23" s="12"/>
       <c r="AQ23" s="12"/>
       <c r="AR23" s="12"/>
@@ -73616,10 +73618,10 @@
       <c r="BS23" s="12"/>
       <c r="BT23" s="12"/>
       <c r="BU23" s="12"/>
-      <c r="BV23" s="115"/>
-      <c r="BW23" s="115"/>
-      <c r="BX23" s="115"/>
-      <c r="BY23" s="115"/>
+      <c r="BV23" s="106"/>
+      <c r="BW23" s="106"/>
+      <c r="BX23" s="106"/>
+      <c r="BY23" s="106"/>
       <c r="BZ23" s="12"/>
       <c r="CA23" s="12"/>
       <c r="CB23" s="12"/>
@@ -73698,7 +73700,7 @@
       <c r="AF24" s="12"/>
       <c r="AG24" s="12"/>
       <c r="AH24" s="12"/>
-      <c r="AI24" s="115"/>
+      <c r="AI24" s="106"/>
       <c r="AJ24" s="12"/>
       <c r="AK24" s="12"/>
       <c r="AL24" s="12"/>
@@ -73713,14 +73715,14 @@
       <c r="AU24" s="12"/>
       <c r="AV24" s="12"/>
       <c r="AW24" s="12"/>
-      <c r="AX24" s="115"/>
-      <c r="AY24" s="115"/>
-      <c r="AZ24" s="115"/>
+      <c r="AX24" s="106"/>
+      <c r="AY24" s="106"/>
+      <c r="AZ24" s="106"/>
       <c r="BA24" s="48"/>
       <c r="BB24" s="48"/>
-      <c r="BC24" s="117"/>
-      <c r="BD24" s="117"/>
-      <c r="BE24" s="115"/>
+      <c r="BC24" s="108"/>
+      <c r="BD24" s="108"/>
+      <c r="BE24" s="106"/>
       <c r="BF24" s="12"/>
       <c r="BG24" s="12"/>
       <c r="BH24" s="12"/>
@@ -73745,11 +73747,11 @@
       <c r="CA24" s="12"/>
       <c r="CB24" s="12"/>
       <c r="CC24" s="12"/>
-      <c r="CD24" s="115"/>
-      <c r="CE24" s="115"/>
-      <c r="CF24" s="115"/>
-      <c r="CG24" s="115"/>
-      <c r="CH24" s="115"/>
+      <c r="CD24" s="106"/>
+      <c r="CE24" s="106"/>
+      <c r="CF24" s="106"/>
+      <c r="CG24" s="106"/>
+      <c r="CH24" s="106"/>
       <c r="CI24" s="12"/>
       <c r="CJ24" s="12"/>
       <c r="CK24" s="12"/>
@@ -73831,22 +73833,22 @@
       <c r="AS25" s="12"/>
       <c r="AT25" s="12"/>
       <c r="AU25" s="12"/>
-      <c r="AV25" s="115"/>
-      <c r="AW25" s="115"/>
-      <c r="AX25" s="115"/>
-      <c r="AY25" s="115"/>
+      <c r="AV25" s="106"/>
+      <c r="AW25" s="106"/>
+      <c r="AX25" s="106"/>
+      <c r="AY25" s="106"/>
       <c r="AZ25" s="12"/>
       <c r="BA25" s="12"/>
       <c r="BB25" s="12"/>
       <c r="BC25" s="12"/>
       <c r="BD25" s="12"/>
       <c r="BE25" s="12"/>
-      <c r="BF25" s="115"/>
-      <c r="BG25" s="115"/>
-      <c r="BH25" s="115"/>
-      <c r="BI25" s="115"/>
+      <c r="BF25" s="106"/>
+      <c r="BG25" s="106"/>
+      <c r="BH25" s="106"/>
+      <c r="BI25" s="106"/>
       <c r="BJ25" s="12"/>
-      <c r="BK25" s="115"/>
+      <c r="BK25" s="106"/>
       <c r="BL25" s="12"/>
       <c r="BM25" s="12"/>
       <c r="BN25" s="12"/>
@@ -73959,22 +73961,22 @@
       <c r="AZ26" s="12"/>
       <c r="BA26" s="12"/>
       <c r="BB26" s="12"/>
-      <c r="BC26" s="115"/>
-      <c r="BD26" s="115"/>
-      <c r="BE26" s="115"/>
-      <c r="BF26" s="115"/>
-      <c r="BG26" s="115"/>
-      <c r="BH26" s="115"/>
+      <c r="BC26" s="106"/>
+      <c r="BD26" s="106"/>
+      <c r="BE26" s="106"/>
+      <c r="BF26" s="106"/>
+      <c r="BG26" s="106"/>
+      <c r="BH26" s="106"/>
       <c r="BI26" s="12"/>
-      <c r="BJ26" s="115"/>
-      <c r="BK26" s="115"/>
-      <c r="BL26" s="115"/>
-      <c r="BM26" s="115"/>
+      <c r="BJ26" s="106"/>
+      <c r="BK26" s="106"/>
+      <c r="BL26" s="106"/>
+      <c r="BM26" s="106"/>
       <c r="BN26" s="12"/>
       <c r="BO26" s="12"/>
       <c r="BP26" s="12"/>
       <c r="BQ26" s="12"/>
-      <c r="BR26" s="115"/>
+      <c r="BR26" s="106"/>
       <c r="BS26" s="12"/>
       <c r="BT26" s="12"/>
       <c r="BU26" s="12"/>
@@ -74068,7 +74070,7 @@
       <c r="AM27" s="12"/>
       <c r="AN27" s="12"/>
       <c r="AO27" s="12"/>
-      <c r="AP27" s="115"/>
+      <c r="AP27" s="106"/>
       <c r="AQ27" s="12"/>
       <c r="AR27" s="12"/>
       <c r="AS27" s="12"/>
@@ -74078,30 +74080,30 @@
       <c r="AW27" s="12"/>
       <c r="AX27" s="12"/>
       <c r="AY27" s="12"/>
-      <c r="AZ27" s="115"/>
-      <c r="BA27" s="115"/>
-      <c r="BB27" s="115"/>
+      <c r="AZ27" s="106"/>
+      <c r="BA27" s="106"/>
+      <c r="BB27" s="106"/>
       <c r="BC27" s="12"/>
       <c r="BD27" s="12"/>
       <c r="BE27" s="12"/>
       <c r="BF27" s="12"/>
       <c r="BG27" s="12"/>
       <c r="BH27" s="12"/>
-      <c r="BI27" s="115"/>
-      <c r="BJ27" s="115"/>
-      <c r="BK27" s="115"/>
+      <c r="BI27" s="106"/>
+      <c r="BJ27" s="106"/>
+      <c r="BK27" s="106"/>
       <c r="BL27" s="12"/>
       <c r="BM27" s="12"/>
       <c r="BN27" s="12"/>
       <c r="BO27" s="12"/>
       <c r="BP27" s="12"/>
       <c r="BQ27" s="12"/>
-      <c r="BR27" s="115"/>
+      <c r="BR27" s="106"/>
       <c r="BS27" s="12"/>
       <c r="BT27" s="12"/>
       <c r="BU27" s="12"/>
-      <c r="BV27" s="115"/>
-      <c r="BW27" s="115"/>
+      <c r="BV27" s="106"/>
+      <c r="BW27" s="106"/>
       <c r="BX27" s="12"/>
       <c r="BY27" s="12"/>
       <c r="BZ27" s="12"/>
@@ -74213,9 +74215,9 @@
       <c r="BL28" s="12"/>
       <c r="BM28" s="12"/>
       <c r="BN28" s="12"/>
-      <c r="BO28" s="115"/>
-      <c r="BP28" s="115"/>
-      <c r="BQ28" s="115"/>
+      <c r="BO28" s="106"/>
+      <c r="BP28" s="106"/>
+      <c r="BQ28" s="106"/>
       <c r="BR28" s="12"/>
       <c r="BS28" s="12"/>
       <c r="BT28" s="12"/>
@@ -74223,10 +74225,10 @@
       <c r="BV28" s="12"/>
       <c r="BW28" s="12"/>
       <c r="BX28" s="12"/>
-      <c r="BY28" s="115"/>
+      <c r="BY28" s="106"/>
       <c r="BZ28" s="12"/>
       <c r="CA28" s="12"/>
-      <c r="CB28" s="115"/>
+      <c r="CB28" s="106"/>
       <c r="CC28" s="12"/>
       <c r="CD28" s="12"/>
       <c r="CE28" s="12"/>
@@ -74310,10 +74312,10 @@
       <c r="AO29" s="12"/>
       <c r="AP29" s="12"/>
       <c r="AQ29" s="12"/>
-      <c r="AR29" s="115"/>
-      <c r="AS29" s="115"/>
-      <c r="AT29" s="115"/>
-      <c r="AU29" s="115"/>
+      <c r="AR29" s="106"/>
+      <c r="AS29" s="106"/>
+      <c r="AT29" s="106"/>
+      <c r="AU29" s="106"/>
       <c r="AV29" s="12"/>
       <c r="AW29" s="12"/>
       <c r="AX29" s="12"/>
@@ -74325,7 +74327,7 @@
       <c r="BD29" s="12"/>
       <c r="BE29" s="12"/>
       <c r="BF29" s="12"/>
-      <c r="BG29" s="115"/>
+      <c r="BG29" s="106"/>
       <c r="BH29" s="12"/>
       <c r="BI29" s="12"/>
       <c r="BJ29" s="12"/>
@@ -74346,7 +74348,7 @@
       <c r="BY29" s="12"/>
       <c r="BZ29" s="12"/>
       <c r="CA29" s="12"/>
-      <c r="CB29" s="115"/>
+      <c r="CB29" s="106"/>
       <c r="CC29" s="12"/>
       <c r="CD29" s="12"/>
       <c r="CE29" s="12"/>
@@ -74441,9 +74443,9 @@
       <c r="AZ30" s="12"/>
       <c r="BA30" s="12"/>
       <c r="BB30" s="12"/>
-      <c r="BC30" s="115"/>
-      <c r="BD30" s="115"/>
-      <c r="BE30" s="115"/>
+      <c r="BC30" s="106"/>
+      <c r="BD30" s="106"/>
+      <c r="BE30" s="106"/>
       <c r="BF30" s="12"/>
       <c r="BG30" s="12"/>
       <c r="BH30" s="12"/>
@@ -74462,15 +74464,15 @@
       <c r="BU30" s="12"/>
       <c r="BV30" s="12"/>
       <c r="BW30" s="12"/>
-      <c r="BX30" s="115"/>
-      <c r="BY30" s="115"/>
+      <c r="BX30" s="106"/>
+      <c r="BY30" s="106"/>
       <c r="BZ30" s="12"/>
       <c r="CA30" s="12"/>
       <c r="CB30" s="12"/>
       <c r="CC30" s="12"/>
       <c r="CD30" s="12"/>
       <c r="CE30" s="12"/>
-      <c r="CF30" s="115"/>
+      <c r="CF30" s="106"/>
       <c r="CG30" s="12"/>
       <c r="CH30" s="12"/>
       <c r="CI30" s="12"/>
@@ -74579,20 +74581,20 @@
       <c r="BT31" s="12"/>
       <c r="BU31" s="12"/>
       <c r="BV31" s="12"/>
-      <c r="BW31" s="115"/>
-      <c r="BX31" s="115"/>
-      <c r="BY31" s="115"/>
-      <c r="BZ31" s="115"/>
-      <c r="CA31" s="115"/>
-      <c r="CB31" s="115"/>
-      <c r="CC31" s="115"/>
+      <c r="BW31" s="106"/>
+      <c r="BX31" s="106"/>
+      <c r="BY31" s="106"/>
+      <c r="BZ31" s="106"/>
+      <c r="CA31" s="106"/>
+      <c r="CB31" s="106"/>
+      <c r="CC31" s="106"/>
       <c r="CD31" s="12"/>
       <c r="CE31" s="12"/>
       <c r="CF31" s="12"/>
       <c r="CG31" s="12"/>
       <c r="CH31" s="12"/>
-      <c r="CI31" s="115"/>
-      <c r="CJ31" s="115"/>
+      <c r="CI31" s="106"/>
+      <c r="CJ31" s="106"/>
       <c r="CK31" s="12"/>
       <c r="CL31" s="12"/>
       <c r="CM31" s="12"/>
@@ -74632,7 +74634,9 @@
       <c r="O32" s="49" t="s">
         <v>1863</v>
       </c>
-      <c r="P32" s="49"/>
+      <c r="P32" s="49" t="s">
+        <v>1864</v>
+      </c>
       <c r="Q32" s="51">
         <v>45649</v>
       </c>
@@ -74707,10 +74711,10 @@
       <c r="CF32" s="12"/>
       <c r="CG32" s="12"/>
       <c r="CH32" s="12"/>
-      <c r="CI32" s="115"/>
-      <c r="CJ32" s="115"/>
-      <c r="CK32" s="115"/>
-      <c r="CL32" s="115"/>
+      <c r="CI32" s="106"/>
+      <c r="CJ32" s="106"/>
+      <c r="CK32" s="106"/>
+      <c r="CL32" s="106"/>
       <c r="CM32" s="12"/>
       <c r="CN32" s="12"/>
       <c r="CO32" s="48"/>
@@ -75769,11 +75773,6 @@
     </sortState>
   </autoFilter>
   <mergeCells count="17">
-    <mergeCell ref="S1:V1"/>
-    <mergeCell ref="W1:AA1"/>
-    <mergeCell ref="AB1:AE1"/>
-    <mergeCell ref="AF1:AI1"/>
-    <mergeCell ref="AJ1:AN1"/>
     <mergeCell ref="CK1:CL1"/>
     <mergeCell ref="AO1:AR1"/>
     <mergeCell ref="AS1:AV1"/>
@@ -75786,6 +75785,11 @@
     <mergeCell ref="BS1:BV1"/>
     <mergeCell ref="BW1:BZ1"/>
     <mergeCell ref="CB1:CE1"/>
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="W1:AA1"/>
+    <mergeCell ref="AB1:AE1"/>
+    <mergeCell ref="AF1:AI1"/>
+    <mergeCell ref="AJ1:AN1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -75915,12 +75919,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="112" t="s">
+      <c r="B1" s="117" t="s">
         <v>1892</v>
       </c>
-      <c r="C1" s="112"/>
-      <c r="D1" s="112"/>
-      <c r="E1" s="112"/>
+      <c r="C1" s="117"/>
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="72" t="s">
@@ -75937,7 +75941,7 @@
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="113" t="s">
+      <c r="B4" s="118" t="s">
         <v>1897</v>
       </c>
       <c r="C4" s="75" t="s">
@@ -75949,7 +75953,7 @@
       <c r="E4" s="77"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="113"/>
+      <c r="B5" s="118"/>
       <c r="C5" s="75" t="s">
         <v>1899</v>
       </c>
@@ -75959,7 +75963,7 @@
       <c r="E5" s="79"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="113"/>
+      <c r="B6" s="118"/>
       <c r="C6" s="75" t="s">
         <v>1900</v>
       </c>
@@ -75969,7 +75973,7 @@
       <c r="E6" s="79"/>
     </row>
     <row r="7" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="114"/>
+      <c r="B7" s="119"/>
       <c r="C7" s="81" t="s">
         <v>1901</v>
       </c>
@@ -75979,7 +75983,7 @@
       <c r="E7" s="83"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="113" t="s">
+      <c r="B8" s="118" t="s">
         <v>1902</v>
       </c>
       <c r="C8" s="75" t="s">
@@ -75991,7 +75995,7 @@
       <c r="E8" s="77"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="113"/>
+      <c r="B9" s="118"/>
       <c r="C9" s="75" t="s">
         <v>1904</v>
       </c>
@@ -76001,7 +76005,7 @@
       <c r="E9" s="79"/>
     </row>
     <row r="10" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="114"/>
+      <c r="B10" s="119"/>
       <c r="C10" s="81" t="s">
         <v>1905</v>
       </c>

</xml_diff>

<commit_message>
actualizacion del plan de trabajo
</commit_message>
<xml_diff>
--- a/00-Documentacion/Listado de reportes totales-TI.xlsx
+++ b/00-Documentacion/Listado de reportes totales-TI.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\pc\raul\Net\migracion_spooler\00-Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repositorios\migracion_spooler\00-Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A57653-D882-43E1-859B-2E130F0298EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22D180C-1D6E-4D8E-A205-293679507CB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="834" activeTab="2" xr2:uid="{1498AA1A-1ACC-4329-A050-ACA05131B658}"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="834" activeTab="2" xr2:uid="{1498AA1A-1ACC-4329-A050-ACA05131B658}"/>
   </bookViews>
   <sheets>
     <sheet name="General - Analisis" sheetId="4" r:id="rId1"/>
@@ -29,7 +29,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId8"/>
+    <pivotCache cacheId="0" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -6313,7 +6313,7 @@
     <xf numFmtId="9" fontId="16" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6546,17 +6546,12 @@
     <xf numFmtId="0" fontId="8" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -6568,7 +6563,10 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -11684,7 +11682,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{94ADBEE8-D536-427C-89A0-0A0A6F573128}" name="TablaDinámica2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{94ADBEE8-D536-427C-89A0-0A0A6F573128}" name="TablaDinámica2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:A58" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="18">
     <pivotField showAll="0"/>
@@ -70580,9 +70578,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9585C0FF-65C5-4BD8-9936-5C9A63F7E604}">
   <dimension ref="A1:CP43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P10" sqref="P10"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -70672,108 +70670,108 @@
     <row r="1" spans="1:94" x14ac:dyDescent="0.25">
       <c r="B1" s="64"/>
       <c r="M1" s="64"/>
-      <c r="S1" s="111">
+      <c r="S1" s="113">
         <v>45536</v>
       </c>
-      <c r="T1" s="112"/>
-      <c r="U1" s="112"/>
-      <c r="V1" s="112"/>
-      <c r="W1" s="111">
+      <c r="T1" s="114"/>
+      <c r="U1" s="114"/>
+      <c r="V1" s="114"/>
+      <c r="W1" s="113">
         <v>45566</v>
       </c>
-      <c r="X1" s="111"/>
-      <c r="Y1" s="111"/>
-      <c r="Z1" s="111"/>
-      <c r="AA1" s="111"/>
-      <c r="AB1" s="113">
+      <c r="X1" s="113"/>
+      <c r="Y1" s="113"/>
+      <c r="Z1" s="113"/>
+      <c r="AA1" s="113"/>
+      <c r="AB1" s="110">
         <v>45597</v>
       </c>
-      <c r="AC1" s="114"/>
-      <c r="AD1" s="114"/>
-      <c r="AE1" s="115"/>
-      <c r="AF1" s="113">
+      <c r="AC1" s="111"/>
+      <c r="AD1" s="111"/>
+      <c r="AE1" s="112"/>
+      <c r="AF1" s="110">
         <v>45627</v>
       </c>
-      <c r="AG1" s="114"/>
-      <c r="AH1" s="114"/>
-      <c r="AI1" s="115"/>
-      <c r="AJ1" s="113">
+      <c r="AG1" s="111"/>
+      <c r="AH1" s="111"/>
+      <c r="AI1" s="112"/>
+      <c r="AJ1" s="110">
         <v>45658</v>
       </c>
-      <c r="AK1" s="114"/>
-      <c r="AL1" s="114"/>
-      <c r="AM1" s="114"/>
-      <c r="AN1" s="115"/>
-      <c r="AO1" s="113">
+      <c r="AK1" s="111"/>
+      <c r="AL1" s="111"/>
+      <c r="AM1" s="111"/>
+      <c r="AN1" s="112"/>
+      <c r="AO1" s="110">
         <v>45689</v>
       </c>
-      <c r="AP1" s="114"/>
-      <c r="AQ1" s="114"/>
-      <c r="AR1" s="115"/>
-      <c r="AS1" s="113">
+      <c r="AP1" s="111"/>
+      <c r="AQ1" s="111"/>
+      <c r="AR1" s="112"/>
+      <c r="AS1" s="110">
         <v>45717</v>
       </c>
-      <c r="AT1" s="114"/>
-      <c r="AU1" s="114"/>
-      <c r="AV1" s="115"/>
-      <c r="AW1" s="113">
+      <c r="AT1" s="111"/>
+      <c r="AU1" s="111"/>
+      <c r="AV1" s="112"/>
+      <c r="AW1" s="110">
         <v>45748</v>
       </c>
-      <c r="AX1" s="114"/>
-      <c r="AY1" s="114"/>
-      <c r="AZ1" s="115"/>
-      <c r="BA1" s="113">
+      <c r="AX1" s="111"/>
+      <c r="AY1" s="111"/>
+      <c r="AZ1" s="112"/>
+      <c r="BA1" s="110">
         <v>45778</v>
       </c>
-      <c r="BB1" s="114"/>
-      <c r="BC1" s="114"/>
-      <c r="BD1" s="114"/>
-      <c r="BE1" s="115"/>
-      <c r="BF1" s="113">
+      <c r="BB1" s="111"/>
+      <c r="BC1" s="111"/>
+      <c r="BD1" s="111"/>
+      <c r="BE1" s="112"/>
+      <c r="BF1" s="110">
         <v>45809</v>
       </c>
-      <c r="BG1" s="114"/>
-      <c r="BH1" s="114"/>
-      <c r="BI1" s="114"/>
-      <c r="BJ1" s="113">
+      <c r="BG1" s="111"/>
+      <c r="BH1" s="111"/>
+      <c r="BI1" s="111"/>
+      <c r="BJ1" s="110">
         <v>45839</v>
       </c>
-      <c r="BK1" s="114"/>
-      <c r="BL1" s="114"/>
-      <c r="BM1" s="114"/>
-      <c r="BN1" s="115"/>
-      <c r="BO1" s="113">
+      <c r="BK1" s="111"/>
+      <c r="BL1" s="111"/>
+      <c r="BM1" s="111"/>
+      <c r="BN1" s="112"/>
+      <c r="BO1" s="110">
         <v>45870</v>
       </c>
-      <c r="BP1" s="114"/>
-      <c r="BQ1" s="114"/>
-      <c r="BR1" s="114"/>
-      <c r="BS1" s="113">
+      <c r="BP1" s="111"/>
+      <c r="BQ1" s="111"/>
+      <c r="BR1" s="111"/>
+      <c r="BS1" s="110">
         <v>45901</v>
       </c>
-      <c r="BT1" s="114"/>
-      <c r="BU1" s="114"/>
-      <c r="BV1" s="114"/>
-      <c r="BW1" s="113">
+      <c r="BT1" s="111"/>
+      <c r="BU1" s="111"/>
+      <c r="BV1" s="111"/>
+      <c r="BW1" s="110">
         <v>45931</v>
       </c>
-      <c r="BX1" s="114"/>
-      <c r="BY1" s="114"/>
-      <c r="BZ1" s="114"/>
-      <c r="CB1" s="113">
+      <c r="BX1" s="111"/>
+      <c r="BY1" s="111"/>
+      <c r="BZ1" s="111"/>
+      <c r="CB1" s="110">
         <v>45962</v>
       </c>
-      <c r="CC1" s="114"/>
-      <c r="CD1" s="114"/>
-      <c r="CE1" s="114"/>
-      <c r="CF1" s="116" t="s">
+      <c r="CC1" s="111"/>
+      <c r="CD1" s="111"/>
+      <c r="CE1" s="111"/>
+      <c r="CF1" s="109" t="s">
         <v>1853</v>
       </c>
-      <c r="CG1" s="116"/>
-      <c r="CK1" s="116" t="s">
+      <c r="CG1" s="109"/>
+      <c r="CK1" s="109" t="s">
         <v>1890</v>
       </c>
-      <c r="CL1" s="116"/>
+      <c r="CL1" s="109"/>
     </row>
     <row r="2" spans="1:94" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
@@ -72091,7 +72089,7 @@
       <c r="E11" s="19" t="s">
         <v>1760</v>
       </c>
-      <c r="F11" s="109" t="s">
+      <c r="F11" s="107" t="s">
         <v>1761</v>
       </c>
       <c r="G11" s="12" t="s">
@@ -72250,7 +72248,6 @@
       <c r="V12" s="12"/>
       <c r="W12" s="12"/>
       <c r="X12" s="12"/>
-      <c r="Y12" s="106"/>
       <c r="Z12" s="12"/>
       <c r="AA12" s="12"/>
       <c r="AB12" s="12"/>
@@ -72362,7 +72359,7 @@
       <c r="T13" s="65"/>
       <c r="U13" s="65"/>
       <c r="V13" s="65"/>
-      <c r="W13" s="107"/>
+      <c r="W13" s="71"/>
       <c r="X13" s="65"/>
       <c r="Y13" s="65"/>
       <c r="Z13" s="65"/>
@@ -72668,12 +72665,11 @@
       <c r="CF15" s="12"/>
       <c r="CG15" s="12"/>
       <c r="CH15" s="12"/>
-      <c r="CI15" s="106"/>
       <c r="CJ15" s="12"/>
       <c r="CK15" s="12"/>
       <c r="CL15" s="12"/>
       <c r="CM15" s="12"/>
-      <c r="CN15" s="110"/>
+      <c r="CN15" s="108"/>
       <c r="CO15" s="71"/>
       <c r="CP15" s="71"/>
     </row>
@@ -73382,10 +73378,6 @@
       <c r="BO21" s="12"/>
       <c r="BP21" s="12"/>
       <c r="BQ21" s="12"/>
-      <c r="BR21" s="106"/>
-      <c r="BS21" s="106"/>
-      <c r="BT21" s="106"/>
-      <c r="BU21" s="106"/>
       <c r="BV21" s="12"/>
       <c r="BW21" s="12"/>
       <c r="BX21" s="12"/>
@@ -73454,7 +73446,6 @@
       <c r="AA22" s="12"/>
       <c r="AB22" s="12"/>
       <c r="AC22" s="12"/>
-      <c r="AD22" s="106"/>
       <c r="AE22" s="12"/>
       <c r="AF22" s="12"/>
       <c r="AG22" s="12"/>
@@ -73482,10 +73473,6 @@
       <c r="BC22" s="12"/>
       <c r="BD22" s="12"/>
       <c r="BE22" s="12"/>
-      <c r="BF22" s="106"/>
-      <c r="BG22" s="106"/>
-      <c r="BH22" s="106"/>
-      <c r="BI22" s="106"/>
       <c r="BJ22" s="12"/>
       <c r="BK22" s="12"/>
       <c r="BL22" s="12"/>
@@ -73585,7 +73572,6 @@
       <c r="AL23" s="12"/>
       <c r="AM23" s="12"/>
       <c r="AN23" s="12"/>
-      <c r="AO23" s="106"/>
       <c r="AP23" s="12"/>
       <c r="AQ23" s="12"/>
       <c r="AR23" s="12"/>
@@ -73618,10 +73604,6 @@
       <c r="BS23" s="12"/>
       <c r="BT23" s="12"/>
       <c r="BU23" s="12"/>
-      <c r="BV23" s="106"/>
-      <c r="BW23" s="106"/>
-      <c r="BX23" s="106"/>
-      <c r="BY23" s="106"/>
       <c r="BZ23" s="12"/>
       <c r="CA23" s="12"/>
       <c r="CB23" s="12"/>
@@ -73700,7 +73682,6 @@
       <c r="AF24" s="12"/>
       <c r="AG24" s="12"/>
       <c r="AH24" s="12"/>
-      <c r="AI24" s="106"/>
       <c r="AJ24" s="12"/>
       <c r="AK24" s="12"/>
       <c r="AL24" s="12"/>
@@ -73715,14 +73696,10 @@
       <c r="AU24" s="12"/>
       <c r="AV24" s="12"/>
       <c r="AW24" s="12"/>
-      <c r="AX24" s="106"/>
-      <c r="AY24" s="106"/>
-      <c r="AZ24" s="106"/>
       <c r="BA24" s="48"/>
       <c r="BB24" s="48"/>
-      <c r="BC24" s="108"/>
-      <c r="BD24" s="108"/>
-      <c r="BE24" s="106"/>
+      <c r="BC24" s="106"/>
+      <c r="BD24" s="106"/>
       <c r="BF24" s="12"/>
       <c r="BG24" s="12"/>
       <c r="BH24" s="12"/>
@@ -73747,11 +73724,6 @@
       <c r="CA24" s="12"/>
       <c r="CB24" s="12"/>
       <c r="CC24" s="12"/>
-      <c r="CD24" s="106"/>
-      <c r="CE24" s="106"/>
-      <c r="CF24" s="106"/>
-      <c r="CG24" s="106"/>
-      <c r="CH24" s="106"/>
       <c r="CI24" s="12"/>
       <c r="CJ24" s="12"/>
       <c r="CK24" s="12"/>
@@ -73833,22 +73805,13 @@
       <c r="AS25" s="12"/>
       <c r="AT25" s="12"/>
       <c r="AU25" s="12"/>
-      <c r="AV25" s="106"/>
-      <c r="AW25" s="106"/>
-      <c r="AX25" s="106"/>
-      <c r="AY25" s="106"/>
       <c r="AZ25" s="12"/>
       <c r="BA25" s="12"/>
       <c r="BB25" s="12"/>
       <c r="BC25" s="12"/>
       <c r="BD25" s="12"/>
       <c r="BE25" s="12"/>
-      <c r="BF25" s="106"/>
-      <c r="BG25" s="106"/>
-      <c r="BH25" s="106"/>
-      <c r="BI25" s="106"/>
       <c r="BJ25" s="12"/>
-      <c r="BK25" s="106"/>
       <c r="BL25" s="12"/>
       <c r="BM25" s="12"/>
       <c r="BN25" s="12"/>
@@ -73961,22 +73924,11 @@
       <c r="AZ26" s="12"/>
       <c r="BA26" s="12"/>
       <c r="BB26" s="12"/>
-      <c r="BC26" s="106"/>
-      <c r="BD26" s="106"/>
-      <c r="BE26" s="106"/>
-      <c r="BF26" s="106"/>
-      <c r="BG26" s="106"/>
-      <c r="BH26" s="106"/>
       <c r="BI26" s="12"/>
-      <c r="BJ26" s="106"/>
-      <c r="BK26" s="106"/>
-      <c r="BL26" s="106"/>
-      <c r="BM26" s="106"/>
       <c r="BN26" s="12"/>
       <c r="BO26" s="12"/>
       <c r="BP26" s="12"/>
       <c r="BQ26" s="12"/>
-      <c r="BR26" s="106"/>
       <c r="BS26" s="12"/>
       <c r="BT26" s="12"/>
       <c r="BU26" s="12"/>
@@ -74070,7 +74022,6 @@
       <c r="AM27" s="12"/>
       <c r="AN27" s="12"/>
       <c r="AO27" s="12"/>
-      <c r="AP27" s="106"/>
       <c r="AQ27" s="12"/>
       <c r="AR27" s="12"/>
       <c r="AS27" s="12"/>
@@ -74080,30 +74031,21 @@
       <c r="AW27" s="12"/>
       <c r="AX27" s="12"/>
       <c r="AY27" s="12"/>
-      <c r="AZ27" s="106"/>
-      <c r="BA27" s="106"/>
-      <c r="BB27" s="106"/>
       <c r="BC27" s="12"/>
       <c r="BD27" s="12"/>
       <c r="BE27" s="12"/>
       <c r="BF27" s="12"/>
       <c r="BG27" s="12"/>
       <c r="BH27" s="12"/>
-      <c r="BI27" s="106"/>
-      <c r="BJ27" s="106"/>
-      <c r="BK27" s="106"/>
       <c r="BL27" s="12"/>
       <c r="BM27" s="12"/>
       <c r="BN27" s="12"/>
       <c r="BO27" s="12"/>
       <c r="BP27" s="12"/>
       <c r="BQ27" s="12"/>
-      <c r="BR27" s="106"/>
       <c r="BS27" s="12"/>
       <c r="BT27" s="12"/>
       <c r="BU27" s="12"/>
-      <c r="BV27" s="106"/>
-      <c r="BW27" s="106"/>
       <c r="BX27" s="12"/>
       <c r="BY27" s="12"/>
       <c r="BZ27" s="12"/>
@@ -74215,9 +74157,6 @@
       <c r="BL28" s="12"/>
       <c r="BM28" s="12"/>
       <c r="BN28" s="12"/>
-      <c r="BO28" s="106"/>
-      <c r="BP28" s="106"/>
-      <c r="BQ28" s="106"/>
       <c r="BR28" s="12"/>
       <c r="BS28" s="12"/>
       <c r="BT28" s="12"/>
@@ -74225,10 +74164,8 @@
       <c r="BV28" s="12"/>
       <c r="BW28" s="12"/>
       <c r="BX28" s="12"/>
-      <c r="BY28" s="106"/>
       <c r="BZ28" s="12"/>
       <c r="CA28" s="12"/>
-      <c r="CB28" s="106"/>
       <c r="CC28" s="12"/>
       <c r="CD28" s="12"/>
       <c r="CE28" s="12"/>
@@ -74312,10 +74249,6 @@
       <c r="AO29" s="12"/>
       <c r="AP29" s="12"/>
       <c r="AQ29" s="12"/>
-      <c r="AR29" s="106"/>
-      <c r="AS29" s="106"/>
-      <c r="AT29" s="106"/>
-      <c r="AU29" s="106"/>
       <c r="AV29" s="12"/>
       <c r="AW29" s="12"/>
       <c r="AX29" s="12"/>
@@ -74327,7 +74260,6 @@
       <c r="BD29" s="12"/>
       <c r="BE29" s="12"/>
       <c r="BF29" s="12"/>
-      <c r="BG29" s="106"/>
       <c r="BH29" s="12"/>
       <c r="BI29" s="12"/>
       <c r="BJ29" s="12"/>
@@ -74348,7 +74280,6 @@
       <c r="BY29" s="12"/>
       <c r="BZ29" s="12"/>
       <c r="CA29" s="12"/>
-      <c r="CB29" s="106"/>
       <c r="CC29" s="12"/>
       <c r="CD29" s="12"/>
       <c r="CE29" s="12"/>
@@ -74443,9 +74374,6 @@
       <c r="AZ30" s="12"/>
       <c r="BA30" s="12"/>
       <c r="BB30" s="12"/>
-      <c r="BC30" s="106"/>
-      <c r="BD30" s="106"/>
-      <c r="BE30" s="106"/>
       <c r="BF30" s="12"/>
       <c r="BG30" s="12"/>
       <c r="BH30" s="12"/>
@@ -74464,15 +74392,12 @@
       <c r="BU30" s="12"/>
       <c r="BV30" s="12"/>
       <c r="BW30" s="12"/>
-      <c r="BX30" s="106"/>
-      <c r="BY30" s="106"/>
       <c r="BZ30" s="12"/>
       <c r="CA30" s="12"/>
       <c r="CB30" s="12"/>
       <c r="CC30" s="12"/>
       <c r="CD30" s="12"/>
       <c r="CE30" s="12"/>
-      <c r="CF30" s="106"/>
       <c r="CG30" s="12"/>
       <c r="CH30" s="12"/>
       <c r="CI30" s="12"/>
@@ -74581,20 +74506,11 @@
       <c r="BT31" s="12"/>
       <c r="BU31" s="12"/>
       <c r="BV31" s="12"/>
-      <c r="BW31" s="106"/>
-      <c r="BX31" s="106"/>
-      <c r="BY31" s="106"/>
-      <c r="BZ31" s="106"/>
-      <c r="CA31" s="106"/>
-      <c r="CB31" s="106"/>
-      <c r="CC31" s="106"/>
       <c r="CD31" s="12"/>
       <c r="CE31" s="12"/>
       <c r="CF31" s="12"/>
       <c r="CG31" s="12"/>
       <c r="CH31" s="12"/>
-      <c r="CI31" s="106"/>
-      <c r="CJ31" s="106"/>
       <c r="CK31" s="12"/>
       <c r="CL31" s="12"/>
       <c r="CM31" s="12"/>
@@ -74711,10 +74627,6 @@
       <c r="CF32" s="12"/>
       <c r="CG32" s="12"/>
       <c r="CH32" s="12"/>
-      <c r="CI32" s="106"/>
-      <c r="CJ32" s="106"/>
-      <c r="CK32" s="106"/>
-      <c r="CL32" s="106"/>
       <c r="CM32" s="12"/>
       <c r="CN32" s="12"/>
       <c r="CO32" s="48"/>
@@ -75773,6 +75685,11 @@
     </sortState>
   </autoFilter>
   <mergeCells count="17">
+    <mergeCell ref="S1:V1"/>
+    <mergeCell ref="W1:AA1"/>
+    <mergeCell ref="AB1:AE1"/>
+    <mergeCell ref="AF1:AI1"/>
+    <mergeCell ref="AJ1:AN1"/>
     <mergeCell ref="CK1:CL1"/>
     <mergeCell ref="AO1:AR1"/>
     <mergeCell ref="AS1:AV1"/>
@@ -75785,11 +75702,6 @@
     <mergeCell ref="BS1:BV1"/>
     <mergeCell ref="BW1:BZ1"/>
     <mergeCell ref="CB1:CE1"/>
-    <mergeCell ref="S1:V1"/>
-    <mergeCell ref="W1:AA1"/>
-    <mergeCell ref="AB1:AE1"/>
-    <mergeCell ref="AF1:AI1"/>
-    <mergeCell ref="AJ1:AN1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -75919,12 +75831,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="117" t="s">
+      <c r="B1" s="115" t="s">
         <v>1892</v>
       </c>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="72" t="s">
@@ -75941,7 +75853,7 @@
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="118" t="s">
+      <c r="B4" s="116" t="s">
         <v>1897</v>
       </c>
       <c r="C4" s="75" t="s">
@@ -75953,7 +75865,7 @@
       <c r="E4" s="77"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="118"/>
+      <c r="B5" s="116"/>
       <c r="C5" s="75" t="s">
         <v>1899</v>
       </c>
@@ -75963,7 +75875,7 @@
       <c r="E5" s="79"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="118"/>
+      <c r="B6" s="116"/>
       <c r="C6" s="75" t="s">
         <v>1900</v>
       </c>
@@ -75973,7 +75885,7 @@
       <c r="E6" s="79"/>
     </row>
     <row r="7" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="119"/>
+      <c r="B7" s="117"/>
       <c r="C7" s="81" t="s">
         <v>1901</v>
       </c>
@@ -75983,7 +75895,7 @@
       <c r="E7" s="83"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="118" t="s">
+      <c r="B8" s="116" t="s">
         <v>1902</v>
       </c>
       <c r="C8" s="75" t="s">
@@ -75995,7 +75907,7 @@
       <c r="E8" s="77"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="118"/>
+      <c r="B9" s="116"/>
       <c r="C9" s="75" t="s">
         <v>1904</v>
       </c>
@@ -76005,7 +75917,7 @@
       <c r="E9" s="79"/>
     </row>
     <row r="10" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="119"/>
+      <c r="B10" s="117"/>
       <c r="C10" s="81" t="s">
         <v>1905</v>
       </c>

</xml_diff>